<commit_message>
Add test equipment calibration dates
</commit_message>
<xml_diff>
--- a/MUSCMammoMonitor.xlsx
+++ b/MUSCMammoMonitor.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="142">
   <si>
     <t>Print Area</t>
   </si>
@@ -438,6 +438,21 @@
   </si>
   <si>
     <t>Revision 1.3-20190606</t>
+  </si>
+  <si>
+    <t>Meter:</t>
+  </si>
+  <si>
+    <t>Calibration Due:</t>
+  </si>
+  <si>
+    <t>Calibration Date:</t>
+  </si>
+  <si>
+    <t>Radcal 9010</t>
+  </si>
+  <si>
+    <t>Test Equipment</t>
   </si>
 </sst>
 </file>
@@ -452,7 +467,7 @@
     <numFmt numFmtId="168" formatCode="0.0"/>
     <numFmt numFmtId="169" formatCode="0.0%"/>
     <numFmt numFmtId="170" formatCode="0.##"/>
-    <numFmt numFmtId="172" formatCode="[$-409]d/mmm/yyyy;@"/>
+    <numFmt numFmtId="171" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -558,7 +573,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -601,8 +616,14 @@
         <bgColor rgb="FFE6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6E6E6"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="47">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -1165,6 +1186,30 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -1184,7 +1229,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="196">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1486,15 +1531,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="168" fontId="3" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1675,6 +1714,90 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="171" fontId="3" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="3" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1684,9 +1807,6 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1699,76 +1819,22 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="3" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="3" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="3" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="3" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="3" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="3" fillId="8" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1782,6 +1848,16 @@
     <cellStyle name="Result2" xfId="2"/>
   </cellStyles>
   <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1849,16 +1925,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2248,7 +2314,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="O4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W23" sqref="W23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -2290,12 +2358,12 @@
       <c r="AA1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="AG1" s="187" t="s">
+      <c r="AG1" s="168" t="s">
         <v>1</v>
       </c>
-      <c r="AH1" s="187"/>
-      <c r="AI1" s="187"/>
-      <c r="AJ1" s="187"/>
+      <c r="AH1" s="168"/>
+      <c r="AI1" s="168"/>
+      <c r="AJ1" s="168"/>
     </row>
     <row r="2" spans="1:36" ht="14.45" customHeight="1">
       <c r="A2" s="2">
@@ -2312,14 +2380,14 @@
       </c>
       <c r="Y2" s="14"/>
       <c r="AA2" s="15"/>
-      <c r="AG2" s="188" t="s">
+      <c r="AG2" s="169" t="s">
         <v>3</v>
       </c>
-      <c r="AH2" s="188"/>
-      <c r="AI2" s="189" t="s">
+      <c r="AH2" s="169"/>
+      <c r="AI2" s="170" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="189"/>
+      <c r="AJ2" s="170"/>
     </row>
     <row r="3" spans="1:36" ht="14.45" customHeight="1">
       <c r="A3" s="2">
@@ -2468,7 +2536,7 @@
       <c r="O7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P7" s="191"/>
+      <c r="P7" s="162"/>
       <c r="Q7" s="31"/>
       <c r="W7" s="1" t="s">
         <v>21</v>
@@ -2529,7 +2597,7 @@
       <c r="O8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P8" s="194" t="str">
+      <c r="P8" s="164" t="str">
         <f>IF(AB8="","",AB8)</f>
         <v/>
       </c>
@@ -2609,19 +2677,19 @@
       <c r="D10" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="190" t="str">
+      <c r="E10" s="171" t="str">
         <f t="shared" ref="E10:E15" si="1">IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="F10" s="190"/>
+      <c r="F10" s="171"/>
       <c r="I10" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="190" t="str">
+      <c r="J10" s="171" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="K10" s="190"/>
+      <c r="K10" s="171"/>
       <c r="M10" s="12"/>
       <c r="O10" s="13"/>
       <c r="Q10" s="21" t="s">
@@ -2662,19 +2730,19 @@
       <c r="D11" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="185" t="str">
+      <c r="E11" s="172" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F11" s="185"/>
+      <c r="F11" s="172"/>
       <c r="I11" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="195" t="str">
+      <c r="J11" s="173" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="K11" s="195"/>
+      <c r="K11" s="173"/>
       <c r="M11" s="12"/>
       <c r="O11" s="13"/>
       <c r="Q11" s="21" t="s">
@@ -2715,19 +2783,19 @@
       <c r="D12" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="185" t="str">
+      <c r="E12" s="172" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F12" s="185"/>
+      <c r="F12" s="172"/>
       <c r="I12" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="185" t="str">
+      <c r="J12" s="172" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="K12" s="185"/>
+      <c r="K12" s="172"/>
       <c r="M12" s="12"/>
       <c r="O12" s="13"/>
       <c r="Q12" s="21" t="s">
@@ -2768,19 +2836,19 @@
       <c r="D13" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="185" t="str">
+      <c r="E13" s="172" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F13" s="185"/>
+      <c r="F13" s="172"/>
       <c r="I13" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="185" t="str">
+      <c r="J13" s="172" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="K13" s="185"/>
+      <c r="K13" s="172"/>
       <c r="M13" s="12"/>
       <c r="O13" s="13"/>
       <c r="Q13" s="21" t="s">
@@ -2821,19 +2889,19 @@
       <c r="D14" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="185" t="str">
+      <c r="E14" s="172" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F14" s="185"/>
+      <c r="F14" s="172"/>
       <c r="I14" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="185" t="str">
+      <c r="J14" s="172" t="str">
         <f>IF(V14="","",V14)</f>
         <v/>
       </c>
-      <c r="K14" s="185"/>
+      <c r="K14" s="172"/>
       <c r="M14" s="12"/>
       <c r="O14" s="13"/>
       <c r="Q14" s="21" t="s">
@@ -2874,11 +2942,11 @@
       <c r="D15" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="185" t="str">
+      <c r="E15" s="172" t="str">
         <f t="shared" si="1"/>
         <v>IMPAX 4.2 2015</v>
       </c>
-      <c r="F15" s="185"/>
+      <c r="F15" s="172"/>
       <c r="M15" s="12"/>
       <c r="O15" s="26"/>
       <c r="P15" s="27"/>
@@ -3009,20 +3077,26 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="186" t="s">
+      <c r="F19" s="174" t="s">
         <v>45</v>
       </c>
-      <c r="G19" s="186"/>
-      <c r="H19" s="186"/>
-      <c r="I19" s="186"/>
-      <c r="J19" s="186"/>
-      <c r="K19" s="186"/>
-      <c r="L19" s="186"/>
+      <c r="G19" s="174"/>
+      <c r="H19" s="174"/>
+      <c r="I19" s="174"/>
+      <c r="J19" s="174"/>
+      <c r="K19" s="174"/>
+      <c r="L19" s="174"/>
       <c r="M19" s="5"/>
       <c r="O19" s="13"/>
       <c r="R19" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="S19" s="40"/>
+      <c r="V19" s="40" t="s">
+        <v>141</v>
+      </c>
+      <c r="W19" s="40"/>
+      <c r="X19" s="40"/>
       <c r="Y19" s="14"/>
       <c r="AA19" s="21" t="s">
         <v>38</v>
@@ -3065,12 +3139,17 @@
         <v>47</v>
       </c>
       <c r="R20" s="76"/>
-      <c r="S20" s="77"/>
-      <c r="T20" s="77"/>
-      <c r="U20" s="77"/>
-      <c r="V20" s="77"/>
-      <c r="W20" s="77"/>
-      <c r="X20" s="77"/>
+      <c r="S20" s="40"/>
+      <c r="V20" s="66" t="s">
+        <v>137</v>
+      </c>
+      <c r="W20" s="197" t="str">
+        <f>IF(X20&lt;&gt;"",X20,IF(AB23="","",AB23))</f>
+        <v>Radcal 9010</v>
+      </c>
+      <c r="X20" s="198" t="s">
+        <v>140</v>
+      </c>
       <c r="Y20" s="14"/>
       <c r="AA20" s="21" t="s">
         <v>40</v>
@@ -3113,12 +3192,17 @@
         <v>48</v>
       </c>
       <c r="R21" s="76"/>
-      <c r="S21" s="77"/>
-      <c r="T21" s="77"/>
-      <c r="U21" s="77"/>
-      <c r="V21" s="77"/>
-      <c r="W21" s="77"/>
-      <c r="X21" s="77"/>
+      <c r="S21" s="40"/>
+      <c r="V21" s="66" t="s">
+        <v>139</v>
+      </c>
+      <c r="W21" s="202">
+        <f t="shared" ref="W21:W22" si="4">IF(X21&lt;&gt;"",X21,IF(AB24="","",AB24))</f>
+        <v>43670</v>
+      </c>
+      <c r="X21" s="199">
+        <v>43670</v>
+      </c>
       <c r="Y21" s="14"/>
       <c r="AB21" s="20"/>
       <c r="AC21" s="20"/>
@@ -3152,24 +3236,20 @@
         <v>49</v>
       </c>
       <c r="R22" s="76"/>
-      <c r="S22" s="77"/>
-      <c r="T22" s="77"/>
-      <c r="U22" s="77"/>
-      <c r="V22" s="77"/>
-      <c r="W22" s="77"/>
-      <c r="X22" s="77"/>
+      <c r="S22" s="40"/>
+      <c r="V22" s="66" t="s">
+        <v>138</v>
+      </c>
+      <c r="W22" s="202">
+        <f t="shared" si="4"/>
+        <v>44036</v>
+      </c>
+      <c r="X22" s="199">
+        <v>44036</v>
+      </c>
       <c r="Y22" s="14"/>
-      <c r="AA22" s="66" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB22" s="34"/>
-      <c r="AC22" s="35" t="str">
-        <f t="shared" ref="AC22:AC28" si="4">IF(AB22&lt;&gt;AD22,"Change","")</f>
-        <v/>
-      </c>
-      <c r="AD22" s="73" t="str">
-        <f>IF(P26="","",P26)</f>
-        <v/>
+      <c r="AA22" s="21" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:30" ht="14.45" customHeight="1">
@@ -3200,24 +3280,24 @@
         <v>51</v>
       </c>
       <c r="R23" s="76"/>
-      <c r="S23" s="77"/>
-      <c r="T23" s="77"/>
-      <c r="U23" s="77"/>
-      <c r="V23" s="77"/>
-      <c r="W23" s="77"/>
-      <c r="X23" s="77"/>
+      <c r="S23" s="40"/>
+      <c r="T23" s="40"/>
+      <c r="U23" s="40"/>
+      <c r="V23" s="40"/>
+      <c r="W23" s="40"/>
+      <c r="X23" s="40"/>
       <c r="Y23" s="14"/>
-      <c r="AA23" s="21" t="s">
-        <v>52</v>
+      <c r="AA23" s="66" t="s">
+        <v>137</v>
       </c>
       <c r="AB23" s="34"/>
       <c r="AC23" s="35" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="AD23" s="79" t="str">
-        <f>IF(R36="","",R36)</f>
-        <v/>
+        <f t="shared" ref="AC23:AC25" si="5">IF(AB23&lt;&gt;AD23,"Change","")</f>
+        <v>Change</v>
+      </c>
+      <c r="AD23" s="73" t="str">
+        <f>IF(X20="","",X20)</f>
+        <v>Radcal 9010</v>
       </c>
     </row>
     <row r="24" spans="1:30" ht="14.45" customHeight="1">
@@ -3228,11 +3308,11 @@
       <c r="D24" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="192" t="str">
+      <c r="E24" s="175" t="str">
         <f>IF(P51="","",P51)</f>
         <v/>
       </c>
-      <c r="F24" s="192"/>
+      <c r="F24" s="175"/>
       <c r="G24" s="40"/>
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
@@ -3242,17 +3322,17 @@
       <c r="M24" s="12"/>
       <c r="O24" s="13"/>
       <c r="Y24" s="14"/>
-      <c r="AA24" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB24" s="34"/>
+      <c r="AA24" s="66" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB24" s="201"/>
       <c r="AC24" s="35" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="AD24" s="79" t="str">
-        <f>IF(S36="","",S36)</f>
-        <v/>
+        <f t="shared" si="5"/>
+        <v>Change</v>
+      </c>
+      <c r="AD24" s="200">
+        <f t="shared" ref="AD24:AD25" si="6">IF(X21="","",X21)</f>
+        <v>43670</v>
       </c>
     </row>
     <row r="25" spans="1:30" ht="14.45" customHeight="1">
@@ -3271,17 +3351,17 @@
         <v>14</v>
       </c>
       <c r="Y25" s="14"/>
-      <c r="AA25" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB25" s="81"/>
+      <c r="AA25" s="66" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB25" s="201"/>
       <c r="AC25" s="35" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="AD25" s="82" t="str">
-        <f>IF(Q92="","",Q92)</f>
-        <v/>
+        <f t="shared" si="5"/>
+        <v>Change</v>
+      </c>
+      <c r="AD25" s="200">
+        <f t="shared" si="6"/>
+        <v>44036</v>
       </c>
     </row>
     <row r="26" spans="1:30" ht="14.45" customHeight="1">
@@ -3301,18 +3381,6 @@
         <v>57</v>
       </c>
       <c r="Y26" s="14"/>
-      <c r="AA26" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB26" s="81"/>
-      <c r="AC26" s="35" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="AD26" s="82" t="str">
-        <f>IF(R92="","",R92)</f>
-        <v/>
-      </c>
     </row>
     <row r="27" spans="1:30" ht="14.45" customHeight="1">
       <c r="A27" s="2">
@@ -3340,7 +3408,7 @@
         <v>62</v>
       </c>
       <c r="P27" s="88" t="str">
-        <f>IF(AB22="","",AB22)</f>
+        <f>IF(AB27="","",AB27)</f>
         <v/>
       </c>
       <c r="Q27" s="1" t="s">
@@ -3353,16 +3421,16 @@
         <v>61</v>
       </c>
       <c r="Y27" s="14"/>
-      <c r="AA27" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB27" s="81"/>
+      <c r="AA27" s="66" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB27" s="34"/>
       <c r="AC27" s="35" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="AD27" s="82" t="str">
-        <f>IF(S92="","",S92)</f>
+        <f t="shared" ref="AC27:AC33" si="7">IF(AB27&lt;&gt;AD27,"Change","")</f>
+        <v/>
+      </c>
+      <c r="AD27" s="73" t="str">
+        <f>IF(P26="","",P26)</f>
         <v/>
       </c>
     </row>
@@ -3402,15 +3470,15 @@
       <c r="X28" s="91"/>
       <c r="Y28" s="14"/>
       <c r="AA28" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB28" s="81"/>
+        <v>52</v>
+      </c>
+      <c r="AB28" s="34"/>
       <c r="AC28" s="35" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="AD28" s="82" t="str">
-        <f>IF(T92="","",T92)</f>
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AD28" s="79" t="str">
+        <f>IF(R36="","",R36)</f>
         <v/>
       </c>
     </row>
@@ -3449,11 +3517,17 @@
       <c r="X29" s="77"/>
       <c r="Y29" s="14"/>
       <c r="AA29" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB29" s="20"/>
-      <c r="AC29" s="20"/>
-      <c r="AD29" s="20"/>
+        <v>53</v>
+      </c>
+      <c r="AB29" s="34"/>
+      <c r="AC29" s="35" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AD29" s="79" t="str">
+        <f>IF(S36="","",S36)</f>
+        <v/>
+      </c>
     </row>
     <row r="30" spans="1:30" ht="14.45" customHeight="1">
       <c r="A30" s="2">
@@ -3487,11 +3561,15 @@
       <c r="X30" s="77"/>
       <c r="Y30" s="14"/>
       <c r="AA30" s="21" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="AB30" s="81"/>
+      <c r="AC30" s="35" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="AD30" s="82" t="str">
-        <f>IF(R70="","",R70)</f>
+        <f>IF(Q92="","",Q92)</f>
         <v/>
       </c>
     </row>
@@ -3504,11 +3582,15 @@
       <c r="O31" s="13"/>
       <c r="Y31" s="14"/>
       <c r="AA31" s="21" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="AB31" s="81"/>
+      <c r="AC31" s="35" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="AD31" s="82" t="str">
-        <f>IF(R72="","",R72)</f>
+        <f>IF(R92="","",R92)</f>
         <v/>
       </c>
     </row>
@@ -3532,11 +3614,15 @@
       </c>
       <c r="Y32" s="14"/>
       <c r="AA32" s="21" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="AB32" s="81"/>
+      <c r="AC32" s="35" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="AD32" s="82" t="str">
-        <f>IF(R74="","",R74)</f>
+        <f>IF(S92="","",S92)</f>
         <v/>
       </c>
     </row>
@@ -3548,11 +3634,11 @@
       <c r="C33" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="192" t="str">
+      <c r="D33" s="175" t="str">
         <f>IF(P33="","",P33)</f>
         <v/>
       </c>
-      <c r="E33" s="192"/>
+      <c r="E33" s="175"/>
       <c r="F33" s="87" t="s">
         <v>74</v>
       </c>
@@ -3570,7 +3656,7 @@
       <c r="O33" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="P33" s="191"/>
+      <c r="P33" s="162"/>
       <c r="R33" s="20" t="str">
         <f>"Left ("&amp;RIGHT($V$13,4)&amp;")"</f>
         <v>Left ()</v>
@@ -3581,11 +3667,15 @@
       </c>
       <c r="Y33" s="14"/>
       <c r="AA33" s="21" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="AB33" s="81"/>
+      <c r="AC33" s="35" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
       <c r="AD33" s="82" t="str">
-        <f>IF(S70="","",S70)</f>
+        <f>IF(T92="","",T92)</f>
         <v/>
       </c>
     </row>
@@ -3621,17 +3711,15 @@
       <c r="Q34" s="100" t="s">
         <v>78</v>
       </c>
-      <c r="R34" s="101"/>
-      <c r="S34" s="101"/>
+      <c r="R34" s="166"/>
+      <c r="S34" s="166"/>
       <c r="Y34" s="14"/>
       <c r="AA34" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB34" s="81"/>
-      <c r="AD34" s="82" t="str">
-        <f>IF(S72="","",S72)</f>
-        <v/>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="AB34" s="20"/>
+      <c r="AC34" s="20"/>
+      <c r="AD34" s="20"/>
     </row>
     <row r="35" spans="1:30" ht="14.45" customHeight="1">
       <c r="A35" s="2">
@@ -3662,18 +3750,18 @@
       <c r="L35" s="97"/>
       <c r="M35" s="12"/>
       <c r="O35" s="13"/>
-      <c r="Q35" s="102" t="s">
+      <c r="Q35" s="101" t="s">
         <v>80</v>
       </c>
-      <c r="R35" s="103"/>
-      <c r="S35" s="103"/>
+      <c r="R35" s="167"/>
+      <c r="S35" s="167"/>
       <c r="Y35" s="14"/>
       <c r="AA35" s="21" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="AB35" s="81"/>
       <c r="AD35" s="82" t="str">
-        <f>IF(S74="","",S74)</f>
+        <f>IF(R70="","",R70)</f>
         <v/>
       </c>
     </row>
@@ -3702,15 +3790,23 @@
       <c r="Q36" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="R36" s="104" t="str">
+      <c r="R36" s="102" t="str">
         <f>IF(OR(R34="",R35=""),"",R35/R34)</f>
         <v/>
       </c>
-      <c r="S36" s="105" t="str">
+      <c r="S36" s="103" t="str">
         <f>IF(OR(S34="",S35=""),"",S35/S34)</f>
         <v/>
       </c>
       <c r="Y36" s="14"/>
+      <c r="AA36" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB36" s="81"/>
+      <c r="AD36" s="82" t="str">
+        <f>IF(R72="","",R72)</f>
+        <v/>
+      </c>
     </row>
     <row r="37" spans="1:30" ht="14.45" customHeight="1">
       <c r="A37" s="2">
@@ -3733,6 +3829,14 @@
       <c r="M37" s="12"/>
       <c r="O37" s="13"/>
       <c r="Y37" s="14"/>
+      <c r="AA37" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB37" s="81"/>
+      <c r="AD37" s="82" t="str">
+        <f>IF(R74="","",R74)</f>
+        <v/>
+      </c>
     </row>
     <row r="38" spans="1:30" ht="14.45" customHeight="1">
       <c r="A38" s="2">
@@ -3767,6 +3871,14 @@
       <c r="U38" s="91"/>
       <c r="X38" s="91"/>
       <c r="Y38" s="14"/>
+      <c r="AA38" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB38" s="81"/>
+      <c r="AD38" s="82" t="str">
+        <f>IF(S70="","",S70)</f>
+        <v/>
+      </c>
     </row>
     <row r="39" spans="1:30" ht="14.45" customHeight="1">
       <c r="A39" s="2">
@@ -3790,6 +3902,14 @@
       <c r="W39" s="77"/>
       <c r="X39" s="77"/>
       <c r="Y39" s="14"/>
+      <c r="AA39" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB39" s="81"/>
+      <c r="AD39" s="82" t="str">
+        <f>IF(S72="","",S72)</f>
+        <v/>
+      </c>
     </row>
     <row r="40" spans="1:30" ht="14.45" customHeight="1">
       <c r="A40" s="2">
@@ -3813,6 +3933,14 @@
       <c r="W40" s="77"/>
       <c r="X40" s="77"/>
       <c r="Y40" s="14"/>
+      <c r="AA40" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB40" s="81"/>
+      <c r="AD40" s="82" t="str">
+        <f>IF(S74="","",S74)</f>
+        <v/>
+      </c>
     </row>
     <row r="41" spans="1:30" ht="14.45" customHeight="1">
       <c r="A41" s="2">
@@ -3822,16 +3950,16 @@
       <c r="C41" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="192" t="str">
+      <c r="D41" s="175" t="str">
         <f>IF(P43="","",P43)</f>
         <v/>
       </c>
-      <c r="E41" s="192"/>
-      <c r="F41" s="106" t="str">
+      <c r="E41" s="175"/>
+      <c r="F41" s="104" t="str">
         <f>R44</f>
         <v>Left ()</v>
       </c>
-      <c r="G41" s="107" t="str">
+      <c r="G41" s="105" t="str">
         <f>S44</f>
         <v>Right ()</v>
       </c>
@@ -3847,11 +3975,11 @@
       <c r="E42" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="F42" s="108" t="str">
+      <c r="F42" s="106" t="str">
         <f>IF(R45="","",IF(R45=1,"YES",IF(R45=2,"NO",IF(R45=3,"NA",""))))</f>
         <v/>
       </c>
-      <c r="G42" s="109" t="str">
+      <c r="G42" s="107" t="str">
         <f>IF(S45="","",IF(S45=1,"YES",IF(S45=2,"NO",IF(S45=3,"NA",""))))</f>
         <v/>
       </c>
@@ -3897,7 +4025,7 @@
       <c r="O43" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="P43" s="191"/>
+      <c r="P43" s="162"/>
       <c r="V43" s="1" t="s">
         <v>84</v>
       </c>
@@ -3907,7 +4035,7 @@
       </c>
       <c r="AB43" s="34"/>
       <c r="AC43" s="35" t="str">
-        <f t="shared" ref="AC43:AC49" si="5">IF(AB43&lt;&gt;AD43,"Change","")</f>
+        <f t="shared" ref="AC43:AC49" si="8">IF(AB43&lt;&gt;AD43,"Change","")</f>
         <v/>
       </c>
       <c r="AD43" s="82" t="str">
@@ -3934,7 +4062,7 @@
       <c r="K44" s="92"/>
       <c r="L44" s="92"/>
       <c r="M44" s="12"/>
-      <c r="O44" s="110" t="s">
+      <c r="O44" s="108" t="s">
         <v>44</v>
       </c>
       <c r="R44" s="20" t="str">
@@ -3951,7 +4079,7 @@
       </c>
       <c r="AB44" s="34"/>
       <c r="AC44" s="35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AD44" s="82" t="str">
@@ -3982,15 +4110,15 @@
       <c r="Q45" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="R45" s="111"/>
-      <c r="S45" s="111"/>
+      <c r="R45" s="109"/>
+      <c r="S45" s="109"/>
       <c r="Y45" s="14"/>
       <c r="AA45" s="21" t="s">
         <v>87</v>
       </c>
       <c r="AB45" s="34"/>
       <c r="AC45" s="35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AD45" s="82" t="str">
@@ -4023,7 +4151,7 @@
       </c>
       <c r="AB46" s="34"/>
       <c r="AC46" s="35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AD46" s="82" t="str">
@@ -4061,7 +4189,7 @@
       </c>
       <c r="AB47" s="34"/>
       <c r="AC47" s="35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AD47" s="82" t="str">
@@ -4074,7 +4202,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="10"/>
-      <c r="C48" s="112" t="s">
+      <c r="C48" s="110" t="s">
         <v>91</v>
       </c>
       <c r="D48" s="97"/>
@@ -4082,7 +4210,7 @@
       <c r="F48" s="97"/>
       <c r="G48" s="97"/>
       <c r="H48" s="97"/>
-      <c r="I48" s="112" t="s">
+      <c r="I48" s="110" t="s">
         <v>92</v>
       </c>
       <c r="J48" s="97"/>
@@ -4107,7 +4235,7 @@
       </c>
       <c r="AB48" s="34"/>
       <c r="AC48" s="35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AD48" s="82" t="str">
@@ -4124,7 +4252,7 @@
         <f>Q57</f>
         <v>Left ()</v>
       </c>
-      <c r="D49" s="53" t="str">
+      <c r="D49" s="165" t="str">
         <f>IF(Q58="","",Q58)</f>
         <v/>
       </c>
@@ -4132,7 +4260,7 @@
         <f>R57</f>
         <v>Right ()</v>
       </c>
-      <c r="F49" s="53" t="str">
+      <c r="F49" s="165" t="str">
         <f>IF(R58="","",R58)</f>
         <v/>
       </c>
@@ -4142,7 +4270,7 @@
         <f>Q57</f>
         <v>Left ()</v>
       </c>
-      <c r="J49" s="53" t="str">
+      <c r="J49" s="165" t="str">
         <f>IF(Q59="","",Q59)</f>
         <v/>
       </c>
@@ -4150,7 +4278,7 @@
         <f>R57</f>
         <v>Right ()</v>
       </c>
-      <c r="L49" s="53" t="str">
+      <c r="L49" s="165" t="str">
         <f>IF(R59="","",R59)</f>
         <v/>
       </c>
@@ -4162,7 +4290,7 @@
       </c>
       <c r="AB49" s="34"/>
       <c r="AC49" s="35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AD49" s="82" t="str">
@@ -4227,7 +4355,7 @@
       <c r="O51" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="P51" s="191"/>
+      <c r="P51" s="162"/>
       <c r="V51" s="1" t="s">
         <v>96</v>
       </c>
@@ -4319,15 +4447,15 @@
         <v>54</v>
       </c>
       <c r="B54" s="10"/>
-      <c r="C54" s="112" t="s">
+      <c r="C54" s="110" t="s">
         <v>97</v>
       </c>
-      <c r="I54" s="184" t="s">
+      <c r="I54" s="176" t="s">
         <v>98</v>
       </c>
-      <c r="J54" s="184"/>
-      <c r="K54" s="184"/>
-      <c r="L54" s="184"/>
+      <c r="J54" s="176"/>
+      <c r="K54" s="176"/>
+      <c r="L54" s="176"/>
       <c r="M54" s="12"/>
       <c r="O54" s="13"/>
       <c r="P54" s="21" t="s">
@@ -4351,24 +4479,24 @@
         <v>55</v>
       </c>
       <c r="B55" s="10"/>
-      <c r="F55" s="106" t="str">
+      <c r="F55" s="104" t="str">
         <f>R65</f>
         <v>Left ()</v>
       </c>
-      <c r="G55" s="107" t="str">
+      <c r="G55" s="105" t="str">
         <f>S65</f>
         <v>Right ()</v>
       </c>
-      <c r="I55" s="172" t="str">
+      <c r="I55" s="177" t="str">
         <f>R65</f>
         <v>Left ()</v>
       </c>
-      <c r="J55" s="172"/>
-      <c r="K55" s="173" t="str">
+      <c r="J55" s="177"/>
+      <c r="K55" s="178" t="str">
         <f>S65</f>
         <v>Right ()</v>
       </c>
-      <c r="L55" s="173"/>
+      <c r="L55" s="178"/>
       <c r="M55" s="12"/>
       <c r="O55" s="13"/>
       <c r="Y55" s="14"/>
@@ -4390,27 +4518,27 @@
       <c r="E56" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="F56" s="113" t="str">
-        <f t="shared" ref="F56:G58" si="6">IF(R66="","",IF(R66=1,"YES",IF(R66=2,"NO",IF(R66=3,"NA",""))))</f>
-        <v/>
-      </c>
-      <c r="G56" s="114" t="str">
-        <f t="shared" si="6"/>
+      <c r="F56" s="111" t="str">
+        <f t="shared" ref="F56:G58" si="9">IF(R66="","",IF(R66=1,"YES",IF(R66=2,"NO",IF(R66=3,"NA",""))))</f>
+        <v/>
+      </c>
+      <c r="G56" s="112" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="H56" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="I56" s="180" t="str">
+      <c r="I56" s="179" t="str">
         <f>IF(R70="","",R70)</f>
         <v/>
       </c>
-      <c r="J56" s="180"/>
-      <c r="K56" s="181" t="str">
+      <c r="J56" s="179"/>
+      <c r="K56" s="180" t="str">
         <f>IF(S70="","",S70)</f>
         <v/>
       </c>
-      <c r="L56" s="181"/>
+      <c r="L56" s="180"/>
       <c r="M56" s="12"/>
       <c r="O56" s="80" t="s">
         <v>89</v>
@@ -4430,29 +4558,29 @@
       <c r="E57" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="F57" s="113" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="G57" s="114" t="str">
-        <f t="shared" si="6"/>
+      <c r="F57" s="111" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="G57" s="112" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="H57" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="I57" s="180" t="str">
+      <c r="I57" s="179" t="str">
         <f>IF(R72="","",R72)</f>
         <v/>
       </c>
-      <c r="J57" s="180"/>
-      <c r="K57" s="181" t="str">
+      <c r="J57" s="179"/>
+      <c r="K57" s="180" t="str">
         <f>IF(S72="","",S72)</f>
         <v/>
       </c>
-      <c r="L57" s="181"/>
+      <c r="L57" s="180"/>
       <c r="M57" s="12"/>
-      <c r="O57" s="115" t="s">
+      <c r="O57" s="113" t="s">
         <v>103</v>
       </c>
       <c r="Q57" s="20" t="str">
@@ -4482,34 +4610,34 @@
       <c r="E58" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="F58" s="108" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="G58" s="109" t="str">
-        <f t="shared" si="6"/>
+      <c r="F58" s="106" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="G58" s="107" t="str">
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="H58" s="52" t="s">
         <v>105</v>
       </c>
-      <c r="I58" s="182" t="str">
+      <c r="I58" s="181" t="str">
         <f>IF(R74="","",R74)</f>
         <v/>
       </c>
-      <c r="J58" s="182"/>
-      <c r="K58" s="183" t="str">
+      <c r="J58" s="181"/>
+      <c r="K58" s="182" t="str">
         <f>IF(S74="","",S74)</f>
         <v/>
       </c>
-      <c r="L58" s="183"/>
+      <c r="L58" s="182"/>
       <c r="M58" s="12"/>
       <c r="O58" s="13"/>
-      <c r="P58" s="116" t="s">
+      <c r="P58" s="114" t="s">
         <v>106</v>
       </c>
-      <c r="Q58" s="101"/>
-      <c r="R58" s="101"/>
+      <c r="Q58" s="166"/>
+      <c r="R58" s="166"/>
       <c r="Y58" s="14"/>
       <c r="AB58" s="20"/>
       <c r="AC58" s="20"/>
@@ -4537,11 +4665,11 @@
       <c r="L59" s="89"/>
       <c r="M59" s="12"/>
       <c r="O59" s="13"/>
-      <c r="P59" s="117" t="s">
+      <c r="P59" s="115" t="s">
         <v>107</v>
       </c>
-      <c r="Q59" s="103"/>
-      <c r="R59" s="103"/>
+      <c r="Q59" s="167"/>
+      <c r="R59" s="167"/>
       <c r="Y59" s="14"/>
       <c r="AB59" s="69"/>
       <c r="AC59" s="35" t="str">
@@ -4692,7 +4820,7 @@
       <c r="K64" s="24"/>
       <c r="L64" s="24"/>
       <c r="M64" s="25"/>
-      <c r="O64" s="115" t="s">
+      <c r="O64" s="113" t="s">
         <v>97</v>
       </c>
       <c r="U64" s="21" t="s">
@@ -4713,18 +4841,18 @@
       <c r="C65" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D65" s="193" t="str">
+      <c r="D65" s="163" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
       <c r="L65" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="M65" s="118" t="str">
+      <c r="M65" s="116" t="str">
         <f>IF($X$7="","",$X$7)</f>
         <v>Eugene Mah</v>
       </c>
-      <c r="O65" s="110" t="s">
+      <c r="O65" s="108" t="s">
         <v>44</v>
       </c>
       <c r="R65" s="20" t="str">
@@ -4753,14 +4881,14 @@
       <c r="C66" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="D66" s="119" t="str">
+      <c r="D66" s="117" t="str">
         <f>IF($E$14="","",$E$14)</f>
         <v/>
       </c>
       <c r="L66" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="M66" s="120" t="str">
+      <c r="M66" s="118" t="str">
         <f>IF($R$13="","",$R$13)</f>
         <v/>
       </c>
@@ -4768,8 +4896,8 @@
       <c r="Q66" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="R66" s="121"/>
-      <c r="S66" s="122"/>
+      <c r="R66" s="119"/>
+      <c r="S66" s="120"/>
       <c r="Y66" s="14"/>
       <c r="AB66" s="20"/>
       <c r="AC66" s="20"/>
@@ -4779,7 +4907,7 @@
       <c r="A67" s="2">
         <v>1</v>
       </c>
-      <c r="M67" s="123" t="str">
+      <c r="M67" s="121" t="str">
         <f>$H$2</f>
         <v>Medical University of South Carolina</v>
       </c>
@@ -4787,8 +4915,8 @@
       <c r="Q67" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="R67" s="124"/>
-      <c r="S67" s="125"/>
+      <c r="R67" s="122"/>
+      <c r="S67" s="123"/>
       <c r="Y67" s="14"/>
       <c r="AB67" s="69"/>
       <c r="AC67" s="35" t="str">
@@ -4812,8 +4940,8 @@
       <c r="Q68" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="R68" s="126"/>
-      <c r="S68" s="127"/>
+      <c r="R68" s="124"/>
+      <c r="S68" s="125"/>
       <c r="Y68" s="14"/>
       <c r="AB68" s="20"/>
       <c r="AC68" s="20"/>
@@ -4842,10 +4970,10 @@
       <c r="R69" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="V69" s="167" t="s">
+      <c r="V69" s="183" t="s">
         <v>111</v>
       </c>
-      <c r="W69" s="167"/>
+      <c r="W69" s="183"/>
       <c r="Y69" s="14"/>
       <c r="AB69" s="69"/>
       <c r="AC69" s="35" t="str">
@@ -4876,17 +5004,17 @@
       <c r="L70" s="4"/>
       <c r="M70" s="5"/>
       <c r="O70" s="13"/>
-      <c r="Q70" s="167" t="s">
+      <c r="Q70" s="183" t="s">
         <v>100</v>
       </c>
-      <c r="R70" s="176"/>
-      <c r="S70" s="177"/>
-      <c r="V70" s="178" t="str">
-        <f>IF(AB30="","",AB30)</f>
-        <v/>
-      </c>
-      <c r="W70" s="179" t="str">
-        <f>IF(AB33="","",AB33)</f>
+      <c r="R70" s="184"/>
+      <c r="S70" s="185"/>
+      <c r="V70" s="186" t="str">
+        <f>IF(AB35="","",AB35)</f>
+        <v/>
+      </c>
+      <c r="W70" s="187" t="str">
+        <f>IF(AB38="","",AB38)</f>
         <v/>
       </c>
       <c r="Y70" s="14"/>
@@ -4900,26 +5028,26 @@
       </c>
       <c r="B71" s="10"/>
       <c r="C71" s="97"/>
-      <c r="D71" s="172" t="str">
+      <c r="D71" s="177" t="str">
         <f>Q83</f>
         <v>UNL-10 (cd/m^2)</v>
       </c>
-      <c r="E71" s="172"/>
-      <c r="F71" s="173" t="str">
+      <c r="E71" s="177"/>
+      <c r="F71" s="178" t="str">
         <f>S83</f>
         <v>UNL-80 (cd/m^2)</v>
       </c>
-      <c r="G71" s="173"/>
+      <c r="G71" s="178"/>
       <c r="I71" s="68" t="s">
         <v>113</v>
       </c>
       <c r="M71" s="12"/>
       <c r="O71" s="13"/>
-      <c r="Q71" s="167"/>
-      <c r="R71" s="176"/>
-      <c r="S71" s="177"/>
-      <c r="V71" s="178"/>
-      <c r="W71" s="179"/>
+      <c r="Q71" s="183"/>
+      <c r="R71" s="184"/>
+      <c r="S71" s="185"/>
+      <c r="V71" s="186"/>
+      <c r="W71" s="187"/>
       <c r="Y71" s="14"/>
       <c r="AB71" s="69"/>
       <c r="AC71" s="35" t="str">
@@ -4937,7 +5065,7 @@
       </c>
       <c r="B72" s="10"/>
       <c r="C72" s="97"/>
-      <c r="D72" s="113" t="str">
+      <c r="D72" s="111" t="str">
         <f>Q84</f>
         <v>Left ()</v>
       </c>
@@ -4949,7 +5077,7 @@
         <f>S84</f>
         <v>Left ()</v>
       </c>
-      <c r="G72" s="114" t="str">
+      <c r="G72" s="112" t="str">
         <f>T84</f>
         <v>Right ()</v>
       </c>
@@ -4962,17 +5090,17 @@
       </c>
       <c r="M72" s="12"/>
       <c r="O72" s="13"/>
-      <c r="Q72" s="167" t="s">
+      <c r="Q72" s="183" t="s">
         <v>102</v>
       </c>
-      <c r="R72" s="174"/>
-      <c r="S72" s="175"/>
-      <c r="V72" s="165" t="str">
-        <f>IF(AB31="","",AB31)</f>
-        <v/>
-      </c>
-      <c r="W72" s="166" t="str">
-        <f>IF(AB34="","",AB34)</f>
+      <c r="R72" s="188"/>
+      <c r="S72" s="189"/>
+      <c r="V72" s="191" t="str">
+        <f>IF(AB36="","",AB36)</f>
+        <v/>
+      </c>
+      <c r="W72" s="192" t="str">
+        <f>IF(AB39="","",AB39)</f>
         <v/>
       </c>
       <c r="Y72" s="14"/>
@@ -4985,20 +5113,20 @@
       <c r="C73" s="52" t="s">
         <v>115</v>
       </c>
-      <c r="D73" s="128" t="str">
-        <f t="shared" ref="D73:G75" si="7">IF(Q90="","",Q90)</f>
+      <c r="D73" s="126" t="str">
+        <f t="shared" ref="D73:G75" si="10">IF(Q90="","",Q90)</f>
         <v/>
       </c>
       <c r="E73" s="99" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F73" s="99" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G73" s="129" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G73" s="127" t="str">
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="I73" s="56" t="str">
@@ -5010,11 +5138,11 @@
       </c>
       <c r="M73" s="12"/>
       <c r="O73" s="13"/>
-      <c r="Q73" s="167"/>
-      <c r="R73" s="174"/>
-      <c r="S73" s="175"/>
-      <c r="V73" s="165"/>
-      <c r="W73" s="166"/>
+      <c r="Q73" s="183"/>
+      <c r="R73" s="188"/>
+      <c r="S73" s="189"/>
+      <c r="V73" s="191"/>
+      <c r="W73" s="192"/>
       <c r="Y73" s="14"/>
     </row>
     <row r="74" spans="1:30" ht="14.45" customHeight="1">
@@ -5025,20 +5153,20 @@
       <c r="C74" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="D74" s="128" t="str">
-        <f t="shared" si="7"/>
+      <c r="D74" s="126" t="str">
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="E74" s="99" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F74" s="99" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G74" s="129" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G74" s="127" t="str">
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="I74" s="56" t="str">
@@ -5050,17 +5178,17 @@
       </c>
       <c r="M74" s="12"/>
       <c r="O74" s="13"/>
-      <c r="Q74" s="167" t="s">
+      <c r="Q74" s="183" t="s">
         <v>105</v>
       </c>
-      <c r="R74" s="168"/>
-      <c r="S74" s="169"/>
-      <c r="V74" s="170" t="str">
-        <f>IF(AB32="","",AB32)</f>
-        <v/>
-      </c>
-      <c r="W74" s="171" t="str">
-        <f>IF(AB35="","",AB35)</f>
+      <c r="R74" s="193"/>
+      <c r="S74" s="194"/>
+      <c r="V74" s="195" t="str">
+        <f>IF(AB37="","",AB37)</f>
+        <v/>
+      </c>
+      <c r="W74" s="196" t="str">
+        <f>IF(AB40="","",AB40)</f>
         <v/>
       </c>
       <c r="Y74" s="14"/>
@@ -5073,29 +5201,29 @@
       <c r="C75" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="D75" s="130" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="E75" s="131" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="F75" s="131" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="G75" s="132" t="str">
-        <f t="shared" si="7"/>
+      <c r="D75" s="128" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="E75" s="129" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="F75" s="129" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G75" s="130" t="str">
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="M75" s="12"/>
       <c r="O75" s="13"/>
-      <c r="Q75" s="167"/>
-      <c r="R75" s="168"/>
-      <c r="S75" s="169"/>
-      <c r="V75" s="170"/>
-      <c r="W75" s="171"/>
+      <c r="Q75" s="183"/>
+      <c r="R75" s="193"/>
+      <c r="S75" s="194"/>
+      <c r="V75" s="195"/>
+      <c r="W75" s="196"/>
       <c r="Y75" s="14"/>
     </row>
     <row r="76" spans="1:30" ht="14.45" customHeight="1">
@@ -5103,19 +5231,19 @@
         <v>10</v>
       </c>
       <c r="B76" s="10"/>
-      <c r="D76" s="108" t="str">
+      <c r="D76" s="106" t="str">
         <f>IF(D75="","",IF(D75&lt;=0.3,"PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="E76" s="133" t="str">
+      <c r="E76" s="131" t="str">
         <f>IF(E75="","",IF(E75&lt;=0.3,"PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="F76" s="133" t="str">
+      <c r="F76" s="131" t="str">
         <f>IF(F75="","",IF(F75&lt;=0.3,"PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="G76" s="109" t="str">
+      <c r="G76" s="107" t="str">
         <f>IF(G75="","",IF(G75&lt;=0.3,"PASS","FAIL"))</f>
         <v/>
       </c>
@@ -5266,7 +5394,7 @@
         <v>16</v>
       </c>
       <c r="B82" s="10"/>
-      <c r="D82" s="119" t="str">
+      <c r="D82" s="117" t="str">
         <f>IF(Q100="","",IF(LEN(Q100)&lt;=135,Q100,IF(LEN(Q100)&lt;=260,LEFT(Q100,SEARCH(" ",Q100,125)),LEFT(Q100,SEARCH(" ",Q100,130)))))</f>
         <v/>
       </c>
@@ -5279,7 +5407,7 @@
       <c r="K82" s="91"/>
       <c r="L82" s="91"/>
       <c r="M82" s="12"/>
-      <c r="O82" s="115" t="s">
+      <c r="O82" s="113" t="s">
         <v>112</v>
       </c>
       <c r="V82" s="68" t="s">
@@ -5292,7 +5420,7 @@
         <v>17</v>
       </c>
       <c r="B83" s="10"/>
-      <c r="D83" s="134" t="str">
+      <c r="D83" s="132" t="str">
         <f>IF(LEN(Q100)&lt;=135,"",IF(LEN(Q100)&lt;=260,RIGHT(Q100,LEN(Q100)-SEARCH(" ",Q100,125)),MID(Q100,SEARCH(" ",Q100,130),IF(LEN(Q100)&lt;=265,LEN(Q100),SEARCH(" ",Q100,255)-SEARCH(" ",Q100,130)))))</f>
         <v/>
       </c>
@@ -5306,15 +5434,15 @@
       <c r="L83" s="77"/>
       <c r="M83" s="12"/>
       <c r="O83" s="13"/>
-      <c r="Q83" s="164" t="s">
+      <c r="Q83" s="190" t="s">
         <v>123</v>
       </c>
-      <c r="R83" s="164"/>
-      <c r="S83" s="164" t="s">
+      <c r="R83" s="190"/>
+      <c r="S83" s="190" t="s">
         <v>124</v>
       </c>
-      <c r="T83" s="164"/>
-      <c r="V83" s="135" t="s">
+      <c r="T83" s="190"/>
+      <c r="V83" s="133" t="s">
         <v>44</v>
       </c>
       <c r="Y83" s="14"/>
@@ -5324,7 +5452,7 @@
         <v>18</v>
       </c>
       <c r="B84" s="10"/>
-      <c r="D84" s="134" t="str">
+      <c r="D84" s="132" t="str">
         <f>IF(LEN(Q100)&lt;=265,"",RIGHT(Q100,LEN(Q100)-SEARCH(" ",Q100,255)))</f>
         <v/>
       </c>
@@ -5338,23 +5466,23 @@
       <c r="L84" s="77"/>
       <c r="M84" s="12"/>
       <c r="O84" s="13"/>
-      <c r="Q84" s="136" t="str">
+      <c r="Q84" s="134" t="str">
         <f>"Left ("&amp;RIGHT($V$13,4)&amp;")"</f>
         <v>Left ()</v>
       </c>
-      <c r="R84" s="137" t="str">
+      <c r="R84" s="135" t="str">
         <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
         <v>Right ()</v>
       </c>
-      <c r="S84" s="136" t="str">
+      <c r="S84" s="134" t="str">
         <f>"Left ("&amp;RIGHT($V$13,4)&amp;")"</f>
         <v>Left ()</v>
       </c>
-      <c r="T84" s="137" t="str">
+      <c r="T84" s="135" t="str">
         <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
         <v>Right ()</v>
       </c>
-      <c r="V84" s="138"/>
+      <c r="V84" s="136"/>
       <c r="W84" s="1" t="s">
         <v>114</v>
       </c>
@@ -5365,7 +5493,7 @@
         <v>19</v>
       </c>
       <c r="B85" s="10"/>
-      <c r="D85" s="134" t="str">
+      <c r="D85" s="132" t="str">
         <f>IF(Q102="","",IF(LEN(Q102)&lt;=135,Q102,IF(LEN(Q102)&lt;=260,LEFT(Q102,SEARCH(" ",Q102,125)),LEFT(Q102,SEARCH(" ",Q102,130)))))</f>
         <v/>
       </c>
@@ -5382,11 +5510,11 @@
       <c r="P85" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="Q85" s="139"/>
-      <c r="R85" s="140"/>
-      <c r="S85" s="141"/>
-      <c r="T85" s="140"/>
-      <c r="V85" s="138"/>
+      <c r="Q85" s="137"/>
+      <c r="R85" s="138"/>
+      <c r="S85" s="139"/>
+      <c r="T85" s="138"/>
+      <c r="V85" s="136"/>
       <c r="W85" s="1" t="s">
         <v>116</v>
       </c>
@@ -5397,7 +5525,7 @@
         <v>20</v>
       </c>
       <c r="B86" s="10"/>
-      <c r="D86" s="134" t="str">
+      <c r="D86" s="132" t="str">
         <f>IF(LEN(Q102)&lt;=135,"",IF(LEN(Q102)&lt;=260,RIGHT(Q102,LEN(Q102)-SEARCH(" ",Q102,125)),MID(Q102,SEARCH(" ",Q102,130),IF(LEN(Q102)&lt;=265,LEN(Q102),SEARCH(" ",Q102,255)-SEARCH(" ",Q102,130)))))</f>
         <v/>
       </c>
@@ -5414,11 +5542,11 @@
       <c r="P86" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="Q86" s="142"/>
-      <c r="R86" s="143"/>
-      <c r="S86" s="144"/>
-      <c r="T86" s="143"/>
-      <c r="V86" s="138"/>
+      <c r="Q86" s="140"/>
+      <c r="R86" s="141"/>
+      <c r="S86" s="142"/>
+      <c r="T86" s="141"/>
+      <c r="V86" s="136"/>
       <c r="W86" s="1" t="s">
         <v>118</v>
       </c>
@@ -5429,7 +5557,7 @@
         <v>21</v>
       </c>
       <c r="B87" s="10"/>
-      <c r="D87" s="134" t="str">
+      <c r="D87" s="132" t="str">
         <f>IF(LEN(Q102)&lt;=265,"",RIGHT(Q102,LEN(Q102)-SEARCH(" ",Q102,255)))</f>
         <v/>
       </c>
@@ -5446,10 +5574,10 @@
       <c r="P87" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="Q87" s="142"/>
-      <c r="R87" s="143"/>
-      <c r="S87" s="144"/>
-      <c r="T87" s="143"/>
+      <c r="Q87" s="140"/>
+      <c r="R87" s="141"/>
+      <c r="S87" s="142"/>
+      <c r="T87" s="141"/>
       <c r="Y87" s="14"/>
     </row>
     <row r="88" spans="1:25" ht="14.45" customHeight="1">
@@ -5457,7 +5585,7 @@
         <v>22</v>
       </c>
       <c r="B88" s="10"/>
-      <c r="D88" s="134" t="str">
+      <c r="D88" s="132" t="str">
         <f>IF(Q104="","",IF(LEN(Q104)&lt;=135,Q104,IF(LEN(Q104)&lt;=260,LEFT(Q104,SEARCH(" ",Q104,125)),LEFT(Q104,SEARCH(" ",Q104,130)))))</f>
         <v/>
       </c>
@@ -5474,10 +5602,10 @@
       <c r="P88" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="Q88" s="142"/>
-      <c r="R88" s="143"/>
-      <c r="S88" s="144"/>
-      <c r="T88" s="143"/>
+      <c r="Q88" s="140"/>
+      <c r="R88" s="141"/>
+      <c r="S88" s="142"/>
+      <c r="T88" s="141"/>
       <c r="Y88" s="14"/>
     </row>
     <row r="89" spans="1:25" ht="14.45" customHeight="1">
@@ -5485,7 +5613,7 @@
         <v>23</v>
       </c>
       <c r="B89" s="10"/>
-      <c r="D89" s="134" t="str">
+      <c r="D89" s="132" t="str">
         <f>IF(LEN(Q104)&lt;=135,"",IF(LEN(Q104)&lt;=260,RIGHT(Q104,LEN(Q104)-SEARCH(" ",Q104,125)),MID(Q104,SEARCH(" ",Q104,130),IF(LEN(Q104)&lt;=265,LEN(Q104),SEARCH(" ",Q104,255)-SEARCH(" ",Q104,130)))))</f>
         <v/>
       </c>
@@ -5502,10 +5630,10 @@
       <c r="P89" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="Q89" s="145"/>
-      <c r="R89" s="146"/>
-      <c r="S89" s="147"/>
-      <c r="T89" s="146"/>
+      <c r="Q89" s="143"/>
+      <c r="R89" s="144"/>
+      <c r="S89" s="145"/>
+      <c r="T89" s="144"/>
       <c r="Y89" s="14"/>
     </row>
     <row r="90" spans="1:25" ht="14.45" customHeight="1">
@@ -5513,7 +5641,7 @@
         <v>24</v>
       </c>
       <c r="B90" s="10"/>
-      <c r="D90" s="134" t="str">
+      <c r="D90" s="132" t="str">
         <f>IF(LEN(Q104)&lt;=265,"",RIGHT(Q104,LEN(Q104)-SEARCH(" ",Q104,255)))</f>
         <v/>
       </c>
@@ -5530,19 +5658,19 @@
       <c r="P90" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="Q90" s="148" t="str">
+      <c r="Q90" s="146" t="str">
         <f>IF(Q85="","",AVERAGE(Q85:Q89))</f>
         <v/>
       </c>
-      <c r="R90" s="149" t="str">
+      <c r="R90" s="147" t="str">
         <f>IF(R85="","",AVERAGE(R85:R89))</f>
         <v/>
       </c>
-      <c r="S90" s="150" t="str">
+      <c r="S90" s="148" t="str">
         <f>IF(S85="","",AVERAGE(S85:S89))</f>
         <v/>
       </c>
-      <c r="T90" s="149" t="str">
+      <c r="T90" s="147" t="str">
         <f>IF(T85="","",AVERAGE(T85:T89))</f>
         <v/>
       </c>
@@ -5553,7 +5681,7 @@
         <v>25</v>
       </c>
       <c r="B91" s="10"/>
-      <c r="D91" s="134" t="str">
+      <c r="D91" s="132" t="str">
         <f>IF(Q106="","",IF(LEN(Q106)&lt;=135,Q106,IF(LEN(Q106)&lt;=260,LEFT(Q106,SEARCH(" ",Q106,125)),LEFT(Q106,SEARCH(" ",Q106,130)))))</f>
         <v/>
       </c>
@@ -5570,19 +5698,19 @@
       <c r="P91" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="Q91" s="151" t="str">
+      <c r="Q91" s="149" t="str">
         <f>IF(Q85="","",STDEV(Q85:Q89))</f>
         <v/>
       </c>
-      <c r="R91" s="152" t="str">
+      <c r="R91" s="150" t="str">
         <f>IF(R85="","",STDEV(R85:R89))</f>
         <v/>
       </c>
-      <c r="S91" s="153" t="str">
+      <c r="S91" s="151" t="str">
         <f>IF(S85="","",STDEV(S85:S89))</f>
         <v/>
       </c>
-      <c r="T91" s="152" t="str">
+      <c r="T91" s="150" t="str">
         <f>IF(T85="","",STDEV(T85:T89))</f>
         <v/>
       </c>
@@ -5593,7 +5721,7 @@
         <v>26</v>
       </c>
       <c r="B92" s="10"/>
-      <c r="D92" s="134" t="str">
+      <c r="D92" s="132" t="str">
         <f>IF(LEN(Q106)&lt;=135,"",IF(LEN(Q106)&lt;=260,RIGHT(Q106,LEN(Q106)-SEARCH(" ",Q106,125)),MID(Q106,SEARCH(" ",Q106,130),IF(LEN(Q106)&lt;=265,LEN(Q106),SEARCH(" ",Q106,255)-SEARCH(" ",Q106,130)))))</f>
         <v/>
       </c>
@@ -5610,19 +5738,19 @@
       <c r="P92" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="Q92" s="154" t="str">
+      <c r="Q92" s="152" t="str">
         <f>IF(Q85="","",(MAX(Q85:Q89)-MIN(Q85:Q89))/(MIN(Q85:Q89)+MAX(Q85:Q89)))</f>
         <v/>
       </c>
-      <c r="R92" s="155" t="str">
+      <c r="R92" s="153" t="str">
         <f>IF(R85="","",(MAX(R85:R89)-MIN(R85:R89))/(MIN(R85:R89)+MAX(R85:R89)))</f>
         <v/>
       </c>
-      <c r="S92" s="156" t="str">
+      <c r="S92" s="154" t="str">
         <f>IF(S85="","",(MAX(S85:S89)-MIN(S85:S89))/(MIN(S85:S89)+MAX(S85:S89)))</f>
         <v/>
       </c>
-      <c r="T92" s="155" t="str">
+      <c r="T92" s="153" t="str">
         <f>IF(T85="","",(MAX(T85:T89)-MIN(T85:T89))/(MIN(T85:T89)+MAX(T85:T89)))</f>
         <v/>
       </c>
@@ -5639,7 +5767,7 @@
         <v>27</v>
       </c>
       <c r="B93" s="10"/>
-      <c r="D93" s="134" t="str">
+      <c r="D93" s="132" t="str">
         <f>IF(LEN(Q106)&lt;=265,"",RIGHT(Q106,LEN(Q106)-SEARCH(" ",Q106,255)))</f>
         <v/>
       </c>
@@ -5672,7 +5800,7 @@
         <v>28</v>
       </c>
       <c r="B94" s="10"/>
-      <c r="D94" s="134" t="str">
+      <c r="D94" s="132" t="str">
         <f>IF(Q108="","",IF(LEN(Q108)&lt;=135,Q108,IF(LEN(Q108)&lt;=260,LEFT(Q108,SEARCH(" ",Q108,125)),LEFT(Q108,SEARCH(" ",Q108,130)))))</f>
         <v/>
       </c>
@@ -5707,7 +5835,7 @@
         <v>29</v>
       </c>
       <c r="B95" s="10"/>
-      <c r="D95" s="134" t="str">
+      <c r="D95" s="132" t="str">
         <f>IF(LEN(Q108)&lt;=135,"",IF(LEN(Q108)&lt;=260,RIGHT(Q108,LEN(Q108)-SEARCH(" ",Q108,125)),MID(Q108,SEARCH(" ",Q108,130),IF(LEN(Q108)&lt;=265,LEN(Q108),SEARCH(" ",Q108,255)-SEARCH(" ",Q108,130)))))</f>
         <v/>
       </c>
@@ -5739,7 +5867,7 @@
         <v>30</v>
       </c>
       <c r="B96" s="10"/>
-      <c r="D96" s="134" t="str">
+      <c r="D96" s="132" t="str">
         <f>IF(LEN(Q108)&lt;=265,"",RIGHT(Q108,LEN(Q108)-SEARCH(" ",Q108,255)))</f>
         <v/>
       </c>
@@ -5769,7 +5897,7 @@
         <v>31</v>
       </c>
       <c r="B97" s="10"/>
-      <c r="D97" s="134" t="str">
+      <c r="D97" s="132" t="str">
         <f>IF(Q110="","",IF(LEN(Q110)&lt;=135,Q110,IF(LEN(Q110)&lt;=260,LEFT(Q110,SEARCH(" ",Q110,125)),LEFT(Q110,SEARCH(" ",Q110,130)))))</f>
         <v/>
       </c>
@@ -5788,7 +5916,7 @@
         <v>32</v>
       </c>
       <c r="B98" s="10"/>
-      <c r="D98" s="134" t="str">
+      <c r="D98" s="132" t="str">
         <f>IF(LEN(Q110)&lt;=135,"",IF(LEN(Q110)&lt;=260,RIGHT(Q110,LEN(Q110)-SEARCH(" ",Q110,125)),MID(Q110,SEARCH(" ",Q110,130),IF(LEN(Q110)&lt;=265,LEN(Q110),SEARCH(" ",Q110,255)-SEARCH(" ",Q110,130)))))</f>
         <v/>
       </c>
@@ -5801,7 +5929,7 @@
       <c r="K98" s="77"/>
       <c r="L98" s="77"/>
       <c r="M98" s="12"/>
-      <c r="T98" s="157" t="s">
+      <c r="T98" s="155" t="s">
         <v>133</v>
       </c>
     </row>
@@ -5810,7 +5938,7 @@
         <v>33</v>
       </c>
       <c r="B99" s="10"/>
-      <c r="D99" s="134" t="str">
+      <c r="D99" s="132" t="str">
         <f>IF(LEN(Q110)&lt;=265,"",RIGHT(Q110,LEN(Q110)-SEARCH(" ",Q110,255)))</f>
         <v/>
       </c>
@@ -5827,7 +5955,7 @@
       <c r="P99" s="7"/>
       <c r="Q99" s="7"/>
       <c r="R99" s="7"/>
-      <c r="S99" s="158" t="s">
+      <c r="S99" s="156" t="s">
         <v>134</v>
       </c>
       <c r="T99" s="7"/>
@@ -5842,7 +5970,7 @@
         <v>34</v>
       </c>
       <c r="B100" s="10"/>
-      <c r="D100" s="134" t="str">
+      <c r="D100" s="132" t="str">
         <f>IF(Q112="","",IF(LEN(Q112)&lt;=135,Q112,IF(LEN(Q112)&lt;=260,LEFT(Q112,SEARCH(" ",Q112,125)),LEFT(Q112,SEARCH(" ",Q112,130)))))</f>
         <v/>
       </c>
@@ -5859,9 +5987,9 @@
       <c r="P100" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="Q100" s="159"/>
-      <c r="R100" s="160"/>
-      <c r="S100" s="161" t="str">
+      <c r="Q100" s="157"/>
+      <c r="R100" s="158"/>
+      <c r="S100" s="159" t="str">
         <f>IF(AB51="","",AB51)</f>
         <v/>
       </c>
@@ -5875,7 +6003,7 @@
         <v>35</v>
       </c>
       <c r="B101" s="10"/>
-      <c r="D101" s="134" t="str">
+      <c r="D101" s="132" t="str">
         <f>IF(LEN(Q112)&lt;=135,"",IF(LEN(Q112)&lt;=260,RIGHT(Q112,LEN(Q112)-SEARCH(" ",Q112,125)),MID(Q112,SEARCH(" ",Q112,130),IF(LEN(Q112)&lt;=265,LEN(Q112),SEARCH(" ",Q112,255)-SEARCH(" ",Q112,130)))))</f>
         <v/>
       </c>
@@ -5893,13 +6021,13 @@
         <v>66</v>
       </c>
       <c r="Q101" s="94"/>
-      <c r="R101" s="162">
+      <c r="R101" s="160">
         <f>LEN(Q100)</f>
         <v>0</v>
       </c>
       <c r="S101" s="77"/>
       <c r="T101" s="77"/>
-      <c r="U101" s="163"/>
+      <c r="U101" s="161"/>
       <c r="V101" s="77"/>
       <c r="W101" s="77"/>
       <c r="X101" s="77"/>
@@ -5910,7 +6038,7 @@
         <v>36</v>
       </c>
       <c r="B102" s="10"/>
-      <c r="D102" s="134" t="str">
+      <c r="D102" s="132" t="str">
         <f>IF(LEN(Q112)&lt;=265,"",RIGHT(Q112,LEN(Q112)-SEARCH(" ",Q112,255)))</f>
         <v/>
       </c>
@@ -5927,9 +6055,9 @@
       <c r="P102" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="Q102" s="159"/>
-      <c r="R102" s="160"/>
-      <c r="S102" s="161" t="str">
+      <c r="Q102" s="157"/>
+      <c r="R102" s="158"/>
+      <c r="S102" s="159" t="str">
         <f>IF(AB53="","",AB53)</f>
         <v/>
       </c>
@@ -5943,7 +6071,7 @@
         <v>37</v>
       </c>
       <c r="B103" s="10"/>
-      <c r="D103" s="134" t="str">
+      <c r="D103" s="132" t="str">
         <f>IF(Q114="","",IF(LEN(Q114)&lt;=135,Q114,IF(LEN(Q114)&lt;=260,LEFT(Q114,SEARCH(" ",Q114,125)),LEFT(Q114,SEARCH(" ",Q114,130)))))</f>
         <v/>
       </c>
@@ -5961,13 +6089,13 @@
         <v>66</v>
       </c>
       <c r="Q103" s="94"/>
-      <c r="R103" s="162">
+      <c r="R103" s="160">
         <f>LEN(Q102)</f>
         <v>0</v>
       </c>
       <c r="S103" s="77"/>
       <c r="T103" s="77"/>
-      <c r="U103" s="163"/>
+      <c r="U103" s="161"/>
       <c r="V103" s="77"/>
       <c r="W103" s="77"/>
       <c r="X103" s="77"/>
@@ -5978,7 +6106,7 @@
         <v>38</v>
       </c>
       <c r="B104" s="10"/>
-      <c r="D104" s="134" t="str">
+      <c r="D104" s="132" t="str">
         <f>IF(LEN(Q114)&lt;=135,"",IF(LEN(Q114)&lt;=260,RIGHT(Q114,LEN(Q114)-SEARCH(" ",Q114,125)),MID(Q114,SEARCH(" ",Q114,130),IF(LEN(Q114)&lt;=265,LEN(Q114),SEARCH(" ",Q114,255)-SEARCH(" ",Q114,130)))))</f>
         <v/>
       </c>
@@ -5995,9 +6123,9 @@
       <c r="P104" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="Q104" s="159"/>
-      <c r="R104" s="160"/>
-      <c r="S104" s="161" t="str">
+      <c r="Q104" s="157"/>
+      <c r="R104" s="158"/>
+      <c r="S104" s="159" t="str">
         <f>IF(AB55="","",AB55)</f>
         <v/>
       </c>
@@ -6011,7 +6139,7 @@
         <v>39</v>
       </c>
       <c r="B105" s="10"/>
-      <c r="D105" s="134" t="str">
+      <c r="D105" s="132" t="str">
         <f>IF(LEN(Q114)&lt;=265,"",RIGHT(Q114,LEN(Q114)-SEARCH(" ",Q114,255)))</f>
         <v/>
       </c>
@@ -6029,13 +6157,13 @@
         <v>66</v>
       </c>
       <c r="Q105" s="94"/>
-      <c r="R105" s="162">
+      <c r="R105" s="160">
         <f>LEN(Q104)</f>
         <v>0</v>
       </c>
       <c r="S105" s="77"/>
       <c r="T105" s="77"/>
-      <c r="U105" s="163"/>
+      <c r="U105" s="161"/>
       <c r="V105" s="77"/>
       <c r="W105" s="77"/>
       <c r="X105" s="77"/>
@@ -6046,7 +6174,7 @@
         <v>40</v>
       </c>
       <c r="B106" s="10"/>
-      <c r="D106" s="134" t="str">
+      <c r="D106" s="132" t="str">
         <f>IF(Q116="","",IF(LEN(Q116)&lt;=135,Q116,IF(LEN(Q116)&lt;=260,LEFT(Q116,SEARCH(" ",Q116,125)),LEFT(Q116,SEARCH(" ",Q116,130)))))</f>
         <v/>
       </c>
@@ -6063,9 +6191,9 @@
       <c r="P106" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="Q106" s="159"/>
-      <c r="R106" s="160"/>
-      <c r="S106" s="161" t="str">
+      <c r="Q106" s="157"/>
+      <c r="R106" s="158"/>
+      <c r="S106" s="159" t="str">
         <f>IF(AB57="","",AB57)</f>
         <v/>
       </c>
@@ -6079,7 +6207,7 @@
         <v>41</v>
       </c>
       <c r="B107" s="10"/>
-      <c r="D107" s="134" t="str">
+      <c r="D107" s="132" t="str">
         <f>IF(LEN(Q116)&lt;=135,"",IF(LEN(Q116)&lt;=260,RIGHT(Q116,LEN(Q116)-SEARCH(" ",Q116,125)),MID(Q116,SEARCH(" ",Q116,130),IF(LEN(Q116)&lt;=265,LEN(Q116),SEARCH(" ",Q116,255)-SEARCH(" ",Q116,130)))))</f>
         <v/>
       </c>
@@ -6097,13 +6225,13 @@
         <v>66</v>
       </c>
       <c r="Q107" s="94"/>
-      <c r="R107" s="162">
+      <c r="R107" s="160">
         <f>LEN(Q106)</f>
         <v>0</v>
       </c>
       <c r="S107" s="77"/>
       <c r="T107" s="77"/>
-      <c r="U107" s="163"/>
+      <c r="U107" s="161"/>
       <c r="V107" s="77"/>
       <c r="W107" s="77"/>
       <c r="X107" s="77"/>
@@ -6114,7 +6242,7 @@
         <v>42</v>
       </c>
       <c r="B108" s="10"/>
-      <c r="D108" s="134" t="str">
+      <c r="D108" s="132" t="str">
         <f>IF(LEN(Q116)&lt;=265,"",RIGHT(Q116,LEN(Q116)-SEARCH(" ",Q116,255)))</f>
         <v/>
       </c>
@@ -6131,9 +6259,9 @@
       <c r="P108" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="Q108" s="159"/>
-      <c r="R108" s="160"/>
-      <c r="S108" s="161" t="str">
+      <c r="Q108" s="157"/>
+      <c r="R108" s="158"/>
+      <c r="S108" s="159" t="str">
         <f>IF(AB59="","",AB59)</f>
         <v/>
       </c>
@@ -6147,7 +6275,7 @@
         <v>43</v>
       </c>
       <c r="B109" s="10"/>
-      <c r="D109" s="134" t="str">
+      <c r="D109" s="132" t="str">
         <f>IF(Q118="","",IF(LEN(Q118)&lt;=135,Q118,IF(LEN(Q118)&lt;=260,LEFT(Q118,SEARCH(" ",Q118,125)),LEFT(Q118,SEARCH(" ",Q118,130)))))</f>
         <v/>
       </c>
@@ -6165,13 +6293,13 @@
         <v>66</v>
       </c>
       <c r="Q109" s="94"/>
-      <c r="R109" s="162">
+      <c r="R109" s="160">
         <f>LEN(Q108)</f>
         <v>0</v>
       </c>
       <c r="S109" s="77"/>
       <c r="T109" s="77"/>
-      <c r="U109" s="163"/>
+      <c r="U109" s="161"/>
       <c r="V109" s="77"/>
       <c r="W109" s="77"/>
       <c r="X109" s="77"/>
@@ -6182,7 +6310,7 @@
         <v>44</v>
       </c>
       <c r="B110" s="10"/>
-      <c r="D110" s="134" t="str">
+      <c r="D110" s="132" t="str">
         <f>IF(LEN(Q118)&lt;=135,"",IF(LEN(Q118)&lt;=260,RIGHT(Q118,LEN(Q118)-SEARCH(" ",Q118,125)),MID(Q118,SEARCH(" ",Q118,130),IF(LEN(Q118)&lt;=265,LEN(Q118),SEARCH(" ",Q118,255)-SEARCH(" ",Q118,130)))))</f>
         <v/>
       </c>
@@ -6199,9 +6327,9 @@
       <c r="P110" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="Q110" s="159"/>
-      <c r="R110" s="160"/>
-      <c r="S110" s="161" t="str">
+      <c r="Q110" s="157"/>
+      <c r="R110" s="158"/>
+      <c r="S110" s="159" t="str">
         <f>IF(AB61="","",AB61)</f>
         <v/>
       </c>
@@ -6215,7 +6343,7 @@
         <v>45</v>
       </c>
       <c r="B111" s="10"/>
-      <c r="D111" s="134" t="str">
+      <c r="D111" s="132" t="str">
         <f>IF(LEN(Q118)&lt;=265,"",RIGHT(Q118,LEN(Q118)-SEARCH(" ",Q118,255)))</f>
         <v/>
       </c>
@@ -6233,7 +6361,7 @@
         <v>66</v>
       </c>
       <c r="Q111" s="94"/>
-      <c r="R111" s="162">
+      <c r="R111" s="160">
         <f>LEN(Q110)</f>
         <v>0</v>
       </c>
@@ -6250,7 +6378,7 @@
         <v>46</v>
       </c>
       <c r="B112" s="10"/>
-      <c r="D112" s="134" t="str">
+      <c r="D112" s="132" t="str">
         <f>IF(Q120="","",IF(LEN(Q120)&lt;=135,Q120,IF(LEN(Q120)&lt;=260,LEFT(Q120,SEARCH(" ",Q120,125)),LEFT(Q120,SEARCH(" ",Q120,130)))))</f>
         <v/>
       </c>
@@ -6267,9 +6395,9 @@
       <c r="P112" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="Q112" s="159"/>
-      <c r="R112" s="160"/>
-      <c r="S112" s="161" t="str">
+      <c r="Q112" s="157"/>
+      <c r="R112" s="158"/>
+      <c r="S112" s="159" t="str">
         <f>IF(AB63="","",AB63)</f>
         <v/>
       </c>
@@ -6283,7 +6411,7 @@
         <v>47</v>
       </c>
       <c r="B113" s="10"/>
-      <c r="D113" s="134" t="str">
+      <c r="D113" s="132" t="str">
         <f>IF(LEN(Q120)&lt;=135,"",IF(LEN(Q120)&lt;=260,RIGHT(Q120,LEN(Q120)-SEARCH(" ",Q120,125)),MID(Q120,SEARCH(" ",Q120,130),IF(LEN(Q120)&lt;=265,LEN(Q120),SEARCH(" ",Q120,255)-SEARCH(" ",Q120,130)))))</f>
         <v/>
       </c>
@@ -6301,7 +6429,7 @@
         <v>66</v>
       </c>
       <c r="Q113" s="94"/>
-      <c r="R113" s="162">
+      <c r="R113" s="160">
         <f>LEN(Q112)</f>
         <v>0</v>
       </c>
@@ -6318,7 +6446,7 @@
         <v>48</v>
       </c>
       <c r="B114" s="10"/>
-      <c r="D114" s="134" t="str">
+      <c r="D114" s="132" t="str">
         <f>IF(LEN(Q120)&lt;=265,"",RIGHT(Q120,LEN(Q120)-SEARCH(" ",Q120,255)))</f>
         <v/>
       </c>
@@ -6335,9 +6463,9 @@
       <c r="P114" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="Q114" s="159"/>
-      <c r="R114" s="160"/>
-      <c r="S114" s="161" t="str">
+      <c r="Q114" s="157"/>
+      <c r="R114" s="158"/>
+      <c r="S114" s="159" t="str">
         <f>IF(AB65="","",AB65)</f>
         <v/>
       </c>
@@ -6357,7 +6485,7 @@
         <v>66</v>
       </c>
       <c r="Q115" s="94"/>
-      <c r="R115" s="162">
+      <c r="R115" s="160">
         <f>LEN(Q114)</f>
         <v>0</v>
       </c>
@@ -6379,9 +6507,9 @@
       <c r="P116" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="Q116" s="159"/>
-      <c r="R116" s="160"/>
-      <c r="S116" s="161" t="str">
+      <c r="Q116" s="157"/>
+      <c r="R116" s="158"/>
+      <c r="S116" s="159" t="str">
         <f>IF(AB67="","",AB67)</f>
         <v/>
       </c>
@@ -6401,7 +6529,7 @@
         <v>66</v>
       </c>
       <c r="Q117" s="94"/>
-      <c r="R117" s="162">
+      <c r="R117" s="160">
         <f>LEN(Q116)</f>
         <v>0</v>
       </c>
@@ -6423,9 +6551,9 @@
       <c r="P118" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="Q118" s="159"/>
-      <c r="R118" s="160"/>
-      <c r="S118" s="161" t="str">
+      <c r="Q118" s="157"/>
+      <c r="R118" s="158"/>
+      <c r="S118" s="159" t="str">
         <f>IF(AB69="","",AB69)</f>
         <v/>
       </c>
@@ -6445,7 +6573,7 @@
         <v>66</v>
       </c>
       <c r="Q119" s="94"/>
-      <c r="R119" s="162">
+      <c r="R119" s="160">
         <f>LEN(Q118)</f>
         <v>0</v>
       </c>
@@ -6467,9 +6595,9 @@
       <c r="P120" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="Q120" s="159"/>
-      <c r="R120" s="160"/>
-      <c r="S120" s="161" t="str">
+      <c r="Q120" s="157"/>
+      <c r="R120" s="158"/>
+      <c r="S120" s="159" t="str">
         <f>IF(AB71="","",AB71)</f>
         <v/>
       </c>
@@ -6489,7 +6617,7 @@
         <v>66</v>
       </c>
       <c r="Q121" s="94"/>
-      <c r="R121" s="162">
+      <c r="R121" s="160">
         <f>LEN(Q120)</f>
         <v>0</v>
       </c>
@@ -6592,14 +6720,14 @@
       <c r="C131" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D131" s="193" t="str">
+      <c r="D131" s="163" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
       <c r="L131" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="M131" s="118" t="str">
+      <c r="M131" s="116" t="str">
         <f>IF($X$7="","",$X$7)</f>
         <v>Eugene Mah</v>
       </c>
@@ -6611,58 +6739,20 @@
       <c r="C132" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="D132" s="119" t="str">
+      <c r="D132" s="117" t="str">
         <f>IF($J$12="","",$J$12)</f>
         <v/>
       </c>
       <c r="L132" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="M132" s="120" t="str">
+      <c r="M132" s="118" t="str">
         <f>IF($R$13="","",$R$13)</f>
         <v/>
       </c>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="AG1:AJ1"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="F19:L19"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="I54:L54"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="I56:J56"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="V69:W69"/>
-    <mergeCell ref="Q70:Q71"/>
-    <mergeCell ref="R70:R71"/>
-    <mergeCell ref="S70:S71"/>
-    <mergeCell ref="V70:V71"/>
-    <mergeCell ref="W70:W71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="Q72:Q73"/>
-    <mergeCell ref="R72:R73"/>
-    <mergeCell ref="S72:S73"/>
     <mergeCell ref="Q83:R83"/>
     <mergeCell ref="S83:T83"/>
     <mergeCell ref="V72:V73"/>
@@ -6672,6 +6762,44 @@
     <mergeCell ref="S74:S75"/>
     <mergeCell ref="V74:V75"/>
     <mergeCell ref="W74:W75"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="Q72:Q73"/>
+    <mergeCell ref="R72:R73"/>
+    <mergeCell ref="S72:S73"/>
+    <mergeCell ref="V69:W69"/>
+    <mergeCell ref="Q70:Q71"/>
+    <mergeCell ref="R70:R71"/>
+    <mergeCell ref="S70:S71"/>
+    <mergeCell ref="V70:V71"/>
+    <mergeCell ref="W70:W71"/>
+    <mergeCell ref="I56:J56"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="I54:L54"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="F19:L19"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="AG1:AJ1"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="J10:K10"/>
   </mergeCells>
   <conditionalFormatting sqref="I72:I74">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
@@ -6690,35 +6818,35 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F56:G58 F42:G42">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"NO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"YES"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
-      <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D76:G76">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"FAIL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"PASS"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D75:G75 Q92:T92">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>0.3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>0.3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:E23">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"NO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"YES"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.92638888888888904" header="0.51180555555555496" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
Fix cell formatting and references
</commit_message>
<xml_diff>
--- a/MUSCMammoMonitor.xlsx
+++ b/MUSCMammoMonitor.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugenem\Documents\GitHub\EquipTestingSpreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D86285C-5C96-4B5B-8074-696614E77EB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Barco" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Barco!$B$1:$M$132</definedName>
     <definedName name="Z_B8088769_C3DE_4DF8_A82B_D0EB46FFCC4A_.wvu.PrintArea" localSheetId="0" hidden="1">Barco!$B$1:$M$132</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <customWorkbookViews>
     <customWorkbookView name="Eugene Mah - Personal View" guid="{B8088769-C3DE-4DF8-A82B-D0EB46FFCC4A}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="784" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
@@ -27,6 +28,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -37,12 +41,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Eugene Mah</author>
   </authors>
   <commentList>
-    <comment ref="Q59" authorId="0" shapeId="0">
+    <comment ref="Q59" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -66,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q88" authorId="0" shapeId="0">
+    <comment ref="Q88" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -95,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="184">
   <si>
     <t>Print Area</t>
   </si>
@@ -652,7 +656,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="dd\-mmm\-yy"/>
@@ -1590,7 +1594,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="236">
+  <cellXfs count="237">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2093,18 +2097,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="47" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="39" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2138,12 +2133,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2174,12 +2163,6 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2189,20 +2172,68 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2237,76 +2268,52 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="47" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="39" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Fail" xfId="6"/>
-    <cellStyle name="Heading" xfId="3"/>
-    <cellStyle name="Heading1" xfId="4"/>
+    <cellStyle name="Fail" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Heading" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Heading1" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Pass" xfId="5"/>
+    <cellStyle name="Pass" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Percent" xfId="7" builtinId="5"/>
-    <cellStyle name="Result" xfId="1"/>
-    <cellStyle name="Result2" xfId="2"/>
+    <cellStyle name="Result" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Result2" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -2822,24 +2829,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="2" width="2.5703125" style="1" customWidth="1"/>
-    <col min="3" max="11" width="11.5703125" style="1"/>
-    <col min="12" max="12" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" style="1"/>
-    <col min="14" max="14" width="2.5703125" style="1" customWidth="1"/>
-    <col min="15" max="36" width="11.5703125" style="1"/>
+    <col min="1" max="2" width="2.5546875" style="1" customWidth="1"/>
+    <col min="3" max="11" width="11.5546875" style="1"/>
+    <col min="12" max="12" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5546875" style="1"/>
+    <col min="14" max="14" width="2.5546875" style="1" customWidth="1"/>
+    <col min="15" max="36" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="14.45" customHeight="1">
+    <row r="1" spans="1:36" ht="14.4" customHeight="1">
       <c r="A1" s="2">
         <v>1</v>
       </c>
@@ -2871,14 +2878,14 @@
       <c r="AA1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="AG1" s="232" t="s">
+      <c r="AG1" s="194" t="s">
         <v>1</v>
       </c>
-      <c r="AH1" s="232"/>
-      <c r="AI1" s="232"/>
-      <c r="AJ1" s="232"/>
-    </row>
-    <row r="2" spans="1:36" ht="14.45" customHeight="1">
+      <c r="AH1" s="194"/>
+      <c r="AI1" s="194"/>
+      <c r="AJ1" s="194"/>
+    </row>
+    <row r="2" spans="1:36" ht="14.4" customHeight="1">
       <c r="A2" s="2">
         <v>2</v>
       </c>
@@ -2893,16 +2900,16 @@
       </c>
       <c r="Y2" s="14"/>
       <c r="AA2" s="15"/>
-      <c r="AG2" s="233" t="s">
+      <c r="AG2" s="195" t="s">
         <v>3</v>
       </c>
-      <c r="AH2" s="233"/>
-      <c r="AI2" s="234" t="s">
+      <c r="AH2" s="195"/>
+      <c r="AI2" s="196" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="234"/>
-    </row>
-    <row r="3" spans="1:36" ht="14.45" customHeight="1">
+      <c r="AJ2" s="196"/>
+    </row>
+    <row r="3" spans="1:36" ht="14.4" customHeight="1">
       <c r="A3" s="2">
         <v>3</v>
       </c>
@@ -2933,7 +2940,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="14.45" customHeight="1">
+    <row r="4" spans="1:36" ht="14.4" customHeight="1">
       <c r="A4" s="2">
         <v>4</v>
       </c>
@@ -2963,7 +2970,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="14.45" customHeight="1">
+    <row r="5" spans="1:36" ht="14.4" customHeight="1">
       <c r="A5" s="2">
         <v>5</v>
       </c>
@@ -2993,7 +3000,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="14.45" customHeight="1">
+    <row r="6" spans="1:36" ht="14.4" customHeight="1">
       <c r="A6" s="2">
         <v>6</v>
       </c>
@@ -3042,7 +3049,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="14.45" customHeight="1">
+    <row r="7" spans="1:36" ht="14.4" customHeight="1">
       <c r="A7" s="2">
         <v>7</v>
       </c>
@@ -3089,7 +3096,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="14.45" customHeight="1">
+    <row r="8" spans="1:36" ht="14.4" customHeight="1">
       <c r="A8" s="2">
         <v>8</v>
       </c>
@@ -3134,7 +3141,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="14.45" customHeight="1">
+    <row r="9" spans="1:36" ht="14.4" customHeight="1">
       <c r="A9" s="2">
         <v>9</v>
       </c>
@@ -3186,7 +3193,7 @@
       </c>
       <c r="AG9" s="2"/>
     </row>
-    <row r="10" spans="1:36" ht="14.45" customHeight="1">
+    <row r="10" spans="1:36" ht="14.4" customHeight="1">
       <c r="A10" s="2">
         <v>10</v>
       </c>
@@ -3194,19 +3201,19 @@
       <c r="D10" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="235" t="str">
+      <c r="E10" s="197" t="str">
         <f t="shared" ref="E10:E15" si="1">IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="F10" s="235"/>
+      <c r="F10" s="197"/>
       <c r="I10" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="235" t="str">
+      <c r="J10" s="197" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="K10" s="235"/>
+      <c r="K10" s="197"/>
       <c r="M10" s="12"/>
       <c r="O10" s="13"/>
       <c r="Q10" s="21" t="s">
@@ -3241,7 +3248,7 @@
       <c r="AF10" s="2"/>
       <c r="AG10" s="2"/>
     </row>
-    <row r="11" spans="1:36" ht="14.45" customHeight="1">
+    <row r="11" spans="1:36" ht="14.4" customHeight="1">
       <c r="A11" s="2">
         <v>11</v>
       </c>
@@ -3249,19 +3256,19 @@
       <c r="D11" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="228" t="str">
+      <c r="E11" s="198" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F11" s="228"/>
+      <c r="F11" s="198"/>
       <c r="I11" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="231" t="str">
+      <c r="J11" s="199" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="K11" s="231"/>
+      <c r="K11" s="199"/>
       <c r="M11" s="12"/>
       <c r="O11" s="13"/>
       <c r="Q11" s="21" t="s">
@@ -3293,14 +3300,14 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="AF11" s="185" t="s">
+      <c r="AF11" s="180" t="s">
         <v>156</v>
       </c>
-      <c r="AG11" s="185" t="s">
+      <c r="AG11" s="180" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="14.45" customHeight="1">
+    <row r="12" spans="1:36" ht="14.4" customHeight="1">
       <c r="A12" s="2">
         <v>12</v>
       </c>
@@ -3308,19 +3315,19 @@
       <c r="D12" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="228" t="str">
+      <c r="E12" s="198" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F12" s="228"/>
+      <c r="F12" s="198"/>
       <c r="I12" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="228" t="str">
+      <c r="J12" s="198" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="K12" s="228"/>
+      <c r="K12" s="198"/>
       <c r="M12" s="12"/>
       <c r="O12" s="13"/>
       <c r="Q12" s="21" t="s">
@@ -3352,11 +3359,12 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="AF12" s="1" t="s">
+      <c r="AF12" s="2" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="13" spans="1:36" ht="14.45" customHeight="1">
+      <c r="AG12" s="2"/>
+    </row>
+    <row r="13" spans="1:36" ht="14.4" customHeight="1">
       <c r="A13" s="2">
         <v>13</v>
       </c>
@@ -3364,19 +3372,19 @@
       <c r="D13" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="228" t="str">
+      <c r="E13" s="198" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F13" s="228"/>
+      <c r="F13" s="198"/>
       <c r="I13" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="228" t="str">
+      <c r="J13" s="198" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="K13" s="228"/>
+      <c r="K13" s="198"/>
       <c r="M13" s="12"/>
       <c r="O13" s="13"/>
       <c r="Q13" s="21" t="s">
@@ -3411,8 +3419,9 @@
       <c r="AF13" s="2" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="14" spans="1:36" ht="14.45" customHeight="1">
+      <c r="AG13" s="2"/>
+    </row>
+    <row r="14" spans="1:36" ht="14.4" customHeight="1">
       <c r="A14" s="2">
         <v>14</v>
       </c>
@@ -3420,19 +3429,19 @@
       <c r="D14" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="228" t="str">
+      <c r="E14" s="198" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F14" s="228"/>
+      <c r="F14" s="198"/>
       <c r="I14" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="228" t="str">
+      <c r="J14" s="198" t="str">
         <f>IF(V14="","",V14)</f>
         <v/>
       </c>
-      <c r="K14" s="228"/>
+      <c r="K14" s="198"/>
       <c r="M14" s="12"/>
       <c r="O14" s="13"/>
       <c r="Q14" s="21" t="s">
@@ -3467,8 +3476,9 @@
       <c r="AF14" s="2" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="15" spans="1:36" ht="14.45" customHeight="1" thickBot="1">
+      <c r="AG14" s="2"/>
+    </row>
+    <row r="15" spans="1:36" ht="14.4" customHeight="1" thickBot="1">
       <c r="A15" s="2">
         <v>15</v>
       </c>
@@ -3476,11 +3486,11 @@
       <c r="D15" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="228" t="str">
+      <c r="E15" s="198" t="str">
         <f t="shared" si="1"/>
         <v>IMPAX 4.2 2015</v>
       </c>
-      <c r="F15" s="228"/>
+      <c r="F15" s="198"/>
       <c r="M15" s="12"/>
       <c r="O15" s="26"/>
       <c r="P15" s="27"/>
@@ -3515,8 +3525,9 @@
       <c r="AF15" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="16" spans="1:36" ht="14.45" customHeight="1" thickBot="1">
+      <c r="AG15" s="2"/>
+    </row>
+    <row r="16" spans="1:36" ht="14.4" customHeight="1" thickBot="1">
       <c r="A16" s="2">
         <v>16</v>
       </c>
@@ -3547,8 +3558,9 @@
       <c r="AF16" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="17" spans="1:32" ht="14.45" customHeight="1" thickTop="1" thickBot="1">
+      <c r="AG16" s="2"/>
+    </row>
+    <row r="17" spans="1:33" ht="14.4" customHeight="1" thickTop="1" thickBot="1">
       <c r="A17" s="2">
         <v>17</v>
       </c>
@@ -3576,8 +3588,9 @@
       <c r="AF17" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="18" spans="1:32" ht="14.45" customHeight="1" thickBot="1">
+      <c r="AG17" s="2"/>
+    </row>
+    <row r="18" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
       <c r="A18" s="2">
         <v>18</v>
       </c>
@@ -3614,8 +3627,9 @@
       <c r="AF18" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="19" spans="1:32" ht="14.45" customHeight="1" thickTop="1">
+      <c r="AG18" s="2"/>
+    </row>
+    <row r="19" spans="1:33" ht="14.4" customHeight="1" thickTop="1">
       <c r="A19" s="2">
         <v>19</v>
       </c>
@@ -3630,10 +3644,10 @@
       <c r="H19" s="154"/>
       <c r="I19" s="154"/>
       <c r="J19" s="154"/>
-      <c r="K19" s="230" t="s">
+      <c r="K19" s="201" t="s">
         <v>129</v>
       </c>
-      <c r="L19" s="230"/>
+      <c r="L19" s="201"/>
       <c r="M19" s="5"/>
       <c r="O19" s="13"/>
       <c r="R19" s="1" t="s">
@@ -3661,8 +3675,9 @@
       <c r="AF19" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="20" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG19" s="2"/>
+    </row>
+    <row r="20" spans="1:33" ht="14.4" customHeight="1">
       <c r="A20" s="2">
         <v>20</v>
       </c>
@@ -3725,8 +3740,9 @@
       <c r="AF20" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="21" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG20" s="2"/>
+    </row>
+    <row r="21" spans="1:33" ht="14.4" customHeight="1">
       <c r="A21" s="2">
         <v>21</v>
       </c>
@@ -3780,8 +3796,9 @@
       <c r="AF21" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="22" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG21" s="2"/>
+    </row>
+    <row r="22" spans="1:33" ht="14.4" customHeight="1">
       <c r="A22" s="2">
         <v>22</v>
       </c>
@@ -3835,8 +3852,9 @@
       <c r="AF22" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="23" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG22" s="2"/>
+    </row>
+    <row r="23" spans="1:33" ht="14.4" customHeight="1">
       <c r="A23" s="2">
         <v>23</v>
       </c>
@@ -3889,8 +3907,9 @@
       <c r="AF23" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="24" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG23" s="2"/>
+    </row>
+    <row r="24" spans="1:33" ht="14.4" customHeight="1">
       <c r="A24" s="2">
         <v>24</v>
       </c>
@@ -3898,11 +3917,11 @@
       <c r="D24" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="229" t="str">
+      <c r="E24" s="200" t="str">
         <f>IF(P52="","",P52)</f>
         <v/>
       </c>
-      <c r="F24" s="229"/>
+      <c r="F24" s="200"/>
       <c r="G24" s="40"/>
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
@@ -3927,8 +3946,9 @@
       <c r="AF24" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="25" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG24" s="2"/>
+    </row>
+    <row r="25" spans="1:33" ht="14.4" customHeight="1">
       <c r="A25" s="2">
         <v>25</v>
       </c>
@@ -3959,8 +3979,9 @@
       <c r="AF25" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="26" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG25" s="2"/>
+    </row>
+    <row r="26" spans="1:33" ht="14.4" customHeight="1">
       <c r="A26" s="2">
         <v>26</v>
       </c>
@@ -3979,7 +4000,7 @@
       <c r="S26" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="T26" s="85" t="str">
+      <c r="T26" s="232" t="str">
         <f>IF(AG12="","",AG12)</f>
         <v/>
       </c>
@@ -3990,8 +4011,9 @@
       <c r="AF26" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="27" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG26" s="2"/>
+    </row>
+    <row r="27" spans="1:33" ht="14.4" customHeight="1">
       <c r="A27" s="2">
         <v>27</v>
       </c>
@@ -4049,8 +4071,9 @@
       <c r="AF27" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="28" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG27" s="2"/>
+    </row>
+    <row r="28" spans="1:33" ht="14.4" customHeight="1">
       <c r="A28" s="2">
         <v>28</v>
       </c>
@@ -4058,7 +4081,7 @@
       <c r="C28" s="52" t="s">
         <v>144</v>
       </c>
-      <c r="D28" s="168" t="str">
+      <c r="D28" s="144" t="str">
         <f>IF(T26="","",T26)</f>
         <v/>
       </c>
@@ -4089,8 +4112,9 @@
       <c r="AF28" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="29" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG28" s="2"/>
+    </row>
+    <row r="29" spans="1:33" ht="14.4" customHeight="1">
       <c r="A29" s="2">
         <v>29</v>
       </c>
@@ -4140,8 +4164,9 @@
       <c r="AF29" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="30" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG29" s="2"/>
+    </row>
+    <row r="30" spans="1:33" ht="14.4" customHeight="1">
       <c r="A30" s="2">
         <v>30</v>
       </c>
@@ -4191,8 +4216,9 @@
       <c r="AF30" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="31" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG30" s="2"/>
+    </row>
+    <row r="31" spans="1:33" ht="14.4" customHeight="1">
       <c r="A31" s="2">
         <v>31</v>
       </c>
@@ -4239,8 +4265,9 @@
       <c r="AF31" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="32" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG31" s="2"/>
+    </row>
+    <row r="32" spans="1:33" ht="14.4" customHeight="1">
       <c r="A32" s="2">
         <v>32</v>
       </c>
@@ -4282,8 +4309,9 @@
       <c r="AF32" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="33" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG32" s="2"/>
+    </row>
+    <row r="33" spans="1:33" ht="14.4" customHeight="1">
       <c r="A33" s="2">
         <v>33</v>
       </c>
@@ -4333,8 +4361,9 @@
       <c r="AF33" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="34" spans="1:32" ht="14.45" customHeight="1" thickBot="1">
+      <c r="AG33" s="2"/>
+    </row>
+    <row r="34" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
       <c r="A34" s="2">
         <v>34</v>
       </c>
@@ -4395,8 +4424,9 @@
       <c r="AF34" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="35" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG34" s="2"/>
+    </row>
+    <row r="35" spans="1:33" ht="14.4" customHeight="1">
       <c r="A35" s="2">
         <v>35</v>
       </c>
@@ -4452,8 +4482,9 @@
       <c r="AF35" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="36" spans="1:32" ht="14.45" customHeight="1" thickBot="1">
+      <c r="AG35" s="2"/>
+    </row>
+    <row r="36" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
       <c r="A36" s="2">
         <v>36</v>
       </c>
@@ -4509,8 +4540,9 @@
       <c r="AF36" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="37" spans="1:32" ht="14.45" customHeight="1" thickBot="1">
+      <c r="AG36" s="2"/>
+    </row>
+    <row r="37" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
       <c r="A37" s="2">
         <v>37</v>
       </c>
@@ -4565,8 +4597,9 @@
       <c r="AF37" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="38" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG37" s="2"/>
+    </row>
+    <row r="38" spans="1:33" ht="14.4" customHeight="1">
       <c r="A38" s="2">
         <v>38</v>
       </c>
@@ -4611,8 +4644,9 @@
       <c r="AF38" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="39" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG38" s="2"/>
+    </row>
+    <row r="39" spans="1:33" ht="14.4" customHeight="1">
       <c r="A39" s="2">
         <v>39</v>
       </c>
@@ -4662,8 +4696,9 @@
       <c r="AF39" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="40" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG39" s="2"/>
+    </row>
+    <row r="40" spans="1:33" ht="14.4" customHeight="1">
       <c r="A40" s="2">
         <v>40</v>
       </c>
@@ -4710,8 +4745,9 @@
       <c r="AF40" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="41" spans="1:32" ht="14.45" customHeight="1" thickBot="1">
+      <c r="AG40" s="2"/>
+    </row>
+    <row r="41" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
       <c r="A41" s="2">
         <v>41</v>
       </c>
@@ -4757,8 +4793,9 @@
       <c r="AF41" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="42" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG41" s="2"/>
+    </row>
+    <row r="42" spans="1:33" ht="14.4" customHeight="1">
       <c r="A42" s="2">
         <v>42</v>
       </c>
@@ -4811,8 +4848,9 @@
       <c r="AF42" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="43" spans="1:32" ht="14.45" customHeight="1" thickBot="1">
+      <c r="AG42" s="2"/>
+    </row>
+    <row r="43" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
       <c r="A43" s="2">
         <v>43</v>
       </c>
@@ -4868,8 +4906,9 @@
       <c r="AF43" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="44" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG43" s="2"/>
+    </row>
+    <row r="44" spans="1:33" ht="14.4" customHeight="1">
       <c r="A44" s="2">
         <v>44</v>
       </c>
@@ -4920,8 +4959,9 @@
       <c r="AF44" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="45" spans="1:32" ht="14.45" customHeight="1" thickBot="1">
+      <c r="AG44" s="2"/>
+    </row>
+    <row r="45" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
       <c r="A45" s="2">
         <v>45</v>
       </c>
@@ -4974,8 +5014,9 @@
       <c r="AF45" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="46" spans="1:32" ht="14.45" customHeight="1" thickBot="1">
+      <c r="AG45" s="2"/>
+    </row>
+    <row r="46" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
       <c r="A46" s="2">
         <v>46</v>
       </c>
@@ -5022,8 +5063,9 @@
       <c r="AF46" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="47" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG46" s="2"/>
+    </row>
+    <row r="47" spans="1:33" ht="14.4" customHeight="1">
       <c r="A47" s="2">
         <v>47</v>
       </c>
@@ -5064,8 +5106,9 @@
       <c r="AF47" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="48" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG47" s="2"/>
+    </row>
+    <row r="48" spans="1:33" ht="14.4" customHeight="1">
       <c r="A48" s="2">
         <v>48</v>
       </c>
@@ -5114,8 +5157,9 @@
       <c r="AF48" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="49" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG48" s="2"/>
+    </row>
+    <row r="49" spans="1:33" ht="14.4" customHeight="1">
       <c r="A49" s="2">
         <v>49</v>
       </c>
@@ -5163,8 +5207,9 @@
       <c r="AF49" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="50" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG49" s="2"/>
+    </row>
+    <row r="50" spans="1:33" ht="14.4" customHeight="1">
       <c r="A50" s="2">
         <v>50</v>
       </c>
@@ -5220,8 +5265,9 @@
       <c r="AF50" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="51" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG50" s="2"/>
+    </row>
+    <row r="51" spans="1:33" ht="14.4" customHeight="1">
       <c r="A51" s="2">
         <v>51</v>
       </c>
@@ -5241,7 +5287,7 @@
         <f>R58</f>
         <v>Right ()</v>
       </c>
-      <c r="J51" s="204" t="str">
+      <c r="J51" s="193" t="str">
         <f>IF(R60="","",R60)</f>
         <v/>
       </c>
@@ -5281,15 +5327,16 @@
       <c r="AF51" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="52" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AG51" s="2"/>
+    </row>
+    <row r="52" spans="1:33" ht="14.4" customHeight="1">
       <c r="A52" s="2">
         <v>52</v>
       </c>
       <c r="B52" s="10"/>
       <c r="F52" s="95"/>
       <c r="I52" s="62"/>
-      <c r="J52" s="199"/>
+      <c r="J52" s="192"/>
       <c r="M52" s="12"/>
       <c r="O52" s="84" t="s">
         <v>20</v>
@@ -5321,13 +5368,14 @@
       <c r="AF52" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="53" spans="1:32" ht="14.45" customHeight="1" thickBot="1">
+      <c r="AG52" s="2"/>
+    </row>
+    <row r="53" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
       <c r="A53" s="2">
         <v>53</v>
       </c>
       <c r="B53" s="10"/>
-      <c r="E53" s="199" t="str">
+      <c r="E53" s="192" t="str">
         <f>Q58</f>
         <v>Left ()</v>
       </c>
@@ -5366,8 +5414,12 @@
         <f>IF(S77="","",S77)</f>
         <v/>
       </c>
-    </row>
-    <row r="54" spans="1:32" ht="14.45" customHeight="1">
+      <c r="AF53" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AG53" s="2"/>
+    </row>
+    <row r="54" spans="1:33" ht="14.4" customHeight="1">
       <c r="A54" s="2">
         <v>54</v>
       </c>
@@ -5375,11 +5427,11 @@
       <c r="D54" s="52" t="s">
         <v>178</v>
       </c>
-      <c r="E54" s="200" t="str">
+      <c r="E54" s="233" t="str">
         <f>IF(Q61="","",Q61)</f>
         <v/>
       </c>
-      <c r="F54" s="201" t="str">
+      <c r="F54" s="234" t="str">
         <f>IF(R61="","",R61)</f>
         <v/>
       </c>
@@ -5401,7 +5453,7 @@
       <c r="X54" s="78"/>
       <c r="Y54" s="14"/>
     </row>
-    <row r="55" spans="1:32" ht="14.45" customHeight="1" thickBot="1">
+    <row r="55" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
       <c r="A55" s="2">
         <v>55</v>
       </c>
@@ -5409,11 +5461,11 @@
       <c r="D55" s="52" t="s">
         <v>179</v>
       </c>
-      <c r="E55" s="202" t="str">
+      <c r="E55" s="235" t="str">
         <f>IF(Q62="","",Q62)</f>
         <v/>
       </c>
-      <c r="F55" s="203" t="str">
+      <c r="F55" s="236" t="str">
         <f>IF(R62="","",R62)</f>
         <v/>
       </c>
@@ -5438,7 +5490,7 @@
       <c r="AC55" s="20"/>
       <c r="AD55" s="20"/>
     </row>
-    <row r="56" spans="1:32" ht="14.45" customHeight="1">
+    <row r="56" spans="1:33" ht="14.4" customHeight="1">
       <c r="A56" s="2">
         <v>56</v>
       </c>
@@ -5468,7 +5520,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:32" ht="14.45" customHeight="1">
+    <row r="57" spans="1:33" ht="14.4" customHeight="1">
       <c r="A57" s="2">
         <v>57</v>
       </c>
@@ -5515,7 +5567,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:32" ht="14.45" customHeight="1" thickBot="1">
+    <row r="58" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
       <c r="A58" s="2">
         <v>58</v>
       </c>
@@ -5574,7 +5626,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:32" ht="14.45" customHeight="1">
+    <row r="59" spans="1:33" ht="14.4" customHeight="1">
       <c r="A59" s="2">
         <v>59</v>
       </c>
@@ -5597,23 +5649,23 @@
       <c r="P59" s="66" t="s">
         <v>147</v>
       </c>
-      <c r="Q59" s="186" t="str">
-        <f>IF(AG12="","",AG12+Lamb)</f>
-        <v/>
-      </c>
-      <c r="R59" s="187" t="str">
-        <f>IF(AG13="","",AG13+Lamb)</f>
+      <c r="Q59" s="181" t="str">
+        <f>IF(AG12="","",AG13+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R59" s="182" t="str">
+        <f>IF(AG13="","",AG14+Lamb)</f>
         <v/>
       </c>
       <c r="S59" s="2"/>
-      <c r="T59" s="182" t="s">
+      <c r="T59" s="179" t="s">
         <v>147</v>
       </c>
-      <c r="U59" s="178" t="str">
+      <c r="U59" s="175" t="str">
         <f>IF(AB31="","",AB31)</f>
         <v/>
       </c>
-      <c r="V59" s="179" t="str">
+      <c r="V59" s="176" t="str">
         <f>IF(AB32="","",AB32)</f>
         <v/>
       </c>
@@ -5633,7 +5685,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:32" ht="14.45" customHeight="1">
+    <row r="60" spans="1:33" ht="14.4" customHeight="1">
       <c r="A60" s="2">
         <v>60</v>
       </c>
@@ -5643,23 +5695,23 @@
       <c r="P60" s="66" t="s">
         <v>148</v>
       </c>
-      <c r="Q60" s="189" t="str">
-        <f>IF(AG14="","",AG14+Lamb)</f>
-        <v/>
-      </c>
-      <c r="R60" s="190" t="str">
-        <f>IF(AG15="","",AG15+Lamb)</f>
+      <c r="Q60" s="184" t="str">
+        <f>IF(AG14="","",AG15+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R60" s="185" t="str">
+        <f>IF(AG15="","",AG16+Lamb)</f>
         <v/>
       </c>
       <c r="S60" s="2"/>
-      <c r="T60" s="182" t="s">
+      <c r="T60" s="179" t="s">
         <v>148</v>
       </c>
-      <c r="U60" s="197" t="str">
+      <c r="U60" s="190" t="str">
         <f>IF(AB33="","",AB33)</f>
         <v/>
       </c>
-      <c r="V60" s="198" t="str">
+      <c r="V60" s="191" t="str">
         <f>IF(AB34="","",AB34)</f>
         <v/>
       </c>
@@ -5679,7 +5731,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:32" ht="14.45" customHeight="1">
+    <row r="61" spans="1:33" ht="14.4" customHeight="1">
       <c r="A61" s="2">
         <v>61</v>
       </c>
@@ -5689,22 +5741,22 @@
       <c r="P61" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="Q61" s="195" t="str">
+      <c r="Q61" s="225" t="str">
         <f>IF(Q59="","",Q60/Q59)</f>
         <v/>
       </c>
-      <c r="R61" s="196" t="str">
+      <c r="R61" s="226" t="str">
         <f>IF(R59="","",R60/R59)</f>
         <v/>
       </c>
       <c r="T61" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="U61" s="197" t="str">
+      <c r="U61" s="190" t="str">
         <f>IF(AB35="","",AB35)</f>
         <v/>
       </c>
-      <c r="V61" s="198" t="str">
+      <c r="V61" s="191" t="str">
         <f>IF(AB36="","",AB36)</f>
         <v/>
       </c>
@@ -5722,7 +5774,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:32" ht="14.45" customHeight="1" thickBot="1">
+    <row r="62" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
       <c r="A62" s="2">
         <v>62</v>
       </c>
@@ -5732,22 +5784,22 @@
       <c r="P62" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="Q62" s="183" t="str">
+      <c r="Q62" s="227" t="str">
         <f>IF(OR(Q59="",Lamb=""),"",Lamb/Q59)</f>
         <v/>
       </c>
-      <c r="R62" s="184" t="str">
+      <c r="R62" s="228" t="str">
         <f>IF(OR(R59="",Lamb=""),"",Lamb/R59)</f>
         <v/>
       </c>
       <c r="T62" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="U62" s="180" t="str">
+      <c r="U62" s="177" t="str">
         <f>IF(AB37="","",AB37)</f>
         <v/>
       </c>
-      <c r="V62" s="181" t="str">
+      <c r="V62" s="178" t="str">
         <f>IF(AB38="","",AB38)</f>
         <v/>
       </c>
@@ -5765,7 +5817,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:32" ht="14.45" customHeight="1">
+    <row r="63" spans="1:33" ht="14.4" customHeight="1">
       <c r="A63" s="2">
         <v>63</v>
       </c>
@@ -5775,7 +5827,7 @@
       <c r="P63" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="Q63" s="169" t="str">
+      <c r="Q63" s="168" t="str">
         <f>IF(Q65&lt;&gt;"",Q65,IF(AB67="","",AB60))</f>
         <v/>
       </c>
@@ -5791,7 +5843,7 @@
       <c r="AC63" s="20"/>
       <c r="AD63" s="20"/>
     </row>
-    <row r="64" spans="1:32" ht="14.45" customHeight="1" thickBot="1">
+    <row r="64" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
       <c r="A64" s="2">
         <v>64</v>
       </c>
@@ -5836,7 +5888,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:30" ht="14.45" customHeight="1" thickTop="1">
+    <row r="65" spans="1:30" ht="14.4" customHeight="1" thickTop="1">
       <c r="A65" s="2">
         <v>65</v>
       </c>
@@ -5871,7 +5923,7 @@
       <c r="AC65" s="20"/>
       <c r="AD65" s="20"/>
     </row>
-    <row r="66" spans="1:30" ht="14.45" customHeight="1">
+    <row r="66" spans="1:30" ht="14.4" customHeight="1">
       <c r="A66" s="2">
         <v>66</v>
       </c>
@@ -5910,7 +5962,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:30" ht="14.45" customHeight="1">
+    <row r="67" spans="1:30" ht="14.4" customHeight="1">
       <c r="A67" s="2">
         <v>1</v>
       </c>
@@ -5939,7 +5991,7 @@
       <c r="AC67" s="20"/>
       <c r="AD67" s="20"/>
     </row>
-    <row r="68" spans="1:30" ht="14.45" customHeight="1" thickBot="1">
+    <row r="68" spans="1:30" ht="14.4" customHeight="1" thickBot="1">
       <c r="A68" s="2">
         <v>2</v>
       </c>
@@ -5976,7 +6028,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:30" ht="14.45" customHeight="1" thickBot="1">
+    <row r="69" spans="1:30" ht="14.4" customHeight="1" thickBot="1">
       <c r="A69" s="2">
         <v>3</v>
       </c>
@@ -6009,7 +6061,7 @@
       <c r="AC69" s="20"/>
       <c r="AD69" s="20"/>
     </row>
-    <row r="70" spans="1:30" ht="14.45" customHeight="1" thickTop="1" thickBot="1">
+    <row r="70" spans="1:30" ht="14.4" customHeight="1" thickTop="1" thickBot="1">
       <c r="A70" s="2">
         <v>4</v>
       </c>
@@ -6050,22 +6102,22 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:30" ht="14.45" customHeight="1" thickBot="1">
+    <row r="71" spans="1:30" ht="14.4" customHeight="1" thickBot="1">
       <c r="A71" s="2">
         <v>5</v>
       </c>
       <c r="B71" s="10"/>
       <c r="C71" s="95"/>
-      <c r="D71" s="224" t="str">
+      <c r="D71" s="202" t="str">
         <f>Q86</f>
         <v>UNL-10 (cd/m^2)</v>
       </c>
-      <c r="E71" s="224"/>
-      <c r="F71" s="225" t="str">
+      <c r="E71" s="202"/>
+      <c r="F71" s="203" t="str">
         <f>S86</f>
         <v>UNL-80 (cd/m^2)</v>
       </c>
-      <c r="G71" s="225"/>
+      <c r="G71" s="203"/>
       <c r="I71" s="68" t="s">
         <v>108</v>
       </c>
@@ -6087,7 +6139,7 @@
       <c r="AC71" s="20"/>
       <c r="AD71" s="20"/>
     </row>
-    <row r="72" spans="1:30" ht="14.45" customHeight="1" thickBot="1">
+    <row r="72" spans="1:30" ht="14.4" customHeight="1" thickBot="1">
       <c r="A72" s="2">
         <v>6</v>
       </c>
@@ -6144,7 +6196,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:30" ht="14.45" customHeight="1">
+    <row r="73" spans="1:30" ht="14.4" customHeight="1">
       <c r="A73" s="2">
         <v>7</v>
       </c>
@@ -6181,15 +6233,15 @@
       <c r="Q73" s="159" t="s">
         <v>97</v>
       </c>
-      <c r="R73" s="208"/>
-      <c r="S73" s="212"/>
+      <c r="R73" s="217"/>
+      <c r="S73" s="221"/>
       <c r="T73" s="2"/>
       <c r="U73" s="2"/>
-      <c r="V73" s="219" t="str">
+      <c r="V73" s="209" t="str">
         <f>IF(AB48="","",AB48)</f>
         <v/>
       </c>
-      <c r="W73" s="220" t="str">
+      <c r="W73" s="210" t="str">
         <f>IF(AB51="","",AB51)</f>
         <v/>
       </c>
@@ -6199,7 +6251,7 @@
       <c r="AC73" s="20"/>
       <c r="AD73" s="20"/>
     </row>
-    <row r="74" spans="1:30" ht="14.45" customHeight="1">
+    <row r="74" spans="1:30" ht="14.4" customHeight="1">
       <c r="A74" s="2">
         <v>8</v>
       </c>
@@ -6234,12 +6286,12 @@
       <c r="O74" s="13"/>
       <c r="P74" s="2"/>
       <c r="Q74" s="159"/>
-      <c r="R74" s="209"/>
-      <c r="S74" s="213"/>
+      <c r="R74" s="218"/>
+      <c r="S74" s="222"/>
       <c r="T74" s="2"/>
       <c r="U74" s="2"/>
-      <c r="V74" s="218"/>
-      <c r="W74" s="221"/>
+      <c r="V74" s="208"/>
+      <c r="W74" s="211"/>
       <c r="X74" s="2"/>
       <c r="Y74" s="14"/>
       <c r="AB74" s="158"/>
@@ -6252,7 +6304,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:30" ht="14.45" customHeight="1">
+    <row r="75" spans="1:30" ht="14.4" customHeight="1">
       <c r="A75" s="2">
         <v>9</v>
       </c>
@@ -6282,15 +6334,15 @@
       <c r="Q75" s="159" t="s">
         <v>99</v>
       </c>
-      <c r="R75" s="210"/>
-      <c r="S75" s="214"/>
+      <c r="R75" s="219"/>
+      <c r="S75" s="223"/>
       <c r="T75" s="2"/>
       <c r="U75" s="2"/>
-      <c r="V75" s="216" t="str">
+      <c r="V75" s="206" t="str">
         <f>IF(AB49="","",AB49)</f>
         <v/>
       </c>
-      <c r="W75" s="222" t="str">
+      <c r="W75" s="212" t="str">
         <f>IF(AB52="","",AB52)</f>
         <v/>
       </c>
@@ -6300,7 +6352,7 @@
       <c r="AC75" s="20"/>
       <c r="AD75" s="20"/>
     </row>
-    <row r="76" spans="1:30" ht="14.45" customHeight="1">
+    <row r="76" spans="1:30" ht="14.4" customHeight="1">
       <c r="A76" s="2">
         <v>10</v>
       </c>
@@ -6334,12 +6386,12 @@
       <c r="O76" s="13"/>
       <c r="P76" s="2"/>
       <c r="Q76" s="159"/>
-      <c r="R76" s="209"/>
-      <c r="S76" s="213"/>
+      <c r="R76" s="218"/>
+      <c r="S76" s="222"/>
       <c r="T76" s="2"/>
       <c r="U76" s="2"/>
-      <c r="V76" s="218"/>
-      <c r="W76" s="221"/>
+      <c r="V76" s="208"/>
+      <c r="W76" s="211"/>
       <c r="X76" s="2"/>
       <c r="Y76" s="14"/>
       <c r="AB76" s="158"/>
@@ -6352,7 +6404,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:30" ht="14.45" customHeight="1" thickBot="1">
+    <row r="77" spans="1:30" ht="14.4" customHeight="1" thickBot="1">
       <c r="A77" s="2">
         <v>11</v>
       </c>
@@ -6382,15 +6434,15 @@
       <c r="Q77" s="159" t="s">
         <v>102</v>
       </c>
-      <c r="R77" s="210"/>
-      <c r="S77" s="214"/>
+      <c r="R77" s="219"/>
+      <c r="S77" s="223"/>
       <c r="T77" s="2"/>
       <c r="U77" s="2"/>
-      <c r="V77" s="216" t="str">
+      <c r="V77" s="206" t="str">
         <f>IF(AB50="","",AB50)</f>
         <v/>
       </c>
-      <c r="W77" s="222" t="str">
+      <c r="W77" s="212" t="str">
         <f>IF(AB53="","",AB53)</f>
         <v/>
       </c>
@@ -6400,7 +6452,7 @@
       <c r="AC77" s="20"/>
       <c r="AD77" s="20"/>
     </row>
-    <row r="78" spans="1:30" ht="14.45" customHeight="1" thickBot="1">
+    <row r="78" spans="1:30" ht="14.4" customHeight="1" thickBot="1">
       <c r="A78" s="2">
         <v>12</v>
       </c>
@@ -6409,12 +6461,12 @@
       <c r="O78" s="13"/>
       <c r="P78" s="2"/>
       <c r="Q78" s="159"/>
-      <c r="R78" s="211"/>
-      <c r="S78" s="215"/>
+      <c r="R78" s="220"/>
+      <c r="S78" s="224"/>
       <c r="T78" s="2"/>
       <c r="U78" s="2"/>
-      <c r="V78" s="217"/>
-      <c r="W78" s="223"/>
+      <c r="V78" s="207"/>
+      <c r="W78" s="213"/>
       <c r="X78" s="2"/>
       <c r="Y78" s="14"/>
       <c r="AB78" s="158"/>
@@ -6427,7 +6479,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:30" ht="14.45" customHeight="1">
+    <row r="79" spans="1:30" ht="14.4" customHeight="1">
       <c r="A79" s="2">
         <v>13</v>
       </c>
@@ -6467,7 +6519,7 @@
       <c r="AC79" s="20"/>
       <c r="AD79" s="20"/>
     </row>
-    <row r="80" spans="1:30" ht="14.45" customHeight="1">
+    <row r="80" spans="1:30" ht="14.4" customHeight="1">
       <c r="A80" s="2">
         <v>14</v>
       </c>
@@ -6507,7 +6559,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:30" ht="14.45" customHeight="1">
+    <row r="81" spans="1:30" ht="14.4" customHeight="1">
       <c r="A81" s="2">
         <v>15</v>
       </c>
@@ -6546,7 +6598,7 @@
       <c r="AC81" s="20"/>
       <c r="AD81" s="20"/>
     </row>
-    <row r="82" spans="1:30" ht="14.45" customHeight="1">
+    <row r="82" spans="1:30" ht="14.4" customHeight="1">
       <c r="A82" s="2">
         <v>16</v>
       </c>
@@ -6578,7 +6630,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:30" ht="14.45" customHeight="1" thickBot="1">
+    <row r="83" spans="1:30" ht="14.4" customHeight="1" thickBot="1">
       <c r="A83" s="2">
         <v>17</v>
       </c>
@@ -6615,7 +6667,7 @@
       <c r="AC83" s="20"/>
       <c r="AD83" s="20"/>
     </row>
-    <row r="84" spans="1:30" ht="14.45" customHeight="1">
+    <row r="84" spans="1:30" ht="14.4" customHeight="1">
       <c r="A84" s="2">
         <v>18</v>
       </c>
@@ -6632,16 +6684,16 @@
         <v>Right ()</v>
       </c>
       <c r="H84" s="2"/>
-      <c r="I84" s="226" t="str">
+      <c r="I84" s="204" t="str">
         <f>R68</f>
         <v>Left ()</v>
       </c>
-      <c r="J84" s="226"/>
-      <c r="K84" s="226" t="str">
+      <c r="J84" s="204"/>
+      <c r="K84" s="204" t="str">
         <f>S68</f>
         <v>Right ()</v>
       </c>
-      <c r="L84" s="226"/>
+      <c r="L84" s="204"/>
       <c r="M84" s="12"/>
       <c r="O84" s="13"/>
       <c r="P84" s="2"/>
@@ -6664,7 +6716,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:30" ht="14.45" customHeight="1" thickBot="1">
+    <row r="85" spans="1:30" ht="14.4" customHeight="1" thickBot="1">
       <c r="A85" s="2">
         <v>19</v>
       </c>
@@ -6685,16 +6737,16 @@
       <c r="H85" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="I85" s="227" t="str">
+      <c r="I85" s="205" t="str">
         <f>IF(R73="","",R73)</f>
         <v/>
       </c>
-      <c r="J85" s="227"/>
-      <c r="K85" s="227" t="str">
+      <c r="J85" s="205"/>
+      <c r="K85" s="205" t="str">
         <f>IF(S73="","",S73)</f>
         <v/>
       </c>
-      <c r="L85" s="227"/>
+      <c r="L85" s="205"/>
       <c r="M85" s="12"/>
       <c r="O85" s="109" t="s">
         <v>107</v>
@@ -6712,7 +6764,7 @@
       <c r="X85" s="2"/>
       <c r="Y85" s="14"/>
     </row>
-    <row r="86" spans="1:30" ht="14.45" customHeight="1">
+    <row r="86" spans="1:30" ht="14.4" customHeight="1">
       <c r="A86" s="2">
         <v>20</v>
       </c>
@@ -6733,27 +6785,27 @@
       <c r="H86" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="I86" s="227" t="str">
+      <c r="I86" s="205" t="str">
         <f>IF(R75="","",R75)</f>
         <v/>
       </c>
-      <c r="J86" s="227"/>
-      <c r="K86" s="227" t="str">
+      <c r="J86" s="205"/>
+      <c r="K86" s="205" t="str">
         <f>IF(S75="","",S75)</f>
         <v/>
       </c>
-      <c r="L86" s="227"/>
+      <c r="L86" s="205"/>
       <c r="M86" s="12"/>
       <c r="O86" s="13"/>
       <c r="P86" s="2"/>
-      <c r="Q86" s="206" t="s">
+      <c r="Q86" s="215" t="s">
         <v>118</v>
       </c>
-      <c r="R86" s="207"/>
-      <c r="S86" s="206" t="s">
+      <c r="R86" s="216"/>
+      <c r="S86" s="215" t="s">
         <v>119</v>
       </c>
-      <c r="T86" s="207"/>
+      <c r="T86" s="216"/>
       <c r="U86" s="2"/>
       <c r="V86" s="127" t="s">
         <v>44</v>
@@ -6762,7 +6814,7 @@
       <c r="X86" s="2"/>
       <c r="Y86" s="14"/>
     </row>
-    <row r="87" spans="1:30" ht="14.45" customHeight="1" thickBot="1">
+    <row r="87" spans="1:30" ht="14.4" customHeight="1" thickBot="1">
       <c r="A87" s="2">
         <v>21</v>
       </c>
@@ -6783,16 +6835,16 @@
       <c r="H87" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="I87" s="205" t="str">
+      <c r="I87" s="214" t="str">
         <f>IF(R77="","",R77)</f>
         <v/>
       </c>
-      <c r="J87" s="205"/>
-      <c r="K87" s="205" t="str">
+      <c r="J87" s="214"/>
+      <c r="K87" s="214" t="str">
         <f>IF(S77="","",S77)</f>
         <v/>
       </c>
-      <c r="L87" s="205"/>
+      <c r="L87" s="214"/>
       <c r="M87" s="12"/>
       <c r="O87" s="13"/>
       <c r="P87" s="2"/>
@@ -6826,7 +6878,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="88" spans="1:30" ht="14.45" customHeight="1">
+    <row r="88" spans="1:30" ht="14.4" customHeight="1">
       <c r="A88" s="2">
         <v>22</v>
       </c>
@@ -6851,20 +6903,20 @@
       <c r="P88" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="Q88" s="186" t="str">
-        <f t="shared" ref="Q88:Q96" si="16">IF(AG16="","",AG16+Lamb)</f>
-        <v/>
-      </c>
-      <c r="R88" s="187" t="str">
-        <f t="shared" ref="R88:R96" si="17">IF(AG25="","",AG25+Lamb)</f>
-        <v/>
-      </c>
-      <c r="S88" s="188" t="str">
-        <f t="shared" ref="S88:S96" si="18">IF(AG34="","",AG34+Lamb)</f>
-        <v/>
-      </c>
-      <c r="T88" s="187" t="str">
-        <f t="shared" ref="T88:T96" si="19">IF(AG43="","",AG43+Lamb)</f>
+      <c r="Q88" s="181" t="str">
+        <f>IF(AG16="","",AG17+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R88" s="182" t="str">
+        <f>IF(AG25="","",AG26+Lamb)</f>
+        <v/>
+      </c>
+      <c r="S88" s="183" t="str">
+        <f>IF(AG34="","",AG35+Lamb)</f>
+        <v/>
+      </c>
+      <c r="T88" s="182" t="str">
+        <f>IF(AG43="","",AG44+Lamb)</f>
         <v/>
       </c>
       <c r="U88" s="2"/>
@@ -6874,24 +6926,24 @@
       </c>
       <c r="X88" s="2"/>
       <c r="Y88" s="14"/>
-      <c r="AA88" s="1" t="e">
+      <c r="AA88" s="231" t="e">
         <f>ABS(Q88-MEDIAN($Q$88:$Q$96))/MEDIAN($Q$88:$Q$96)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AB88" s="2" t="e">
+      <c r="AB88" s="231" t="e">
         <f>ABS(R88-MEDIAN($R$88:$R$96))/MEDIAN($R$88:$R$96)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AC88" s="2" t="e">
+      <c r="AC88" s="231" t="e">
         <f>ABS(S88-MEDIAN($S$88:$S$96))/MEDIAN($S$88:$S$96)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AD88" s="2" t="e">
+      <c r="AD88" s="231" t="e">
         <f>ABS(T88-MEDIAN($T$88:$T$96))/MEDIAN($T$88:$T$96)</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="89" spans="1:30" ht="14.45" customHeight="1">
+    <row r="89" spans="1:30" ht="14.4" customHeight="1">
       <c r="A89" s="2">
         <v>23</v>
       </c>
@@ -6914,20 +6966,20 @@
       <c r="P89" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="Q89" s="189" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="R89" s="190" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="S89" s="191" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="T89" s="190" t="str">
-        <f t="shared" si="19"/>
+      <c r="Q89" s="184" t="str">
+        <f>IF(AG17="","",AG18+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R89" s="185" t="str">
+        <f>IF(AG26="","",AG27+Lamb)</f>
+        <v/>
+      </c>
+      <c r="S89" s="186" t="str">
+        <f>IF(AG35="","",AG36+Lamb)</f>
+        <v/>
+      </c>
+      <c r="T89" s="185" t="str">
+        <f>IF(AG44="","",AG45+Lamb)</f>
         <v/>
       </c>
       <c r="U89" s="2"/>
@@ -6937,24 +6989,24 @@
       </c>
       <c r="X89" s="2"/>
       <c r="Y89" s="14"/>
-      <c r="AA89" s="2" t="e">
-        <f t="shared" ref="AA89:AA96" si="20">ABS(Q89-MEDIAN($Q$88:$Q$96))/MEDIAN($Q$88:$Q$96)</f>
+      <c r="AA89" s="231" t="e">
+        <f t="shared" ref="AA89:AA96" si="16">ABS(Q89-MEDIAN($Q$88:$Q$96))/MEDIAN($Q$88:$Q$96)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AB89" s="2" t="e">
-        <f t="shared" ref="AB89:AB96" si="21">ABS(R89-MEDIAN($R$88:$R$96))/MEDIAN($R$88:$R$96)</f>
+      <c r="AB89" s="231" t="e">
+        <f t="shared" ref="AB89:AB96" si="17">ABS(R89-MEDIAN($R$88:$R$96))/MEDIAN($R$88:$R$96)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AC89" s="2" t="e">
-        <f t="shared" ref="AC89:AC96" si="22">ABS(S89-MEDIAN($S$88:$S$96))/MEDIAN($S$88:$S$96)</f>
+      <c r="AC89" s="231" t="e">
+        <f t="shared" ref="AC89:AC96" si="18">ABS(S89-MEDIAN($S$88:$S$96))/MEDIAN($S$88:$S$96)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AD89" s="2" t="e">
-        <f t="shared" ref="AD89:AD96" si="23">ABS(T89-MEDIAN($T$88:$T$96))/MEDIAN($T$88:$T$96)</f>
+      <c r="AD89" s="231" t="e">
+        <f t="shared" ref="AD89:AD96" si="19">ABS(T89-MEDIAN($T$88:$T$96))/MEDIAN($T$88:$T$96)</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="90" spans="1:30" ht="14.45" customHeight="1">
+    <row r="90" spans="1:30" ht="14.4" customHeight="1">
       <c r="A90" s="2">
         <v>24</v>
       </c>
@@ -6977,20 +7029,20 @@
       <c r="P90" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="Q90" s="189" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="R90" s="190" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="S90" s="191" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="T90" s="190" t="str">
-        <f t="shared" si="19"/>
+      <c r="Q90" s="184" t="str">
+        <f>IF(AG18="","",AG19+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R90" s="185" t="str">
+        <f>IF(AG27="","",AG28+Lamb)</f>
+        <v/>
+      </c>
+      <c r="S90" s="186" t="str">
+        <f>IF(AG36="","",AG37+Lamb)</f>
+        <v/>
+      </c>
+      <c r="T90" s="185" t="str">
+        <f>IF(AG45="","",AG46+Lamb)</f>
         <v/>
       </c>
       <c r="U90" s="2"/>
@@ -6998,24 +7050,24 @@
       <c r="W90" s="2"/>
       <c r="X90" s="2"/>
       <c r="Y90" s="14"/>
-      <c r="AA90" s="2" t="e">
-        <f t="shared" si="20"/>
+      <c r="AA90" s="231" t="e">
+        <f t="shared" si="16"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB90" s="2" t="e">
-        <f t="shared" si="21"/>
+      <c r="AB90" s="231" t="e">
+        <f t="shared" si="17"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AC90" s="2" t="e">
-        <f t="shared" si="22"/>
+      <c r="AC90" s="231" t="e">
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AD90" s="2" t="e">
-        <f t="shared" si="23"/>
+      <c r="AD90" s="231" t="e">
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="91" spans="1:30" ht="14.45" customHeight="1">
+    <row r="91" spans="1:30" ht="14.4" customHeight="1">
       <c r="A91" s="2">
         <v>25</v>
       </c>
@@ -7025,20 +7077,20 @@
       <c r="P91" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="Q91" s="189" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="R91" s="190" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="S91" s="191" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="T91" s="190" t="str">
-        <f t="shared" si="19"/>
+      <c r="Q91" s="184" t="str">
+        <f>IF(AG19="","",AG20+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R91" s="185" t="str">
+        <f>IF(AG28="","",AG29+Lamb)</f>
+        <v/>
+      </c>
+      <c r="S91" s="186" t="str">
+        <f>IF(AG37="","",AG38+Lamb)</f>
+        <v/>
+      </c>
+      <c r="T91" s="185" t="str">
+        <f>IF(AG46="","",AG47+Lamb)</f>
         <v/>
       </c>
       <c r="U91" s="2"/>
@@ -7046,24 +7098,24 @@
       <c r="W91" s="2"/>
       <c r="X91" s="2"/>
       <c r="Y91" s="14"/>
-      <c r="AA91" s="2" t="e">
-        <f t="shared" si="20"/>
+      <c r="AA91" s="231" t="e">
+        <f t="shared" si="16"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB91" s="2" t="e">
-        <f t="shared" si="21"/>
+      <c r="AB91" s="231" t="e">
+        <f t="shared" si="17"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AC91" s="2" t="e">
-        <f t="shared" si="22"/>
+      <c r="AC91" s="231" t="e">
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AD91" s="2" t="e">
-        <f t="shared" si="23"/>
+      <c r="AD91" s="231" t="e">
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="92" spans="1:30" ht="14.45" customHeight="1">
+    <row r="92" spans="1:30" ht="14.4" customHeight="1">
       <c r="A92" s="2">
         <v>26</v>
       </c>
@@ -7076,20 +7128,20 @@
       <c r="P92" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="Q92" s="189" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="R92" s="190" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="S92" s="191" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="T92" s="190" t="str">
-        <f t="shared" si="19"/>
+      <c r="Q92" s="184" t="str">
+        <f>IF(AG20="","",AG21+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R92" s="185" t="str">
+        <f>IF(AG29="","",AG30+Lamb)</f>
+        <v/>
+      </c>
+      <c r="S92" s="186" t="str">
+        <f>IF(AG38="","",AG39+Lamb)</f>
+        <v/>
+      </c>
+      <c r="T92" s="185" t="str">
+        <f>IF(AG47="","",AG48+Lamb)</f>
         <v/>
       </c>
       <c r="U92" s="2"/>
@@ -7097,24 +7149,24 @@
       <c r="W92" s="2"/>
       <c r="X92" s="2"/>
       <c r="Y92" s="14"/>
-      <c r="AA92" s="2" t="e">
-        <f t="shared" si="20"/>
+      <c r="AA92" s="231" t="e">
+        <f t="shared" si="16"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB92" s="2" t="e">
-        <f t="shared" si="21"/>
+      <c r="AB92" s="231" t="e">
+        <f t="shared" si="17"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AC92" s="2" t="e">
-        <f t="shared" si="22"/>
+      <c r="AC92" s="231" t="e">
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AD92" s="2" t="e">
-        <f t="shared" si="23"/>
+      <c r="AD92" s="231" t="e">
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="93" spans="1:30" ht="14.45" customHeight="1">
+    <row r="93" spans="1:30" ht="14.4" customHeight="1">
       <c r="A93" s="2">
         <v>27</v>
       </c>
@@ -7136,41 +7188,41 @@
       <c r="P93" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="Q93" s="189" t="str">
+      <c r="Q93" s="184" t="str">
+        <f>IF(AG21="","",AG22+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R93" s="185" t="str">
+        <f>IF(AG30="","",AG31+Lamb)</f>
+        <v/>
+      </c>
+      <c r="S93" s="186" t="str">
+        <f>IF(AG39="","",AG40+Lamb)</f>
+        <v/>
+      </c>
+      <c r="T93" s="185" t="str">
+        <f>IF(AG48="","",AG49+Lamb)</f>
+        <v/>
+      </c>
+      <c r="Y93" s="14"/>
+      <c r="AA93" s="231" t="e">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="R93" s="190" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AB93" s="231" t="e">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="S93" s="191" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AC93" s="231" t="e">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="T93" s="190" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AD93" s="231" t="e">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="Y93" s="14"/>
-      <c r="AA93" s="2" t="e">
-        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB93" s="2" t="e">
-        <f t="shared" si="21"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AC93" s="2" t="e">
-        <f t="shared" si="22"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AD93" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="94" spans="1:30" ht="14.45" customHeight="1">
+    </row>
+    <row r="94" spans="1:30" ht="14.4" customHeight="1">
       <c r="A94" s="2">
         <v>28</v>
       </c>
@@ -7192,41 +7244,41 @@
       <c r="P94" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="Q94" s="189" t="str">
+      <c r="Q94" s="184" t="str">
+        <f>IF(AG22="","",AG23+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R94" s="185" t="str">
+        <f>IF(AG31="","",AG32+Lamb)</f>
+        <v/>
+      </c>
+      <c r="S94" s="186" t="str">
+        <f>IF(AG40="","",AG41+Lamb)</f>
+        <v/>
+      </c>
+      <c r="T94" s="185" t="str">
+        <f>IF(AG49="","",AG50+Lamb)</f>
+        <v/>
+      </c>
+      <c r="Y94" s="14"/>
+      <c r="AA94" s="231" t="e">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="R94" s="190" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AB94" s="231" t="e">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="S94" s="191" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AC94" s="231" t="e">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="T94" s="190" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AD94" s="231" t="e">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="Y94" s="14"/>
-      <c r="AA94" s="2" t="e">
-        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB94" s="2" t="e">
-        <f t="shared" si="21"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AC94" s="2" t="e">
-        <f t="shared" si="22"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AD94" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="95" spans="1:30" ht="14.45" customHeight="1">
+    </row>
+    <row r="95" spans="1:30" ht="14.4" customHeight="1">
       <c r="A95" s="2">
         <v>29</v>
       </c>
@@ -7248,41 +7300,41 @@
       <c r="P95" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="Q95" s="189" t="str">
+      <c r="Q95" s="184" t="str">
+        <f>IF(AG23="","",AG24+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R95" s="185" t="str">
+        <f>IF(AG32="","",AG33+Lamb)</f>
+        <v/>
+      </c>
+      <c r="S95" s="186" t="str">
+        <f>IF(AG41="","",AG42+Lamb)</f>
+        <v/>
+      </c>
+      <c r="T95" s="185" t="str">
+        <f>IF(AG50="","",AG51+Lamb)</f>
+        <v/>
+      </c>
+      <c r="Y95" s="14"/>
+      <c r="AA95" s="231" t="e">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="R95" s="190" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AB95" s="231" t="e">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="S95" s="191" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AC95" s="231" t="e">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="T95" s="190" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AD95" s="231" t="e">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="Y95" s="14"/>
-      <c r="AA95" s="2" t="e">
-        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB95" s="2" t="e">
-        <f t="shared" si="21"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AC95" s="2" t="e">
-        <f t="shared" si="22"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AD95" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="96" spans="1:30" ht="14.45" customHeight="1" thickBot="1">
+    </row>
+    <row r="96" spans="1:30" ht="14.4" customHeight="1" thickBot="1">
       <c r="A96" s="2">
         <v>30</v>
       </c>
@@ -7304,41 +7356,41 @@
       <c r="P96" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="Q96" s="192" t="str">
+      <c r="Q96" s="187" t="str">
+        <f>IF(AG24="","",AG25+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R96" s="188" t="str">
+        <f>IF(AG33="","",AG34+Lamb)</f>
+        <v/>
+      </c>
+      <c r="S96" s="189" t="str">
+        <f>IF(AG42="","",AG43+Lamb)</f>
+        <v/>
+      </c>
+      <c r="T96" s="188" t="str">
+        <f>IF(AG51="","",AG52+Lamb)</f>
+        <v/>
+      </c>
+      <c r="Y96" s="14"/>
+      <c r="AA96" s="231" t="e">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="R96" s="193" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AB96" s="231" t="e">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="S96" s="194" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AC96" s="231" t="e">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="T96" s="193" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AD96" s="231" t="e">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="Y96" s="14"/>
-      <c r="AA96" s="2" t="e">
-        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB96" s="2" t="e">
-        <f t="shared" si="21"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AC96" s="2" t="e">
-        <f t="shared" si="22"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AD96" s="2" t="e">
-        <f t="shared" si="23"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="97" spans="1:25" ht="14.45" customHeight="1">
+    </row>
+    <row r="97" spans="1:25" ht="14.4" customHeight="1">
       <c r="A97" s="2">
         <v>31</v>
       </c>
@@ -7382,7 +7434,7 @@
       <c r="X97" s="2"/>
       <c r="Y97" s="14"/>
     </row>
-    <row r="98" spans="1:25" ht="14.45" customHeight="1" thickBot="1">
+    <row r="98" spans="1:25" ht="14.4" customHeight="1" thickBot="1">
       <c r="A98" s="2">
         <v>32</v>
       </c>
@@ -7404,19 +7456,19 @@
       <c r="P98" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="Q98" s="172" t="str">
+      <c r="Q98" s="169" t="str">
         <f>IF(Q88="","",STDEV(Q88:Q92))</f>
         <v/>
       </c>
-      <c r="R98" s="173" t="str">
+      <c r="R98" s="170" t="str">
         <f>IF(R88="","",STDEV(R88:R92))</f>
         <v/>
       </c>
-      <c r="S98" s="174" t="str">
+      <c r="S98" s="171" t="str">
         <f>IF(S88="","",STDEV(S88:S92))</f>
         <v/>
       </c>
-      <c r="T98" s="173" t="str">
+      <c r="T98" s="170" t="str">
         <f>IF(T88="","",STDEV(T88:T92))</f>
         <v/>
       </c>
@@ -7426,7 +7478,7 @@
       <c r="X98" s="2"/>
       <c r="Y98" s="14"/>
     </row>
-    <row r="99" spans="1:25" ht="14.45" customHeight="1" thickBot="1">
+    <row r="99" spans="1:25" ht="14.4" customHeight="1" thickBot="1">
       <c r="A99" s="2">
         <v>33</v>
       </c>
@@ -7448,19 +7500,19 @@
       <c r="P99" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="Q99" s="175" t="str">
+      <c r="Q99" s="172" t="str">
         <f>IF(Q88="","",2*(MAX(Q88:Q96)-MIN(Q88:Q96))/(MIN(Q88:Q96)+MAX(Q88:Q96)))</f>
         <v/>
       </c>
-      <c r="R99" s="176" t="str">
+      <c r="R99" s="173" t="str">
         <f>IF(R88="","",2*(MAX(R88:R96)-MIN(R88:R96))/(MIN(R88:R96)+MAX(R88:R96)))</f>
         <v/>
       </c>
-      <c r="S99" s="177" t="str">
+      <c r="S99" s="174" t="str">
         <f>IF(S88="","",2*(MAX(S88:S96)-MIN(S88:S96))/(MIN(S88:S96)+MAX(S88:S96)))</f>
         <v/>
       </c>
-      <c r="T99" s="176" t="str">
+      <c r="T99" s="173" t="str">
         <f>IF(T88="","",2*(MAX(T88:T96)-MIN(T88:T96))/(MIN(T88:T96)+MAX(T88:T96)))</f>
         <v/>
       </c>
@@ -7474,7 +7526,7 @@
       <c r="X99" s="2"/>
       <c r="Y99" s="14"/>
     </row>
-    <row r="100" spans="1:25" ht="14.45" customHeight="1" thickBot="1">
+    <row r="100" spans="1:25" ht="14.4" customHeight="1" thickBot="1">
       <c r="A100" s="2">
         <v>34</v>
       </c>
@@ -7496,19 +7548,19 @@
       <c r="P100" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="Q100" s="170" t="str">
+      <c r="Q100" s="229" t="str">
         <f>IF(Q88="","",MAX(AA88:AA96))</f>
         <v/>
       </c>
-      <c r="R100" s="171" t="str">
+      <c r="R100" s="230" t="str">
         <f>IF(R88="","",MAX(AB88:AB96))</f>
         <v/>
       </c>
-      <c r="S100" s="170" t="str">
+      <c r="S100" s="229" t="str">
         <f>IF(S88="","",MAX(AC88:AC96))</f>
         <v/>
       </c>
-      <c r="T100" s="171" t="str">
+      <c r="T100" s="230" t="str">
         <f>IF(T88="","",MAX(AD88:AD96))</f>
         <v/>
       </c>
@@ -7517,7 +7569,7 @@
       </c>
       <c r="Y100" s="14"/>
     </row>
-    <row r="101" spans="1:25" ht="14.45" customHeight="1">
+    <row r="101" spans="1:25" ht="14.4" customHeight="1">
       <c r="A101" s="2">
         <v>35</v>
       </c>
@@ -7539,7 +7591,7 @@
       <c r="P101" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="Q101" s="169" t="str">
+      <c r="Q101" s="168" t="str">
         <f>IF(Q103&lt;&gt;"",Q103,IF(AB62="","",AB62))</f>
         <v/>
       </c>
@@ -7552,7 +7604,7 @@
       <c r="X101" s="90"/>
       <c r="Y101" s="14"/>
     </row>
-    <row r="102" spans="1:25" ht="14.45" customHeight="1">
+    <row r="102" spans="1:25" ht="14.4" customHeight="1">
       <c r="A102" s="2">
         <v>36</v>
       </c>
@@ -7587,7 +7639,7 @@
       <c r="X102" s="78"/>
       <c r="Y102" s="14"/>
     </row>
-    <row r="103" spans="1:25" ht="14.45" customHeight="1">
+    <row r="103" spans="1:25" ht="14.4" customHeight="1">
       <c r="A103" s="2">
         <v>37</v>
       </c>
@@ -7619,7 +7671,7 @@
       <c r="X103" s="78"/>
       <c r="Y103" s="14"/>
     </row>
-    <row r="104" spans="1:25" ht="14.45" customHeight="1" thickBot="1">
+    <row r="104" spans="1:25" ht="14.4" customHeight="1" thickBot="1">
       <c r="A104" s="2">
         <v>38</v>
       </c>
@@ -7649,7 +7701,7 @@
       <c r="X104" s="44"/>
       <c r="Y104" s="28"/>
     </row>
-    <row r="105" spans="1:25" ht="14.45" customHeight="1">
+    <row r="105" spans="1:25" ht="14.4" customHeight="1">
       <c r="A105" s="2">
         <v>39</v>
       </c>
@@ -7679,7 +7731,7 @@
       <c r="X105" s="2"/>
       <c r="Y105" s="2"/>
     </row>
-    <row r="106" spans="1:25" ht="14.45" customHeight="1" thickBot="1">
+    <row r="106" spans="1:25" ht="14.4" customHeight="1" thickBot="1">
       <c r="A106" s="2">
         <v>40</v>
       </c>
@@ -7711,7 +7763,7 @@
       <c r="X106" s="2"/>
       <c r="Y106" s="2"/>
     </row>
-    <row r="107" spans="1:25" ht="14.45" customHeight="1">
+    <row r="107" spans="1:25" ht="14.4" customHeight="1">
       <c r="A107" s="2">
         <v>41</v>
       </c>
@@ -7743,7 +7795,7 @@
       <c r="X107" s="7"/>
       <c r="Y107" s="8"/>
     </row>
-    <row r="108" spans="1:25" ht="14.45" customHeight="1">
+    <row r="108" spans="1:25" ht="14.4" customHeight="1">
       <c r="A108" s="2">
         <v>42</v>
       </c>
@@ -7778,7 +7830,7 @@
       <c r="X108" s="90"/>
       <c r="Y108" s="14"/>
     </row>
-    <row r="109" spans="1:25" ht="14.45" customHeight="1">
+    <row r="109" spans="1:25" ht="14.4" customHeight="1">
       <c r="A109" s="2">
         <v>43</v>
       </c>
@@ -7813,7 +7865,7 @@
       <c r="X109" s="78"/>
       <c r="Y109" s="14"/>
     </row>
-    <row r="110" spans="1:25" ht="14.45" customHeight="1">
+    <row r="110" spans="1:25" ht="14.4" customHeight="1">
       <c r="A110" s="2">
         <v>44</v>
       </c>
@@ -7848,7 +7900,7 @@
       <c r="X110" s="90"/>
       <c r="Y110" s="14"/>
     </row>
-    <row r="111" spans="1:25" ht="14.45" customHeight="1">
+    <row r="111" spans="1:25" ht="14.4" customHeight="1">
       <c r="A111" s="2">
         <v>45</v>
       </c>
@@ -7883,7 +7935,7 @@
       <c r="X111" s="78"/>
       <c r="Y111" s="14"/>
     </row>
-    <row r="112" spans="1:25" ht="14.45" customHeight="1">
+    <row r="112" spans="1:25" ht="14.4" customHeight="1">
       <c r="A112" s="2">
         <v>46</v>
       </c>
@@ -7918,7 +7970,7 @@
       <c r="X112" s="90"/>
       <c r="Y112" s="14"/>
     </row>
-    <row r="113" spans="1:25" ht="14.45" customHeight="1">
+    <row r="113" spans="1:25" ht="14.4" customHeight="1">
       <c r="A113" s="2">
         <v>47</v>
       </c>
@@ -7953,7 +8005,7 @@
       <c r="X113" s="78"/>
       <c r="Y113" s="14"/>
     </row>
-    <row r="114" spans="1:25" ht="14.45" customHeight="1">
+    <row r="114" spans="1:25" ht="14.4" customHeight="1">
       <c r="A114" s="2">
         <v>48</v>
       </c>
@@ -7988,7 +8040,7 @@
       <c r="X114" s="90"/>
       <c r="Y114" s="14"/>
     </row>
-    <row r="115" spans="1:25" ht="14.45" customHeight="1">
+    <row r="115" spans="1:25" ht="14.4" customHeight="1">
       <c r="A115" s="2">
         <v>49</v>
       </c>
@@ -8023,7 +8075,7 @@
       <c r="X115" s="78"/>
       <c r="Y115" s="14"/>
     </row>
-    <row r="116" spans="1:25" ht="14.45" customHeight="1">
+    <row r="116" spans="1:25" ht="14.4" customHeight="1">
       <c r="A116" s="2">
         <v>50</v>
       </c>
@@ -8058,7 +8110,7 @@
       <c r="X116" s="90"/>
       <c r="Y116" s="14"/>
     </row>
-    <row r="117" spans="1:25" ht="14.45" customHeight="1">
+    <row r="117" spans="1:25" ht="14.4" customHeight="1">
       <c r="A117" s="2">
         <v>51</v>
       </c>
@@ -8093,7 +8145,7 @@
       <c r="X117" s="78"/>
       <c r="Y117" s="14"/>
     </row>
-    <row r="118" spans="1:25" ht="14.45" customHeight="1">
+    <row r="118" spans="1:25" ht="14.4" customHeight="1">
       <c r="A118" s="2">
         <v>52</v>
       </c>
@@ -8128,7 +8180,7 @@
       <c r="X118" s="90"/>
       <c r="Y118" s="14"/>
     </row>
-    <row r="119" spans="1:25" ht="14.45" customHeight="1">
+    <row r="119" spans="1:25" ht="14.4" customHeight="1">
       <c r="A119" s="2">
         <v>53</v>
       </c>
@@ -8163,7 +8215,7 @@
       <c r="X119" s="78"/>
       <c r="Y119" s="14"/>
     </row>
-    <row r="120" spans="1:25" ht="14.45" customHeight="1">
+    <row r="120" spans="1:25" ht="14.4" customHeight="1">
       <c r="A120" s="2">
         <v>54</v>
       </c>
@@ -8198,7 +8250,7 @@
       <c r="X120" s="90"/>
       <c r="Y120" s="14"/>
     </row>
-    <row r="121" spans="1:25" ht="14.45" customHeight="1">
+    <row r="121" spans="1:25" ht="14.4" customHeight="1">
       <c r="A121" s="2">
         <v>55</v>
       </c>
@@ -8233,7 +8285,7 @@
       <c r="X121" s="78"/>
       <c r="Y121" s="14"/>
     </row>
-    <row r="122" spans="1:25" ht="14.45" customHeight="1">
+    <row r="122" spans="1:25" ht="14.4" customHeight="1">
       <c r="A122" s="2">
         <v>56</v>
       </c>
@@ -8268,7 +8320,7 @@
       <c r="X122" s="90"/>
       <c r="Y122" s="14"/>
     </row>
-    <row r="123" spans="1:25" ht="14.45" customHeight="1">
+    <row r="123" spans="1:25" ht="14.4" customHeight="1">
       <c r="A123" s="2">
         <v>57</v>
       </c>
@@ -8303,7 +8355,7 @@
       <c r="X123" s="78"/>
       <c r="Y123" s="14"/>
     </row>
-    <row r="124" spans="1:25" ht="14.45" customHeight="1">
+    <row r="124" spans="1:25" ht="14.4" customHeight="1">
       <c r="A124" s="2">
         <v>58</v>
       </c>
@@ -8338,7 +8390,7 @@
       <c r="X124" s="90"/>
       <c r="Y124" s="14"/>
     </row>
-    <row r="125" spans="1:25" ht="14.45" customHeight="1">
+    <row r="125" spans="1:25" ht="14.4" customHeight="1">
       <c r="A125" s="2">
         <v>59</v>
       </c>
@@ -8373,7 +8425,7 @@
       <c r="X125" s="78"/>
       <c r="Y125" s="14"/>
     </row>
-    <row r="126" spans="1:25" ht="14.45" customHeight="1">
+    <row r="126" spans="1:25" ht="14.4" customHeight="1">
       <c r="A126" s="2">
         <v>60</v>
       </c>
@@ -8396,7 +8448,7 @@
       <c r="X126" s="90"/>
       <c r="Y126" s="14"/>
     </row>
-    <row r="127" spans="1:25" ht="14.45" customHeight="1">
+    <row r="127" spans="1:25" ht="14.4" customHeight="1">
       <c r="A127" s="2">
         <v>61</v>
       </c>
@@ -8419,7 +8471,7 @@
       <c r="X127" s="78"/>
       <c r="Y127" s="14"/>
     </row>
-    <row r="128" spans="1:25" ht="14.45" customHeight="1">
+    <row r="128" spans="1:25" ht="14.4" customHeight="1">
       <c r="A128" s="2">
         <v>62</v>
       </c>
@@ -8442,7 +8494,7 @@
       <c r="X128" s="90"/>
       <c r="Y128" s="14"/>
     </row>
-    <row r="129" spans="1:25" ht="14.45" customHeight="1">
+    <row r="129" spans="1:25" ht="14.4" customHeight="1">
       <c r="A129" s="2">
         <v>63</v>
       </c>
@@ -8465,7 +8517,7 @@
       <c r="X129" s="78"/>
       <c r="Y129" s="14"/>
     </row>
-    <row r="130" spans="1:25" ht="14.45" customHeight="1" thickBot="1">
+    <row r="130" spans="1:25" ht="14.4" customHeight="1" thickBot="1">
       <c r="A130" s="2">
         <v>64</v>
       </c>
@@ -8493,7 +8545,7 @@
       <c r="X130" s="44"/>
       <c r="Y130" s="28"/>
     </row>
-    <row r="131" spans="1:25" ht="14.45" customHeight="1" thickTop="1">
+    <row r="131" spans="1:25" ht="14.4" customHeight="1" thickTop="1">
       <c r="A131" s="2">
         <v>65</v>
       </c>
@@ -8512,7 +8564,7 @@
         <v>Eugene Mah</v>
       </c>
     </row>
-    <row r="132" spans="1:25" ht="14.45" customHeight="1">
+    <row r="132" spans="1:25" ht="14.4" customHeight="1">
       <c r="A132" s="2">
         <v>66</v>
       </c>
@@ -8545,34 +8597,6 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="40">
-    <mergeCell ref="AG1:AJ1"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="I84:J84"/>
-    <mergeCell ref="K84:L84"/>
-    <mergeCell ref="I85:J85"/>
-    <mergeCell ref="K85:L85"/>
-    <mergeCell ref="V77:V78"/>
-    <mergeCell ref="V75:V76"/>
-    <mergeCell ref="V73:V74"/>
-    <mergeCell ref="W73:W74"/>
-    <mergeCell ref="W75:W76"/>
-    <mergeCell ref="W77:W78"/>
     <mergeCell ref="I87:J87"/>
     <mergeCell ref="K87:L87"/>
     <mergeCell ref="Q86:R86"/>
@@ -8585,6 +8609,34 @@
     <mergeCell ref="S77:S78"/>
     <mergeCell ref="I86:J86"/>
     <mergeCell ref="K86:L86"/>
+    <mergeCell ref="V77:V78"/>
+    <mergeCell ref="V75:V76"/>
+    <mergeCell ref="V73:V74"/>
+    <mergeCell ref="W73:W74"/>
+    <mergeCell ref="W75:W76"/>
+    <mergeCell ref="W77:W78"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="I84:J84"/>
+    <mergeCell ref="K84:L84"/>
+    <mergeCell ref="I85:J85"/>
+    <mergeCell ref="K85:L85"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="AG1:AJ1"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="J10:K10"/>
   </mergeCells>
   <conditionalFormatting sqref="I72:I74">
     <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">

</xml_diff>

<commit_message>
Fix formulas in uniformity section
</commit_message>
<xml_diff>
--- a/MUSCMammoMonitor.xlsx
+++ b/MUSCMammoMonitor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D86285C-5C96-4B5B-8074-696614E77EB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6861AF77-9C69-4059-93C2-C46413026BB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2118,18 +2118,6 @@
     <xf numFmtId="169" fontId="3" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -2163,18 +2151,48 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="47" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="39" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2268,40 +2286,22 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="47" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="39" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2833,7 +2833,7 @@
   <dimension ref="A1:AJ132"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -2878,12 +2878,12 @@
       <c r="AA1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="AG1" s="194" t="s">
+      <c r="AG1" s="200" t="s">
         <v>1</v>
       </c>
-      <c r="AH1" s="194"/>
-      <c r="AI1" s="194"/>
-      <c r="AJ1" s="194"/>
+      <c r="AH1" s="200"/>
+      <c r="AI1" s="200"/>
+      <c r="AJ1" s="200"/>
     </row>
     <row r="2" spans="1:36" ht="14.4" customHeight="1">
       <c r="A2" s="2">
@@ -2900,14 +2900,14 @@
       </c>
       <c r="Y2" s="14"/>
       <c r="AA2" s="15"/>
-      <c r="AG2" s="195" t="s">
+      <c r="AG2" s="201" t="s">
         <v>3</v>
       </c>
-      <c r="AH2" s="195"/>
-      <c r="AI2" s="196" t="s">
+      <c r="AH2" s="201"/>
+      <c r="AI2" s="202" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="196"/>
+      <c r="AJ2" s="202"/>
     </row>
     <row r="3" spans="1:36" ht="14.4" customHeight="1">
       <c r="A3" s="2">
@@ -3201,19 +3201,19 @@
       <c r="D10" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="197" t="str">
+      <c r="E10" s="203" t="str">
         <f t="shared" ref="E10:E15" si="1">IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="F10" s="197"/>
+      <c r="F10" s="203"/>
       <c r="I10" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="197" t="str">
+      <c r="J10" s="203" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="K10" s="197"/>
+      <c r="K10" s="203"/>
       <c r="M10" s="12"/>
       <c r="O10" s="13"/>
       <c r="Q10" s="21" t="s">
@@ -3256,19 +3256,19 @@
       <c r="D11" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="198" t="str">
+      <c r="E11" s="204" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F11" s="198"/>
+      <c r="F11" s="204"/>
       <c r="I11" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="199" t="str">
+      <c r="J11" s="205" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="K11" s="199"/>
+      <c r="K11" s="205"/>
       <c r="M11" s="12"/>
       <c r="O11" s="13"/>
       <c r="Q11" s="21" t="s">
@@ -3300,10 +3300,10 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="AF11" s="180" t="s">
+      <c r="AF11" s="176" t="s">
         <v>156</v>
       </c>
-      <c r="AG11" s="180" t="s">
+      <c r="AG11" s="176" t="s">
         <v>157</v>
       </c>
     </row>
@@ -3315,19 +3315,19 @@
       <c r="D12" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="198" t="str">
+      <c r="E12" s="204" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F12" s="198"/>
+      <c r="F12" s="204"/>
       <c r="I12" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="198" t="str">
+      <c r="J12" s="204" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="K12" s="198"/>
+      <c r="K12" s="204"/>
       <c r="M12" s="12"/>
       <c r="O12" s="13"/>
       <c r="Q12" s="21" t="s">
@@ -3372,19 +3372,19 @@
       <c r="D13" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="198" t="str">
+      <c r="E13" s="204" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F13" s="198"/>
+      <c r="F13" s="204"/>
       <c r="I13" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="198" t="str">
+      <c r="J13" s="204" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="K13" s="198"/>
+      <c r="K13" s="204"/>
       <c r="M13" s="12"/>
       <c r="O13" s="13"/>
       <c r="Q13" s="21" t="s">
@@ -3429,19 +3429,19 @@
       <c r="D14" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="198" t="str">
+      <c r="E14" s="204" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F14" s="198"/>
+      <c r="F14" s="204"/>
       <c r="I14" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="198" t="str">
+      <c r="J14" s="204" t="str">
         <f>IF(V14="","",V14)</f>
         <v/>
       </c>
-      <c r="K14" s="198"/>
+      <c r="K14" s="204"/>
       <c r="M14" s="12"/>
       <c r="O14" s="13"/>
       <c r="Q14" s="21" t="s">
@@ -3486,11 +3486,11 @@
       <c r="D15" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="198" t="str">
+      <c r="E15" s="204" t="str">
         <f t="shared" si="1"/>
         <v>IMPAX 4.2 2015</v>
       </c>
-      <c r="F15" s="198"/>
+      <c r="F15" s="204"/>
       <c r="M15" s="12"/>
       <c r="O15" s="26"/>
       <c r="P15" s="27"/>
@@ -3644,10 +3644,10 @@
       <c r="H19" s="154"/>
       <c r="I19" s="154"/>
       <c r="J19" s="154"/>
-      <c r="K19" s="201" t="s">
+      <c r="K19" s="207" t="s">
         <v>129</v>
       </c>
-      <c r="L19" s="201"/>
+      <c r="L19" s="207"/>
       <c r="M19" s="5"/>
       <c r="O19" s="13"/>
       <c r="R19" s="1" t="s">
@@ -3917,11 +3917,11 @@
       <c r="D24" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="200" t="str">
+      <c r="E24" s="206" t="str">
         <f>IF(P52="","",P52)</f>
         <v/>
       </c>
-      <c r="F24" s="200"/>
+      <c r="F24" s="206"/>
       <c r="G24" s="40"/>
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
@@ -4000,7 +4000,7 @@
       <c r="S26" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="T26" s="232" t="str">
+      <c r="T26" s="195" t="str">
         <f>IF(AG12="","",AG12)</f>
         <v/>
       </c>
@@ -5287,7 +5287,7 @@
         <f>R58</f>
         <v>Right ()</v>
       </c>
-      <c r="J51" s="193" t="str">
+      <c r="J51" s="187" t="str">
         <f>IF(R60="","",R60)</f>
         <v/>
       </c>
@@ -5336,7 +5336,7 @@
       <c r="B52" s="10"/>
       <c r="F52" s="95"/>
       <c r="I52" s="62"/>
-      <c r="J52" s="192"/>
+      <c r="J52" s="186"/>
       <c r="M52" s="12"/>
       <c r="O52" s="84" t="s">
         <v>20</v>
@@ -5375,7 +5375,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="10"/>
-      <c r="E53" s="192" t="str">
+      <c r="E53" s="186" t="str">
         <f>Q58</f>
         <v>Left ()</v>
       </c>
@@ -5427,11 +5427,11 @@
       <c r="D54" s="52" t="s">
         <v>178</v>
       </c>
-      <c r="E54" s="233" t="str">
+      <c r="E54" s="196" t="str">
         <f>IF(Q61="","",Q61)</f>
         <v/>
       </c>
-      <c r="F54" s="234" t="str">
+      <c r="F54" s="197" t="str">
         <f>IF(R61="","",R61)</f>
         <v/>
       </c>
@@ -5461,11 +5461,11 @@
       <c r="D55" s="52" t="s">
         <v>179</v>
       </c>
-      <c r="E55" s="235" t="str">
+      <c r="E55" s="198" t="str">
         <f>IF(Q62="","",Q62)</f>
         <v/>
       </c>
-      <c r="F55" s="236" t="str">
+      <c r="F55" s="199" t="str">
         <f>IF(R62="","",R62)</f>
         <v/>
       </c>
@@ -5649,23 +5649,23 @@
       <c r="P59" s="66" t="s">
         <v>147</v>
       </c>
-      <c r="Q59" s="181" t="str">
+      <c r="Q59" s="177" t="str">
         <f>IF(AG12="","",AG13+Lamb)</f>
         <v/>
       </c>
-      <c r="R59" s="182" t="str">
+      <c r="R59" s="178" t="str">
         <f>IF(AG13="","",AG14+Lamb)</f>
         <v/>
       </c>
       <c r="S59" s="2"/>
-      <c r="T59" s="179" t="s">
+      <c r="T59" s="175" t="s">
         <v>147</v>
       </c>
-      <c r="U59" s="175" t="str">
+      <c r="U59" s="231" t="str">
         <f>IF(AB31="","",AB31)</f>
         <v/>
       </c>
-      <c r="V59" s="176" t="str">
+      <c r="V59" s="232" t="str">
         <f>IF(AB32="","",AB32)</f>
         <v/>
       </c>
@@ -5695,23 +5695,23 @@
       <c r="P60" s="66" t="s">
         <v>148</v>
       </c>
-      <c r="Q60" s="184" t="str">
+      <c r="Q60" s="180" t="str">
         <f>IF(AG14="","",AG15+Lamb)</f>
         <v/>
       </c>
-      <c r="R60" s="185" t="str">
+      <c r="R60" s="181" t="str">
         <f>IF(AG15="","",AG16+Lamb)</f>
         <v/>
       </c>
       <c r="S60" s="2"/>
-      <c r="T60" s="179" t="s">
+      <c r="T60" s="175" t="s">
         <v>148</v>
       </c>
-      <c r="U60" s="190" t="str">
+      <c r="U60" s="233" t="str">
         <f>IF(AB33="","",AB33)</f>
         <v/>
       </c>
-      <c r="V60" s="191" t="str">
+      <c r="V60" s="234" t="str">
         <f>IF(AB34="","",AB34)</f>
         <v/>
       </c>
@@ -5741,22 +5741,22 @@
       <c r="P61" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="Q61" s="225" t="str">
+      <c r="Q61" s="188" t="str">
         <f>IF(Q59="","",Q60/Q59)</f>
         <v/>
       </c>
-      <c r="R61" s="226" t="str">
+      <c r="R61" s="189" t="str">
         <f>IF(R59="","",R60/R59)</f>
         <v/>
       </c>
       <c r="T61" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="U61" s="190" t="str">
+      <c r="U61" s="233" t="str">
         <f>IF(AB35="","",AB35)</f>
         <v/>
       </c>
-      <c r="V61" s="191" t="str">
+      <c r="V61" s="234" t="str">
         <f>IF(AB36="","",AB36)</f>
         <v/>
       </c>
@@ -5784,22 +5784,22 @@
       <c r="P62" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="Q62" s="227" t="str">
+      <c r="Q62" s="190" t="str">
         <f>IF(OR(Q59="",Lamb=""),"",Lamb/Q59)</f>
         <v/>
       </c>
-      <c r="R62" s="228" t="str">
+      <c r="R62" s="191" t="str">
         <f>IF(OR(R59="",Lamb=""),"",Lamb/R59)</f>
         <v/>
       </c>
       <c r="T62" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="U62" s="177" t="str">
+      <c r="U62" s="235" t="str">
         <f>IF(AB37="","",AB37)</f>
         <v/>
       </c>
-      <c r="V62" s="178" t="str">
+      <c r="V62" s="236" t="str">
         <f>IF(AB38="","",AB38)</f>
         <v/>
       </c>
@@ -6108,16 +6108,16 @@
       </c>
       <c r="B71" s="10"/>
       <c r="C71" s="95"/>
-      <c r="D71" s="202" t="str">
+      <c r="D71" s="208" t="str">
         <f>Q86</f>
         <v>UNL-10 (cd/m^2)</v>
       </c>
-      <c r="E71" s="202"/>
-      <c r="F71" s="203" t="str">
+      <c r="E71" s="208"/>
+      <c r="F71" s="209" t="str">
         <f>S86</f>
         <v>UNL-80 (cd/m^2)</v>
       </c>
-      <c r="G71" s="203"/>
+      <c r="G71" s="209"/>
       <c r="I71" s="68" t="s">
         <v>108</v>
       </c>
@@ -6233,15 +6233,15 @@
       <c r="Q73" s="159" t="s">
         <v>97</v>
       </c>
-      <c r="R73" s="217"/>
-      <c r="S73" s="221"/>
+      <c r="R73" s="223"/>
+      <c r="S73" s="227"/>
       <c r="T73" s="2"/>
       <c r="U73" s="2"/>
-      <c r="V73" s="209" t="str">
+      <c r="V73" s="215" t="str">
         <f>IF(AB48="","",AB48)</f>
         <v/>
       </c>
-      <c r="W73" s="210" t="str">
+      <c r="W73" s="216" t="str">
         <f>IF(AB51="","",AB51)</f>
         <v/>
       </c>
@@ -6286,12 +6286,12 @@
       <c r="O74" s="13"/>
       <c r="P74" s="2"/>
       <c r="Q74" s="159"/>
-      <c r="R74" s="218"/>
-      <c r="S74" s="222"/>
+      <c r="R74" s="224"/>
+      <c r="S74" s="228"/>
       <c r="T74" s="2"/>
       <c r="U74" s="2"/>
-      <c r="V74" s="208"/>
-      <c r="W74" s="211"/>
+      <c r="V74" s="214"/>
+      <c r="W74" s="217"/>
       <c r="X74" s="2"/>
       <c r="Y74" s="14"/>
       <c r="AB74" s="158"/>
@@ -6334,15 +6334,15 @@
       <c r="Q75" s="159" t="s">
         <v>99</v>
       </c>
-      <c r="R75" s="219"/>
-      <c r="S75" s="223"/>
+      <c r="R75" s="225"/>
+      <c r="S75" s="229"/>
       <c r="T75" s="2"/>
       <c r="U75" s="2"/>
-      <c r="V75" s="206" t="str">
+      <c r="V75" s="212" t="str">
         <f>IF(AB49="","",AB49)</f>
         <v/>
       </c>
-      <c r="W75" s="212" t="str">
+      <c r="W75" s="218" t="str">
         <f>IF(AB52="","",AB52)</f>
         <v/>
       </c>
@@ -6386,12 +6386,12 @@
       <c r="O76" s="13"/>
       <c r="P76" s="2"/>
       <c r="Q76" s="159"/>
-      <c r="R76" s="218"/>
-      <c r="S76" s="222"/>
+      <c r="R76" s="224"/>
+      <c r="S76" s="228"/>
       <c r="T76" s="2"/>
       <c r="U76" s="2"/>
-      <c r="V76" s="208"/>
-      <c r="W76" s="211"/>
+      <c r="V76" s="214"/>
+      <c r="W76" s="217"/>
       <c r="X76" s="2"/>
       <c r="Y76" s="14"/>
       <c r="AB76" s="158"/>
@@ -6434,15 +6434,15 @@
       <c r="Q77" s="159" t="s">
         <v>102</v>
       </c>
-      <c r="R77" s="219"/>
-      <c r="S77" s="223"/>
+      <c r="R77" s="225"/>
+      <c r="S77" s="229"/>
       <c r="T77" s="2"/>
       <c r="U77" s="2"/>
-      <c r="V77" s="206" t="str">
+      <c r="V77" s="212" t="str">
         <f>IF(AB50="","",AB50)</f>
         <v/>
       </c>
-      <c r="W77" s="212" t="str">
+      <c r="W77" s="218" t="str">
         <f>IF(AB53="","",AB53)</f>
         <v/>
       </c>
@@ -6461,12 +6461,12 @@
       <c r="O78" s="13"/>
       <c r="P78" s="2"/>
       <c r="Q78" s="159"/>
-      <c r="R78" s="220"/>
-      <c r="S78" s="224"/>
+      <c r="R78" s="226"/>
+      <c r="S78" s="230"/>
       <c r="T78" s="2"/>
       <c r="U78" s="2"/>
-      <c r="V78" s="207"/>
-      <c r="W78" s="213"/>
+      <c r="V78" s="213"/>
+      <c r="W78" s="219"/>
       <c r="X78" s="2"/>
       <c r="Y78" s="14"/>
       <c r="AB78" s="158"/>
@@ -6684,16 +6684,16 @@
         <v>Right ()</v>
       </c>
       <c r="H84" s="2"/>
-      <c r="I84" s="204" t="str">
+      <c r="I84" s="210" t="str">
         <f>R68</f>
         <v>Left ()</v>
       </c>
-      <c r="J84" s="204"/>
-      <c r="K84" s="204" t="str">
+      <c r="J84" s="210"/>
+      <c r="K84" s="210" t="str">
         <f>S68</f>
         <v>Right ()</v>
       </c>
-      <c r="L84" s="204"/>
+      <c r="L84" s="210"/>
       <c r="M84" s="12"/>
       <c r="O84" s="13"/>
       <c r="P84" s="2"/>
@@ -6737,16 +6737,16 @@
       <c r="H85" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="I85" s="205" t="str">
+      <c r="I85" s="211" t="str">
         <f>IF(R73="","",R73)</f>
         <v/>
       </c>
-      <c r="J85" s="205"/>
-      <c r="K85" s="205" t="str">
+      <c r="J85" s="211"/>
+      <c r="K85" s="211" t="str">
         <f>IF(S73="","",S73)</f>
         <v/>
       </c>
-      <c r="L85" s="205"/>
+      <c r="L85" s="211"/>
       <c r="M85" s="12"/>
       <c r="O85" s="109" t="s">
         <v>107</v>
@@ -6785,27 +6785,27 @@
       <c r="H86" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="I86" s="205" t="str">
+      <c r="I86" s="211" t="str">
         <f>IF(R75="","",R75)</f>
         <v/>
       </c>
-      <c r="J86" s="205"/>
-      <c r="K86" s="205" t="str">
+      <c r="J86" s="211"/>
+      <c r="K86" s="211" t="str">
         <f>IF(S75="","",S75)</f>
         <v/>
       </c>
-      <c r="L86" s="205"/>
+      <c r="L86" s="211"/>
       <c r="M86" s="12"/>
       <c r="O86" s="13"/>
       <c r="P86" s="2"/>
-      <c r="Q86" s="215" t="s">
+      <c r="Q86" s="221" t="s">
         <v>118</v>
       </c>
-      <c r="R86" s="216"/>
-      <c r="S86" s="215" t="s">
+      <c r="R86" s="222"/>
+      <c r="S86" s="221" t="s">
         <v>119</v>
       </c>
-      <c r="T86" s="216"/>
+      <c r="T86" s="222"/>
       <c r="U86" s="2"/>
       <c r="V86" s="127" t="s">
         <v>44</v>
@@ -6835,16 +6835,16 @@
       <c r="H87" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="I87" s="214" t="str">
+      <c r="I87" s="220" t="str">
         <f>IF(R77="","",R77)</f>
         <v/>
       </c>
-      <c r="J87" s="214"/>
-      <c r="K87" s="214" t="str">
+      <c r="J87" s="220"/>
+      <c r="K87" s="220" t="str">
         <f>IF(S77="","",S77)</f>
         <v/>
       </c>
-      <c r="L87" s="214"/>
+      <c r="L87" s="220"/>
       <c r="M87" s="12"/>
       <c r="O87" s="13"/>
       <c r="P87" s="2"/>
@@ -6903,20 +6903,20 @@
       <c r="P88" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="Q88" s="181" t="str">
-        <f>IF(AG16="","",AG17+Lamb)</f>
-        <v/>
-      </c>
-      <c r="R88" s="182" t="str">
-        <f>IF(AG25="","",AG26+Lamb)</f>
-        <v/>
-      </c>
-      <c r="S88" s="183" t="str">
-        <f>IF(AG34="","",AG35+Lamb)</f>
-        <v/>
-      </c>
-      <c r="T88" s="182" t="str">
-        <f>IF(AG43="","",AG44+Lamb)</f>
+      <c r="Q88" s="177" t="str">
+        <f t="shared" ref="Q88:Q96" si="16">IF(AG17="","",AG17+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R88" s="178" t="str">
+        <f t="shared" ref="R88:R96" si="17">IF(AG26="","",AG26+Lamb)</f>
+        <v/>
+      </c>
+      <c r="S88" s="179" t="str">
+        <f t="shared" ref="S88:S96" si="18">IF(AG35="","",AG35+Lamb)</f>
+        <v/>
+      </c>
+      <c r="T88" s="178" t="str">
+        <f t="shared" ref="T88:T96" si="19">IF(AG44="","",AG44+Lamb)</f>
         <v/>
       </c>
       <c r="U88" s="2"/>
@@ -6926,19 +6926,19 @@
       </c>
       <c r="X88" s="2"/>
       <c r="Y88" s="14"/>
-      <c r="AA88" s="231" t="e">
+      <c r="AA88" s="194" t="e">
         <f>ABS(Q88-MEDIAN($Q$88:$Q$96))/MEDIAN($Q$88:$Q$96)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AB88" s="231" t="e">
+      <c r="AB88" s="194" t="e">
         <f>ABS(R88-MEDIAN($R$88:$R$96))/MEDIAN($R$88:$R$96)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AC88" s="231" t="e">
+      <c r="AC88" s="194" t="e">
         <f>ABS(S88-MEDIAN($S$88:$S$96))/MEDIAN($S$88:$S$96)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AD88" s="231" t="e">
+      <c r="AD88" s="194" t="e">
         <f>ABS(T88-MEDIAN($T$88:$T$96))/MEDIAN($T$88:$T$96)</f>
         <v>#VALUE!</v>
       </c>
@@ -6966,20 +6966,20 @@
       <c r="P89" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="Q89" s="184" t="str">
-        <f>IF(AG17="","",AG18+Lamb)</f>
-        <v/>
-      </c>
-      <c r="R89" s="185" t="str">
-        <f>IF(AG26="","",AG27+Lamb)</f>
-        <v/>
-      </c>
-      <c r="S89" s="186" t="str">
-        <f>IF(AG35="","",AG36+Lamb)</f>
-        <v/>
-      </c>
-      <c r="T89" s="185" t="str">
-        <f>IF(AG44="","",AG45+Lamb)</f>
+      <c r="Q89" s="180" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="R89" s="181" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="S89" s="182" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="T89" s="181" t="str">
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="U89" s="2"/>
@@ -6989,20 +6989,20 @@
       </c>
       <c r="X89" s="2"/>
       <c r="Y89" s="14"/>
-      <c r="AA89" s="231" t="e">
-        <f t="shared" ref="AA89:AA96" si="16">ABS(Q89-MEDIAN($Q$88:$Q$96))/MEDIAN($Q$88:$Q$96)</f>
+      <c r="AA89" s="194" t="e">
+        <f t="shared" ref="AA89:AA96" si="20">ABS(Q89-MEDIAN($Q$88:$Q$96))/MEDIAN($Q$88:$Q$96)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AB89" s="231" t="e">
-        <f t="shared" ref="AB89:AB96" si="17">ABS(R89-MEDIAN($R$88:$R$96))/MEDIAN($R$88:$R$96)</f>
+      <c r="AB89" s="194" t="e">
+        <f t="shared" ref="AB89:AB96" si="21">ABS(R89-MEDIAN($R$88:$R$96))/MEDIAN($R$88:$R$96)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AC89" s="231" t="e">
-        <f t="shared" ref="AC89:AC96" si="18">ABS(S89-MEDIAN($S$88:$S$96))/MEDIAN($S$88:$S$96)</f>
+      <c r="AC89" s="194" t="e">
+        <f t="shared" ref="AC89:AC96" si="22">ABS(S89-MEDIAN($S$88:$S$96))/MEDIAN($S$88:$S$96)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AD89" s="231" t="e">
-        <f t="shared" ref="AD89:AD96" si="19">ABS(T89-MEDIAN($T$88:$T$96))/MEDIAN($T$88:$T$96)</f>
+      <c r="AD89" s="194" t="e">
+        <f t="shared" ref="AD89:AD96" si="23">ABS(T89-MEDIAN($T$88:$T$96))/MEDIAN($T$88:$T$96)</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7029,20 +7029,20 @@
       <c r="P90" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="Q90" s="184" t="str">
-        <f>IF(AG18="","",AG19+Lamb)</f>
-        <v/>
-      </c>
-      <c r="R90" s="185" t="str">
-        <f>IF(AG27="","",AG28+Lamb)</f>
-        <v/>
-      </c>
-      <c r="S90" s="186" t="str">
-        <f>IF(AG36="","",AG37+Lamb)</f>
-        <v/>
-      </c>
-      <c r="T90" s="185" t="str">
-        <f>IF(AG45="","",AG46+Lamb)</f>
+      <c r="Q90" s="180" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="R90" s="181" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="S90" s="182" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="T90" s="181" t="str">
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="U90" s="2"/>
@@ -7050,20 +7050,20 @@
       <c r="W90" s="2"/>
       <c r="X90" s="2"/>
       <c r="Y90" s="14"/>
-      <c r="AA90" s="231" t="e">
-        <f t="shared" si="16"/>
+      <c r="AA90" s="194" t="e">
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB90" s="231" t="e">
-        <f t="shared" si="17"/>
+      <c r="AB90" s="194" t="e">
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AC90" s="231" t="e">
-        <f t="shared" si="18"/>
+      <c r="AC90" s="194" t="e">
+        <f t="shared" si="22"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AD90" s="231" t="e">
-        <f t="shared" si="19"/>
+      <c r="AD90" s="194" t="e">
+        <f t="shared" si="23"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7077,20 +7077,20 @@
       <c r="P91" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="Q91" s="184" t="str">
-        <f>IF(AG19="","",AG20+Lamb)</f>
-        <v/>
-      </c>
-      <c r="R91" s="185" t="str">
-        <f>IF(AG28="","",AG29+Lamb)</f>
-        <v/>
-      </c>
-      <c r="S91" s="186" t="str">
-        <f>IF(AG37="","",AG38+Lamb)</f>
-        <v/>
-      </c>
-      <c r="T91" s="185" t="str">
-        <f>IF(AG46="","",AG47+Lamb)</f>
+      <c r="Q91" s="180" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="R91" s="181" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="S91" s="182" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="T91" s="181" t="str">
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="U91" s="2"/>
@@ -7098,20 +7098,20 @@
       <c r="W91" s="2"/>
       <c r="X91" s="2"/>
       <c r="Y91" s="14"/>
-      <c r="AA91" s="231" t="e">
-        <f t="shared" si="16"/>
+      <c r="AA91" s="194" t="e">
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB91" s="231" t="e">
-        <f t="shared" si="17"/>
+      <c r="AB91" s="194" t="e">
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AC91" s="231" t="e">
-        <f t="shared" si="18"/>
+      <c r="AC91" s="194" t="e">
+        <f t="shared" si="22"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AD91" s="231" t="e">
-        <f t="shared" si="19"/>
+      <c r="AD91" s="194" t="e">
+        <f t="shared" si="23"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7128,20 +7128,20 @@
       <c r="P92" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="Q92" s="184" t="str">
-        <f>IF(AG20="","",AG21+Lamb)</f>
-        <v/>
-      </c>
-      <c r="R92" s="185" t="str">
-        <f>IF(AG29="","",AG30+Lamb)</f>
-        <v/>
-      </c>
-      <c r="S92" s="186" t="str">
-        <f>IF(AG38="","",AG39+Lamb)</f>
-        <v/>
-      </c>
-      <c r="T92" s="185" t="str">
-        <f>IF(AG47="","",AG48+Lamb)</f>
+      <c r="Q92" s="180" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="R92" s="181" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="S92" s="182" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="T92" s="181" t="str">
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="U92" s="2"/>
@@ -7149,20 +7149,20 @@
       <c r="W92" s="2"/>
       <c r="X92" s="2"/>
       <c r="Y92" s="14"/>
-      <c r="AA92" s="231" t="e">
-        <f t="shared" si="16"/>
+      <c r="AA92" s="194" t="e">
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB92" s="231" t="e">
-        <f t="shared" si="17"/>
+      <c r="AB92" s="194" t="e">
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AC92" s="231" t="e">
-        <f t="shared" si="18"/>
+      <c r="AC92" s="194" t="e">
+        <f t="shared" si="22"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AD92" s="231" t="e">
-        <f t="shared" si="19"/>
+      <c r="AD92" s="194" t="e">
+        <f t="shared" si="23"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7188,37 +7188,37 @@
       <c r="P93" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="Q93" s="184" t="str">
-        <f>IF(AG21="","",AG22+Lamb)</f>
-        <v/>
-      </c>
-      <c r="R93" s="185" t="str">
-        <f>IF(AG30="","",AG31+Lamb)</f>
-        <v/>
-      </c>
-      <c r="S93" s="186" t="str">
-        <f>IF(AG39="","",AG40+Lamb)</f>
-        <v/>
-      </c>
-      <c r="T93" s="185" t="str">
-        <f>IF(AG48="","",AG49+Lamb)</f>
+      <c r="Q93" s="180" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="R93" s="181" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="S93" s="182" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="T93" s="181" t="str">
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="Y93" s="14"/>
-      <c r="AA93" s="231" t="e">
-        <f t="shared" si="16"/>
+      <c r="AA93" s="194" t="e">
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB93" s="231" t="e">
-        <f t="shared" si="17"/>
+      <c r="AB93" s="194" t="e">
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AC93" s="231" t="e">
-        <f t="shared" si="18"/>
+      <c r="AC93" s="194" t="e">
+        <f t="shared" si="22"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AD93" s="231" t="e">
-        <f t="shared" si="19"/>
+      <c r="AD93" s="194" t="e">
+        <f t="shared" si="23"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7244,37 +7244,37 @@
       <c r="P94" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="Q94" s="184" t="str">
-        <f>IF(AG22="","",AG23+Lamb)</f>
-        <v/>
-      </c>
-      <c r="R94" s="185" t="str">
-        <f>IF(AG31="","",AG32+Lamb)</f>
-        <v/>
-      </c>
-      <c r="S94" s="186" t="str">
-        <f>IF(AG40="","",AG41+Lamb)</f>
-        <v/>
-      </c>
-      <c r="T94" s="185" t="str">
-        <f>IF(AG49="","",AG50+Lamb)</f>
+      <c r="Q94" s="180" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="R94" s="181" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="S94" s="182" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="T94" s="181" t="str">
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="Y94" s="14"/>
-      <c r="AA94" s="231" t="e">
-        <f t="shared" si="16"/>
+      <c r="AA94" s="194" t="e">
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB94" s="231" t="e">
-        <f t="shared" si="17"/>
+      <c r="AB94" s="194" t="e">
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AC94" s="231" t="e">
-        <f t="shared" si="18"/>
+      <c r="AC94" s="194" t="e">
+        <f t="shared" si="22"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AD94" s="231" t="e">
-        <f t="shared" si="19"/>
+      <c r="AD94" s="194" t="e">
+        <f t="shared" si="23"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7300,37 +7300,37 @@
       <c r="P95" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="Q95" s="184" t="str">
-        <f>IF(AG23="","",AG24+Lamb)</f>
-        <v/>
-      </c>
-      <c r="R95" s="185" t="str">
-        <f>IF(AG32="","",AG33+Lamb)</f>
-        <v/>
-      </c>
-      <c r="S95" s="186" t="str">
-        <f>IF(AG41="","",AG42+Lamb)</f>
-        <v/>
-      </c>
-      <c r="T95" s="185" t="str">
-        <f>IF(AG50="","",AG51+Lamb)</f>
+      <c r="Q95" s="180" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="R95" s="181" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="S95" s="182" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="T95" s="181" t="str">
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="Y95" s="14"/>
-      <c r="AA95" s="231" t="e">
-        <f t="shared" si="16"/>
+      <c r="AA95" s="194" t="e">
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB95" s="231" t="e">
-        <f t="shared" si="17"/>
+      <c r="AB95" s="194" t="e">
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AC95" s="231" t="e">
-        <f t="shared" si="18"/>
+      <c r="AC95" s="194" t="e">
+        <f t="shared" si="22"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AD95" s="231" t="e">
-        <f t="shared" si="19"/>
+      <c r="AD95" s="194" t="e">
+        <f t="shared" si="23"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7356,37 +7356,37 @@
       <c r="P96" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="Q96" s="187" t="str">
-        <f>IF(AG24="","",AG25+Lamb)</f>
-        <v/>
-      </c>
-      <c r="R96" s="188" t="str">
-        <f>IF(AG33="","",AG34+Lamb)</f>
-        <v/>
-      </c>
-      <c r="S96" s="189" t="str">
-        <f>IF(AG42="","",AG43+Lamb)</f>
-        <v/>
-      </c>
-      <c r="T96" s="188" t="str">
-        <f>IF(AG51="","",AG52+Lamb)</f>
+      <c r="Q96" s="183" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="R96" s="184" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="S96" s="185" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="T96" s="184" t="str">
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="Y96" s="14"/>
-      <c r="AA96" s="231" t="e">
-        <f t="shared" si="16"/>
+      <c r="AA96" s="194" t="e">
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB96" s="231" t="e">
-        <f t="shared" si="17"/>
+      <c r="AB96" s="194" t="e">
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AC96" s="231" t="e">
-        <f t="shared" si="18"/>
+      <c r="AC96" s="194" t="e">
+        <f t="shared" si="22"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AD96" s="231" t="e">
-        <f t="shared" si="19"/>
+      <c r="AD96" s="194" t="e">
+        <f t="shared" si="23"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7548,19 +7548,19 @@
       <c r="P100" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="Q100" s="229" t="str">
+      <c r="Q100" s="192" t="str">
         <f>IF(Q88="","",MAX(AA88:AA96))</f>
         <v/>
       </c>
-      <c r="R100" s="230" t="str">
+      <c r="R100" s="193" t="str">
         <f>IF(R88="","",MAX(AB88:AB96))</f>
         <v/>
       </c>
-      <c r="S100" s="229" t="str">
+      <c r="S100" s="192" t="str">
         <f>IF(S88="","",MAX(AC88:AC96))</f>
         <v/>
       </c>
-      <c r="T100" s="230" t="str">
+      <c r="T100" s="193" t="str">
         <f>IF(T88="","",MAX(AD88:AD96))</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
Add overall luminance calc
</commit_message>
<xml_diff>
--- a/MUSCMammoMonitor.xlsx
+++ b/MUSCMammoMonitor.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\EquipTestingSpreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugenem\Documents\GitHub\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6861AF77-9C69-4059-93C2-C46413026BB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D79B9E-EBEF-43BE-9B71-DFA2A16884CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Barco" sheetId="1" r:id="rId1"/>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="186">
   <si>
     <t>Print Area</t>
   </si>
@@ -651,6 +651,12 @@
   </si>
   <si>
     <t>Lum Dev from Median (%):</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>SD</t>
   </si>
 </sst>
 </file>
@@ -1594,7 +1600,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="237">
+  <cellXfs count="238">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2193,38 +2199,56 @@
     <xf numFmtId="2" fontId="10" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2253,56 +2277,41 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -2832,21 +2841,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
+    <sheetView tabSelected="1" topLeftCell="N82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X98" sqref="X98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="2.5546875" style="1" customWidth="1"/>
-    <col min="3" max="11" width="11.5546875" style="1"/>
-    <col min="12" max="12" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5546875" style="1"/>
-    <col min="14" max="14" width="2.5546875" style="1" customWidth="1"/>
-    <col min="15" max="36" width="11.5546875" style="1"/>
+    <col min="1" max="2" width="2.5703125" style="1" customWidth="1"/>
+    <col min="3" max="11" width="11.5703125" style="1"/>
+    <col min="12" max="12" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" style="1"/>
+    <col min="14" max="14" width="2.5703125" style="1" customWidth="1"/>
+    <col min="15" max="36" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="14.4" customHeight="1">
+    <row r="1" spans="1:36" ht="14.45" customHeight="1">
       <c r="A1" s="2">
         <v>1</v>
       </c>
@@ -2878,14 +2887,14 @@
       <c r="AA1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="AG1" s="200" t="s">
+      <c r="AG1" s="233" t="s">
         <v>1</v>
       </c>
-      <c r="AH1" s="200"/>
-      <c r="AI1" s="200"/>
-      <c r="AJ1" s="200"/>
-    </row>
-    <row r="2" spans="1:36" ht="14.4" customHeight="1">
+      <c r="AH1" s="233"/>
+      <c r="AI1" s="233"/>
+      <c r="AJ1" s="233"/>
+    </row>
+    <row r="2" spans="1:36" ht="14.45" customHeight="1">
       <c r="A2" s="2">
         <v>2</v>
       </c>
@@ -2900,16 +2909,16 @@
       </c>
       <c r="Y2" s="14"/>
       <c r="AA2" s="15"/>
-      <c r="AG2" s="201" t="s">
+      <c r="AG2" s="234" t="s">
         <v>3</v>
       </c>
-      <c r="AH2" s="201"/>
-      <c r="AI2" s="202" t="s">
+      <c r="AH2" s="234"/>
+      <c r="AI2" s="235" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="202"/>
-    </row>
-    <row r="3" spans="1:36" ht="14.4" customHeight="1">
+      <c r="AJ2" s="235"/>
+    </row>
+    <row r="3" spans="1:36" ht="14.45" customHeight="1">
       <c r="A3" s="2">
         <v>3</v>
       </c>
@@ -2940,7 +2949,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="14.4" customHeight="1">
+    <row r="4" spans="1:36" ht="14.45" customHeight="1">
       <c r="A4" s="2">
         <v>4</v>
       </c>
@@ -2970,7 +2979,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="14.4" customHeight="1">
+    <row r="5" spans="1:36" ht="14.45" customHeight="1">
       <c r="A5" s="2">
         <v>5</v>
       </c>
@@ -3000,7 +3009,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="14.4" customHeight="1">
+    <row r="6" spans="1:36" ht="14.45" customHeight="1">
       <c r="A6" s="2">
         <v>6</v>
       </c>
@@ -3049,7 +3058,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="14.4" customHeight="1">
+    <row r="7" spans="1:36" ht="14.45" customHeight="1">
       <c r="A7" s="2">
         <v>7</v>
       </c>
@@ -3096,7 +3105,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="14.4" customHeight="1">
+    <row r="8" spans="1:36" ht="14.45" customHeight="1">
       <c r="A8" s="2">
         <v>8</v>
       </c>
@@ -3141,7 +3150,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="14.4" customHeight="1">
+    <row r="9" spans="1:36" ht="14.45" customHeight="1">
       <c r="A9" s="2">
         <v>9</v>
       </c>
@@ -3193,7 +3202,7 @@
       </c>
       <c r="AG9" s="2"/>
     </row>
-    <row r="10" spans="1:36" ht="14.4" customHeight="1">
+    <row r="10" spans="1:36" ht="14.45" customHeight="1">
       <c r="A10" s="2">
         <v>10</v>
       </c>
@@ -3201,19 +3210,19 @@
       <c r="D10" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="203" t="str">
+      <c r="E10" s="236" t="str">
         <f t="shared" ref="E10:E15" si="1">IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="F10" s="203"/>
+      <c r="F10" s="236"/>
       <c r="I10" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="203" t="str">
+      <c r="J10" s="236" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="K10" s="203"/>
+      <c r="K10" s="236"/>
       <c r="M10" s="12"/>
       <c r="O10" s="13"/>
       <c r="Q10" s="21" t="s">
@@ -3248,7 +3257,7 @@
       <c r="AF10" s="2"/>
       <c r="AG10" s="2"/>
     </row>
-    <row r="11" spans="1:36" ht="14.4" customHeight="1">
+    <row r="11" spans="1:36" ht="14.45" customHeight="1">
       <c r="A11" s="2">
         <v>11</v>
       </c>
@@ -3256,19 +3265,19 @@
       <c r="D11" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="204" t="str">
+      <c r="E11" s="229" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F11" s="204"/>
+      <c r="F11" s="229"/>
       <c r="I11" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="205" t="str">
+      <c r="J11" s="232" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="K11" s="205"/>
+      <c r="K11" s="232"/>
       <c r="M11" s="12"/>
       <c r="O11" s="13"/>
       <c r="Q11" s="21" t="s">
@@ -3307,7 +3316,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="14.4" customHeight="1">
+    <row r="12" spans="1:36" ht="14.45" customHeight="1">
       <c r="A12" s="2">
         <v>12</v>
       </c>
@@ -3315,19 +3324,19 @@
       <c r="D12" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="204" t="str">
+      <c r="E12" s="229" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F12" s="204"/>
+      <c r="F12" s="229"/>
       <c r="I12" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="204" t="str">
+      <c r="J12" s="229" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="K12" s="204"/>
+      <c r="K12" s="229"/>
       <c r="M12" s="12"/>
       <c r="O12" s="13"/>
       <c r="Q12" s="21" t="s">
@@ -3364,7 +3373,7 @@
       </c>
       <c r="AG12" s="2"/>
     </row>
-    <row r="13" spans="1:36" ht="14.4" customHeight="1">
+    <row r="13" spans="1:36" ht="14.45" customHeight="1">
       <c r="A13" s="2">
         <v>13</v>
       </c>
@@ -3372,19 +3381,19 @@
       <c r="D13" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="204" t="str">
+      <c r="E13" s="229" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F13" s="204"/>
+      <c r="F13" s="229"/>
       <c r="I13" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="204" t="str">
+      <c r="J13" s="229" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="K13" s="204"/>
+      <c r="K13" s="229"/>
       <c r="M13" s="12"/>
       <c r="O13" s="13"/>
       <c r="Q13" s="21" t="s">
@@ -3421,7 +3430,7 @@
       </c>
       <c r="AG13" s="2"/>
     </row>
-    <row r="14" spans="1:36" ht="14.4" customHeight="1">
+    <row r="14" spans="1:36" ht="14.45" customHeight="1">
       <c r="A14" s="2">
         <v>14</v>
       </c>
@@ -3429,19 +3438,19 @@
       <c r="D14" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="204" t="str">
+      <c r="E14" s="229" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F14" s="204"/>
+      <c r="F14" s="229"/>
       <c r="I14" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="204" t="str">
+      <c r="J14" s="229" t="str">
         <f>IF(V14="","",V14)</f>
         <v/>
       </c>
-      <c r="K14" s="204"/>
+      <c r="K14" s="229"/>
       <c r="M14" s="12"/>
       <c r="O14" s="13"/>
       <c r="Q14" s="21" t="s">
@@ -3478,7 +3487,7 @@
       </c>
       <c r="AG14" s="2"/>
     </row>
-    <row r="15" spans="1:36" ht="14.4" customHeight="1" thickBot="1">
+    <row r="15" spans="1:36" ht="14.45" customHeight="1" thickBot="1">
       <c r="A15" s="2">
         <v>15</v>
       </c>
@@ -3486,11 +3495,11 @@
       <c r="D15" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="204" t="str">
+      <c r="E15" s="229" t="str">
         <f t="shared" si="1"/>
         <v>IMPAX 4.2 2015</v>
       </c>
-      <c r="F15" s="204"/>
+      <c r="F15" s="229"/>
       <c r="M15" s="12"/>
       <c r="O15" s="26"/>
       <c r="P15" s="27"/>
@@ -3527,7 +3536,7 @@
       </c>
       <c r="AG15" s="2"/>
     </row>
-    <row r="16" spans="1:36" ht="14.4" customHeight="1" thickBot="1">
+    <row r="16" spans="1:36" ht="14.45" customHeight="1" thickBot="1">
       <c r="A16" s="2">
         <v>16</v>
       </c>
@@ -3560,7 +3569,7 @@
       </c>
       <c r="AG16" s="2"/>
     </row>
-    <row r="17" spans="1:33" ht="14.4" customHeight="1" thickTop="1" thickBot="1">
+    <row r="17" spans="1:33" ht="14.45" customHeight="1" thickTop="1" thickBot="1">
       <c r="A17" s="2">
         <v>17</v>
       </c>
@@ -3590,7 +3599,7 @@
       </c>
       <c r="AG17" s="2"/>
     </row>
-    <row r="18" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
+    <row r="18" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A18" s="2">
         <v>18</v>
       </c>
@@ -3629,7 +3638,7 @@
       </c>
       <c r="AG18" s="2"/>
     </row>
-    <row r="19" spans="1:33" ht="14.4" customHeight="1" thickTop="1">
+    <row r="19" spans="1:33" ht="14.45" customHeight="1" thickTop="1">
       <c r="A19" s="2">
         <v>19</v>
       </c>
@@ -3644,10 +3653,10 @@
       <c r="H19" s="154"/>
       <c r="I19" s="154"/>
       <c r="J19" s="154"/>
-      <c r="K19" s="207" t="s">
+      <c r="K19" s="231" t="s">
         <v>129</v>
       </c>
-      <c r="L19" s="207"/>
+      <c r="L19" s="231"/>
       <c r="M19" s="5"/>
       <c r="O19" s="13"/>
       <c r="R19" s="1" t="s">
@@ -3677,7 +3686,7 @@
       </c>
       <c r="AG19" s="2"/>
     </row>
-    <row r="20" spans="1:33" ht="14.4" customHeight="1">
+    <row r="20" spans="1:33" ht="14.45" customHeight="1">
       <c r="A20" s="2">
         <v>20</v>
       </c>
@@ -3742,7 +3751,7 @@
       </c>
       <c r="AG20" s="2"/>
     </row>
-    <row r="21" spans="1:33" ht="14.4" customHeight="1">
+    <row r="21" spans="1:33" ht="14.45" customHeight="1">
       <c r="A21" s="2">
         <v>21</v>
       </c>
@@ -3798,7 +3807,7 @@
       </c>
       <c r="AG21" s="2"/>
     </row>
-    <row r="22" spans="1:33" ht="14.4" customHeight="1">
+    <row r="22" spans="1:33" ht="14.45" customHeight="1">
       <c r="A22" s="2">
         <v>22</v>
       </c>
@@ -3854,7 +3863,7 @@
       </c>
       <c r="AG22" s="2"/>
     </row>
-    <row r="23" spans="1:33" ht="14.4" customHeight="1">
+    <row r="23" spans="1:33" ht="14.45" customHeight="1">
       <c r="A23" s="2">
         <v>23</v>
       </c>
@@ -3909,7 +3918,7 @@
       </c>
       <c r="AG23" s="2"/>
     </row>
-    <row r="24" spans="1:33" ht="14.4" customHeight="1">
+    <row r="24" spans="1:33" ht="14.45" customHeight="1">
       <c r="A24" s="2">
         <v>24</v>
       </c>
@@ -3917,11 +3926,11 @@
       <c r="D24" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="206" t="str">
+      <c r="E24" s="230" t="str">
         <f>IF(P52="","",P52)</f>
         <v/>
       </c>
-      <c r="F24" s="206"/>
+      <c r="F24" s="230"/>
       <c r="G24" s="40"/>
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
@@ -3948,7 +3957,7 @@
       </c>
       <c r="AG24" s="2"/>
     </row>
-    <row r="25" spans="1:33" ht="14.4" customHeight="1">
+    <row r="25" spans="1:33" ht="14.45" customHeight="1">
       <c r="A25" s="2">
         <v>25</v>
       </c>
@@ -3981,7 +3990,7 @@
       </c>
       <c r="AG25" s="2"/>
     </row>
-    <row r="26" spans="1:33" ht="14.4" customHeight="1">
+    <row r="26" spans="1:33" ht="14.45" customHeight="1">
       <c r="A26" s="2">
         <v>26</v>
       </c>
@@ -4013,7 +4022,7 @@
       </c>
       <c r="AG26" s="2"/>
     </row>
-    <row r="27" spans="1:33" ht="14.4" customHeight="1">
+    <row r="27" spans="1:33" ht="14.45" customHeight="1">
       <c r="A27" s="2">
         <v>27</v>
       </c>
@@ -4073,7 +4082,7 @@
       </c>
       <c r="AG27" s="2"/>
     </row>
-    <row r="28" spans="1:33" ht="14.4" customHeight="1">
+    <row r="28" spans="1:33" ht="14.45" customHeight="1">
       <c r="A28" s="2">
         <v>28</v>
       </c>
@@ -4114,7 +4123,7 @@
       </c>
       <c r="AG28" s="2"/>
     </row>
-    <row r="29" spans="1:33" ht="14.4" customHeight="1">
+    <row r="29" spans="1:33" ht="14.45" customHeight="1">
       <c r="A29" s="2">
         <v>29</v>
       </c>
@@ -4166,7 +4175,7 @@
       </c>
       <c r="AG29" s="2"/>
     </row>
-    <row r="30" spans="1:33" ht="14.4" customHeight="1">
+    <row r="30" spans="1:33" ht="14.45" customHeight="1">
       <c r="A30" s="2">
         <v>30</v>
       </c>
@@ -4218,7 +4227,7 @@
       </c>
       <c r="AG30" s="2"/>
     </row>
-    <row r="31" spans="1:33" ht="14.4" customHeight="1">
+    <row r="31" spans="1:33" ht="14.45" customHeight="1">
       <c r="A31" s="2">
         <v>31</v>
       </c>
@@ -4267,7 +4276,7 @@
       </c>
       <c r="AG31" s="2"/>
     </row>
-    <row r="32" spans="1:33" ht="14.4" customHeight="1">
+    <row r="32" spans="1:33" ht="14.45" customHeight="1">
       <c r="A32" s="2">
         <v>32</v>
       </c>
@@ -4311,7 +4320,7 @@
       </c>
       <c r="AG32" s="2"/>
     </row>
-    <row r="33" spans="1:33" ht="14.4" customHeight="1">
+    <row r="33" spans="1:33" ht="14.45" customHeight="1">
       <c r="A33" s="2">
         <v>33</v>
       </c>
@@ -4363,7 +4372,7 @@
       </c>
       <c r="AG33" s="2"/>
     </row>
-    <row r="34" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
+    <row r="34" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A34" s="2">
         <v>34</v>
       </c>
@@ -4426,7 +4435,7 @@
       </c>
       <c r="AG34" s="2"/>
     </row>
-    <row r="35" spans="1:33" ht="14.4" customHeight="1">
+    <row r="35" spans="1:33" ht="14.45" customHeight="1">
       <c r="A35" s="2">
         <v>35</v>
       </c>
@@ -4484,7 +4493,7 @@
       </c>
       <c r="AG35" s="2"/>
     </row>
-    <row r="36" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
+    <row r="36" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A36" s="2">
         <v>36</v>
       </c>
@@ -4542,7 +4551,7 @@
       </c>
       <c r="AG36" s="2"/>
     </row>
-    <row r="37" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
+    <row r="37" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A37" s="2">
         <v>37</v>
       </c>
@@ -4599,7 +4608,7 @@
       </c>
       <c r="AG37" s="2"/>
     </row>
-    <row r="38" spans="1:33" ht="14.4" customHeight="1">
+    <row r="38" spans="1:33" ht="14.45" customHeight="1">
       <c r="A38" s="2">
         <v>38</v>
       </c>
@@ -4646,7 +4655,7 @@
       </c>
       <c r="AG38" s="2"/>
     </row>
-    <row r="39" spans="1:33" ht="14.4" customHeight="1">
+    <row r="39" spans="1:33" ht="14.45" customHeight="1">
       <c r="A39" s="2">
         <v>39</v>
       </c>
@@ -4698,7 +4707,7 @@
       </c>
       <c r="AG39" s="2"/>
     </row>
-    <row r="40" spans="1:33" ht="14.4" customHeight="1">
+    <row r="40" spans="1:33" ht="14.45" customHeight="1">
       <c r="A40" s="2">
         <v>40</v>
       </c>
@@ -4747,7 +4756,7 @@
       </c>
       <c r="AG40" s="2"/>
     </row>
-    <row r="41" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
+    <row r="41" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A41" s="2">
         <v>41</v>
       </c>
@@ -4795,7 +4804,7 @@
       </c>
       <c r="AG41" s="2"/>
     </row>
-    <row r="42" spans="1:33" ht="14.4" customHeight="1">
+    <row r="42" spans="1:33" ht="14.45" customHeight="1">
       <c r="A42" s="2">
         <v>42</v>
       </c>
@@ -4850,7 +4859,7 @@
       </c>
       <c r="AG42" s="2"/>
     </row>
-    <row r="43" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
+    <row r="43" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A43" s="2">
         <v>43</v>
       </c>
@@ -4908,7 +4917,7 @@
       </c>
       <c r="AG43" s="2"/>
     </row>
-    <row r="44" spans="1:33" ht="14.4" customHeight="1">
+    <row r="44" spans="1:33" ht="14.45" customHeight="1">
       <c r="A44" s="2">
         <v>44</v>
       </c>
@@ -4961,7 +4970,7 @@
       </c>
       <c r="AG44" s="2"/>
     </row>
-    <row r="45" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
+    <row r="45" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A45" s="2">
         <v>45</v>
       </c>
@@ -5016,7 +5025,7 @@
       </c>
       <c r="AG45" s="2"/>
     </row>
-    <row r="46" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
+    <row r="46" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A46" s="2">
         <v>46</v>
       </c>
@@ -5065,7 +5074,7 @@
       </c>
       <c r="AG46" s="2"/>
     </row>
-    <row r="47" spans="1:33" ht="14.4" customHeight="1">
+    <row r="47" spans="1:33" ht="14.45" customHeight="1">
       <c r="A47" s="2">
         <v>47</v>
       </c>
@@ -5108,7 +5117,7 @@
       </c>
       <c r="AG47" s="2"/>
     </row>
-    <row r="48" spans="1:33" ht="14.4" customHeight="1">
+    <row r="48" spans="1:33" ht="14.45" customHeight="1">
       <c r="A48" s="2">
         <v>48</v>
       </c>
@@ -5159,7 +5168,7 @@
       </c>
       <c r="AG48" s="2"/>
     </row>
-    <row r="49" spans="1:33" ht="14.4" customHeight="1">
+    <row r="49" spans="1:33" ht="14.45" customHeight="1">
       <c r="A49" s="2">
         <v>49</v>
       </c>
@@ -5209,7 +5218,7 @@
       </c>
       <c r="AG49" s="2"/>
     </row>
-    <row r="50" spans="1:33" ht="14.4" customHeight="1">
+    <row r="50" spans="1:33" ht="14.45" customHeight="1">
       <c r="A50" s="2">
         <v>50</v>
       </c>
@@ -5267,7 +5276,7 @@
       </c>
       <c r="AG50" s="2"/>
     </row>
-    <row r="51" spans="1:33" ht="14.4" customHeight="1">
+    <row r="51" spans="1:33" ht="14.45" customHeight="1">
       <c r="A51" s="2">
         <v>51</v>
       </c>
@@ -5329,7 +5338,7 @@
       </c>
       <c r="AG51" s="2"/>
     </row>
-    <row r="52" spans="1:33" ht="14.4" customHeight="1">
+    <row r="52" spans="1:33" ht="14.45" customHeight="1">
       <c r="A52" s="2">
         <v>52</v>
       </c>
@@ -5370,7 +5379,7 @@
       </c>
       <c r="AG52" s="2"/>
     </row>
-    <row r="53" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
+    <row r="53" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A53" s="2">
         <v>53</v>
       </c>
@@ -5419,7 +5428,7 @@
       </c>
       <c r="AG53" s="2"/>
     </row>
-    <row r="54" spans="1:33" ht="14.4" customHeight="1">
+    <row r="54" spans="1:33" ht="14.45" customHeight="1">
       <c r="A54" s="2">
         <v>54</v>
       </c>
@@ -5453,7 +5462,7 @@
       <c r="X54" s="78"/>
       <c r="Y54" s="14"/>
     </row>
-    <row r="55" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
+    <row r="55" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A55" s="2">
         <v>55</v>
       </c>
@@ -5490,7 +5499,7 @@
       <c r="AC55" s="20"/>
       <c r="AD55" s="20"/>
     </row>
-    <row r="56" spans="1:33" ht="14.4" customHeight="1">
+    <row r="56" spans="1:33" ht="14.45" customHeight="1">
       <c r="A56" s="2">
         <v>56</v>
       </c>
@@ -5520,7 +5529,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:33" ht="14.4" customHeight="1">
+    <row r="57" spans="1:33" ht="14.45" customHeight="1">
       <c r="A57" s="2">
         <v>57</v>
       </c>
@@ -5567,7 +5576,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
+    <row r="58" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A58" s="2">
         <v>58</v>
       </c>
@@ -5626,7 +5635,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:33" ht="14.4" customHeight="1">
+    <row r="59" spans="1:33" ht="14.45" customHeight="1">
       <c r="A59" s="2">
         <v>59</v>
       </c>
@@ -5661,11 +5670,11 @@
       <c r="T59" s="175" t="s">
         <v>147</v>
       </c>
-      <c r="U59" s="231" t="str">
+      <c r="U59" s="200" t="str">
         <f>IF(AB31="","",AB31)</f>
         <v/>
       </c>
-      <c r="V59" s="232" t="str">
+      <c r="V59" s="201" t="str">
         <f>IF(AB32="","",AB32)</f>
         <v/>
       </c>
@@ -5685,7 +5694,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:33" ht="14.4" customHeight="1">
+    <row r="60" spans="1:33" ht="14.45" customHeight="1">
       <c r="A60" s="2">
         <v>60</v>
       </c>
@@ -5707,11 +5716,11 @@
       <c r="T60" s="175" t="s">
         <v>148</v>
       </c>
-      <c r="U60" s="233" t="str">
+      <c r="U60" s="202" t="str">
         <f>IF(AB33="","",AB33)</f>
         <v/>
       </c>
-      <c r="V60" s="234" t="str">
+      <c r="V60" s="203" t="str">
         <f>IF(AB34="","",AB34)</f>
         <v/>
       </c>
@@ -5731,7 +5740,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:33" ht="14.4" customHeight="1">
+    <row r="61" spans="1:33" ht="14.45" customHeight="1">
       <c r="A61" s="2">
         <v>61</v>
       </c>
@@ -5752,11 +5761,11 @@
       <c r="T61" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="U61" s="233" t="str">
+      <c r="U61" s="202" t="str">
         <f>IF(AB35="","",AB35)</f>
         <v/>
       </c>
-      <c r="V61" s="234" t="str">
+      <c r="V61" s="203" t="str">
         <f>IF(AB36="","",AB36)</f>
         <v/>
       </c>
@@ -5774,7 +5783,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
+    <row r="62" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A62" s="2">
         <v>62</v>
       </c>
@@ -5795,11 +5804,11 @@
       <c r="T62" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="U62" s="235" t="str">
+      <c r="U62" s="204" t="str">
         <f>IF(AB37="","",AB37)</f>
         <v/>
       </c>
-      <c r="V62" s="236" t="str">
+      <c r="V62" s="205" t="str">
         <f>IF(AB38="","",AB38)</f>
         <v/>
       </c>
@@ -5817,7 +5826,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:33" ht="14.4" customHeight="1">
+    <row r="63" spans="1:33" ht="14.45" customHeight="1">
       <c r="A63" s="2">
         <v>63</v>
       </c>
@@ -5843,7 +5852,7 @@
       <c r="AC63" s="20"/>
       <c r="AD63" s="20"/>
     </row>
-    <row r="64" spans="1:33" ht="14.4" customHeight="1" thickBot="1">
+    <row r="64" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A64" s="2">
         <v>64</v>
       </c>
@@ -5888,7 +5897,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:30" ht="14.4" customHeight="1" thickTop="1">
+    <row r="65" spans="1:30" ht="14.45" customHeight="1" thickTop="1">
       <c r="A65" s="2">
         <v>65</v>
       </c>
@@ -5923,7 +5932,7 @@
       <c r="AC65" s="20"/>
       <c r="AD65" s="20"/>
     </row>
-    <row r="66" spans="1:30" ht="14.4" customHeight="1">
+    <row r="66" spans="1:30" ht="14.45" customHeight="1">
       <c r="A66" s="2">
         <v>66</v>
       </c>
@@ -5962,7 +5971,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:30" ht="14.4" customHeight="1">
+    <row r="67" spans="1:30" ht="14.45" customHeight="1">
       <c r="A67" s="2">
         <v>1</v>
       </c>
@@ -5991,7 +6000,7 @@
       <c r="AC67" s="20"/>
       <c r="AD67" s="20"/>
     </row>
-    <row r="68" spans="1:30" ht="14.4" customHeight="1" thickBot="1">
+    <row r="68" spans="1:30" ht="14.45" customHeight="1" thickBot="1">
       <c r="A68" s="2">
         <v>2</v>
       </c>
@@ -6028,7 +6037,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:30" ht="14.4" customHeight="1" thickBot="1">
+    <row r="69" spans="1:30" ht="14.45" customHeight="1" thickBot="1">
       <c r="A69" s="2">
         <v>3</v>
       </c>
@@ -6061,7 +6070,7 @@
       <c r="AC69" s="20"/>
       <c r="AD69" s="20"/>
     </row>
-    <row r="70" spans="1:30" ht="14.4" customHeight="1" thickTop="1" thickBot="1">
+    <row r="70" spans="1:30" ht="14.45" customHeight="1" thickTop="1" thickBot="1">
       <c r="A70" s="2">
         <v>4</v>
       </c>
@@ -6102,22 +6111,22 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:30" ht="14.4" customHeight="1" thickBot="1">
+    <row r="71" spans="1:30" ht="14.45" customHeight="1" thickBot="1">
       <c r="A71" s="2">
         <v>5</v>
       </c>
       <c r="B71" s="10"/>
       <c r="C71" s="95"/>
-      <c r="D71" s="208" t="str">
+      <c r="D71" s="226" t="str">
         <f>Q86</f>
         <v>UNL-10 (cd/m^2)</v>
       </c>
-      <c r="E71" s="208"/>
-      <c r="F71" s="209" t="str">
+      <c r="E71" s="226"/>
+      <c r="F71" s="227" t="str">
         <f>S86</f>
         <v>UNL-80 (cd/m^2)</v>
       </c>
-      <c r="G71" s="209"/>
+      <c r="G71" s="227"/>
       <c r="I71" s="68" t="s">
         <v>108</v>
       </c>
@@ -6139,7 +6148,7 @@
       <c r="AC71" s="20"/>
       <c r="AD71" s="20"/>
     </row>
-    <row r="72" spans="1:30" ht="14.4" customHeight="1" thickBot="1">
+    <row r="72" spans="1:30" ht="14.45" customHeight="1" thickBot="1">
       <c r="A72" s="2">
         <v>6</v>
       </c>
@@ -6196,7 +6205,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:30" ht="14.4" customHeight="1">
+    <row r="73" spans="1:30" ht="14.45" customHeight="1">
       <c r="A73" s="2">
         <v>7</v>
       </c>
@@ -6233,15 +6242,15 @@
       <c r="Q73" s="159" t="s">
         <v>97</v>
       </c>
-      <c r="R73" s="223"/>
-      <c r="S73" s="227"/>
+      <c r="R73" s="209"/>
+      <c r="S73" s="213"/>
       <c r="T73" s="2"/>
       <c r="U73" s="2"/>
-      <c r="V73" s="215" t="str">
+      <c r="V73" s="221" t="str">
         <f>IF(AB48="","",AB48)</f>
         <v/>
       </c>
-      <c r="W73" s="216" t="str">
+      <c r="W73" s="222" t="str">
         <f>IF(AB51="","",AB51)</f>
         <v/>
       </c>
@@ -6251,7 +6260,7 @@
       <c r="AC73" s="20"/>
       <c r="AD73" s="20"/>
     </row>
-    <row r="74" spans="1:30" ht="14.4" customHeight="1">
+    <row r="74" spans="1:30" ht="14.45" customHeight="1">
       <c r="A74" s="2">
         <v>8</v>
       </c>
@@ -6286,12 +6295,12 @@
       <c r="O74" s="13"/>
       <c r="P74" s="2"/>
       <c r="Q74" s="159"/>
-      <c r="R74" s="224"/>
-      <c r="S74" s="228"/>
+      <c r="R74" s="210"/>
+      <c r="S74" s="214"/>
       <c r="T74" s="2"/>
       <c r="U74" s="2"/>
-      <c r="V74" s="214"/>
-      <c r="W74" s="217"/>
+      <c r="V74" s="220"/>
+      <c r="W74" s="223"/>
       <c r="X74" s="2"/>
       <c r="Y74" s="14"/>
       <c r="AB74" s="158"/>
@@ -6304,7 +6313,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:30" ht="14.4" customHeight="1">
+    <row r="75" spans="1:30" ht="14.45" customHeight="1">
       <c r="A75" s="2">
         <v>9</v>
       </c>
@@ -6334,15 +6343,15 @@
       <c r="Q75" s="159" t="s">
         <v>99</v>
       </c>
-      <c r="R75" s="225"/>
-      <c r="S75" s="229"/>
+      <c r="R75" s="211"/>
+      <c r="S75" s="215"/>
       <c r="T75" s="2"/>
       <c r="U75" s="2"/>
-      <c r="V75" s="212" t="str">
+      <c r="V75" s="218" t="str">
         <f>IF(AB49="","",AB49)</f>
         <v/>
       </c>
-      <c r="W75" s="218" t="str">
+      <c r="W75" s="224" t="str">
         <f>IF(AB52="","",AB52)</f>
         <v/>
       </c>
@@ -6352,7 +6361,7 @@
       <c r="AC75" s="20"/>
       <c r="AD75" s="20"/>
     </row>
-    <row r="76" spans="1:30" ht="14.4" customHeight="1">
+    <row r="76" spans="1:30" ht="14.45" customHeight="1">
       <c r="A76" s="2">
         <v>10</v>
       </c>
@@ -6386,12 +6395,12 @@
       <c r="O76" s="13"/>
       <c r="P76" s="2"/>
       <c r="Q76" s="159"/>
-      <c r="R76" s="224"/>
-      <c r="S76" s="228"/>
+      <c r="R76" s="210"/>
+      <c r="S76" s="214"/>
       <c r="T76" s="2"/>
       <c r="U76" s="2"/>
-      <c r="V76" s="214"/>
-      <c r="W76" s="217"/>
+      <c r="V76" s="220"/>
+      <c r="W76" s="223"/>
       <c r="X76" s="2"/>
       <c r="Y76" s="14"/>
       <c r="AB76" s="158"/>
@@ -6404,7 +6413,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:30" ht="14.4" customHeight="1" thickBot="1">
+    <row r="77" spans="1:30" ht="14.45" customHeight="1" thickBot="1">
       <c r="A77" s="2">
         <v>11</v>
       </c>
@@ -6434,15 +6443,15 @@
       <c r="Q77" s="159" t="s">
         <v>102</v>
       </c>
-      <c r="R77" s="225"/>
-      <c r="S77" s="229"/>
+      <c r="R77" s="211"/>
+      <c r="S77" s="215"/>
       <c r="T77" s="2"/>
       <c r="U77" s="2"/>
-      <c r="V77" s="212" t="str">
+      <c r="V77" s="218" t="str">
         <f>IF(AB50="","",AB50)</f>
         <v/>
       </c>
-      <c r="W77" s="218" t="str">
+      <c r="W77" s="224" t="str">
         <f>IF(AB53="","",AB53)</f>
         <v/>
       </c>
@@ -6452,7 +6461,7 @@
       <c r="AC77" s="20"/>
       <c r="AD77" s="20"/>
     </row>
-    <row r="78" spans="1:30" ht="14.4" customHeight="1" thickBot="1">
+    <row r="78" spans="1:30" ht="14.45" customHeight="1" thickBot="1">
       <c r="A78" s="2">
         <v>12</v>
       </c>
@@ -6461,12 +6470,12 @@
       <c r="O78" s="13"/>
       <c r="P78" s="2"/>
       <c r="Q78" s="159"/>
-      <c r="R78" s="226"/>
-      <c r="S78" s="230"/>
+      <c r="R78" s="212"/>
+      <c r="S78" s="216"/>
       <c r="T78" s="2"/>
       <c r="U78" s="2"/>
-      <c r="V78" s="213"/>
-      <c r="W78" s="219"/>
+      <c r="V78" s="219"/>
+      <c r="W78" s="225"/>
       <c r="X78" s="2"/>
       <c r="Y78" s="14"/>
       <c r="AB78" s="158"/>
@@ -6479,7 +6488,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:30" ht="14.4" customHeight="1">
+    <row r="79" spans="1:30" ht="14.45" customHeight="1">
       <c r="A79" s="2">
         <v>13</v>
       </c>
@@ -6519,7 +6528,7 @@
       <c r="AC79" s="20"/>
       <c r="AD79" s="20"/>
     </row>
-    <row r="80" spans="1:30" ht="14.4" customHeight="1">
+    <row r="80" spans="1:30" ht="14.45" customHeight="1">
       <c r="A80" s="2">
         <v>14</v>
       </c>
@@ -6559,7 +6568,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:30" ht="14.4" customHeight="1">
+    <row r="81" spans="1:30" ht="14.45" customHeight="1">
       <c r="A81" s="2">
         <v>15</v>
       </c>
@@ -6598,7 +6607,7 @@
       <c r="AC81" s="20"/>
       <c r="AD81" s="20"/>
     </row>
-    <row r="82" spans="1:30" ht="14.4" customHeight="1">
+    <row r="82" spans="1:30" ht="14.45" customHeight="1">
       <c r="A82" s="2">
         <v>16</v>
       </c>
@@ -6630,7 +6639,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:30" ht="14.4" customHeight="1" thickBot="1">
+    <row r="83" spans="1:30" ht="14.45" customHeight="1" thickBot="1">
       <c r="A83" s="2">
         <v>17</v>
       </c>
@@ -6667,7 +6676,7 @@
       <c r="AC83" s="20"/>
       <c r="AD83" s="20"/>
     </row>
-    <row r="84" spans="1:30" ht="14.4" customHeight="1">
+    <row r="84" spans="1:30" ht="14.45" customHeight="1">
       <c r="A84" s="2">
         <v>18</v>
       </c>
@@ -6684,16 +6693,16 @@
         <v>Right ()</v>
       </c>
       <c r="H84" s="2"/>
-      <c r="I84" s="210" t="str">
+      <c r="I84" s="228" t="str">
         <f>R68</f>
         <v>Left ()</v>
       </c>
-      <c r="J84" s="210"/>
-      <c r="K84" s="210" t="str">
+      <c r="J84" s="228"/>
+      <c r="K84" s="228" t="str">
         <f>S68</f>
         <v>Right ()</v>
       </c>
-      <c r="L84" s="210"/>
+      <c r="L84" s="228"/>
       <c r="M84" s="12"/>
       <c r="O84" s="13"/>
       <c r="P84" s="2"/>
@@ -6716,7 +6725,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:30" ht="14.4" customHeight="1" thickBot="1">
+    <row r="85" spans="1:30" ht="14.45" customHeight="1" thickBot="1">
       <c r="A85" s="2">
         <v>19</v>
       </c>
@@ -6737,16 +6746,16 @@
       <c r="H85" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="I85" s="211" t="str">
+      <c r="I85" s="217" t="str">
         <f>IF(R73="","",R73)</f>
         <v/>
       </c>
-      <c r="J85" s="211"/>
-      <c r="K85" s="211" t="str">
+      <c r="J85" s="217"/>
+      <c r="K85" s="217" t="str">
         <f>IF(S73="","",S73)</f>
         <v/>
       </c>
-      <c r="L85" s="211"/>
+      <c r="L85" s="217"/>
       <c r="M85" s="12"/>
       <c r="O85" s="109" t="s">
         <v>107</v>
@@ -6764,7 +6773,7 @@
       <c r="X85" s="2"/>
       <c r="Y85" s="14"/>
     </row>
-    <row r="86" spans="1:30" ht="14.4" customHeight="1">
+    <row r="86" spans="1:30" ht="14.45" customHeight="1">
       <c r="A86" s="2">
         <v>20</v>
       </c>
@@ -6785,27 +6794,27 @@
       <c r="H86" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="I86" s="211" t="str">
+      <c r="I86" s="217" t="str">
         <f>IF(R75="","",R75)</f>
         <v/>
       </c>
-      <c r="J86" s="211"/>
-      <c r="K86" s="211" t="str">
+      <c r="J86" s="217"/>
+      <c r="K86" s="217" t="str">
         <f>IF(S75="","",S75)</f>
         <v/>
       </c>
-      <c r="L86" s="211"/>
+      <c r="L86" s="217"/>
       <c r="M86" s="12"/>
       <c r="O86" s="13"/>
       <c r="P86" s="2"/>
-      <c r="Q86" s="221" t="s">
+      <c r="Q86" s="207" t="s">
         <v>118</v>
       </c>
-      <c r="R86" s="222"/>
-      <c r="S86" s="221" t="s">
+      <c r="R86" s="208"/>
+      <c r="S86" s="207" t="s">
         <v>119</v>
       </c>
-      <c r="T86" s="222"/>
+      <c r="T86" s="208"/>
       <c r="U86" s="2"/>
       <c r="V86" s="127" t="s">
         <v>44</v>
@@ -6814,7 +6823,7 @@
       <c r="X86" s="2"/>
       <c r="Y86" s="14"/>
     </row>
-    <row r="87" spans="1:30" ht="14.4" customHeight="1" thickBot="1">
+    <row r="87" spans="1:30" ht="14.45" customHeight="1" thickBot="1">
       <c r="A87" s="2">
         <v>21</v>
       </c>
@@ -6835,16 +6844,16 @@
       <c r="H87" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="I87" s="220" t="str">
+      <c r="I87" s="206" t="str">
         <f>IF(R77="","",R77)</f>
         <v/>
       </c>
-      <c r="J87" s="220"/>
-      <c r="K87" s="220" t="str">
+      <c r="J87" s="206"/>
+      <c r="K87" s="206" t="str">
         <f>IF(S77="","",S77)</f>
         <v/>
       </c>
-      <c r="L87" s="220"/>
+      <c r="L87" s="206"/>
       <c r="M87" s="12"/>
       <c r="O87" s="13"/>
       <c r="P87" s="2"/>
@@ -6878,7 +6887,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="88" spans="1:30" ht="14.4" customHeight="1">
+    <row r="88" spans="1:30" ht="14.45" customHeight="1">
       <c r="A88" s="2">
         <v>22</v>
       </c>
@@ -6943,7 +6952,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="89" spans="1:30" ht="14.4" customHeight="1">
+    <row r="89" spans="1:30" ht="14.45" customHeight="1">
       <c r="A89" s="2">
         <v>23</v>
       </c>
@@ -7006,7 +7015,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="90" spans="1:30" ht="14.4" customHeight="1">
+    <row r="90" spans="1:30" ht="14.45" customHeight="1">
       <c r="A90" s="2">
         <v>24</v>
       </c>
@@ -7067,7 +7076,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="91" spans="1:30" ht="14.4" customHeight="1">
+    <row r="91" spans="1:30" ht="14.45" customHeight="1">
       <c r="A91" s="2">
         <v>25</v>
       </c>
@@ -7115,7 +7124,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="92" spans="1:30" ht="14.4" customHeight="1">
+    <row r="92" spans="1:30" ht="14.45" customHeight="1">
       <c r="A92" s="2">
         <v>26</v>
       </c>
@@ -7146,8 +7155,12 @@
       </c>
       <c r="U92" s="2"/>
       <c r="V92" s="2"/>
-      <c r="W92" s="2"/>
-      <c r="X92" s="2"/>
+      <c r="W92" s="159" t="s">
+        <v>184</v>
+      </c>
+      <c r="X92" s="159" t="s">
+        <v>185</v>
+      </c>
       <c r="Y92" s="14"/>
       <c r="AA92" s="194" t="e">
         <f t="shared" si="20"/>
@@ -7166,7 +7179,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="93" spans="1:30" ht="14.4" customHeight="1">
+    <row r="93" spans="1:30" ht="14.45" customHeight="1">
       <c r="A93" s="2">
         <v>27</v>
       </c>
@@ -7204,6 +7217,17 @@
         <f t="shared" si="19"/>
         <v/>
       </c>
+      <c r="V93" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="W93" s="237" t="e">
+        <f>AVERAGE(Q88:R96)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X93" s="1" t="e">
+        <f>STDEV(Q88:R96)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="Y93" s="14"/>
       <c r="AA93" s="194" t="e">
         <f t="shared" si="20"/>
@@ -7222,7 +7246,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="94" spans="1:30" ht="14.4" customHeight="1">
+    <row r="94" spans="1:30" ht="14.45" customHeight="1">
       <c r="A94" s="2">
         <v>28</v>
       </c>
@@ -7260,6 +7284,17 @@
         <f t="shared" si="19"/>
         <v/>
       </c>
+      <c r="V94" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="W94" s="237" t="e">
+        <f>AVERAGE(S88:T96)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X94" s="1" t="e">
+        <f>STDEV(S88:T96)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="Y94" s="14"/>
       <c r="AA94" s="194" t="e">
         <f t="shared" si="20"/>
@@ -7278,7 +7313,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="95" spans="1:30" ht="14.4" customHeight="1">
+    <row r="95" spans="1:30" ht="14.45" customHeight="1">
       <c r="A95" s="2">
         <v>29</v>
       </c>
@@ -7334,7 +7369,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="96" spans="1:30" ht="14.4" customHeight="1" thickBot="1">
+    <row r="96" spans="1:30" ht="14.45" customHeight="1" thickBot="1">
       <c r="A96" s="2">
         <v>30</v>
       </c>
@@ -7390,7 +7425,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="97" spans="1:25" ht="14.4" customHeight="1">
+    <row r="97" spans="1:25" ht="14.45" customHeight="1">
       <c r="A97" s="2">
         <v>31</v>
       </c>
@@ -7434,7 +7469,7 @@
       <c r="X97" s="2"/>
       <c r="Y97" s="14"/>
     </row>
-    <row r="98" spans="1:25" ht="14.4" customHeight="1" thickBot="1">
+    <row r="98" spans="1:25" ht="14.45" customHeight="1" thickBot="1">
       <c r="A98" s="2">
         <v>32</v>
       </c>
@@ -7478,7 +7513,7 @@
       <c r="X98" s="2"/>
       <c r="Y98" s="14"/>
     </row>
-    <row r="99" spans="1:25" ht="14.4" customHeight="1" thickBot="1">
+    <row r="99" spans="1:25" ht="14.45" customHeight="1" thickBot="1">
       <c r="A99" s="2">
         <v>33</v>
       </c>
@@ -7526,7 +7561,7 @@
       <c r="X99" s="2"/>
       <c r="Y99" s="14"/>
     </row>
-    <row r="100" spans="1:25" ht="14.4" customHeight="1" thickBot="1">
+    <row r="100" spans="1:25" ht="14.45" customHeight="1" thickBot="1">
       <c r="A100" s="2">
         <v>34</v>
       </c>
@@ -7569,7 +7604,7 @@
       </c>
       <c r="Y100" s="14"/>
     </row>
-    <row r="101" spans="1:25" ht="14.4" customHeight="1">
+    <row r="101" spans="1:25" ht="14.45" customHeight="1">
       <c r="A101" s="2">
         <v>35</v>
       </c>
@@ -7604,7 +7639,7 @@
       <c r="X101" s="90"/>
       <c r="Y101" s="14"/>
     </row>
-    <row r="102" spans="1:25" ht="14.4" customHeight="1">
+    <row r="102" spans="1:25" ht="14.45" customHeight="1">
       <c r="A102" s="2">
         <v>36</v>
       </c>
@@ -7639,7 +7674,7 @@
       <c r="X102" s="78"/>
       <c r="Y102" s="14"/>
     </row>
-    <row r="103" spans="1:25" ht="14.4" customHeight="1">
+    <row r="103" spans="1:25" ht="14.45" customHeight="1">
       <c r="A103" s="2">
         <v>37</v>
       </c>
@@ -7671,7 +7706,7 @@
       <c r="X103" s="78"/>
       <c r="Y103" s="14"/>
     </row>
-    <row r="104" spans="1:25" ht="14.4" customHeight="1" thickBot="1">
+    <row r="104" spans="1:25" ht="14.45" customHeight="1" thickBot="1">
       <c r="A104" s="2">
         <v>38</v>
       </c>
@@ -7701,7 +7736,7 @@
       <c r="X104" s="44"/>
       <c r="Y104" s="28"/>
     </row>
-    <row r="105" spans="1:25" ht="14.4" customHeight="1">
+    <row r="105" spans="1:25" ht="14.45" customHeight="1">
       <c r="A105" s="2">
         <v>39</v>
       </c>
@@ -7731,7 +7766,7 @@
       <c r="X105" s="2"/>
       <c r="Y105" s="2"/>
     </row>
-    <row r="106" spans="1:25" ht="14.4" customHeight="1" thickBot="1">
+    <row r="106" spans="1:25" ht="14.45" customHeight="1" thickBot="1">
       <c r="A106" s="2">
         <v>40</v>
       </c>
@@ -7763,7 +7798,7 @@
       <c r="X106" s="2"/>
       <c r="Y106" s="2"/>
     </row>
-    <row r="107" spans="1:25" ht="14.4" customHeight="1">
+    <row r="107" spans="1:25" ht="14.45" customHeight="1">
       <c r="A107" s="2">
         <v>41</v>
       </c>
@@ -7795,7 +7830,7 @@
       <c r="X107" s="7"/>
       <c r="Y107" s="8"/>
     </row>
-    <row r="108" spans="1:25" ht="14.4" customHeight="1">
+    <row r="108" spans="1:25" ht="14.45" customHeight="1">
       <c r="A108" s="2">
         <v>42</v>
       </c>
@@ -7830,7 +7865,7 @@
       <c r="X108" s="90"/>
       <c r="Y108" s="14"/>
     </row>
-    <row r="109" spans="1:25" ht="14.4" customHeight="1">
+    <row r="109" spans="1:25" ht="14.45" customHeight="1">
       <c r="A109" s="2">
         <v>43</v>
       </c>
@@ -7865,7 +7900,7 @@
       <c r="X109" s="78"/>
       <c r="Y109" s="14"/>
     </row>
-    <row r="110" spans="1:25" ht="14.4" customHeight="1">
+    <row r="110" spans="1:25" ht="14.45" customHeight="1">
       <c r="A110" s="2">
         <v>44</v>
       </c>
@@ -7900,7 +7935,7 @@
       <c r="X110" s="90"/>
       <c r="Y110" s="14"/>
     </row>
-    <row r="111" spans="1:25" ht="14.4" customHeight="1">
+    <row r="111" spans="1:25" ht="14.45" customHeight="1">
       <c r="A111" s="2">
         <v>45</v>
       </c>
@@ -7935,7 +7970,7 @@
       <c r="X111" s="78"/>
       <c r="Y111" s="14"/>
     </row>
-    <row r="112" spans="1:25" ht="14.4" customHeight="1">
+    <row r="112" spans="1:25" ht="14.45" customHeight="1">
       <c r="A112" s="2">
         <v>46</v>
       </c>
@@ -7970,7 +8005,7 @@
       <c r="X112" s="90"/>
       <c r="Y112" s="14"/>
     </row>
-    <row r="113" spans="1:25" ht="14.4" customHeight="1">
+    <row r="113" spans="1:25" ht="14.45" customHeight="1">
       <c r="A113" s="2">
         <v>47</v>
       </c>
@@ -8005,7 +8040,7 @@
       <c r="X113" s="78"/>
       <c r="Y113" s="14"/>
     </row>
-    <row r="114" spans="1:25" ht="14.4" customHeight="1">
+    <row r="114" spans="1:25" ht="14.45" customHeight="1">
       <c r="A114" s="2">
         <v>48</v>
       </c>
@@ -8040,7 +8075,7 @@
       <c r="X114" s="90"/>
       <c r="Y114" s="14"/>
     </row>
-    <row r="115" spans="1:25" ht="14.4" customHeight="1">
+    <row r="115" spans="1:25" ht="14.45" customHeight="1">
       <c r="A115" s="2">
         <v>49</v>
       </c>
@@ -8075,7 +8110,7 @@
       <c r="X115" s="78"/>
       <c r="Y115" s="14"/>
     </row>
-    <row r="116" spans="1:25" ht="14.4" customHeight="1">
+    <row r="116" spans="1:25" ht="14.45" customHeight="1">
       <c r="A116" s="2">
         <v>50</v>
       </c>
@@ -8110,7 +8145,7 @@
       <c r="X116" s="90"/>
       <c r="Y116" s="14"/>
     </row>
-    <row r="117" spans="1:25" ht="14.4" customHeight="1">
+    <row r="117" spans="1:25" ht="14.45" customHeight="1">
       <c r="A117" s="2">
         <v>51</v>
       </c>
@@ -8145,7 +8180,7 @@
       <c r="X117" s="78"/>
       <c r="Y117" s="14"/>
     </row>
-    <row r="118" spans="1:25" ht="14.4" customHeight="1">
+    <row r="118" spans="1:25" ht="14.45" customHeight="1">
       <c r="A118" s="2">
         <v>52</v>
       </c>
@@ -8180,7 +8215,7 @@
       <c r="X118" s="90"/>
       <c r="Y118" s="14"/>
     </row>
-    <row r="119" spans="1:25" ht="14.4" customHeight="1">
+    <row r="119" spans="1:25" ht="14.45" customHeight="1">
       <c r="A119" s="2">
         <v>53</v>
       </c>
@@ -8215,7 +8250,7 @@
       <c r="X119" s="78"/>
       <c r="Y119" s="14"/>
     </row>
-    <row r="120" spans="1:25" ht="14.4" customHeight="1">
+    <row r="120" spans="1:25" ht="14.45" customHeight="1">
       <c r="A120" s="2">
         <v>54</v>
       </c>
@@ -8250,7 +8285,7 @@
       <c r="X120" s="90"/>
       <c r="Y120" s="14"/>
     </row>
-    <row r="121" spans="1:25" ht="14.4" customHeight="1">
+    <row r="121" spans="1:25" ht="14.45" customHeight="1">
       <c r="A121" s="2">
         <v>55</v>
       </c>
@@ -8285,7 +8320,7 @@
       <c r="X121" s="78"/>
       <c r="Y121" s="14"/>
     </row>
-    <row r="122" spans="1:25" ht="14.4" customHeight="1">
+    <row r="122" spans="1:25" ht="14.45" customHeight="1">
       <c r="A122" s="2">
         <v>56</v>
       </c>
@@ -8320,7 +8355,7 @@
       <c r="X122" s="90"/>
       <c r="Y122" s="14"/>
     </row>
-    <row r="123" spans="1:25" ht="14.4" customHeight="1">
+    <row r="123" spans="1:25" ht="14.45" customHeight="1">
       <c r="A123" s="2">
         <v>57</v>
       </c>
@@ -8355,7 +8390,7 @@
       <c r="X123" s="78"/>
       <c r="Y123" s="14"/>
     </row>
-    <row r="124" spans="1:25" ht="14.4" customHeight="1">
+    <row r="124" spans="1:25" ht="14.45" customHeight="1">
       <c r="A124" s="2">
         <v>58</v>
       </c>
@@ -8390,7 +8425,7 @@
       <c r="X124" s="90"/>
       <c r="Y124" s="14"/>
     </row>
-    <row r="125" spans="1:25" ht="14.4" customHeight="1">
+    <row r="125" spans="1:25" ht="14.45" customHeight="1">
       <c r="A125" s="2">
         <v>59</v>
       </c>
@@ -8425,7 +8460,7 @@
       <c r="X125" s="78"/>
       <c r="Y125" s="14"/>
     </row>
-    <row r="126" spans="1:25" ht="14.4" customHeight="1">
+    <row r="126" spans="1:25" ht="14.45" customHeight="1">
       <c r="A126" s="2">
         <v>60</v>
       </c>
@@ -8448,7 +8483,7 @@
       <c r="X126" s="90"/>
       <c r="Y126" s="14"/>
     </row>
-    <row r="127" spans="1:25" ht="14.4" customHeight="1">
+    <row r="127" spans="1:25" ht="14.45" customHeight="1">
       <c r="A127" s="2">
         <v>61</v>
       </c>
@@ -8471,7 +8506,7 @@
       <c r="X127" s="78"/>
       <c r="Y127" s="14"/>
     </row>
-    <row r="128" spans="1:25" ht="14.4" customHeight="1">
+    <row r="128" spans="1:25" ht="14.45" customHeight="1">
       <c r="A128" s="2">
         <v>62</v>
       </c>
@@ -8494,7 +8529,7 @@
       <c r="X128" s="90"/>
       <c r="Y128" s="14"/>
     </row>
-    <row r="129" spans="1:25" ht="14.4" customHeight="1">
+    <row r="129" spans="1:25" ht="14.45" customHeight="1">
       <c r="A129" s="2">
         <v>63</v>
       </c>
@@ -8517,7 +8552,7 @@
       <c r="X129" s="78"/>
       <c r="Y129" s="14"/>
     </row>
-    <row r="130" spans="1:25" ht="14.4" customHeight="1" thickBot="1">
+    <row r="130" spans="1:25" ht="14.45" customHeight="1" thickBot="1">
       <c r="A130" s="2">
         <v>64</v>
       </c>
@@ -8545,7 +8580,7 @@
       <c r="X130" s="44"/>
       <c r="Y130" s="28"/>
     </row>
-    <row r="131" spans="1:25" ht="14.4" customHeight="1" thickTop="1">
+    <row r="131" spans="1:25" ht="14.45" customHeight="1" thickTop="1">
       <c r="A131" s="2">
         <v>65</v>
       </c>
@@ -8564,7 +8599,7 @@
         <v>Eugene Mah</v>
       </c>
     </row>
-    <row r="132" spans="1:25" ht="14.4" customHeight="1">
+    <row r="132" spans="1:25" ht="14.45" customHeight="1">
       <c r="A132" s="2">
         <v>66</v>
       </c>
@@ -8597,6 +8632,34 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="40">
+    <mergeCell ref="AG1:AJ1"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="I84:J84"/>
+    <mergeCell ref="K84:L84"/>
+    <mergeCell ref="I85:J85"/>
+    <mergeCell ref="K85:L85"/>
+    <mergeCell ref="V77:V78"/>
+    <mergeCell ref="V75:V76"/>
+    <mergeCell ref="V73:V74"/>
+    <mergeCell ref="W73:W74"/>
+    <mergeCell ref="W75:W76"/>
+    <mergeCell ref="W77:W78"/>
     <mergeCell ref="I87:J87"/>
     <mergeCell ref="K87:L87"/>
     <mergeCell ref="Q86:R86"/>
@@ -8609,34 +8672,6 @@
     <mergeCell ref="S77:S78"/>
     <mergeCell ref="I86:J86"/>
     <mergeCell ref="K86:L86"/>
-    <mergeCell ref="V77:V78"/>
-    <mergeCell ref="V75:V76"/>
-    <mergeCell ref="V73:V74"/>
-    <mergeCell ref="W73:W74"/>
-    <mergeCell ref="W75:W76"/>
-    <mergeCell ref="W77:W78"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="I84:J84"/>
-    <mergeCell ref="K84:L84"/>
-    <mergeCell ref="I85:J85"/>
-    <mergeCell ref="K85:L85"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="AG1:AJ1"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="J10:K10"/>
   </mergeCells>
   <conditionalFormatting sqref="I72:I74">
     <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">

</xml_diff>

<commit_message>
Move Ocean data to separate spreadsheet tab
</commit_message>
<xml_diff>
--- a/MUSCMammoMonitor.xlsx
+++ b/MUSCMammoMonitor.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugenem\Documents\GitHub\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D79B9E-EBEF-43BE-9B71-DFA2A16884CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B78240B-419B-4DF7-8F4E-FCE73FCACBDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Barco" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Lamb">Barco!$T$26</definedName>
+    <definedName name="Page1">Barco!$B$1:$M$66</definedName>
+    <definedName name="Page2">Barco!$B$67:$M$132</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Barco!$B$1:$M$132</definedName>
     <definedName name="Z_B8088769_C3DE_4DF8_A82B_D0EB46FFCC4A_.wvu.PrintArea" localSheetId="0" hidden="1">Barco!$B$1:$M$132</definedName>
   </definedNames>
@@ -99,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="188">
   <si>
     <t>Print Area</t>
   </si>
@@ -506,9 +509,6 @@
     <t>Piranha CB2-19020491</t>
   </si>
   <si>
-    <t>Revision 1.5-20210527</t>
-  </si>
-  <si>
     <t>Ambient light illuminance measured at the surface of the monitor(s) must be less than 20 lux</t>
   </si>
   <si>
@@ -569,9 +569,6 @@
     <t>Measurements</t>
   </si>
   <si>
-    <t>Set text</t>
-  </si>
-  <si>
     <t>Light_x000D_(cd/m²)</t>
   </si>
   <si>
@@ -581,12 +578,6 @@
     <t>LN18</t>
   </si>
   <si>
-    <t>UNL10</t>
-  </si>
-  <si>
-    <t>UNL80</t>
-  </si>
-  <si>
     <t>LUDM UNL 10 L:</t>
   </si>
   <si>
@@ -641,9 +632,6 @@
     <t>Ambience Ratio:</t>
   </si>
   <si>
-    <t>L_amb</t>
-  </si>
-  <si>
     <t>Luminance deviation from median is &lt; 30%</t>
   </si>
   <si>
@@ -657,6 +645,27 @@
   </si>
   <si>
     <t>SD</t>
+  </si>
+  <si>
+    <t>Test Pattern</t>
+  </si>
+  <si>
+    <t>Lamb</t>
+  </si>
+  <si>
+    <t>UN10</t>
+  </si>
+  <si>
+    <t>UN80</t>
+  </si>
+  <si>
+    <t>Waveforms</t>
+  </si>
+  <si>
+    <t>Revision 1.6-20220607</t>
+  </si>
+  <si>
+    <t>Page1,Page2</t>
   </si>
 </sst>
 </file>
@@ -672,7 +681,7 @@
     <numFmt numFmtId="169" formatCode="0.0%"/>
     <numFmt numFmtId="170" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -781,13 +790,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -798,6 +800,19 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1600,7 +1615,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="238">
+  <cellXfs count="239">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2127,9 +2142,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2217,6 +2229,66 @@
     <xf numFmtId="2" fontId="3" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2250,68 +2322,10 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -2841,9 +2855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X98" sqref="X98"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -2872,7 +2884,7 @@
       <c r="L1" s="4"/>
       <c r="M1" s="5"/>
       <c r="O1" s="6" t="s">
-        <v>135</v>
+        <v>186</v>
       </c>
       <c r="P1" s="7"/>
       <c r="Q1" s="7"/>
@@ -2887,12 +2899,12 @@
       <c r="AA1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="AG1" s="233" t="s">
+      <c r="AG1" s="205" t="s">
         <v>1</v>
       </c>
-      <c r="AH1" s="233"/>
-      <c r="AI1" s="233"/>
-      <c r="AJ1" s="233"/>
+      <c r="AH1" s="205"/>
+      <c r="AI1" s="205"/>
+      <c r="AJ1" s="205"/>
     </row>
     <row r="2" spans="1:36" ht="14.45" customHeight="1">
       <c r="A2" s="2">
@@ -2908,15 +2920,17 @@
         <v>2</v>
       </c>
       <c r="Y2" s="14"/>
-      <c r="AA2" s="15"/>
-      <c r="AG2" s="234" t="s">
+      <c r="AA2" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="AG2" s="206" t="s">
         <v>3</v>
       </c>
-      <c r="AH2" s="234"/>
-      <c r="AI2" s="235" t="s">
+      <c r="AH2" s="206"/>
+      <c r="AI2" s="207" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="235"/>
+      <c r="AJ2" s="207"/>
     </row>
     <row r="3" spans="1:36" ht="14.45" customHeight="1">
       <c r="A3" s="2">
@@ -2962,7 +2976,9 @@
       <c r="AA4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="AB4" s="22"/>
+      <c r="AB4" s="22" t="s">
+        <v>187</v>
+      </c>
       <c r="AF4" s="21" t="s">
         <v>9</v>
       </c>
@@ -3083,11 +3099,11 @@
       <c r="AB7" s="34"/>
       <c r="AC7" s="35" t="str">
         <f t="shared" ref="AC7:AC20" si="0">IF(AB7&lt;&gt;AD7,"Change","")</f>
-        <v/>
+        <v>Change</v>
       </c>
       <c r="AD7" s="36" t="str">
         <f>IF(OR(AA2="",AA2=0),"",AA2)</f>
-        <v/>
+        <v>Page1,Page2</v>
       </c>
       <c r="AF7" s="21" t="s">
         <v>23</v>
@@ -3197,10 +3213,8 @@
         <f>IF(X7="","",X7)</f>
         <v>Eugene Mah</v>
       </c>
-      <c r="AF9" s="68" t="s">
-        <v>155</v>
-      </c>
-      <c r="AG9" s="2"/>
+      <c r="AF9"/>
+      <c r="AG9"/>
     </row>
     <row r="10" spans="1:36" ht="14.45" customHeight="1">
       <c r="A10" s="2">
@@ -3210,19 +3224,19 @@
       <c r="D10" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="236" t="str">
+      <c r="E10" s="208" t="str">
         <f t="shared" ref="E10:E15" si="1">IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="F10" s="236"/>
+      <c r="F10" s="208"/>
       <c r="I10" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="236" t="str">
+      <c r="J10" s="208" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="K10" s="236"/>
+      <c r="K10" s="208"/>
       <c r="M10" s="12"/>
       <c r="O10" s="13"/>
       <c r="Q10" s="21" t="s">
@@ -3254,8 +3268,8 @@
         <f t="shared" ref="AD10:AD15" si="3">IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="AF10" s="2"/>
-      <c r="AG10" s="2"/>
+      <c r="AF10"/>
+      <c r="AG10"/>
     </row>
     <row r="11" spans="1:36" ht="14.45" customHeight="1">
       <c r="A11" s="2">
@@ -3265,19 +3279,19 @@
       <c r="D11" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="229" t="str">
+      <c r="E11" s="209" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F11" s="229"/>
+      <c r="F11" s="209"/>
       <c r="I11" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="232" t="str">
+      <c r="J11" s="210" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="K11" s="232"/>
+      <c r="K11" s="210"/>
       <c r="M11" s="12"/>
       <c r="O11" s="13"/>
       <c r="Q11" s="21" t="s">
@@ -3309,12 +3323,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="AF11" s="176" t="s">
-        <v>156</v>
-      </c>
-      <c r="AG11" s="176" t="s">
-        <v>157</v>
-      </c>
+      <c r="AF11"/>
+      <c r="AG11"/>
     </row>
     <row r="12" spans="1:36" ht="14.45" customHeight="1">
       <c r="A12" s="2">
@@ -3324,19 +3334,19 @@
       <c r="D12" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="229" t="str">
+      <c r="E12" s="209" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F12" s="229"/>
+      <c r="F12" s="209"/>
       <c r="I12" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="229" t="str">
+      <c r="J12" s="209" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="K12" s="229"/>
+      <c r="K12" s="209"/>
       <c r="M12" s="12"/>
       <c r="O12" s="13"/>
       <c r="Q12" s="21" t="s">
@@ -3368,10 +3378,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="AF12" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="AG12" s="2"/>
+      <c r="AF12"/>
+      <c r="AG12"/>
     </row>
     <row r="13" spans="1:36" ht="14.45" customHeight="1">
       <c r="A13" s="2">
@@ -3381,19 +3389,19 @@
       <c r="D13" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="229" t="str">
+      <c r="E13" s="209" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F13" s="229"/>
+      <c r="F13" s="209"/>
       <c r="I13" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="229" t="str">
+      <c r="J13" s="209" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="K13" s="229"/>
+      <c r="K13" s="209"/>
       <c r="M13" s="12"/>
       <c r="O13" s="13"/>
       <c r="Q13" s="21" t="s">
@@ -3425,10 +3433,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="AF13" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AG13" s="2"/>
+      <c r="AF13"/>
+      <c r="AG13"/>
     </row>
     <row r="14" spans="1:36" ht="14.45" customHeight="1">
       <c r="A14" s="2">
@@ -3438,19 +3444,19 @@
       <c r="D14" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="229" t="str">
+      <c r="E14" s="209" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F14" s="229"/>
+      <c r="F14" s="209"/>
       <c r="I14" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="229" t="str">
+      <c r="J14" s="209" t="str">
         <f>IF(V14="","",V14)</f>
         <v/>
       </c>
-      <c r="K14" s="229"/>
+      <c r="K14" s="209"/>
       <c r="M14" s="12"/>
       <c r="O14" s="13"/>
       <c r="Q14" s="21" t="s">
@@ -3482,10 +3488,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="AF14" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AG14" s="2"/>
+      <c r="AF14"/>
+      <c r="AG14"/>
     </row>
     <row r="15" spans="1:36" ht="14.45" customHeight="1" thickBot="1">
       <c r="A15" s="2">
@@ -3495,11 +3499,11 @@
       <c r="D15" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="229" t="str">
+      <c r="E15" s="209" t="str">
         <f t="shared" si="1"/>
         <v>IMPAX 4.2 2015</v>
       </c>
-      <c r="F15" s="229"/>
+      <c r="F15" s="209"/>
       <c r="M15" s="12"/>
       <c r="O15" s="26"/>
       <c r="P15" s="27"/>
@@ -3531,10 +3535,8 @@
         <f t="shared" si="3"/>
         <v>IMPAX 4.2 2015</v>
       </c>
-      <c r="AF15" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="AG15" s="2"/>
+      <c r="AF15"/>
+      <c r="AG15"/>
     </row>
     <row r="16" spans="1:36" ht="14.45" customHeight="1" thickBot="1">
       <c r="A16" s="2">
@@ -3564,10 +3566,8 @@
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="AF16" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="AG16" s="2"/>
+      <c r="AF16"/>
+      <c r="AG16"/>
     </row>
     <row r="17" spans="1:33" ht="14.45" customHeight="1" thickTop="1" thickBot="1">
       <c r="A17" s="2">
@@ -3594,10 +3594,8 @@
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="AF17" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG17" s="2"/>
+      <c r="AF17"/>
+      <c r="AG17"/>
     </row>
     <row r="18" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A18" s="2">
@@ -3633,10 +3631,8 @@
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="AF18" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG18" s="2"/>
+      <c r="AF18"/>
+      <c r="AG18"/>
     </row>
     <row r="19" spans="1:33" ht="14.45" customHeight="1" thickTop="1">
       <c r="A19" s="2">
@@ -3653,10 +3649,10 @@
       <c r="H19" s="154"/>
       <c r="I19" s="154"/>
       <c r="J19" s="154"/>
-      <c r="K19" s="231" t="s">
+      <c r="K19" s="212" t="s">
         <v>129</v>
       </c>
-      <c r="L19" s="231"/>
+      <c r="L19" s="212"/>
       <c r="M19" s="5"/>
       <c r="O19" s="13"/>
       <c r="R19" s="1" t="s">
@@ -3681,10 +3677,8 @@
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="AF19" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG19" s="2"/>
+      <c r="AF19"/>
+      <c r="AG19"/>
     </row>
     <row r="20" spans="1:33" ht="14.45" customHeight="1">
       <c r="A20" s="2">
@@ -3746,10 +3740,8 @@
         <f>IF(V14="","",V14)</f>
         <v/>
       </c>
-      <c r="AF20" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG20" s="2"/>
+      <c r="AF20"/>
+      <c r="AG20"/>
     </row>
     <row r="21" spans="1:33" ht="14.45" customHeight="1">
       <c r="A21" s="2">
@@ -3802,10 +3794,8 @@
       <c r="AB21" s="20"/>
       <c r="AC21" s="20"/>
       <c r="AD21" s="20"/>
-      <c r="AF21" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG21" s="2"/>
+      <c r="AF21"/>
+      <c r="AG21"/>
     </row>
     <row r="22" spans="1:33" ht="14.45" customHeight="1">
       <c r="A22" s="2">
@@ -3858,10 +3848,8 @@
       <c r="AA22" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="AF22" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG22" s="2"/>
+      <c r="AF22"/>
+      <c r="AG22"/>
     </row>
     <row r="23" spans="1:33" ht="14.45" customHeight="1">
       <c r="A23" s="2">
@@ -3913,10 +3901,8 @@
         <f>IF(X20="","",X20)</f>
         <v>Piranha CB2-19020491</v>
       </c>
-      <c r="AF23" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG23" s="2"/>
+      <c r="AF23"/>
+      <c r="AG23"/>
     </row>
     <row r="24" spans="1:33" ht="14.45" customHeight="1">
       <c r="A24" s="2">
@@ -3926,11 +3912,11 @@
       <c r="D24" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="230" t="str">
+      <c r="E24" s="211" t="str">
         <f>IF(P52="","",P52)</f>
         <v/>
       </c>
-      <c r="F24" s="230"/>
+      <c r="F24" s="211"/>
       <c r="G24" s="40"/>
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
@@ -3952,10 +3938,8 @@
         <f t="shared" ref="AD24:AD25" si="8">IF(X21="","",X21)</f>
         <v>43549</v>
       </c>
-      <c r="AF24" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG24" s="2"/>
+      <c r="AF24"/>
+      <c r="AG24"/>
     </row>
     <row r="25" spans="1:33" ht="14.45" customHeight="1">
       <c r="A25" s="2">
@@ -3985,10 +3969,8 @@
         <f t="shared" si="8"/>
         <v>44280</v>
       </c>
-      <c r="AF25" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG25" s="2"/>
+      <c r="AF25"/>
+      <c r="AG25"/>
     </row>
     <row r="26" spans="1:33" ht="14.45" customHeight="1">
       <c r="A26" s="2">
@@ -4000,27 +3982,25 @@
       </c>
       <c r="M26" s="12"/>
       <c r="O26" s="84" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P26" s="85"/>
       <c r="Q26" s="1" t="s">
         <v>55</v>
       </c>
       <c r="S26" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="T26" s="195" t="str">
-        <f>IF(AG12="","",AG12)</f>
+        <v>139</v>
+      </c>
+      <c r="T26" s="194" t="str">
+        <f>IF(Sheet1!B4="","",Sheet1!B4)</f>
         <v/>
       </c>
       <c r="U26" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Y26" s="14"/>
-      <c r="AF26" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG26" s="2"/>
+      <c r="AF26"/>
+      <c r="AG26"/>
     </row>
     <row r="27" spans="1:33" ht="14.45" customHeight="1">
       <c r="A27" s="2">
@@ -4028,7 +4008,7 @@
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="52" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D27" s="147" t="str">
         <f>IF(P26="","",P26)</f>
@@ -4062,11 +4042,11 @@
         <v/>
       </c>
       <c r="U27" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Y27" s="14"/>
       <c r="AA27" s="66" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AB27" s="34"/>
       <c r="AC27" s="35" t="str">
@@ -4077,10 +4057,8 @@
         <f>IF(P26="","",P26)</f>
         <v/>
       </c>
-      <c r="AF27" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG27" s="2"/>
+      <c r="AF27"/>
+      <c r="AG27"/>
     </row>
     <row r="28" spans="1:33" ht="14.45" customHeight="1">
       <c r="A28" s="2">
@@ -4088,14 +4066,14 @@
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="52" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D28" s="144" t="str">
         <f>IF(T26="","",T26)</f>
         <v/>
       </c>
       <c r="E28" s="167" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M28" s="12"/>
       <c r="O28" s="13"/>
@@ -4103,11 +4081,11 @@
         <v>57</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Y28" s="14"/>
       <c r="AA28" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AB28" s="34"/>
       <c r="AC28" s="35" t="str">
@@ -4118,10 +4096,8 @@
         <f>IF(T26="","",T26)</f>
         <v/>
       </c>
-      <c r="AF28" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG28" s="2"/>
+      <c r="AF28"/>
+      <c r="AG28"/>
     </row>
     <row r="29" spans="1:33" ht="14.45" customHeight="1">
       <c r="A29" s="2">
@@ -4170,10 +4146,8 @@
         <f>IF(R37="","",R37)</f>
         <v/>
       </c>
-      <c r="AF29" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG29" s="2"/>
+      <c r="AF29"/>
+      <c r="AG29"/>
     </row>
     <row r="30" spans="1:33" ht="14.45" customHeight="1">
       <c r="A30" s="2">
@@ -4222,10 +4196,8 @@
         <f>IF(S37="","",S37)</f>
         <v/>
       </c>
-      <c r="AF30" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG30" s="2"/>
+      <c r="AF30"/>
+      <c r="AG30"/>
     </row>
     <row r="31" spans="1:33" ht="14.45" customHeight="1">
       <c r="A31" s="2">
@@ -4260,7 +4232,7 @@
       <c r="X31" s="78"/>
       <c r="Y31" s="14"/>
       <c r="AA31" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AB31" s="34"/>
       <c r="AC31" s="35" t="str">
@@ -4271,10 +4243,8 @@
         <f>IF(Q59="","",Q59)</f>
         <v/>
       </c>
-      <c r="AF31" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG31" s="2"/>
+      <c r="AF31"/>
+      <c r="AG31"/>
     </row>
     <row r="32" spans="1:33" ht="14.45" customHeight="1">
       <c r="A32" s="2">
@@ -4304,7 +4274,7 @@
       <c r="X32" s="2"/>
       <c r="Y32" s="14"/>
       <c r="AA32" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AB32" s="34"/>
       <c r="AC32" s="35" t="str">
@@ -4315,10 +4285,8 @@
         <f>IF(R59="","",R59)</f>
         <v/>
       </c>
-      <c r="AF32" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG32" s="2"/>
+      <c r="AF32"/>
+      <c r="AG32"/>
     </row>
     <row r="33" spans="1:33" ht="14.45" customHeight="1">
       <c r="A33" s="2">
@@ -4356,7 +4324,7 @@
       <c r="X33" s="2"/>
       <c r="Y33" s="14"/>
       <c r="AA33" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AB33" s="34"/>
       <c r="AC33" s="35" t="str">
@@ -4367,10 +4335,8 @@
         <f>IF(Q60="","",Q60)</f>
         <v/>
       </c>
-      <c r="AF33" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG33" s="2"/>
+      <c r="AF33"/>
+      <c r="AG33"/>
     </row>
     <row r="34" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A34" s="2">
@@ -4419,7 +4385,7 @@
       <c r="X34" s="2"/>
       <c r="Y34" s="14"/>
       <c r="AA34" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AB34" s="34"/>
       <c r="AC34" s="35" t="str">
@@ -4430,10 +4396,8 @@
         <f>IF(R60="","",R60)</f>
         <v/>
       </c>
-      <c r="AF34" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG34" s="2"/>
+      <c r="AF34"/>
+      <c r="AG34"/>
     </row>
     <row r="35" spans="1:33" ht="14.45" customHeight="1">
       <c r="A35" s="2">
@@ -4477,7 +4441,7 @@
       <c r="X35" s="2"/>
       <c r="Y35" s="14"/>
       <c r="AA35" s="21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AB35" s="34"/>
       <c r="AC35" s="35" t="str">
@@ -4488,10 +4452,8 @@
         <f>IF(Q61="","",Q61)</f>
         <v/>
       </c>
-      <c r="AF35" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AG35" s="2"/>
+      <c r="AF35"/>
+      <c r="AG35"/>
     </row>
     <row r="36" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A36" s="2">
@@ -4535,7 +4497,7 @@
       <c r="X36" s="2"/>
       <c r="Y36" s="14"/>
       <c r="AA36" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AB36" s="34"/>
       <c r="AC36" s="35" t="str">
@@ -4546,10 +4508,8 @@
         <f>IF(R61="","",R61)</f>
         <v/>
       </c>
-      <c r="AF36" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AG36" s="2"/>
+      <c r="AF36"/>
+      <c r="AG36"/>
     </row>
     <row r="37" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A37" s="2">
@@ -4592,7 +4552,7 @@
       <c r="X37" s="2"/>
       <c r="Y37" s="14"/>
       <c r="AA37" s="21" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="AB37" s="34"/>
       <c r="AC37" s="35" t="str">
@@ -4603,10 +4563,8 @@
         <f>IF(Q62="","",Q62)</f>
         <v/>
       </c>
-      <c r="AF37" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AG37" s="2"/>
+      <c r="AF37"/>
+      <c r="AG37"/>
     </row>
     <row r="38" spans="1:33" ht="14.45" customHeight="1">
       <c r="A38" s="2">
@@ -4639,7 +4597,7 @@
       <c r="X38" s="2"/>
       <c r="Y38" s="14"/>
       <c r="AA38" s="21" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AB38" s="34"/>
       <c r="AC38" s="35" t="str">
@@ -4650,10 +4608,8 @@
         <f>IF(R62="","",R62)</f>
         <v/>
       </c>
-      <c r="AF38" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AG38" s="2"/>
+      <c r="AF38"/>
+      <c r="AG38"/>
     </row>
     <row r="39" spans="1:33" ht="14.45" customHeight="1">
       <c r="A39" s="2">
@@ -4702,10 +4658,8 @@
         <f>IF(Q99="","",Q99)</f>
         <v/>
       </c>
-      <c r="AF39" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AG39" s="2"/>
+      <c r="AF39"/>
+      <c r="AG39"/>
     </row>
     <row r="40" spans="1:33" ht="14.45" customHeight="1">
       <c r="A40" s="2">
@@ -4751,10 +4705,8 @@
         <f>IF(R99="","",R99)</f>
         <v/>
       </c>
-      <c r="AF40" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AG40" s="2"/>
+      <c r="AF40"/>
+      <c r="AG40"/>
     </row>
     <row r="41" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A41" s="2">
@@ -4799,10 +4751,8 @@
         <f>IF(S99="","",S99)</f>
         <v/>
       </c>
-      <c r="AF41" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AG41" s="2"/>
+      <c r="AF41"/>
+      <c r="AG41"/>
     </row>
     <row r="42" spans="1:33" ht="14.45" customHeight="1">
       <c r="A42" s="2">
@@ -4854,10 +4804,8 @@
         <f>IF(T99="","",T99)</f>
         <v/>
       </c>
-      <c r="AF42" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AG42" s="2"/>
+      <c r="AF42"/>
+      <c r="AG42"/>
     </row>
     <row r="43" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A43" s="2">
@@ -4901,7 +4849,7 @@
       <c r="X43" s="2"/>
       <c r="Y43" s="14"/>
       <c r="AA43" s="21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="AB43" s="81"/>
       <c r="AC43" s="35" t="str">
@@ -4912,10 +4860,8 @@
         <f>IF(Q100="","",Q100)</f>
         <v/>
       </c>
-      <c r="AF43" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AG43" s="2"/>
+      <c r="AF43"/>
+      <c r="AG43"/>
     </row>
     <row r="44" spans="1:33" ht="14.45" customHeight="1">
       <c r="A44" s="2">
@@ -4954,7 +4900,7 @@
       <c r="X44" s="2"/>
       <c r="Y44" s="14"/>
       <c r="AA44" s="21" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="AB44" s="81"/>
       <c r="AC44" s="35" t="str">
@@ -4965,10 +4911,8 @@
         <f>IF(R100="","",R100)</f>
         <v/>
       </c>
-      <c r="AF44" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AG44" s="2"/>
+      <c r="AF44"/>
+      <c r="AG44"/>
     </row>
     <row r="45" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A45" s="2">
@@ -5009,7 +4953,7 @@
       <c r="X45" s="2"/>
       <c r="Y45" s="14"/>
       <c r="AA45" s="21" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="AB45" s="81"/>
       <c r="AC45" s="35" t="str">
@@ -5020,10 +4964,8 @@
         <f>IF(S100="","",S100)</f>
         <v/>
       </c>
-      <c r="AF45" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AG45" s="2"/>
+      <c r="AF45"/>
+      <c r="AG45"/>
     </row>
     <row r="46" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A46" s="2">
@@ -5058,7 +5000,7 @@
       <c r="X46" s="2"/>
       <c r="Y46" s="14"/>
       <c r="AA46" s="21" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="AB46" s="81"/>
       <c r="AC46" s="35" t="str">
@@ -5069,10 +5011,8 @@
         <f>IF(T100="","",T100)</f>
         <v/>
       </c>
-      <c r="AF46" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AG46" s="2"/>
+      <c r="AF46"/>
+      <c r="AG46"/>
     </row>
     <row r="47" spans="1:33" ht="14.45" customHeight="1">
       <c r="A47" s="2">
@@ -5112,10 +5052,8 @@
       <c r="AB47" s="20"/>
       <c r="AC47" s="20"/>
       <c r="AD47" s="20"/>
-      <c r="AF47" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AG47" s="2"/>
+      <c r="AF47"/>
+      <c r="AG47"/>
     </row>
     <row r="48" spans="1:33" ht="14.45" customHeight="1">
       <c r="A48" s="2">
@@ -5163,10 +5101,8 @@
         <f>IF(R73="","",R73)</f>
         <v/>
       </c>
-      <c r="AF48" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AG48" s="2"/>
+      <c r="AF48"/>
+      <c r="AG48"/>
     </row>
     <row r="49" spans="1:33" ht="14.45" customHeight="1">
       <c r="A49" s="2">
@@ -5213,10 +5149,8 @@
         <f>IF(R75="","",R75)</f>
         <v/>
       </c>
-      <c r="AF49" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AG49" s="2"/>
+      <c r="AF49"/>
+      <c r="AG49"/>
     </row>
     <row r="50" spans="1:33" ht="14.45" customHeight="1">
       <c r="A50" s="2">
@@ -5232,7 +5166,7 @@
         <v/>
       </c>
       <c r="F50" s="167" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G50" s="95"/>
       <c r="H50" s="95"/>
@@ -5245,7 +5179,7 @@
         <v/>
       </c>
       <c r="K50" s="167" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M50" s="12"/>
       <c r="O50" s="13"/>
@@ -5271,10 +5205,8 @@
         <f>IF(R77="","",R77)</f>
         <v/>
       </c>
-      <c r="AF50" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AG50" s="2"/>
+      <c r="AF50"/>
+      <c r="AG50"/>
     </row>
     <row r="51" spans="1:33" ht="14.45" customHeight="1">
       <c r="A51" s="2">
@@ -5290,18 +5222,18 @@
         <v/>
       </c>
       <c r="F51" s="167" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I51" s="167" t="str">
         <f>R58</f>
         <v>Right ()</v>
       </c>
-      <c r="J51" s="187" t="str">
+      <c r="J51" s="186" t="str">
         <f>IF(R60="","",R60)</f>
         <v/>
       </c>
       <c r="K51" s="167" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M51" s="12"/>
       <c r="O51" s="80" t="s">
@@ -5333,10 +5265,8 @@
         <f>IF(S73="","",S73)</f>
         <v/>
       </c>
-      <c r="AF51" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AG51" s="2"/>
+      <c r="AF51"/>
+      <c r="AG51"/>
     </row>
     <row r="52" spans="1:33" ht="14.45" customHeight="1">
       <c r="A52" s="2">
@@ -5345,7 +5275,7 @@
       <c r="B52" s="10"/>
       <c r="F52" s="95"/>
       <c r="I52" s="62"/>
-      <c r="J52" s="186"/>
+      <c r="J52" s="185"/>
       <c r="M52" s="12"/>
       <c r="O52" s="84" t="s">
         <v>20</v>
@@ -5374,17 +5304,15 @@
         <f>IF(S75="","",S75)</f>
         <v/>
       </c>
-      <c r="AF52" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AG52" s="2"/>
+      <c r="AF52"/>
+      <c r="AG52"/>
     </row>
     <row r="53" spans="1:33" ht="14.45" customHeight="1" thickBot="1">
       <c r="A53" s="2">
         <v>53</v>
       </c>
       <c r="B53" s="10"/>
-      <c r="E53" s="186" t="str">
+      <c r="E53" s="185" t="str">
         <f>Q58</f>
         <v>Left ()</v>
       </c>
@@ -5423,10 +5351,8 @@
         <f>IF(S77="","",S77)</f>
         <v/>
       </c>
-      <c r="AF53" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AG53" s="2"/>
+      <c r="AF53"/>
+      <c r="AG53"/>
     </row>
     <row r="54" spans="1:33" ht="14.45" customHeight="1">
       <c r="A54" s="2">
@@ -5434,13 +5360,13 @@
       </c>
       <c r="B54" s="10"/>
       <c r="D54" s="52" t="s">
-        <v>178</v>
-      </c>
-      <c r="E54" s="196" t="str">
+        <v>174</v>
+      </c>
+      <c r="E54" s="195" t="str">
         <f>IF(Q61="","",Q61)</f>
         <v/>
       </c>
-      <c r="F54" s="197" t="str">
+      <c r="F54" s="196" t="str">
         <f>IF(R61="","",R61)</f>
         <v/>
       </c>
@@ -5468,13 +5394,13 @@
       </c>
       <c r="B55" s="10"/>
       <c r="D55" s="52" t="s">
-        <v>179</v>
-      </c>
-      <c r="E55" s="198" t="str">
+        <v>175</v>
+      </c>
+      <c r="E55" s="197" t="str">
         <f>IF(Q62="","",Q62)</f>
         <v/>
       </c>
-      <c r="F55" s="199" t="str">
+      <c r="F55" s="198" t="str">
         <f>IF(R62="","",R62)</f>
         <v/>
       </c>
@@ -5609,7 +5535,7 @@
       </c>
       <c r="S58" s="2"/>
       <c r="T58" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="U58" s="159" t="str">
         <f>"Left ("&amp;RIGHT($V$13,4)&amp;")"</f>
@@ -5656,25 +5582,25 @@
       <c r="M59" s="12"/>
       <c r="O59" s="13"/>
       <c r="P59" s="66" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q59" s="177" t="str">
-        <f>IF(AG12="","",AG13+Lamb)</f>
-        <v/>
-      </c>
-      <c r="R59" s="178" t="str">
-        <f>IF(AG13="","",AG14+Lamb)</f>
+        <v>146</v>
+      </c>
+      <c r="Q59" s="176" t="str">
+        <f>IF(Sheet1!B5="","",Sheet1!B5+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R59" s="177" t="str">
+        <f>IF(Sheet1!B6="","",Sheet1!B6+Lamb)</f>
         <v/>
       </c>
       <c r="S59" s="2"/>
       <c r="T59" s="175" t="s">
-        <v>147</v>
-      </c>
-      <c r="U59" s="200" t="str">
+        <v>146</v>
+      </c>
+      <c r="U59" s="199" t="str">
         <f>IF(AB31="","",AB31)</f>
         <v/>
       </c>
-      <c r="V59" s="201" t="str">
+      <c r="V59" s="200" t="str">
         <f>IF(AB32="","",AB32)</f>
         <v/>
       </c>
@@ -5702,25 +5628,25 @@
       <c r="M60" s="12"/>
       <c r="O60" s="13"/>
       <c r="P60" s="66" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q60" s="180" t="str">
-        <f>IF(AG14="","",AG15+Lamb)</f>
-        <v/>
-      </c>
-      <c r="R60" s="181" t="str">
-        <f>IF(AG15="","",AG16+Lamb)</f>
+        <v>147</v>
+      </c>
+      <c r="Q60" s="179" t="str">
+        <f>IF(Sheet1!B7="","",Sheet1!B7+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R60" s="180" t="str">
+        <f>IF(Sheet1!B8="","",Sheet1!B8+Lamb)</f>
         <v/>
       </c>
       <c r="S60" s="2"/>
       <c r="T60" s="175" t="s">
-        <v>148</v>
-      </c>
-      <c r="U60" s="202" t="str">
+        <v>147</v>
+      </c>
+      <c r="U60" s="201" t="str">
         <f>IF(AB33="","",AB33)</f>
         <v/>
       </c>
-      <c r="V60" s="203" t="str">
+      <c r="V60" s="202" t="str">
         <f>IF(AB34="","",AB34)</f>
         <v/>
       </c>
@@ -5748,24 +5674,24 @@
       <c r="M61" s="12"/>
       <c r="O61" s="13"/>
       <c r="P61" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="Q61" s="188" t="str">
+        <v>145</v>
+      </c>
+      <c r="Q61" s="187" t="str">
         <f>IF(Q59="","",Q60/Q59)</f>
         <v/>
       </c>
-      <c r="R61" s="189" t="str">
+      <c r="R61" s="188" t="str">
         <f>IF(R59="","",R60/R59)</f>
         <v/>
       </c>
       <c r="T61" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="U61" s="202" t="str">
+        <v>145</v>
+      </c>
+      <c r="U61" s="201" t="str">
         <f>IF(AB35="","",AB35)</f>
         <v/>
       </c>
-      <c r="V61" s="203" t="str">
+      <c r="V61" s="202" t="str">
         <f>IF(AB36="","",AB36)</f>
         <v/>
       </c>
@@ -5791,24 +5717,24 @@
       <c r="M62" s="12"/>
       <c r="O62" s="13"/>
       <c r="P62" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q62" s="190" t="str">
+        <v>171</v>
+      </c>
+      <c r="Q62" s="189" t="str">
         <f>IF(OR(Q59="",Lamb=""),"",Lamb/Q59)</f>
         <v/>
       </c>
-      <c r="R62" s="191" t="str">
+      <c r="R62" s="190" t="str">
         <f>IF(OR(R59="",Lamb=""),"",Lamb/R59)</f>
         <v/>
       </c>
       <c r="T62" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="U62" s="204" t="str">
+        <v>171</v>
+      </c>
+      <c r="U62" s="203" t="str">
         <f>IF(AB37="","",AB37)</f>
         <v/>
       </c>
-      <c r="V62" s="205" t="str">
+      <c r="V62" s="204" t="str">
         <f>IF(AB38="","",AB38)</f>
         <v/>
       </c>
@@ -6117,16 +6043,16 @@
       </c>
       <c r="B71" s="10"/>
       <c r="C71" s="95"/>
-      <c r="D71" s="226" t="str">
+      <c r="D71" s="213" t="str">
         <f>Q86</f>
         <v>UNL-10 (cd/m^2)</v>
       </c>
-      <c r="E71" s="226"/>
-      <c r="F71" s="227" t="str">
+      <c r="E71" s="213"/>
+      <c r="F71" s="214" t="str">
         <f>S86</f>
         <v>UNL-80 (cd/m^2)</v>
       </c>
-      <c r="G71" s="227"/>
+      <c r="G71" s="214"/>
       <c r="I71" s="68" t="s">
         <v>108</v>
       </c>
@@ -6242,15 +6168,15 @@
       <c r="Q73" s="159" t="s">
         <v>97</v>
       </c>
-      <c r="R73" s="209"/>
-      <c r="S73" s="213"/>
+      <c r="R73" s="228"/>
+      <c r="S73" s="232"/>
       <c r="T73" s="2"/>
       <c r="U73" s="2"/>
-      <c r="V73" s="221" t="str">
+      <c r="V73" s="220" t="str">
         <f>IF(AB48="","",AB48)</f>
         <v/>
       </c>
-      <c r="W73" s="222" t="str">
+      <c r="W73" s="221" t="str">
         <f>IF(AB51="","",AB51)</f>
         <v/>
       </c>
@@ -6295,12 +6221,12 @@
       <c r="O74" s="13"/>
       <c r="P74" s="2"/>
       <c r="Q74" s="159"/>
-      <c r="R74" s="210"/>
-      <c r="S74" s="214"/>
+      <c r="R74" s="229"/>
+      <c r="S74" s="233"/>
       <c r="T74" s="2"/>
       <c r="U74" s="2"/>
-      <c r="V74" s="220"/>
-      <c r="W74" s="223"/>
+      <c r="V74" s="219"/>
+      <c r="W74" s="222"/>
       <c r="X74" s="2"/>
       <c r="Y74" s="14"/>
       <c r="AB74" s="158"/>
@@ -6343,15 +6269,15 @@
       <c r="Q75" s="159" t="s">
         <v>99</v>
       </c>
-      <c r="R75" s="211"/>
-      <c r="S75" s="215"/>
+      <c r="R75" s="230"/>
+      <c r="S75" s="234"/>
       <c r="T75" s="2"/>
       <c r="U75" s="2"/>
-      <c r="V75" s="218" t="str">
+      <c r="V75" s="217" t="str">
         <f>IF(AB49="","",AB49)</f>
         <v/>
       </c>
-      <c r="W75" s="224" t="str">
+      <c r="W75" s="223" t="str">
         <f>IF(AB52="","",AB52)</f>
         <v/>
       </c>
@@ -6367,7 +6293,7 @@
       </c>
       <c r="B76" s="10"/>
       <c r="C76" s="52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D76" s="122" t="str">
         <f t="shared" si="13"/>
@@ -6395,12 +6321,12 @@
       <c r="O76" s="13"/>
       <c r="P76" s="2"/>
       <c r="Q76" s="159"/>
-      <c r="R76" s="210"/>
-      <c r="S76" s="214"/>
+      <c r="R76" s="229"/>
+      <c r="S76" s="233"/>
       <c r="T76" s="2"/>
       <c r="U76" s="2"/>
-      <c r="V76" s="220"/>
-      <c r="W76" s="223"/>
+      <c r="V76" s="219"/>
+      <c r="W76" s="222"/>
       <c r="X76" s="2"/>
       <c r="Y76" s="14"/>
       <c r="AB76" s="158"/>
@@ -6435,7 +6361,7 @@
         <v/>
       </c>
       <c r="J77" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="M77" s="12"/>
       <c r="O77" s="13"/>
@@ -6443,15 +6369,15 @@
       <c r="Q77" s="159" t="s">
         <v>102</v>
       </c>
-      <c r="R77" s="211"/>
-      <c r="S77" s="215"/>
+      <c r="R77" s="230"/>
+      <c r="S77" s="234"/>
       <c r="T77" s="2"/>
       <c r="U77" s="2"/>
-      <c r="V77" s="218" t="str">
+      <c r="V77" s="217" t="str">
         <f>IF(AB50="","",AB50)</f>
         <v/>
       </c>
-      <c r="W77" s="224" t="str">
+      <c r="W77" s="223" t="str">
         <f>IF(AB53="","",AB53)</f>
         <v/>
       </c>
@@ -6470,12 +6396,12 @@
       <c r="O78" s="13"/>
       <c r="P78" s="2"/>
       <c r="Q78" s="159"/>
-      <c r="R78" s="212"/>
-      <c r="S78" s="216"/>
+      <c r="R78" s="231"/>
+      <c r="S78" s="235"/>
       <c r="T78" s="2"/>
       <c r="U78" s="2"/>
-      <c r="V78" s="219"/>
-      <c r="W78" s="225"/>
+      <c r="V78" s="218"/>
+      <c r="W78" s="224"/>
       <c r="X78" s="2"/>
       <c r="Y78" s="14"/>
       <c r="AB78" s="158"/>
@@ -6693,16 +6619,16 @@
         <v>Right ()</v>
       </c>
       <c r="H84" s="2"/>
-      <c r="I84" s="228" t="str">
+      <c r="I84" s="215" t="str">
         <f>R68</f>
         <v>Left ()</v>
       </c>
-      <c r="J84" s="228"/>
-      <c r="K84" s="228" t="str">
+      <c r="J84" s="215"/>
+      <c r="K84" s="215" t="str">
         <f>S68</f>
         <v>Right ()</v>
       </c>
-      <c r="L84" s="228"/>
+      <c r="L84" s="215"/>
       <c r="M84" s="12"/>
       <c r="O84" s="13"/>
       <c r="P84" s="2"/>
@@ -6746,16 +6672,16 @@
       <c r="H85" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="I85" s="217" t="str">
+      <c r="I85" s="216" t="str">
         <f>IF(R73="","",R73)</f>
         <v/>
       </c>
-      <c r="J85" s="217"/>
-      <c r="K85" s="217" t="str">
+      <c r="J85" s="216"/>
+      <c r="K85" s="216" t="str">
         <f>IF(S73="","",S73)</f>
         <v/>
       </c>
-      <c r="L85" s="217"/>
+      <c r="L85" s="216"/>
       <c r="M85" s="12"/>
       <c r="O85" s="109" t="s">
         <v>107</v>
@@ -6794,27 +6720,27 @@
       <c r="H86" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="I86" s="217" t="str">
+      <c r="I86" s="216" t="str">
         <f>IF(R75="","",R75)</f>
         <v/>
       </c>
-      <c r="J86" s="217"/>
-      <c r="K86" s="217" t="str">
+      <c r="J86" s="216"/>
+      <c r="K86" s="216" t="str">
         <f>IF(S75="","",S75)</f>
         <v/>
       </c>
-      <c r="L86" s="217"/>
+      <c r="L86" s="216"/>
       <c r="M86" s="12"/>
       <c r="O86" s="13"/>
       <c r="P86" s="2"/>
-      <c r="Q86" s="207" t="s">
+      <c r="Q86" s="226" t="s">
         <v>118</v>
       </c>
-      <c r="R86" s="208"/>
-      <c r="S86" s="207" t="s">
+      <c r="R86" s="227"/>
+      <c r="S86" s="226" t="s">
         <v>119</v>
       </c>
-      <c r="T86" s="208"/>
+      <c r="T86" s="227"/>
       <c r="U86" s="2"/>
       <c r="V86" s="127" t="s">
         <v>44</v>
@@ -6844,16 +6770,16 @@
       <c r="H87" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="I87" s="206" t="str">
+      <c r="I87" s="225" t="str">
         <f>IF(R77="","",R77)</f>
         <v/>
       </c>
-      <c r="J87" s="206"/>
-      <c r="K87" s="206" t="str">
+      <c r="J87" s="225"/>
+      <c r="K87" s="225" t="str">
         <f>IF(S77="","",S77)</f>
         <v/>
       </c>
-      <c r="L87" s="206"/>
+      <c r="L87" s="225"/>
       <c r="M87" s="12"/>
       <c r="O87" s="13"/>
       <c r="P87" s="2"/>
@@ -6881,10 +6807,10 @@
       <c r="X87" s="2"/>
       <c r="Y87" s="14"/>
       <c r="AA87" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC87" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="AC87" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="88" spans="1:30" ht="14.45" customHeight="1">
@@ -6910,22 +6836,22 @@
       <c r="M88" s="12"/>
       <c r="O88" s="13"/>
       <c r="P88" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q88" s="177" t="str">
-        <f t="shared" ref="Q88:Q96" si="16">IF(AG17="","",AG17+Lamb)</f>
-        <v/>
-      </c>
-      <c r="R88" s="178" t="str">
-        <f t="shared" ref="R88:R96" si="17">IF(AG26="","",AG26+Lamb)</f>
-        <v/>
-      </c>
-      <c r="S88" s="179" t="str">
-        <f t="shared" ref="S88:S96" si="18">IF(AG35="","",AG35+Lamb)</f>
-        <v/>
-      </c>
-      <c r="T88" s="178" t="str">
-        <f t="shared" ref="T88:T96" si="19">IF(AG44="","",AG44+Lamb)</f>
+        <v>162</v>
+      </c>
+      <c r="Q88" s="176" t="str">
+        <f>IF(Sheet1!B9="","",Sheet1!B9+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R88" s="177" t="str">
+        <f>IF(Sheet1!B18="","",Sheet1!B18+Lamb)</f>
+        <v/>
+      </c>
+      <c r="S88" s="178" t="str">
+        <f>IF(Sheet1!B27="","",Sheet1!B27+Lamb)</f>
+        <v/>
+      </c>
+      <c r="T88" s="177" t="str">
+        <f>IF(Sheet1!B36="","",Sheet1!B36+Lamb)</f>
         <v/>
       </c>
       <c r="U88" s="2"/>
@@ -6935,19 +6861,19 @@
       </c>
       <c r="X88" s="2"/>
       <c r="Y88" s="14"/>
-      <c r="AA88" s="194" t="e">
+      <c r="AA88" s="193" t="e">
         <f>ABS(Q88-MEDIAN($Q$88:$Q$96))/MEDIAN($Q$88:$Q$96)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AB88" s="194" t="e">
+      <c r="AB88" s="193" t="e">
         <f>ABS(R88-MEDIAN($R$88:$R$96))/MEDIAN($R$88:$R$96)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AC88" s="194" t="e">
+      <c r="AC88" s="193" t="e">
         <f>ABS(S88-MEDIAN($S$88:$S$96))/MEDIAN($S$88:$S$96)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AD88" s="194" t="e">
+      <c r="AD88" s="193" t="e">
         <f>ABS(T88-MEDIAN($T$88:$T$96))/MEDIAN($T$88:$T$96)</f>
         <v>#VALUE!</v>
       </c>
@@ -6973,22 +6899,22 @@
       <c r="M89" s="12"/>
       <c r="O89" s="13"/>
       <c r="P89" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q89" s="180" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="R89" s="181" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="S89" s="182" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="T89" s="181" t="str">
-        <f t="shared" si="19"/>
+        <v>163</v>
+      </c>
+      <c r="Q89" s="179" t="str">
+        <f>IF(Sheet1!B10="","",Sheet1!B10+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R89" s="180" t="str">
+        <f>IF(Sheet1!B19="","",Sheet1!B19+Lamb)</f>
+        <v/>
+      </c>
+      <c r="S89" s="181" t="str">
+        <f>IF(Sheet1!B28="","",Sheet1!B28+Lamb)</f>
+        <v/>
+      </c>
+      <c r="T89" s="180" t="str">
+        <f>IF(Sheet1!B37="","",Sheet1!B37+Lamb)</f>
         <v/>
       </c>
       <c r="U89" s="2"/>
@@ -6998,20 +6924,20 @@
       </c>
       <c r="X89" s="2"/>
       <c r="Y89" s="14"/>
-      <c r="AA89" s="194" t="e">
-        <f t="shared" ref="AA89:AA96" si="20">ABS(Q89-MEDIAN($Q$88:$Q$96))/MEDIAN($Q$88:$Q$96)</f>
+      <c r="AA89" s="193" t="e">
+        <f t="shared" ref="AA89:AA96" si="16">ABS(Q89-MEDIAN($Q$88:$Q$96))/MEDIAN($Q$88:$Q$96)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AB89" s="194" t="e">
-        <f t="shared" ref="AB89:AB96" si="21">ABS(R89-MEDIAN($R$88:$R$96))/MEDIAN($R$88:$R$96)</f>
+      <c r="AB89" s="193" t="e">
+        <f t="shared" ref="AB89:AB96" si="17">ABS(R89-MEDIAN($R$88:$R$96))/MEDIAN($R$88:$R$96)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AC89" s="194" t="e">
-        <f t="shared" ref="AC89:AC96" si="22">ABS(S89-MEDIAN($S$88:$S$96))/MEDIAN($S$88:$S$96)</f>
+      <c r="AC89" s="193" t="e">
+        <f t="shared" ref="AC89:AC96" si="18">ABS(S89-MEDIAN($S$88:$S$96))/MEDIAN($S$88:$S$96)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AD89" s="194" t="e">
-        <f t="shared" ref="AD89:AD96" si="23">ABS(T89-MEDIAN($T$88:$T$96))/MEDIAN($T$88:$T$96)</f>
+      <c r="AD89" s="193" t="e">
+        <f t="shared" ref="AD89:AD96" si="19">ABS(T89-MEDIAN($T$88:$T$96))/MEDIAN($T$88:$T$96)</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7036,22 +6962,22 @@
       <c r="M90" s="12"/>
       <c r="O90" s="13"/>
       <c r="P90" s="21" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q90" s="180" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="R90" s="181" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="S90" s="182" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="T90" s="181" t="str">
-        <f t="shared" si="19"/>
+        <v>164</v>
+      </c>
+      <c r="Q90" s="179" t="str">
+        <f>IF(Sheet1!B11="","",Sheet1!B11+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R90" s="180" t="str">
+        <f>IF(Sheet1!B20="","",Sheet1!B20+Lamb)</f>
+        <v/>
+      </c>
+      <c r="S90" s="181" t="str">
+        <f>IF(Sheet1!B29="","",Sheet1!B29+Lamb)</f>
+        <v/>
+      </c>
+      <c r="T90" s="180" t="str">
+        <f>IF(Sheet1!B38="","",Sheet1!B38+Lamb)</f>
         <v/>
       </c>
       <c r="U90" s="2"/>
@@ -7059,20 +6985,20 @@
       <c r="W90" s="2"/>
       <c r="X90" s="2"/>
       <c r="Y90" s="14"/>
-      <c r="AA90" s="194" t="e">
-        <f t="shared" si="20"/>
+      <c r="AA90" s="193" t="e">
+        <f t="shared" si="16"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB90" s="194" t="e">
-        <f t="shared" si="21"/>
+      <c r="AB90" s="193" t="e">
+        <f t="shared" si="17"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AC90" s="194" t="e">
-        <f t="shared" si="22"/>
+      <c r="AC90" s="193" t="e">
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AD90" s="194" t="e">
-        <f t="shared" si="23"/>
+      <c r="AD90" s="193" t="e">
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7084,22 +7010,22 @@
       <c r="M91" s="12"/>
       <c r="O91" s="13"/>
       <c r="P91" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q91" s="180" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="R91" s="181" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="S91" s="182" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="T91" s="181" t="str">
-        <f t="shared" si="19"/>
+        <v>165</v>
+      </c>
+      <c r="Q91" s="179" t="str">
+        <f>IF(Sheet1!B12="","",Sheet1!B12+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R91" s="180" t="str">
+        <f>IF(Sheet1!B21="","",Sheet1!B21+Lamb)</f>
+        <v/>
+      </c>
+      <c r="S91" s="181" t="str">
+        <f>IF(Sheet1!B30="","",Sheet1!B30+Lamb)</f>
+        <v/>
+      </c>
+      <c r="T91" s="180" t="str">
+        <f>IF(Sheet1!B39="","",Sheet1!B39+Lamb)</f>
         <v/>
       </c>
       <c r="U91" s="2"/>
@@ -7107,20 +7033,20 @@
       <c r="W91" s="2"/>
       <c r="X91" s="2"/>
       <c r="Y91" s="14"/>
-      <c r="AA91" s="194" t="e">
-        <f t="shared" si="20"/>
+      <c r="AA91" s="193" t="e">
+        <f t="shared" si="16"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB91" s="194" t="e">
-        <f t="shared" si="21"/>
+      <c r="AB91" s="193" t="e">
+        <f t="shared" si="17"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AC91" s="194" t="e">
-        <f t="shared" si="22"/>
+      <c r="AC91" s="193" t="e">
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AD91" s="194" t="e">
-        <f t="shared" si="23"/>
+      <c r="AD91" s="193" t="e">
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7135,47 +7061,47 @@
       <c r="M92" s="12"/>
       <c r="O92" s="13"/>
       <c r="P92" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="Q92" s="180" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="R92" s="181" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="S92" s="182" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="T92" s="181" t="str">
-        <f t="shared" si="19"/>
+        <v>166</v>
+      </c>
+      <c r="Q92" s="179" t="str">
+        <f>IF(Sheet1!B13="","",Sheet1!B13+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R92" s="180" t="str">
+        <f>IF(Sheet1!B22="","",Sheet1!B22+Lamb)</f>
+        <v/>
+      </c>
+      <c r="S92" s="181" t="str">
+        <f>IF(Sheet1!B31="","",Sheet1!B31+Lamb)</f>
+        <v/>
+      </c>
+      <c r="T92" s="180" t="str">
+        <f>IF(Sheet1!B40="","",Sheet1!B40+Lamb)</f>
         <v/>
       </c>
       <c r="U92" s="2"/>
       <c r="V92" s="2"/>
       <c r="W92" s="159" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="X92" s="159" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="Y92" s="14"/>
-      <c r="AA92" s="194" t="e">
-        <f t="shared" si="20"/>
+      <c r="AA92" s="193" t="e">
+        <f t="shared" si="16"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB92" s="194" t="e">
-        <f t="shared" si="21"/>
+      <c r="AB92" s="193" t="e">
+        <f t="shared" si="17"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AC92" s="194" t="e">
-        <f t="shared" si="22"/>
+      <c r="AC92" s="193" t="e">
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AD92" s="194" t="e">
-        <f t="shared" si="23"/>
+      <c r="AD92" s="193" t="e">
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7199,50 +7125,50 @@
       <c r="M93" s="12"/>
       <c r="O93" s="13"/>
       <c r="P93" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q93" s="180" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="R93" s="181" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="S93" s="182" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="T93" s="181" t="str">
-        <f t="shared" si="19"/>
+        <v>167</v>
+      </c>
+      <c r="Q93" s="179" t="str">
+        <f>IF(Sheet1!B14="","",Sheet1!B14+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R93" s="180" t="str">
+        <f>IF(Sheet1!B23="","",Sheet1!B23+Lamb)</f>
+        <v/>
+      </c>
+      <c r="S93" s="181" t="str">
+        <f>IF(Sheet1!B32="","",Sheet1!B32+Lamb)</f>
+        <v/>
+      </c>
+      <c r="T93" s="180" t="str">
+        <f>IF(Sheet1!B41="","",Sheet1!B41+Lamb)</f>
         <v/>
       </c>
       <c r="V93" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="W93" s="237" t="e">
+      <c r="W93" s="238" t="e">
         <f>AVERAGE(Q88:R96)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="X93" s="1" t="e">
+      <c r="X93" s="159" t="e">
         <f>STDEV(Q88:R96)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Y93" s="14"/>
-      <c r="AA93" s="194" t="e">
-        <f t="shared" si="20"/>
+      <c r="AA93" s="193" t="e">
+        <f t="shared" si="16"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB93" s="194" t="e">
-        <f t="shared" si="21"/>
+      <c r="AB93" s="193" t="e">
+        <f t="shared" si="17"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AC93" s="194" t="e">
-        <f t="shared" si="22"/>
+      <c r="AC93" s="193" t="e">
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AD93" s="194" t="e">
-        <f t="shared" si="23"/>
+      <c r="AD93" s="193" t="e">
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7266,50 +7192,50 @@
       <c r="M94" s="12"/>
       <c r="O94" s="13"/>
       <c r="P94" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q94" s="180" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="R94" s="181" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="S94" s="182" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="T94" s="181" t="str">
-        <f t="shared" si="19"/>
+        <v>168</v>
+      </c>
+      <c r="Q94" s="179" t="str">
+        <f>IF(Sheet1!B15="","",Sheet1!B15+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R94" s="180" t="str">
+        <f>IF(Sheet1!B24="","",Sheet1!B24+Lamb)</f>
+        <v/>
+      </c>
+      <c r="S94" s="181" t="str">
+        <f>IF(Sheet1!B33="","",Sheet1!B33+Lamb)</f>
+        <v/>
+      </c>
+      <c r="T94" s="180" t="str">
+        <f>IF(Sheet1!B42="","",Sheet1!B42+Lamb)</f>
         <v/>
       </c>
       <c r="V94" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="W94" s="237" t="e">
+      <c r="W94" s="238" t="e">
         <f>AVERAGE(S88:T96)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="X94" s="1" t="e">
+      <c r="X94" s="159" t="e">
         <f>STDEV(S88:T96)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Y94" s="14"/>
-      <c r="AA94" s="194" t="e">
-        <f t="shared" si="20"/>
+      <c r="AA94" s="193" t="e">
+        <f t="shared" si="16"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AB94" s="194" t="e">
-        <f t="shared" si="21"/>
+      <c r="AB94" s="193" t="e">
+        <f t="shared" si="17"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AC94" s="194" t="e">
-        <f t="shared" si="22"/>
+      <c r="AC94" s="193" t="e">
+        <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AD94" s="194" t="e">
-        <f t="shared" si="23"/>
+      <c r="AD94" s="193" t="e">
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7333,39 +7259,39 @@
       <c r="M95" s="12"/>
       <c r="O95" s="13"/>
       <c r="P95" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q95" s="180" t="str">
+        <v>169</v>
+      </c>
+      <c r="Q95" s="179" t="str">
+        <f>IF(Sheet1!B16="","",Sheet1!B16+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R95" s="180" t="str">
+        <f>IF(Sheet1!B25="","",Sheet1!B25+Lamb)</f>
+        <v/>
+      </c>
+      <c r="S95" s="181" t="str">
+        <f>IF(Sheet1!B34="","",Sheet1!B34+Lamb)</f>
+        <v/>
+      </c>
+      <c r="T95" s="180" t="str">
+        <f>IF(Sheet1!B43="","",Sheet1!B43+Lamb)</f>
+        <v/>
+      </c>
+      <c r="Y95" s="14"/>
+      <c r="AA95" s="193" t="e">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="R95" s="181" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AB95" s="193" t="e">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="S95" s="182" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AC95" s="193" t="e">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="T95" s="181" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AD95" s="193" t="e">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="Y95" s="14"/>
-      <c r="AA95" s="194" t="e">
-        <f t="shared" si="20"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AB95" s="194" t="e">
-        <f t="shared" si="21"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AC95" s="194" t="e">
-        <f t="shared" si="22"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AD95" s="194" t="e">
-        <f t="shared" si="23"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7389,39 +7315,39 @@
       <c r="M96" s="12"/>
       <c r="O96" s="13"/>
       <c r="P96" s="21" t="s">
-        <v>174</v>
-      </c>
-      <c r="Q96" s="183" t="str">
+        <v>170</v>
+      </c>
+      <c r="Q96" s="182" t="str">
+        <f>IF(Sheet1!B17="","",Sheet1!B17+Lamb)</f>
+        <v/>
+      </c>
+      <c r="R96" s="183" t="str">
+        <f>IF(Sheet1!B26="","",Sheet1!B26+Lamb)</f>
+        <v/>
+      </c>
+      <c r="S96" s="184" t="str">
+        <f>IF(Sheet1!B35="","",Sheet1!B35+Lamb)</f>
+        <v/>
+      </c>
+      <c r="T96" s="183" t="str">
+        <f>IF(Sheet1!B44="","",Sheet1!B44+Lamb)</f>
+        <v/>
+      </c>
+      <c r="Y96" s="14"/>
+      <c r="AA96" s="193" t="e">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="R96" s="184" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AB96" s="193" t="e">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="S96" s="185" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AC96" s="193" t="e">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="T96" s="184" t="str">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AD96" s="193" t="e">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="Y96" s="14"/>
-      <c r="AA96" s="194" t="e">
-        <f t="shared" si="20"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AB96" s="194" t="e">
-        <f t="shared" si="21"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AC96" s="194" t="e">
-        <f t="shared" si="22"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AD96" s="194" t="e">
-        <f t="shared" si="23"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7581,26 +7507,26 @@
       <c r="M100" s="12"/>
       <c r="O100" s="13"/>
       <c r="P100" s="21" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q100" s="192" t="str">
+        <v>178</v>
+      </c>
+      <c r="Q100" s="191" t="str">
         <f>IF(Q88="","",MAX(AA88:AA96))</f>
         <v/>
       </c>
-      <c r="R100" s="193" t="str">
+      <c r="R100" s="192" t="str">
         <f>IF(R88="","",MAX(AB88:AB96))</f>
         <v/>
       </c>
-      <c r="S100" s="192" t="str">
+      <c r="S100" s="191" t="str">
         <f>IF(S88="","",MAX(AC88:AC96))</f>
         <v/>
       </c>
-      <c r="T100" s="193" t="str">
+      <c r="T100" s="192" t="str">
         <f>IF(T88="","",MAX(AD88:AD96))</f>
         <v/>
       </c>
       <c r="V100" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="Y100" s="14"/>
     </row>
@@ -8632,34 +8558,6 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="40">
-    <mergeCell ref="AG1:AJ1"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="I84:J84"/>
-    <mergeCell ref="K84:L84"/>
-    <mergeCell ref="I85:J85"/>
-    <mergeCell ref="K85:L85"/>
-    <mergeCell ref="V77:V78"/>
-    <mergeCell ref="V75:V76"/>
-    <mergeCell ref="V73:V74"/>
-    <mergeCell ref="W73:W74"/>
-    <mergeCell ref="W75:W76"/>
-    <mergeCell ref="W77:W78"/>
     <mergeCell ref="I87:J87"/>
     <mergeCell ref="K87:L87"/>
     <mergeCell ref="Q86:R86"/>
@@ -8672,6 +8570,34 @@
     <mergeCell ref="S77:S78"/>
     <mergeCell ref="I86:J86"/>
     <mergeCell ref="K86:L86"/>
+    <mergeCell ref="V77:V78"/>
+    <mergeCell ref="V75:V76"/>
+    <mergeCell ref="V73:V74"/>
+    <mergeCell ref="W73:W74"/>
+    <mergeCell ref="W75:W76"/>
+    <mergeCell ref="W77:W78"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="I84:J84"/>
+    <mergeCell ref="K84:L84"/>
+    <mergeCell ref="I85:J85"/>
+    <mergeCell ref="K85:L85"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="AG1:AJ1"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="J10:K10"/>
   </mergeCells>
   <conditionalFormatting sqref="I72:I74">
     <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
@@ -8744,7 +8670,7 @@
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.92638888888888904" header="0.51180555555555496" footer="0.78749999999999998"/>
+  <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.78740157480314965" bottom="0.94488188976377963" header="0.51181102362204722" footer="0.78740157480314965"/>
   <pageSetup scale="65" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -8754,4 +8680,240 @@
   </rowBreaks>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C29263F-D78E-4F41-860C-A3D9FC1D1372}">
+  <dimension ref="A1:B46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="236" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="237" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" s="237" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="236" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Start sheet for yearly checks
</commit_message>
<xml_diff>
--- a/MUSCMammoMonitor.xlsx
+++ b/MUSCMammoMonitor.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugenem\Documents\GitHub\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EEE753-CF3D-4373-8CBD-38EBD29031D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D603258B-BD81-4957-86C2-8F9DAFDF04E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Barco" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="BarcoYearlyChecks" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Lamb">Barco!$T$26</definedName>
     <definedName name="Page1">Barco!$B$1:$M$66</definedName>
     <definedName name="Page2">Barco!$B$67:$M$132</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Barco!$B$1:$M$132</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">BarcoYearlyChecks!$B$1:$L$46</definedName>
     <definedName name="Z_B8088769_C3DE_4DF8_A82B_D0EB46FFCC4A_.wvu.PrintArea" localSheetId="0" hidden="1">Barco!$B$1:$M$132</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -102,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="202">
   <si>
     <t>Print Area</t>
   </si>
@@ -666,6 +668,48 @@
   </si>
   <si>
     <t>Barco K5905277 v16</t>
+  </si>
+  <si>
+    <t>Barco Yearly Checks</t>
+  </si>
+  <si>
+    <t>Visual test - Temporal response</t>
+  </si>
+  <si>
+    <t>Visual test - TG18 OIQ</t>
+  </si>
+  <si>
+    <t>Artifacts, non-uniformities</t>
+  </si>
+  <si>
+    <t>Grayscale continuity</t>
+  </si>
+  <si>
+    <t>0-5% Contrast</t>
+  </si>
+  <si>
+    <t>Gray Steps</t>
+  </si>
+  <si>
+    <t>Alphanumerics</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>5%/95%</t>
+  </si>
+  <si>
+    <t>Line Pairs</t>
   </si>
 </sst>
 </file>
@@ -681,7 +725,7 @@
     <numFmt numFmtId="169" formatCode="0.0%"/>
     <numFmt numFmtId="170" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -815,8 +859,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -871,8 +920,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="59">
+  <borders count="61">
     <border>
       <left/>
       <right/>
@@ -1596,6 +1651,32 @@
       </right>
       <top/>
       <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -1615,7 +1696,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="239">
+  <cellXfs count="255">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2234,6 +2315,66 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2267,66 +2408,52 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Fail" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2578,6 +2705,9 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFFFFF99"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2855,8 +2985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65:M66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2901,12 +3031,12 @@
       <c r="AA1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="AG1" s="235" t="s">
+      <c r="AG1" s="208" t="s">
         <v>1</v>
       </c>
-      <c r="AH1" s="235"/>
-      <c r="AI1" s="235"/>
-      <c r="AJ1" s="235"/>
+      <c r="AH1" s="208"/>
+      <c r="AI1" s="208"/>
+      <c r="AJ1" s="208"/>
     </row>
     <row r="2" spans="1:36" ht="14.45" customHeight="1">
       <c r="A2" s="2">
@@ -2925,14 +3055,14 @@
       <c r="AA2" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="AG2" s="236" t="s">
+      <c r="AG2" s="209" t="s">
         <v>3</v>
       </c>
-      <c r="AH2" s="236"/>
-      <c r="AI2" s="237" t="s">
+      <c r="AH2" s="209"/>
+      <c r="AI2" s="210" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="237"/>
+      <c r="AJ2" s="210"/>
     </row>
     <row r="3" spans="1:36" ht="14.45" customHeight="1">
       <c r="A3" s="2">
@@ -3226,19 +3356,19 @@
       <c r="D10" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="238" t="str">
+      <c r="E10" s="211" t="str">
         <f t="shared" ref="E10:E15" si="1">IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="F10" s="238"/>
+      <c r="F10" s="211"/>
       <c r="I10" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="238" t="str">
+      <c r="J10" s="211" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="K10" s="238"/>
+      <c r="K10" s="211"/>
       <c r="M10" s="12"/>
       <c r="O10" s="13"/>
       <c r="Q10" s="21" t="s">
@@ -3281,19 +3411,19 @@
       <c r="D11" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="231" t="str">
+      <c r="E11" s="212" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F11" s="231"/>
+      <c r="F11" s="212"/>
       <c r="I11" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="234" t="str">
+      <c r="J11" s="213" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="K11" s="234"/>
+      <c r="K11" s="213"/>
       <c r="M11" s="12"/>
       <c r="O11" s="13"/>
       <c r="Q11" s="21" t="s">
@@ -3336,19 +3466,19 @@
       <c r="D12" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="231" t="str">
+      <c r="E12" s="212" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F12" s="231"/>
+      <c r="F12" s="212"/>
       <c r="I12" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="231" t="str">
+      <c r="J12" s="212" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="K12" s="231"/>
+      <c r="K12" s="212"/>
       <c r="M12" s="12"/>
       <c r="O12" s="13"/>
       <c r="Q12" s="21" t="s">
@@ -3391,19 +3521,19 @@
       <c r="D13" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="231" t="str">
+      <c r="E13" s="212" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F13" s="231"/>
+      <c r="F13" s="212"/>
       <c r="I13" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="231" t="str">
+      <c r="J13" s="212" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="K13" s="231"/>
+      <c r="K13" s="212"/>
       <c r="M13" s="12"/>
       <c r="O13" s="13"/>
       <c r="Q13" s="21" t="s">
@@ -3446,19 +3576,19 @@
       <c r="D14" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="231" t="str">
+      <c r="E14" s="212" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F14" s="231"/>
+      <c r="F14" s="212"/>
       <c r="I14" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="231" t="str">
+      <c r="J14" s="212" t="str">
         <f>IF(V14="","",V14)</f>
         <v/>
       </c>
-      <c r="K14" s="231"/>
+      <c r="K14" s="212"/>
       <c r="M14" s="12"/>
       <c r="O14" s="13"/>
       <c r="Q14" s="21" t="s">
@@ -3501,11 +3631,11 @@
       <c r="D15" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="231" t="str">
+      <c r="E15" s="212" t="str">
         <f t="shared" si="1"/>
         <v>Barco K5905277 v16</v>
       </c>
-      <c r="F15" s="231"/>
+      <c r="F15" s="212"/>
       <c r="M15" s="12"/>
       <c r="O15" s="26"/>
       <c r="P15" s="27"/>
@@ -3651,10 +3781,10 @@
       <c r="H19" s="154"/>
       <c r="I19" s="154"/>
       <c r="J19" s="154"/>
-      <c r="K19" s="233" t="s">
+      <c r="K19" s="215" t="s">
         <v>128</v>
       </c>
-      <c r="L19" s="233"/>
+      <c r="L19" s="215"/>
       <c r="M19" s="5"/>
       <c r="O19" s="13"/>
       <c r="R19" s="1" t="s">
@@ -3914,11 +4044,11 @@
       <c r="D24" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="E24" s="232" t="str">
+      <c r="E24" s="214" t="str">
         <f>IF(P52="","",P52)</f>
         <v/>
       </c>
-      <c r="F24" s="232"/>
+      <c r="F24" s="214"/>
       <c r="G24" s="40"/>
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
@@ -6045,16 +6175,16 @@
       </c>
       <c r="B71" s="10"/>
       <c r="C71" s="95"/>
-      <c r="D71" s="228" t="str">
+      <c r="D71" s="216" t="str">
         <f>Q86</f>
         <v>UNL-10 (cd/m^2)</v>
       </c>
-      <c r="E71" s="228"/>
-      <c r="F71" s="229" t="str">
+      <c r="E71" s="216"/>
+      <c r="F71" s="217" t="str">
         <f>S86</f>
         <v>UNL-80 (cd/m^2)</v>
       </c>
-      <c r="G71" s="229"/>
+      <c r="G71" s="217"/>
       <c r="I71" s="68" t="s">
         <v>107</v>
       </c>
@@ -6170,8 +6300,8 @@
       <c r="Q73" s="159" t="s">
         <v>96</v>
       </c>
-      <c r="R73" s="211"/>
-      <c r="S73" s="215"/>
+      <c r="R73" s="231"/>
+      <c r="S73" s="235"/>
       <c r="T73" s="2"/>
       <c r="U73" s="2"/>
       <c r="V73" s="223" t="str">
@@ -6223,8 +6353,8 @@
       <c r="O74" s="13"/>
       <c r="P74" s="2"/>
       <c r="Q74" s="159"/>
-      <c r="R74" s="212"/>
-      <c r="S74" s="216"/>
+      <c r="R74" s="232"/>
+      <c r="S74" s="236"/>
       <c r="T74" s="2"/>
       <c r="U74" s="2"/>
       <c r="V74" s="222"/>
@@ -6271,8 +6401,8 @@
       <c r="Q75" s="159" t="s">
         <v>98</v>
       </c>
-      <c r="R75" s="213"/>
-      <c r="S75" s="217"/>
+      <c r="R75" s="233"/>
+      <c r="S75" s="237"/>
       <c r="T75" s="2"/>
       <c r="U75" s="2"/>
       <c r="V75" s="220" t="str">
@@ -6323,8 +6453,8 @@
       <c r="O76" s="13"/>
       <c r="P76" s="2"/>
       <c r="Q76" s="159"/>
-      <c r="R76" s="212"/>
-      <c r="S76" s="216"/>
+      <c r="R76" s="232"/>
+      <c r="S76" s="236"/>
       <c r="T76" s="2"/>
       <c r="U76" s="2"/>
       <c r="V76" s="222"/>
@@ -6371,8 +6501,8 @@
       <c r="Q77" s="159" t="s">
         <v>101</v>
       </c>
-      <c r="R77" s="213"/>
-      <c r="S77" s="217"/>
+      <c r="R77" s="233"/>
+      <c r="S77" s="237"/>
       <c r="T77" s="2"/>
       <c r="U77" s="2"/>
       <c r="V77" s="220" t="str">
@@ -6398,8 +6528,8 @@
       <c r="O78" s="13"/>
       <c r="P78" s="2"/>
       <c r="Q78" s="159"/>
-      <c r="R78" s="214"/>
-      <c r="S78" s="218"/>
+      <c r="R78" s="234"/>
+      <c r="S78" s="238"/>
       <c r="T78" s="2"/>
       <c r="U78" s="2"/>
       <c r="V78" s="221"/>
@@ -6621,16 +6751,16 @@
         <v>Right ()</v>
       </c>
       <c r="H84" s="2"/>
-      <c r="I84" s="230" t="str">
+      <c r="I84" s="218" t="str">
         <f>R68</f>
         <v>Left ()</v>
       </c>
-      <c r="J84" s="230"/>
-      <c r="K84" s="230" t="str">
+      <c r="J84" s="218"/>
+      <c r="K84" s="218" t="str">
         <f>S68</f>
         <v>Right ()</v>
       </c>
-      <c r="L84" s="230"/>
+      <c r="L84" s="218"/>
       <c r="M84" s="12"/>
       <c r="O84" s="13"/>
       <c r="P84" s="2"/>
@@ -6735,14 +6865,14 @@
       <c r="M86" s="12"/>
       <c r="O86" s="13"/>
       <c r="P86" s="2"/>
-      <c r="Q86" s="209" t="s">
+      <c r="Q86" s="229" t="s">
         <v>117</v>
       </c>
-      <c r="R86" s="210"/>
-      <c r="S86" s="209" t="s">
+      <c r="R86" s="230"/>
+      <c r="S86" s="229" t="s">
         <v>118</v>
       </c>
-      <c r="T86" s="210"/>
+      <c r="T86" s="230"/>
       <c r="U86" s="2"/>
       <c r="V86" s="127" t="s">
         <v>43</v>
@@ -6772,16 +6902,16 @@
       <c r="H87" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="I87" s="208" t="str">
+      <c r="I87" s="228" t="str">
         <f>IF(R77="","",R77)</f>
         <v/>
       </c>
-      <c r="J87" s="208"/>
-      <c r="K87" s="208" t="str">
+      <c r="J87" s="228"/>
+      <c r="K87" s="228" t="str">
         <f>IF(S77="","",S77)</f>
         <v/>
       </c>
-      <c r="L87" s="208"/>
+      <c r="L87" s="228"/>
       <c r="M87" s="12"/>
       <c r="O87" s="13"/>
       <c r="P87" s="2"/>
@@ -8560,34 +8690,6 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="40">
-    <mergeCell ref="AG1:AJ1"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="I84:J84"/>
-    <mergeCell ref="K84:L84"/>
-    <mergeCell ref="I85:J85"/>
-    <mergeCell ref="K85:L85"/>
-    <mergeCell ref="V77:V78"/>
-    <mergeCell ref="V75:V76"/>
-    <mergeCell ref="V73:V74"/>
-    <mergeCell ref="W73:W74"/>
-    <mergeCell ref="W75:W76"/>
-    <mergeCell ref="W77:W78"/>
     <mergeCell ref="I87:J87"/>
     <mergeCell ref="K87:L87"/>
     <mergeCell ref="Q86:R86"/>
@@ -8600,6 +8702,34 @@
     <mergeCell ref="S77:S78"/>
     <mergeCell ref="I86:J86"/>
     <mergeCell ref="K86:L86"/>
+    <mergeCell ref="V77:V78"/>
+    <mergeCell ref="V75:V76"/>
+    <mergeCell ref="V73:V74"/>
+    <mergeCell ref="W73:W74"/>
+    <mergeCell ref="W75:W76"/>
+    <mergeCell ref="W77:W78"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="I84:J84"/>
+    <mergeCell ref="K84:L84"/>
+    <mergeCell ref="I85:J85"/>
+    <mergeCell ref="K85:L85"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="AG1:AJ1"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="J10:K10"/>
   </mergeCells>
   <conditionalFormatting sqref="I72:I74">
     <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
@@ -8685,6 +8815,868 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{756B15AE-536E-4AE5-82F4-E521E392C0F6}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:R46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" style="247" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="95"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="16.5" thickTop="1">
+      <c r="A1" s="247">
+        <v>1</v>
+      </c>
+      <c r="B1" s="239"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="154"/>
+      <c r="K1" s="154"/>
+      <c r="L1" s="240"/>
+      <c r="R1" s="95" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="20.25">
+      <c r="A2" s="247">
+        <v>2</v>
+      </c>
+      <c r="B2" s="241"/>
+      <c r="G2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="242"/>
+      <c r="R2" s="95" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="20.25">
+      <c r="A3" s="247">
+        <v>3</v>
+      </c>
+      <c r="B3" s="241"/>
+      <c r="G3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="242"/>
+      <c r="R3" s="95" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="247">
+        <v>4</v>
+      </c>
+      <c r="B4" s="241"/>
+      <c r="G4" s="159"/>
+      <c r="L4" s="242"/>
+    </row>
+    <row r="5" spans="1:18" ht="20.25">
+      <c r="A5" s="247">
+        <v>5</v>
+      </c>
+      <c r="B5" s="241"/>
+      <c r="G5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="242"/>
+    </row>
+    <row r="6" spans="1:18" ht="16.5" thickBot="1">
+      <c r="A6" s="247">
+        <v>6</v>
+      </c>
+      <c r="B6" s="243"/>
+      <c r="C6" s="244"/>
+      <c r="D6" s="244"/>
+      <c r="E6" s="244"/>
+      <c r="F6" s="244"/>
+      <c r="G6" s="244"/>
+      <c r="H6" s="244"/>
+      <c r="I6" s="244"/>
+      <c r="J6" s="244"/>
+      <c r="K6" s="244"/>
+      <c r="L6" s="245"/>
+    </row>
+    <row r="7" spans="1:18" ht="16.5" thickTop="1">
+      <c r="A7" s="247">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="16.5" thickBot="1">
+      <c r="A8" s="247">
+        <v>8</v>
+      </c>
+      <c r="B8" s="185"/>
+      <c r="C8" s="185"/>
+      <c r="D8" s="185"/>
+      <c r="E8" s="185"/>
+      <c r="F8" s="185"/>
+      <c r="G8" s="185"/>
+      <c r="H8" s="246" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="185"/>
+      <c r="J8" s="185"/>
+      <c r="K8" s="185"/>
+      <c r="L8" s="185"/>
+    </row>
+    <row r="9" spans="1:18" ht="16.5" thickTop="1">
+      <c r="A9" s="247">
+        <v>9</v>
+      </c>
+      <c r="B9" s="239"/>
+      <c r="C9" s="154"/>
+      <c r="D9" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="154"/>
+      <c r="F9" s="154"/>
+      <c r="G9" s="154"/>
+      <c r="H9" s="154"/>
+      <c r="I9" s="154"/>
+      <c r="J9" s="154"/>
+      <c r="K9" s="154"/>
+      <c r="L9" s="240"/>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="247">
+        <v>10</v>
+      </c>
+      <c r="B10" s="241"/>
+      <c r="D10" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="211" t="str">
+        <f>Barco!E10</f>
+        <v/>
+      </c>
+      <c r="F10" s="211"/>
+      <c r="I10" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="211" t="str">
+        <f>Barco!J10</f>
+        <v/>
+      </c>
+      <c r="K10" s="211"/>
+      <c r="L10" s="242"/>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="247">
+        <v>11</v>
+      </c>
+      <c r="B11" s="241"/>
+      <c r="D11" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="211" t="str">
+        <f>Barco!E11</f>
+        <v/>
+      </c>
+      <c r="F11" s="211"/>
+      <c r="I11" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="211" t="str">
+        <f>Barco!J11</f>
+        <v/>
+      </c>
+      <c r="K11" s="211"/>
+      <c r="L11" s="242"/>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="247">
+        <v>12</v>
+      </c>
+      <c r="B12" s="241"/>
+      <c r="D12" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="211" t="str">
+        <f>Barco!E12</f>
+        <v/>
+      </c>
+      <c r="F12" s="211"/>
+      <c r="I12" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="211" t="str">
+        <f>Barco!J12</f>
+        <v/>
+      </c>
+      <c r="K12" s="211"/>
+      <c r="L12" s="242"/>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="247">
+        <v>13</v>
+      </c>
+      <c r="B13" s="241"/>
+      <c r="D13" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="211" t="str">
+        <f>Barco!E13</f>
+        <v/>
+      </c>
+      <c r="F13" s="211"/>
+      <c r="I13" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="211" t="str">
+        <f>Barco!J13</f>
+        <v/>
+      </c>
+      <c r="K13" s="211"/>
+      <c r="L13" s="242"/>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="247">
+        <v>14</v>
+      </c>
+      <c r="B14" s="241"/>
+      <c r="D14" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="211" t="str">
+        <f>Barco!E14</f>
+        <v/>
+      </c>
+      <c r="F14" s="211"/>
+      <c r="I14" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" s="211" t="str">
+        <f>Barco!J14</f>
+        <v/>
+      </c>
+      <c r="K14" s="211"/>
+      <c r="L14" s="242"/>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="247">
+        <v>15</v>
+      </c>
+      <c r="B15" s="241"/>
+      <c r="D15" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="211" t="str">
+        <f>Barco!E15</f>
+        <v>Barco K5905277 v16</v>
+      </c>
+      <c r="F15" s="211"/>
+      <c r="L15" s="242"/>
+    </row>
+    <row r="16" spans="1:18" ht="16.5" thickBot="1">
+      <c r="A16" s="247">
+        <v>16</v>
+      </c>
+      <c r="B16" s="243"/>
+      <c r="C16" s="244"/>
+      <c r="D16" s="244"/>
+      <c r="E16" s="244"/>
+      <c r="F16" s="244"/>
+      <c r="G16" s="244"/>
+      <c r="H16" s="244"/>
+      <c r="I16" s="244"/>
+      <c r="J16" s="244"/>
+      <c r="K16" s="244"/>
+      <c r="L16" s="245"/>
+    </row>
+    <row r="17" spans="1:12" ht="17.25" thickTop="1" thickBot="1">
+      <c r="A17" s="247">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="16.5" thickTop="1">
+      <c r="A18" s="247">
+        <v>18</v>
+      </c>
+      <c r="B18" s="253" t="s">
+        <v>188</v>
+      </c>
+      <c r="C18" s="154"/>
+      <c r="D18" s="154"/>
+      <c r="E18" s="154"/>
+      <c r="F18" s="154"/>
+      <c r="G18" s="154"/>
+      <c r="H18" s="154"/>
+      <c r="I18" s="154"/>
+      <c r="J18" s="154"/>
+      <c r="K18" s="154"/>
+      <c r="L18" s="240"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="247">
+        <v>19</v>
+      </c>
+      <c r="B19" s="241"/>
+      <c r="C19" s="185"/>
+      <c r="D19" s="185"/>
+      <c r="E19" s="185"/>
+      <c r="F19" s="185"/>
+      <c r="G19" s="185"/>
+      <c r="H19" s="185"/>
+      <c r="I19" s="185"/>
+      <c r="J19" s="185"/>
+      <c r="K19" s="185"/>
+      <c r="L19" s="242"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="247">
+        <v>20</v>
+      </c>
+      <c r="B20" s="241"/>
+      <c r="C20" s="185"/>
+      <c r="D20" s="185"/>
+      <c r="E20" s="185"/>
+      <c r="F20" s="249" t="s">
+        <v>196</v>
+      </c>
+      <c r="G20" s="249"/>
+      <c r="H20" s="249" t="s">
+        <v>197</v>
+      </c>
+      <c r="I20" s="249"/>
+      <c r="J20" s="185"/>
+      <c r="K20" s="185"/>
+      <c r="L20" s="242"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="247">
+        <v>21</v>
+      </c>
+      <c r="B21" s="241"/>
+      <c r="C21" s="185"/>
+      <c r="D21" s="185"/>
+      <c r="E21" s="185"/>
+      <c r="F21" s="249" t="str">
+        <f>J13</f>
+        <v/>
+      </c>
+      <c r="G21" s="249"/>
+      <c r="H21" s="249" t="str">
+        <f>J14</f>
+        <v/>
+      </c>
+      <c r="I21" s="249"/>
+      <c r="J21" s="185"/>
+      <c r="K21" s="185"/>
+      <c r="L21" s="242"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="247">
+        <v>22</v>
+      </c>
+      <c r="B22" s="241"/>
+      <c r="C22" s="185"/>
+      <c r="D22" s="185"/>
+      <c r="E22" s="62" t="s">
+        <v>189</v>
+      </c>
+      <c r="F22" s="248" t="str">
+        <f>IF(Barco!E23="","",IF(Barco!E23="YES","PASS","FAIL"))</f>
+        <v/>
+      </c>
+      <c r="G22" s="248"/>
+      <c r="H22" s="248"/>
+      <c r="I22" s="248"/>
+      <c r="J22" s="185"/>
+      <c r="K22" s="185"/>
+      <c r="L22" s="242"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="247">
+        <v>23</v>
+      </c>
+      <c r="B23" s="241"/>
+      <c r="C23" s="185"/>
+      <c r="D23" s="185"/>
+      <c r="E23" s="62" t="s">
+        <v>190</v>
+      </c>
+      <c r="F23" s="248" t="str">
+        <f>IF(Barco!E22="","",IF(Barco!E22="YES","PASS","FAIL"))</f>
+        <v/>
+      </c>
+      <c r="G23" s="248"/>
+      <c r="H23" s="248"/>
+      <c r="I23" s="248"/>
+      <c r="J23" s="185"/>
+      <c r="K23" s="185"/>
+      <c r="L23" s="242"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="247">
+        <v>24</v>
+      </c>
+      <c r="B24" s="241"/>
+      <c r="C24" s="185"/>
+      <c r="D24" s="185"/>
+      <c r="E24" s="62" t="s">
+        <v>191</v>
+      </c>
+      <c r="F24" s="248" t="str">
+        <f>IF(OR(Barco!I72="TBD",Barco!I73="TBD"),"",IF(AND(Barco!I72="YES",Barco!I73="YES"),"PASS","FAIL"))</f>
+        <v/>
+      </c>
+      <c r="G24" s="248"/>
+      <c r="H24" s="248"/>
+      <c r="I24" s="248"/>
+      <c r="J24" s="185"/>
+      <c r="K24" s="185"/>
+      <c r="L24" s="242"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="247">
+        <v>25</v>
+      </c>
+      <c r="B25" s="241"/>
+      <c r="C25" s="185"/>
+      <c r="D25" s="185"/>
+      <c r="E25" s="62" t="s">
+        <v>192</v>
+      </c>
+      <c r="F25" s="252"/>
+      <c r="G25" s="252"/>
+      <c r="H25" s="252"/>
+      <c r="I25" s="252"/>
+      <c r="J25" s="185"/>
+      <c r="K25" s="185"/>
+      <c r="L25" s="242"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="247">
+        <v>26</v>
+      </c>
+      <c r="B26" s="241"/>
+      <c r="C26" s="185"/>
+      <c r="D26" s="185" t="s">
+        <v>200</v>
+      </c>
+      <c r="E26" s="62" t="s">
+        <v>193</v>
+      </c>
+      <c r="F26" s="248" t="str">
+        <f>IF(Barco!F85="","",IF(Barco!F85="YES","PASS","FAIL"))</f>
+        <v/>
+      </c>
+      <c r="G26" s="248"/>
+      <c r="H26" s="248"/>
+      <c r="I26" s="248"/>
+      <c r="J26" s="185"/>
+      <c r="K26" s="185"/>
+      <c r="L26" s="242"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="247">
+        <v>27</v>
+      </c>
+      <c r="B27" s="241"/>
+      <c r="C27" s="185"/>
+      <c r="D27" s="185"/>
+      <c r="E27" s="62" t="s">
+        <v>194</v>
+      </c>
+      <c r="F27" s="252"/>
+      <c r="G27" s="252"/>
+      <c r="H27" s="252"/>
+      <c r="I27" s="252"/>
+      <c r="J27" s="185"/>
+      <c r="K27" s="185"/>
+      <c r="L27" s="242"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="247">
+        <v>28</v>
+      </c>
+      <c r="B28" s="241"/>
+      <c r="C28" s="185"/>
+      <c r="D28" s="185"/>
+      <c r="E28" s="62" t="s">
+        <v>195</v>
+      </c>
+      <c r="F28" s="252"/>
+      <c r="G28" s="252"/>
+      <c r="H28" s="252"/>
+      <c r="I28" s="252"/>
+      <c r="J28" s="185"/>
+      <c r="K28" s="185"/>
+      <c r="L28" s="242"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="247">
+        <v>29</v>
+      </c>
+      <c r="B29" s="241"/>
+      <c r="C29" s="185"/>
+      <c r="D29" s="185"/>
+      <c r="E29" s="62" t="s">
+        <v>201</v>
+      </c>
+      <c r="F29" s="250" t="str">
+        <f>IF(Barco!F86="","",IF(Barco!F86="YES","PASS","FAIL"))</f>
+        <v/>
+      </c>
+      <c r="G29" s="251"/>
+      <c r="H29" s="250" t="str">
+        <f>IF(Barco!G86="","",IF(Barco!G86="YES","PASS","FAIL"))</f>
+        <v/>
+      </c>
+      <c r="I29" s="251"/>
+      <c r="J29" s="185"/>
+      <c r="K29" s="185"/>
+      <c r="L29" s="242"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="247">
+        <v>30</v>
+      </c>
+      <c r="B30" s="241"/>
+      <c r="C30" s="185"/>
+      <c r="D30" s="185"/>
+      <c r="E30" s="254"/>
+      <c r="F30" s="254"/>
+      <c r="G30" s="254"/>
+      <c r="H30" s="254"/>
+      <c r="I30" s="254"/>
+      <c r="J30" s="185"/>
+      <c r="K30" s="185"/>
+      <c r="L30" s="242"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="247">
+        <v>31</v>
+      </c>
+      <c r="B31" s="241"/>
+      <c r="C31" s="185"/>
+      <c r="D31" s="185"/>
+      <c r="E31" s="185"/>
+      <c r="F31" s="185"/>
+      <c r="G31" s="185"/>
+      <c r="H31" s="185"/>
+      <c r="I31" s="185"/>
+      <c r="J31" s="185"/>
+      <c r="K31" s="185"/>
+      <c r="L31" s="242"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="247">
+        <v>32</v>
+      </c>
+      <c r="B32" s="241"/>
+      <c r="C32" s="185"/>
+      <c r="D32" s="185"/>
+      <c r="E32" s="185"/>
+      <c r="F32" s="185"/>
+      <c r="G32" s="185"/>
+      <c r="H32" s="185"/>
+      <c r="I32" s="185"/>
+      <c r="J32" s="185"/>
+      <c r="K32" s="185"/>
+      <c r="L32" s="242"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="247">
+        <v>33</v>
+      </c>
+      <c r="B33" s="241"/>
+      <c r="C33" s="185"/>
+      <c r="D33" s="185"/>
+      <c r="E33" s="185"/>
+      <c r="F33" s="185"/>
+      <c r="G33" s="185"/>
+      <c r="H33" s="185"/>
+      <c r="I33" s="185"/>
+      <c r="J33" s="185"/>
+      <c r="K33" s="185"/>
+      <c r="L33" s="242"/>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="247">
+        <v>34</v>
+      </c>
+      <c r="B34" s="241"/>
+      <c r="C34" s="185"/>
+      <c r="D34" s="185"/>
+      <c r="E34" s="185"/>
+      <c r="F34" s="185"/>
+      <c r="G34" s="185"/>
+      <c r="H34" s="185"/>
+      <c r="I34" s="185"/>
+      <c r="J34" s="185"/>
+      <c r="K34" s="185"/>
+      <c r="L34" s="242"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="247">
+        <v>35</v>
+      </c>
+      <c r="B35" s="241"/>
+      <c r="C35" s="185"/>
+      <c r="D35" s="185"/>
+      <c r="E35" s="185"/>
+      <c r="F35" s="185"/>
+      <c r="G35" s="185"/>
+      <c r="H35" s="185"/>
+      <c r="I35" s="185"/>
+      <c r="J35" s="185"/>
+      <c r="K35" s="185"/>
+      <c r="L35" s="242"/>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="247">
+        <v>36</v>
+      </c>
+      <c r="B36" s="241"/>
+      <c r="C36" s="185"/>
+      <c r="D36" s="185"/>
+      <c r="E36" s="185"/>
+      <c r="F36" s="185"/>
+      <c r="G36" s="185"/>
+      <c r="H36" s="185"/>
+      <c r="I36" s="185"/>
+      <c r="J36" s="185"/>
+      <c r="K36" s="185"/>
+      <c r="L36" s="242"/>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="247">
+        <v>37</v>
+      </c>
+      <c r="B37" s="241"/>
+      <c r="C37" s="185"/>
+      <c r="D37" s="185"/>
+      <c r="E37" s="185"/>
+      <c r="F37" s="185"/>
+      <c r="G37" s="185"/>
+      <c r="H37" s="185"/>
+      <c r="I37" s="185"/>
+      <c r="J37" s="185"/>
+      <c r="K37" s="185"/>
+      <c r="L37" s="242"/>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="247">
+        <v>38</v>
+      </c>
+      <c r="B38" s="241"/>
+      <c r="C38" s="185"/>
+      <c r="D38" s="185"/>
+      <c r="E38" s="185"/>
+      <c r="F38" s="185"/>
+      <c r="G38" s="185"/>
+      <c r="H38" s="185"/>
+      <c r="I38" s="185"/>
+      <c r="J38" s="185"/>
+      <c r="K38" s="185"/>
+      <c r="L38" s="242"/>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="247">
+        <v>39</v>
+      </c>
+      <c r="B39" s="241"/>
+      <c r="C39" s="185"/>
+      <c r="D39" s="185"/>
+      <c r="E39" s="185"/>
+      <c r="F39" s="185"/>
+      <c r="G39" s="185"/>
+      <c r="H39" s="185"/>
+      <c r="I39" s="185"/>
+      <c r="J39" s="185"/>
+      <c r="K39" s="185"/>
+      <c r="L39" s="242"/>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="247">
+        <v>40</v>
+      </c>
+      <c r="B40" s="241"/>
+      <c r="C40" s="185"/>
+      <c r="D40" s="185"/>
+      <c r="E40" s="185"/>
+      <c r="F40" s="185"/>
+      <c r="G40" s="185"/>
+      <c r="H40" s="185"/>
+      <c r="I40" s="185"/>
+      <c r="J40" s="185"/>
+      <c r="K40" s="185"/>
+      <c r="L40" s="242"/>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="247">
+        <v>41</v>
+      </c>
+      <c r="B41" s="241"/>
+      <c r="C41" s="185"/>
+      <c r="D41" s="185"/>
+      <c r="E41" s="185"/>
+      <c r="F41" s="185"/>
+      <c r="G41" s="185"/>
+      <c r="H41" s="185"/>
+      <c r="I41" s="185"/>
+      <c r="J41" s="185"/>
+      <c r="K41" s="185"/>
+      <c r="L41" s="242"/>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="247">
+        <v>42</v>
+      </c>
+      <c r="B42" s="241"/>
+      <c r="C42" s="185"/>
+      <c r="D42" s="185"/>
+      <c r="E42" s="185"/>
+      <c r="F42" s="185"/>
+      <c r="G42" s="185"/>
+      <c r="H42" s="185"/>
+      <c r="I42" s="185"/>
+      <c r="J42" s="185"/>
+      <c r="K42" s="185"/>
+      <c r="L42" s="242"/>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="247">
+        <v>43</v>
+      </c>
+      <c r="B43" s="241"/>
+      <c r="C43" s="185"/>
+      <c r="D43" s="185"/>
+      <c r="E43" s="185"/>
+      <c r="F43" s="185"/>
+      <c r="G43" s="185"/>
+      <c r="H43" s="185"/>
+      <c r="I43" s="185"/>
+      <c r="J43" s="185"/>
+      <c r="K43" s="185"/>
+      <c r="L43" s="242"/>
+    </row>
+    <row r="44" spans="1:12" ht="16.5" thickBot="1">
+      <c r="A44" s="247">
+        <v>44</v>
+      </c>
+      <c r="B44" s="243"/>
+      <c r="C44" s="244"/>
+      <c r="D44" s="244"/>
+      <c r="E44" s="244"/>
+      <c r="F44" s="244"/>
+      <c r="G44" s="244"/>
+      <c r="H44" s="244"/>
+      <c r="I44" s="244"/>
+      <c r="J44" s="244"/>
+      <c r="K44" s="244"/>
+      <c r="L44" s="245"/>
+    </row>
+    <row r="45" spans="1:12" ht="16.5" thickTop="1">
+      <c r="A45" s="247">
+        <v>45</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" s="142" t="str">
+        <f>Barco!D65</f>
+        <v/>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="L45" s="112" t="str">
+        <f>Barco!M65</f>
+        <v>Eugene Mah</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="247">
+        <v>46</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D46" s="142" t="str">
+        <f>Barco!D66</f>
+        <v/>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="L46" s="112" t="str">
+        <f>Barco!M66</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="31">
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="J12:K12"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F25:I25 F27:I28" xr:uid="{CEAD9B4F-4A05-4883-9435-EBBC3722EE42}">
+      <formula1>$R$1:$R$3</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="90" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C29263F-D78E-4F41-860C-A3D9FC1D1372}">
   <dimension ref="A1:B46"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update QC manual version, add max illumination criteria check
Added monitor model so that max illumination criteria can be based on monitor model
</commit_message>
<xml_diff>
--- a/MUSCMammoMonitor.xlsx
+++ b/MUSCMammoMonitor.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EA8C08-EF7F-46D5-B9CB-145D66892A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA916DD7-E49E-40BF-A8DC-0931A4D97E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="211">
   <si>
     <t>Print Area</t>
   </si>
@@ -277,9 +277,6 @@
     <t>Criteria:</t>
   </si>
   <si>
-    <t>Ambient light measured at the surface of the monitor(s) must be less than 20 lux</t>
-  </si>
-  <si>
     <t>Previous:</t>
   </si>
   <si>
@@ -508,9 +505,6 @@
     <t>Piranha CB2-19020491</t>
   </si>
   <si>
-    <t>Ambient light illuminance measured at the surface of the monitor(s) must be less than 20 lux</t>
-  </si>
-  <si>
     <t>cd/m^2</t>
   </si>
   <si>
@@ -667,9 +661,6 @@
     <t>Page1,Page2</t>
   </si>
   <si>
-    <t>Barco K5905277 v16</t>
-  </si>
-  <si>
     <t>Barco Yearly Checks</t>
   </si>
   <si>
@@ -710,6 +701,42 @@
   </si>
   <si>
     <t>Line Pairs</t>
+  </si>
+  <si>
+    <t>Barco K5905277 v18</t>
+  </si>
+  <si>
+    <t>Monitor model:</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Max ambient illumination</t>
+  </si>
+  <si>
+    <t>Monitor model</t>
+  </si>
+  <si>
+    <t>Max illumination (lux)</t>
+  </si>
+  <si>
+    <t>MDMC-12133</t>
+  </si>
+  <si>
+    <t>MDMC-32133</t>
+  </si>
+  <si>
+    <t>MDMG-5221</t>
+  </si>
+  <si>
+    <t>MDMNC-12130</t>
+  </si>
+  <si>
+    <t>MDNC-6121</t>
+  </si>
+  <si>
+    <t>MDNG-6221</t>
   </si>
 </sst>
 </file>
@@ -927,7 +954,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="61">
+  <borders count="64">
     <border>
       <left/>
       <right/>
@@ -1674,6 +1701,45 @@
         <color auto="1"/>
       </right>
       <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -1696,7 +1762,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="225">
+  <cellXfs count="229">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2246,6 +2312,75 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2279,92 +2414,35 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -2377,7 +2455,157 @@
     <cellStyle name="Result" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Result2" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2877,8 +3105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P52" activeCellId="4" sqref="P7:P8 X21:X22 P34 P44 P52"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D42" activeCellId="1" sqref="D34 D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -2908,7 +3136,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
       <c r="O1" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
@@ -2923,12 +3151,12 @@
       <c r="AA1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="AG1" s="211" t="s">
+      <c r="AG1" s="188" t="s">
         <v>1</v>
       </c>
-      <c r="AH1" s="211"/>
-      <c r="AI1" s="211"/>
-      <c r="AJ1" s="211"/>
+      <c r="AH1" s="188"/>
+      <c r="AI1" s="188"/>
+      <c r="AJ1" s="188"/>
     </row>
     <row r="2" spans="1:36" ht="14.4" customHeight="1">
       <c r="A2" s="1">
@@ -2945,16 +3173,16 @@
       </c>
       <c r="Y2" s="13"/>
       <c r="AA2" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="AG2" s="212" t="s">
+        <v>184</v>
+      </c>
+      <c r="AG2" s="189" t="s">
         <v>3</v>
       </c>
-      <c r="AH2" s="212"/>
-      <c r="AI2" s="213" t="s">
+      <c r="AH2" s="189"/>
+      <c r="AI2" s="190" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="213"/>
+      <c r="AJ2" s="190"/>
     </row>
     <row r="3" spans="1:36" ht="14.4" customHeight="1">
       <c r="A3" s="1">
@@ -3001,7 +3229,7 @@
         <v>8</v>
       </c>
       <c r="AB4" s="21" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="AF4" s="20" t="s">
         <v>9</v>
@@ -3145,7 +3373,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="14.4" customHeight="1">
+    <row r="8" spans="1:36" ht="14.4" customHeight="1" thickBot="1">
       <c r="A8" s="1">
         <v>8</v>
       </c>
@@ -3179,7 +3407,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="14.4" customHeight="1">
+    <row r="9" spans="1:36" ht="14.4" customHeight="1" thickTop="1">
       <c r="A9" s="1">
         <v>9</v>
       </c>
@@ -3227,7 +3455,10 @@
         <v>Eugene Mah</v>
       </c>
       <c r="AF9"/>
-      <c r="AG9"/>
+      <c r="AG9" s="226" t="s">
+        <v>202</v>
+      </c>
+      <c r="AH9" s="227"/>
     </row>
     <row r="10" spans="1:36" ht="14.4" customHeight="1">
       <c r="A10" s="1">
@@ -3237,19 +3468,19 @@
       <c r="D10" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="214" t="str">
+      <c r="E10" s="191" t="str">
         <f t="shared" ref="E10:E15" si="1">IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="F10" s="214"/>
+      <c r="F10" s="191"/>
       <c r="I10" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="214" t="str">
+      <c r="J10" s="191" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="K10" s="214"/>
+      <c r="K10" s="191"/>
       <c r="M10" s="11"/>
       <c r="O10" s="12"/>
       <c r="Q10" s="20" t="s">
@@ -3282,7 +3513,12 @@
         <v/>
       </c>
       <c r="AF10"/>
-      <c r="AG10"/>
+      <c r="AG10" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="AH10" s="225" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="11" spans="1:36" ht="14.4" customHeight="1">
       <c r="A11" s="1">
@@ -3292,19 +3528,19 @@
       <c r="D11" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="208" t="str">
+      <c r="E11" s="192" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F11" s="208"/>
+      <c r="F11" s="192"/>
       <c r="I11" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="221" t="str">
+      <c r="J11" s="193" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="K11" s="221"/>
+      <c r="K11" s="193"/>
       <c r="M11" s="11"/>
       <c r="O11" s="12"/>
       <c r="Q11" s="20" t="s">
@@ -3337,7 +3573,12 @@
         <v/>
       </c>
       <c r="AF11"/>
-      <c r="AG11"/>
+      <c r="AG11" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="AH11" s="16">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="1:36" ht="14.4" customHeight="1">
       <c r="A12" s="1">
@@ -3347,19 +3588,19 @@
       <c r="D12" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="208" t="str">
+      <c r="E12" s="192" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F12" s="208"/>
+      <c r="F12" s="192"/>
       <c r="I12" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="208" t="str">
+      <c r="J12" s="192" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="K12" s="208"/>
+      <c r="K12" s="192"/>
       <c r="M12" s="11"/>
       <c r="O12" s="12"/>
       <c r="Q12" s="20" t="s">
@@ -3392,7 +3633,12 @@
         <v/>
       </c>
       <c r="AF12"/>
-      <c r="AG12"/>
+      <c r="AG12" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="AH12" s="16">
+        <v>40</v>
+      </c>
     </row>
     <row r="13" spans="1:36" ht="14.4" customHeight="1">
       <c r="A13" s="1">
@@ -3402,19 +3648,19 @@
       <c r="D13" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="208" t="str">
+      <c r="E13" s="192" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F13" s="208"/>
+      <c r="F13" s="192"/>
       <c r="I13" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="J13" s="208" t="str">
+        <v>200</v>
+      </c>
+      <c r="J13" s="192" t="str">
         <f>IF(V13="","",V13)</f>
         <v/>
       </c>
-      <c r="K13" s="208"/>
+      <c r="K13" s="192"/>
       <c r="M13" s="11"/>
       <c r="O13" s="12"/>
       <c r="Q13" s="20" t="s">
@@ -3426,13 +3672,13 @@
       </c>
       <c r="S13" s="51"/>
       <c r="U13" s="20" t="s">
-        <v>38</v>
+        <v>200</v>
       </c>
       <c r="V13" s="55" t="str">
         <f>IF(W13&lt;&gt;"",W13,IF(AB19="","",AB19))</f>
         <v/>
       </c>
-      <c r="W13" s="51"/>
+      <c r="W13" s="32"/>
       <c r="Y13" s="13"/>
       <c r="AA13" s="20" t="s">
         <v>37</v>
@@ -3447,7 +3693,12 @@
         <v/>
       </c>
       <c r="AF13"/>
-      <c r="AG13"/>
+      <c r="AG13" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="AH13" s="16">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:36" ht="14.4" customHeight="1">
       <c r="A14" s="1">
@@ -3457,19 +3708,19 @@
       <c r="D14" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="208" t="str">
+      <c r="E14" s="192" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F14" s="208"/>
+      <c r="F14" s="192"/>
       <c r="I14" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="J14" s="208" t="str">
+        <v>38</v>
+      </c>
+      <c r="J14" s="192">
         <f>IF(V14="","",V14)</f>
-        <v/>
-      </c>
-      <c r="K14" s="208"/>
+        <v>2590411503</v>
+      </c>
+      <c r="K14" s="192"/>
       <c r="M14" s="11"/>
       <c r="O14" s="12"/>
       <c r="Q14" s="20" t="s">
@@ -3481,11 +3732,11 @@
       </c>
       <c r="S14" s="51"/>
       <c r="U14" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="V14" s="55" t="str">
+        <v>38</v>
+      </c>
+      <c r="V14" s="55">
         <f>IF(W14&lt;&gt;"",W14,IF(AB20="","",AB20))</f>
-        <v/>
+        <v>2590411503</v>
       </c>
       <c r="W14" s="51"/>
       <c r="Y14" s="13"/>
@@ -3502,7 +3753,12 @@
         <v/>
       </c>
       <c r="AF14"/>
-      <c r="AG14"/>
+      <c r="AG14" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="AH14" s="16">
+        <v>40</v>
+      </c>
     </row>
     <row r="15" spans="1:36" ht="14.4" customHeight="1" thickBot="1">
       <c r="A15" s="1">
@@ -3512,11 +3768,19 @@
       <c r="D15" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="208" t="str">
+      <c r="E15" s="192" t="str">
         <f t="shared" si="1"/>
-        <v>Barco K5905277 v16</v>
-      </c>
-      <c r="F15" s="208"/>
+        <v>Barco K5905277 v18</v>
+      </c>
+      <c r="F15" s="192"/>
+      <c r="I15" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" s="192" t="str">
+        <f>IF(V15="","",V15)</f>
+        <v/>
+      </c>
+      <c r="K15" s="192"/>
       <c r="M15" s="11"/>
       <c r="O15" s="25"/>
       <c r="P15" s="26"/>
@@ -3525,15 +3789,20 @@
       </c>
       <c r="R15" s="57" t="str">
         <f t="shared" si="2"/>
-        <v>Barco K5905277 v16</v>
+        <v>Barco K5905277 v18</v>
       </c>
       <c r="S15" s="58" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="T15" s="26"/>
-      <c r="U15" s="26"/>
-      <c r="V15" s="26"/>
-      <c r="W15" s="26"/>
+      <c r="U15" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="V15" s="224" t="str">
+        <f>IF(W15&lt;&gt;"",W15,IF(AB21="","",AB21))</f>
+        <v/>
+      </c>
+      <c r="W15" s="58"/>
       <c r="X15" s="26"/>
       <c r="Y15" s="27"/>
       <c r="AA15" s="20" t="s">
@@ -3546,10 +3815,15 @@
       </c>
       <c r="AD15" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>Barco K5905277 v16</v>
+        <v>Barco K5905277 v18</v>
       </c>
       <c r="AF15"/>
-      <c r="AG15"/>
+      <c r="AG15" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="AH15" s="16">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:36" ht="14.4" customHeight="1" thickBot="1">
       <c r="A16" s="1">
@@ -3580,7 +3854,12 @@
         <v/>
       </c>
       <c r="AF16"/>
-      <c r="AG16"/>
+      <c r="AG16" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="AH16" s="38">
+        <v>20</v>
+      </c>
     </row>
     <row r="17" spans="1:33" ht="14.4" customHeight="1" thickTop="1" thickBot="1">
       <c r="A17" s="1">
@@ -3660,25 +3939,25 @@
       <c r="H19" s="136"/>
       <c r="I19" s="136"/>
       <c r="J19" s="136"/>
-      <c r="K19" s="210" t="s">
-        <v>128</v>
-      </c>
-      <c r="L19" s="210"/>
+      <c r="K19" s="195" t="s">
+        <v>127</v>
+      </c>
+      <c r="L19" s="195"/>
       <c r="M19" s="4"/>
       <c r="O19" s="12"/>
       <c r="R19" s="1" t="s">
         <v>44</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Y19" s="13"/>
       <c r="AA19" s="20" t="s">
-        <v>38</v>
+        <v>200</v>
       </c>
       <c r="AB19" s="33"/>
       <c r="AC19" s="34" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(AB19&lt;&gt;AD19,"Change","")</f>
         <v/>
       </c>
       <c r="AD19" s="35" t="str">
@@ -3694,7 +3973,7 @@
       </c>
       <c r="B20" s="9"/>
       <c r="D20" s="48" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E20" s="49" t="str">
         <f>IF(O20="","",IF(O20=1,"YES",IF(O20=2,"NO",IF(O20=3,"NA",""))))</f>
@@ -3709,7 +3988,7 @@
         <v/>
       </c>
       <c r="K20" s="48" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L20" s="77" t="str">
         <f>IF(W20="","",W20)</f>
@@ -3722,27 +4001,29 @@
       </c>
       <c r="R20" s="66"/>
       <c r="V20" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W20" s="131" t="str">
         <f>IF(X20&lt;&gt;"",X20,IF(AB23="","",AB23))</f>
         <v>Piranha CB2-19020491</v>
       </c>
       <c r="X20" s="132" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Y20" s="13"/>
       <c r="AA20" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB20" s="61"/>
+        <v>38</v>
+      </c>
+      <c r="AB20" s="33">
+        <v>2590411503</v>
+      </c>
       <c r="AC20" s="34" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="AD20" s="35" t="str">
+        <f>IF(AB20&lt;&gt;AD20,"Change","")</f>
+        <v/>
+      </c>
+      <c r="AD20" s="35">
         <f>IF(V14="","",V14)</f>
-        <v/>
+        <v>2590411503</v>
       </c>
       <c r="AF20"/>
       <c r="AG20"/>
@@ -3753,7 +4034,7 @@
       </c>
       <c r="B21" s="9"/>
       <c r="D21" s="48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E21" s="52" t="str">
         <f>IF(O21="","",IF(O21=1,"YES",IF(O21=2,"NO",IF(O21=3,"NA",""))))</f>
@@ -3768,9 +4049,9 @@
         <v/>
       </c>
       <c r="K21" s="48" t="s">
-        <v>127</v>
-      </c>
-      <c r="L21" s="220">
+        <v>126</v>
+      </c>
+      <c r="L21" s="185">
         <f t="shared" ref="L21:L22" si="5">IF(W21="","",W21)</f>
         <v>45089</v>
       </c>
@@ -3781,19 +4062,30 @@
       </c>
       <c r="R21" s="66"/>
       <c r="V21" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="W21" s="135">
         <f t="shared" ref="W21:W22" si="6">IF(X21&lt;&gt;"",X21,IF(AB24="","",AB24))</f>
         <v>45089</v>
       </c>
-      <c r="X21" s="224">
+      <c r="X21" s="187">
         <v>45089</v>
       </c>
       <c r="Y21" s="13"/>
-      <c r="AB21" s="19"/>
-      <c r="AC21" s="19"/>
-      <c r="AD21" s="19"/>
+      <c r="AA21" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB21" s="61" t="s">
+        <v>201</v>
+      </c>
+      <c r="AC21" s="34" t="str">
+        <f>IF(AB21&lt;&gt;AD21,"Change","")</f>
+        <v/>
+      </c>
+      <c r="AD21" s="35" t="str">
+        <f>IF(V15="","",V15)</f>
+        <v/>
+      </c>
       <c r="AF21"/>
       <c r="AG21"/>
     </row>
@@ -3803,7 +4095,7 @@
       </c>
       <c r="B22" s="9"/>
       <c r="D22" s="48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E22" s="52" t="str">
         <f>IF(O22="","",IF(O22=1,"YES",IF(O22=2,"NO",IF(O22=3,"NA",""))))</f>
@@ -3818,9 +4110,9 @@
         <v/>
       </c>
       <c r="K22" s="48" t="s">
-        <v>126</v>
-      </c>
-      <c r="L22" s="220">
+        <v>125</v>
+      </c>
+      <c r="L22" s="185">
         <f t="shared" si="5"/>
         <v>45820</v>
       </c>
@@ -3831,18 +4123,18 @@
       </c>
       <c r="R22" s="66"/>
       <c r="V22" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="W22" s="135">
         <f t="shared" si="6"/>
         <v>45820</v>
       </c>
-      <c r="X22" s="224">
+      <c r="X22" s="187">
         <v>45820</v>
       </c>
       <c r="Y22" s="13"/>
       <c r="AA22" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AF22"/>
       <c r="AG22"/>
@@ -3853,7 +4145,7 @@
       </c>
       <c r="B23" s="9"/>
       <c r="D23" s="48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E23" s="52" t="str">
         <f>IF(O23="","",IF(O23=1,"YES",IF(O23=2,"NO",IF(O23=3,"NA",""))))</f>
@@ -3875,7 +4167,7 @@
       <c r="R23" s="66"/>
       <c r="Y23" s="13"/>
       <c r="AA23" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AB23" s="33"/>
       <c r="AC23" s="34" t="str">
@@ -3895,18 +4187,18 @@
       </c>
       <c r="B24" s="9"/>
       <c r="D24" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="E24" s="209" t="str">
+        <v>83</v>
+      </c>
+      <c r="E24" s="194" t="str">
         <f>IF(P52="","",P52)</f>
         <v/>
       </c>
-      <c r="F24" s="209"/>
+      <c r="F24" s="194"/>
       <c r="M24" s="11"/>
       <c r="O24" s="12"/>
       <c r="Y24" s="13"/>
       <c r="AA24" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AB24" s="134"/>
       <c r="AC24" s="34" t="str">
@@ -3937,7 +4229,7 @@
       </c>
       <c r="Y25" s="13"/>
       <c r="AA25" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AB25" s="134"/>
       <c r="AC25" s="34" t="str">
@@ -3961,21 +4253,21 @@
       </c>
       <c r="M26" s="11"/>
       <c r="O26" s="73" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="P26" s="74"/>
       <c r="Q26" s="1" t="s">
         <v>54</v>
       </c>
       <c r="S26" s="20" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="T26" s="161" t="str">
         <f>IF(Sheet1!B4="","",Sheet1!B4)</f>
         <v/>
       </c>
       <c r="U26" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="Y26" s="13"/>
       <c r="AF26"/>
@@ -3987,7 +4279,7 @@
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="48" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D27" s="49" t="str">
         <f>IF(P26="","",P26)</f>
@@ -3999,12 +4291,13 @@
       <c r="G27" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>57</v>
+      <c r="H27" s="1" t="str">
+        <f>Q28</f>
+        <v>Ambient light illuminance measured at the surface of the monitor(s) is less than __ lux</v>
       </c>
       <c r="M27" s="11"/>
       <c r="O27" s="73" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P27" s="76" t="str">
         <f>IF(AB27="","",AB27)</f>
@@ -4014,18 +4307,18 @@
         <v>54</v>
       </c>
       <c r="S27" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="T27" s="76" t="str">
         <f>IF(AB28="","",AB28)</f>
         <v/>
       </c>
       <c r="U27" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="Y27" s="13"/>
       <c r="AA27" s="20" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AB27" s="33"/>
       <c r="AC27" s="34" t="str">
@@ -4045,26 +4338,27 @@
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="48" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D28" s="128" t="str">
         <f>IF(T26="","",T26)</f>
         <v/>
       </c>
       <c r="E28" s="75" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M28" s="11"/>
       <c r="O28" s="12"/>
       <c r="P28" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="Q28" s="1" t="s">
-        <v>134</v>
+      <c r="Q28" s="1" t="str">
+        <f>"Ambient light illuminance measured at the surface of the monitor(s) is less than "&amp;IF(V13="","__",VLOOKUP(V13,AG10:AH16,2))&amp;" lux"</f>
+        <v>Ambient light illuminance measured at the surface of the monitor(s) is less than __ lux</v>
       </c>
       <c r="Y28" s="13"/>
       <c r="AA28" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="AB28" s="33"/>
       <c r="AC28" s="34" t="str">
@@ -4084,7 +4378,7 @@
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D29" s="77" t="str">
         <f>IF(Q29="","",IF(LEN(Q29)&lt;=135,Q29,IF(LEN(Q29)&lt;=260,LEFT(Q29,SEARCH(" ",Q29,125)),LEFT(Q29,SEARCH(" ",Q29,130)))))</f>
@@ -4101,7 +4395,7 @@
       <c r="M29" s="11"/>
       <c r="O29" s="12"/>
       <c r="P29" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q29" s="78" t="str">
         <f>IF(Q31&lt;&gt;"",Q31,IF(AB56="","",AB56))</f>
@@ -4148,7 +4442,7 @@
       <c r="M30" s="11"/>
       <c r="O30" s="12"/>
       <c r="P30" s="80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q30" s="112"/>
       <c r="R30" s="81">
@@ -4197,7 +4491,7 @@
       <c r="M31" s="11"/>
       <c r="O31" s="12"/>
       <c r="P31" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q31" s="66"/>
       <c r="R31" s="67"/>
@@ -4209,7 +4503,7 @@
       <c r="X31" s="67"/>
       <c r="Y31" s="13"/>
       <c r="AA31" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AB31" s="33"/>
       <c r="AC31" s="34" t="str">
@@ -4232,7 +4526,7 @@
       <c r="O32" s="12"/>
       <c r="Y32" s="13"/>
       <c r="AA32" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AB32" s="33"/>
       <c r="AC32" s="34" t="str">
@@ -4252,21 +4546,21 @@
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="72" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M33" s="11"/>
       <c r="O33" s="69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U33" s="20" t="s">
         <v>52</v>
       </c>
       <c r="V33" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Y33" s="13"/>
       <c r="AA33" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AB33" s="33"/>
       <c r="AC33" s="34" t="str">
@@ -4288,19 +4582,19 @@
       <c r="C34" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="D34" s="222" t="str">
+      <c r="D34" s="228" t="str">
         <f>IF(P34="","",P34)</f>
         <v/>
       </c>
       <c r="E34" s="142"/>
       <c r="F34" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="G34" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="G34" s="75" t="s">
+      <c r="H34" s="82" t="s">
         <v>71</v>
-      </c>
-      <c r="H34" s="82" t="s">
-        <v>72</v>
       </c>
       <c r="I34" s="83"/>
       <c r="J34" s="83"/>
@@ -4317,11 +4611,11 @@
       </c>
       <c r="S34" s="19" t="str">
         <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
-        <v>Right ()</v>
+        <v>Right (1503)</v>
       </c>
       <c r="Y34" s="13"/>
       <c r="AA34" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="AB34" s="33"/>
       <c r="AC34" s="34" t="str">
@@ -4365,13 +4659,13 @@
       <c r="M35" s="11"/>
       <c r="O35" s="12"/>
       <c r="Q35" s="86" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R35" s="129"/>
       <c r="S35" s="129"/>
       <c r="Y35" s="13"/>
       <c r="AA35" s="20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AB35" s="33"/>
       <c r="AC35" s="34" t="str">
@@ -4394,7 +4688,7 @@
       <c r="D36" s="83"/>
       <c r="E36" s="48" t="str">
         <f>S34</f>
-        <v>Right ()</v>
+        <v>Right (1503)</v>
       </c>
       <c r="F36" s="84" t="str">
         <f>IF(S35="","",S35)</f>
@@ -4415,13 +4709,13 @@
       <c r="M36" s="11"/>
       <c r="O36" s="12"/>
       <c r="Q36" s="87" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R36" s="130"/>
       <c r="S36" s="130"/>
       <c r="Y36" s="13"/>
       <c r="AA36" s="20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AB36" s="33"/>
       <c r="AC36" s="34" t="str">
@@ -4441,7 +4735,7 @@
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D37" s="77" t="str">
         <f>IF(Q39="","",IF(LEN(Q39)&lt;=135,Q39,IF(LEN(Q39)&lt;=260,LEFT(Q39,SEARCH(" ",Q39,125)),LEFT(Q39,SEARCH(" ",Q39,130)))))</f>
@@ -4458,7 +4752,7 @@
       <c r="M37" s="11"/>
       <c r="O37" s="12"/>
       <c r="Q37" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R37" s="88" t="str">
         <f>IF(OR(R35="",R36=""),"",R36/R35)</f>
@@ -4470,7 +4764,7 @@
       </c>
       <c r="Y37" s="13"/>
       <c r="AA37" s="20" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AB37" s="33"/>
       <c r="AC37" s="34" t="str">
@@ -4506,7 +4800,7 @@
       <c r="O38" s="12"/>
       <c r="Y38" s="13"/>
       <c r="AA38" s="20" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AB38" s="33"/>
       <c r="AC38" s="34" t="str">
@@ -4541,7 +4835,7 @@
       <c r="M39" s="11"/>
       <c r="O39" s="12"/>
       <c r="P39" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q39" s="78" t="str">
         <f>IF(Q41&lt;&gt;"",Q41,IF(AB57="","",AB57))</f>
@@ -4576,7 +4870,7 @@
       <c r="M40" s="11"/>
       <c r="O40" s="12"/>
       <c r="P40" s="80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q40" s="112"/>
       <c r="R40" s="81">
@@ -4616,7 +4910,7 @@
       <c r="M41" s="11"/>
       <c r="O41" s="12"/>
       <c r="P41" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q41" s="66"/>
       <c r="R41" s="67"/>
@@ -4628,7 +4922,7 @@
       <c r="X41" s="67"/>
       <c r="Y41" s="13"/>
       <c r="AA41" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB41" s="70"/>
       <c r="AC41" s="34" t="str">
@@ -4650,7 +4944,7 @@
       <c r="C42" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="D42" s="222" t="str">
+      <c r="D42" s="228" t="str">
         <f>IF(P44="","",P44)</f>
         <v/>
       </c>
@@ -4661,13 +4955,13 @@
       </c>
       <c r="G42" s="141" t="str">
         <f>S45</f>
-        <v>Right ()</v>
+        <v>Right (1503)</v>
       </c>
       <c r="M42" s="11"/>
       <c r="O42" s="12"/>
       <c r="Y42" s="13"/>
       <c r="AA42" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AB42" s="70"/>
       <c r="AC42" s="34" t="str">
@@ -4687,7 +4981,7 @@
       </c>
       <c r="B43" s="9"/>
       <c r="E43" s="48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F43" s="90" t="str">
         <f>IF(R46="","",IF(R46=1,"YES",IF(R46=2,"NO",IF(R46=3,"NA",""))))</f>
@@ -4705,11 +4999,11 @@
         <v>52</v>
       </c>
       <c r="V43" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Y43" s="13"/>
       <c r="AA43" s="20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="AB43" s="70"/>
       <c r="AC43" s="34" t="str">
@@ -4729,7 +5023,7 @@
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D44" s="77" t="str">
         <f>IF(Q47="","",IF(LEN(Q47)&lt;=135,Q47,IF(LEN(Q47)&lt;=260,LEFT(Q47,SEARCH(" ",Q47,125)),LEFT(Q47,SEARCH(" ",Q47,130)))))</f>
@@ -4749,11 +5043,11 @@
       </c>
       <c r="P44" s="54"/>
       <c r="V44" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Y44" s="13"/>
       <c r="AA44" s="20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AB44" s="70"/>
       <c r="AC44" s="34" t="str">
@@ -4795,11 +5089,11 @@
       </c>
       <c r="S45" s="19" t="str">
         <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
-        <v>Right ()</v>
+        <v>Right (1503)</v>
       </c>
       <c r="Y45" s="13"/>
       <c r="AA45" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AB45" s="70"/>
       <c r="AC45" s="34" t="str">
@@ -4834,13 +5128,13 @@
       <c r="M46" s="11"/>
       <c r="O46" s="12"/>
       <c r="Q46" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R46" s="93"/>
       <c r="S46" s="93"/>
       <c r="Y46" s="13"/>
       <c r="AA46" s="20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AB46" s="70"/>
       <c r="AC46" s="34" t="str">
@@ -4862,7 +5156,7 @@
       <c r="M47" s="11"/>
       <c r="O47" s="12"/>
       <c r="P47" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q47" s="78" t="str">
         <f>IF(Q49&lt;&gt;"",Q49,IF(AB58="","",AB58))</f>
@@ -4875,7 +5169,7 @@
       <c r="X47" s="64"/>
       <c r="Y47" s="13"/>
       <c r="AA47" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AB47" s="19"/>
       <c r="AC47" s="19"/>
@@ -4889,12 +5183,12 @@
       </c>
       <c r="B48" s="9"/>
       <c r="C48" s="72" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M48" s="11"/>
       <c r="O48" s="12"/>
       <c r="P48" s="80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q48" s="112"/>
       <c r="R48" s="81">
@@ -4909,7 +5203,7 @@
       <c r="X48" s="67"/>
       <c r="Y48" s="13"/>
       <c r="AA48" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AB48" s="137"/>
       <c r="AC48" s="34" t="str">
@@ -4929,7 +5223,7 @@
       </c>
       <c r="B49" s="9"/>
       <c r="C49" s="94" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D49" s="83"/>
       <c r="E49" s="83"/>
@@ -4937,7 +5231,7 @@
       <c r="G49" s="83"/>
       <c r="H49" s="83"/>
       <c r="I49" s="94" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J49" s="83"/>
       <c r="K49" s="83"/>
@@ -4945,7 +5239,7 @@
       <c r="M49" s="11"/>
       <c r="O49" s="12"/>
       <c r="P49" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q49" s="66"/>
       <c r="R49" s="67"/>
@@ -4957,7 +5251,7 @@
       <c r="X49" s="67"/>
       <c r="Y49" s="13"/>
       <c r="AA49" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AB49" s="137"/>
       <c r="AC49" s="34" t="str">
@@ -4985,7 +5279,7 @@
         <v/>
       </c>
       <c r="F50" s="75" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G50" s="83"/>
       <c r="H50" s="83"/>
@@ -4998,13 +5292,13 @@
         <v/>
       </c>
       <c r="K50" s="75" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M50" s="11"/>
       <c r="O50" s="12"/>
       <c r="Y50" s="13"/>
       <c r="AA50" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB50" s="137"/>
       <c r="AC50" s="34" t="str">
@@ -5025,25 +5319,25 @@
       <c r="B51" s="9"/>
       <c r="D51" s="75" t="str">
         <f>R58</f>
-        <v>Right ()</v>
+        <v>Right (1503)</v>
       </c>
       <c r="E51" s="128" t="str">
         <f>IF(R59="","",R59)</f>
         <v/>
       </c>
       <c r="F51" s="75" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I51" s="75" t="str">
         <f>R58</f>
-        <v>Right ()</v>
+        <v>Right (1503)</v>
       </c>
       <c r="J51" s="157" t="str">
         <f>IF(R60="","",R60)</f>
         <v/>
       </c>
       <c r="K51" s="75" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M51" s="11"/>
       <c r="O51" s="69" t="s">
@@ -5053,11 +5347,11 @@
         <v>52</v>
       </c>
       <c r="V51" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Y51" s="13"/>
       <c r="AA51" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AB51" s="137"/>
       <c r="AC51" s="34" t="str">
@@ -5085,11 +5379,11 @@
       </c>
       <c r="P52" s="54"/>
       <c r="V52" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Y52" s="13"/>
       <c r="AA52" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AB52" s="137"/>
       <c r="AC52" s="34" t="str">
@@ -5114,14 +5408,14 @@
       </c>
       <c r="F53" s="83" t="str">
         <f>R58</f>
-        <v>Right ()</v>
+        <v>Right (1503)</v>
       </c>
       <c r="I53" s="48"/>
       <c r="J53" s="48"/>
       <c r="M53" s="11"/>
       <c r="O53" s="12"/>
       <c r="P53" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q53" s="78" t="str">
         <f>IF(Q55&lt;&gt;"",Q55,IF(AB59="","",AB59))</f>
@@ -5134,7 +5428,7 @@
       <c r="X53" s="64"/>
       <c r="Y53" s="13"/>
       <c r="AA53" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB53" s="137"/>
       <c r="AC53" s="34" t="str">
@@ -5154,7 +5448,7 @@
       </c>
       <c r="B54" s="9"/>
       <c r="D54" s="48" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E54" s="162" t="str">
         <f>IF(Q61="","",Q61)</f>
@@ -5167,7 +5461,7 @@
       <c r="M54" s="11"/>
       <c r="O54" s="12"/>
       <c r="P54" s="80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q54" s="112"/>
       <c r="R54" s="81">
@@ -5188,7 +5482,7 @@
       </c>
       <c r="B55" s="9"/>
       <c r="D55" s="48" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E55" s="164" t="str">
         <f>IF(Q62="","",Q62)</f>
@@ -5201,7 +5495,7 @@
       <c r="M55" s="11"/>
       <c r="O55" s="12"/>
       <c r="P55" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q55" s="66"/>
       <c r="R55" s="67"/>
@@ -5228,7 +5522,7 @@
       <c r="O56" s="12"/>
       <c r="Y56" s="13"/>
       <c r="AA56" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AB56" s="138"/>
       <c r="AC56" s="34" t="str">
@@ -5246,7 +5540,7 @@
       </c>
       <c r="B57" s="9"/>
       <c r="C57" s="48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D57" s="77" t="str">
         <f>IF(Q63="","",IF(LEN(Q63)&lt;=135,Q63,IF(LEN(Q63)&lt;=260,LEFT(Q63,SEARCH(" ",Q63,125)),LEFT(Q63,SEARCH(" ",Q63,130)))))</f>
@@ -5262,13 +5556,13 @@
       <c r="L57" s="77"/>
       <c r="M57" s="11"/>
       <c r="O57" s="69" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U57"/>
       <c r="V57"/>
       <c r="Y57" s="13"/>
       <c r="AA57" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AB57" s="138"/>
       <c r="AC57" s="34" t="str">
@@ -5300,7 +5594,7 @@
       <c r="L58" s="79"/>
       <c r="M58" s="11"/>
       <c r="O58" s="97" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Q58" s="19" t="str">
         <f>"Left ("&amp;RIGHT($V$13,4)&amp;")"</f>
@@ -5308,10 +5602,10 @@
       </c>
       <c r="R58" s="19" t="str">
         <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
-        <v>Right ()</v>
+        <v>Right (1503)</v>
       </c>
       <c r="T58" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="U58" s="19" t="str">
         <f>"Left ("&amp;RIGHT($V$13,4)&amp;")"</f>
@@ -5319,11 +5613,11 @@
       </c>
       <c r="V58" s="19" t="str">
         <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
-        <v>Right ()</v>
+        <v>Right (1503)</v>
       </c>
       <c r="Y58" s="13"/>
       <c r="AA58" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AB58" s="138"/>
       <c r="AC58" s="34" t="str">
@@ -5356,7 +5650,7 @@
       <c r="M59" s="11"/>
       <c r="O59" s="12"/>
       <c r="P59" s="20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="Q59" s="117" t="str">
         <f>IF(Sheet1!B5="","",Sheet1!B5+Lamb)</f>
@@ -5367,7 +5661,7 @@
         <v/>
       </c>
       <c r="T59" s="150" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="U59" s="166" t="str">
         <f>IF(AB31="","",AB31)</f>
@@ -5379,7 +5673,7 @@
       </c>
       <c r="Y59" s="13"/>
       <c r="AA59" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AB59" s="138"/>
       <c r="AC59" s="34" t="str">
@@ -5399,7 +5693,7 @@
       <c r="M60" s="11"/>
       <c r="O60" s="12"/>
       <c r="P60" s="20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="Q60" s="151" t="str">
         <f>IF(Sheet1!B7="","",Sheet1!B7+Lamb)</f>
@@ -5410,7 +5704,7 @@
         <v/>
       </c>
       <c r="T60" s="150" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="U60" s="168" t="str">
         <f>IF(AB33="","",AB33)</f>
@@ -5422,7 +5716,7 @@
       </c>
       <c r="Y60" s="13"/>
       <c r="AA60" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AB60" s="138"/>
       <c r="AC60" s="34" t="str">
@@ -5442,7 +5736,7 @@
       <c r="M61" s="11"/>
       <c r="O61" s="12"/>
       <c r="P61" s="20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="Q61" s="151" t="str">
         <f>IF(Q59="","",Q60/Q59)</f>
@@ -5453,7 +5747,7 @@
         <v/>
       </c>
       <c r="T61" s="20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="U61" s="168" t="str">
         <f>IF(AB35="","",AB35)</f>
@@ -5465,7 +5759,7 @@
       </c>
       <c r="Y61" s="13"/>
       <c r="AA61" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AB61" s="138"/>
       <c r="AC61" s="34" t="str">
@@ -5485,7 +5779,7 @@
       <c r="M62" s="11"/>
       <c r="O62" s="12"/>
       <c r="P62" s="20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q62" s="154" t="str">
         <f>IF(OR(Q59="",Lamb=""),"",Lamb/Q59)</f>
@@ -5496,7 +5790,7 @@
         <v/>
       </c>
       <c r="T62" s="20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="U62" s="170" t="str">
         <f>IF(AB37="","",AB37)</f>
@@ -5508,7 +5802,7 @@
       </c>
       <c r="Y62" s="13"/>
       <c r="AA62" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AB62" s="138"/>
       <c r="AC62" s="34" t="str">
@@ -5528,7 +5822,7 @@
       <c r="M63" s="11"/>
       <c r="O63" s="12"/>
       <c r="P63" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q63" s="143" t="str">
         <f>IF(Q65&lt;&gt;"",Q65,IF(AB67="","",AB60))</f>
@@ -5562,7 +5856,7 @@
       <c r="M64" s="24"/>
       <c r="O64" s="12"/>
       <c r="P64" s="80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q64" s="112"/>
       <c r="R64" s="81">
@@ -5596,7 +5890,7 @@
       <c r="C65" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D65" s="223" t="str">
+      <c r="D65" s="186" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -5609,7 +5903,7 @@
       </c>
       <c r="O65" s="12"/>
       <c r="P65" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q65" s="66"/>
       <c r="R65" s="67"/>
@@ -5628,7 +5922,7 @@
         <v>66</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D66" s="99" t="str">
         <f>IF($E$14="","",$E$14)</f>
@@ -5662,13 +5956,13 @@
         <v>Medical University of South Carolina</v>
       </c>
       <c r="O67" s="97" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="U67" s="20" t="s">
         <v>52</v>
       </c>
       <c r="V67" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y67" s="13"/>
       <c r="AC67" s="19"/>
@@ -5691,7 +5985,7 @@
       </c>
       <c r="S68" s="19" t="str">
         <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
-        <v>Right ()</v>
+        <v>Right (1503)</v>
       </c>
       <c r="Y68" s="13"/>
       <c r="AB68" s="139"/>
@@ -5710,7 +6004,7 @@
       </c>
       <c r="O69" s="12"/>
       <c r="Q69" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R69" s="100"/>
       <c r="S69" s="101"/>
@@ -5724,7 +6018,7 @@
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="44" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
@@ -5738,7 +6032,7 @@
       <c r="M70" s="4"/>
       <c r="O70" s="12"/>
       <c r="Q70" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="R70" s="102"/>
       <c r="S70" s="103"/>
@@ -5759,23 +6053,23 @@
       </c>
       <c r="B71" s="9"/>
       <c r="C71" s="83"/>
-      <c r="D71" s="205" t="str">
+      <c r="D71" s="196" t="str">
         <f>Q86</f>
         <v>UNL-10 (cd/m^2)</v>
       </c>
-      <c r="E71" s="205"/>
-      <c r="F71" s="206" t="str">
+      <c r="E71" s="196"/>
+      <c r="F71" s="197" t="str">
         <f>S86</f>
         <v>UNL-80 (cd/m^2)</v>
       </c>
-      <c r="G71" s="206"/>
+      <c r="G71" s="197"/>
       <c r="I71" s="60" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M71" s="11"/>
       <c r="O71" s="12"/>
       <c r="Q71" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R71" s="104"/>
       <c r="S71" s="105"/>
@@ -5795,7 +6089,7 @@
       </c>
       <c r="E72" s="84" t="str">
         <f>R87</f>
-        <v>Right ()</v>
+        <v>Right (1503)</v>
       </c>
       <c r="F72" s="84" t="str">
         <f>S87</f>
@@ -5803,25 +6097,25 @@
       </c>
       <c r="G72" s="96" t="str">
         <f>T87</f>
-        <v>Right ()</v>
+        <v>Right (1503)</v>
       </c>
       <c r="I72" s="49" t="str">
         <f>IF(V87="","TBD",IF(V87=1,"YES",IF(V87=2,"NO",IF(V87=3,"NA",""))))</f>
         <v>TBD</v>
       </c>
       <c r="J72" s="83" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M72" s="11"/>
       <c r="O72" s="12"/>
       <c r="Q72" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R72" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="V72" s="19" t="s">
         <v>104</v>
-      </c>
-      <c r="V72" s="19" t="s">
-        <v>105</v>
       </c>
       <c r="W72" s="19"/>
       <c r="Y72" s="13"/>
@@ -5841,7 +6135,7 @@
       </c>
       <c r="B73" s="9"/>
       <c r="C73" s="48" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D73" s="106" t="str">
         <f t="shared" ref="D73:G76" si="13">IF(Q97="","",Q97)</f>
@@ -5864,20 +6158,20 @@
         <v>TBD</v>
       </c>
       <c r="J73" s="83" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M73" s="11"/>
       <c r="O73" s="12"/>
       <c r="Q73" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="R73" s="188"/>
-      <c r="S73" s="192"/>
-      <c r="V73" s="200" t="str">
+        <v>95</v>
+      </c>
+      <c r="R73" s="211"/>
+      <c r="S73" s="215"/>
+      <c r="V73" s="203" t="str">
         <f>IF(AB48="","",AB48)</f>
         <v/>
       </c>
-      <c r="W73" s="201" t="str">
+      <c r="W73" s="204" t="str">
         <f>IF(AB51="","",AB51)</f>
         <v/>
       </c>
@@ -5891,7 +6185,7 @@
       </c>
       <c r="B74" s="9"/>
       <c r="C74" s="48" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D74" s="106" t="str">
         <f t="shared" si="13"/>
@@ -5914,15 +6208,15 @@
         <v>TBD</v>
       </c>
       <c r="J74" s="83" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M74" s="11"/>
       <c r="O74" s="12"/>
       <c r="Q74" s="19"/>
-      <c r="R74" s="189"/>
-      <c r="S74" s="193"/>
-      <c r="V74" s="199"/>
-      <c r="W74" s="202"/>
+      <c r="R74" s="212"/>
+      <c r="S74" s="216"/>
+      <c r="V74" s="202"/>
+      <c r="W74" s="205"/>
       <c r="Y74" s="13"/>
       <c r="AB74" s="139"/>
       <c r="AC74" s="34" t="str">
@@ -5940,7 +6234,7 @@
       </c>
       <c r="B75" s="9"/>
       <c r="C75" s="48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D75" s="108" t="str">
         <f t="shared" si="13"/>
@@ -5961,15 +6255,15 @@
       <c r="M75" s="11"/>
       <c r="O75" s="12"/>
       <c r="Q75" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="R75" s="190"/>
-      <c r="S75" s="194"/>
-      <c r="V75" s="197" t="str">
+        <v>97</v>
+      </c>
+      <c r="R75" s="213"/>
+      <c r="S75" s="217"/>
+      <c r="V75" s="200" t="str">
         <f>IF(AB49="","",AB49)</f>
         <v/>
       </c>
-      <c r="W75" s="203" t="str">
+      <c r="W75" s="206" t="str">
         <f>IF(AB52="","",AB52)</f>
         <v/>
       </c>
@@ -5983,7 +6277,7 @@
       </c>
       <c r="B76" s="9"/>
       <c r="C76" s="48" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D76" s="108" t="str">
         <f t="shared" si="13"/>
@@ -6005,15 +6299,15 @@
         <v>56</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M76" s="11"/>
       <c r="O76" s="12"/>
       <c r="Q76" s="19"/>
-      <c r="R76" s="189"/>
-      <c r="S76" s="193"/>
-      <c r="V76" s="199"/>
-      <c r="W76" s="202"/>
+      <c r="R76" s="212"/>
+      <c r="S76" s="216"/>
+      <c r="V76" s="202"/>
+      <c r="W76" s="205"/>
       <c r="Y76" s="13"/>
       <c r="AB76" s="139"/>
       <c r="AC76" s="34" t="str">
@@ -6047,20 +6341,20 @@
         <v/>
       </c>
       <c r="J77" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="M77" s="11"/>
       <c r="O77" s="12"/>
       <c r="Q77" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="R77" s="190"/>
-      <c r="S77" s="194"/>
-      <c r="V77" s="197" t="str">
+        <v>100</v>
+      </c>
+      <c r="R77" s="213"/>
+      <c r="S77" s="217"/>
+      <c r="V77" s="200" t="str">
         <f>IF(AB50="","",AB50)</f>
         <v/>
       </c>
-      <c r="W77" s="203" t="str">
+      <c r="W77" s="206" t="str">
         <f>IF(AB53="","",AB53)</f>
         <v/>
       </c>
@@ -6076,10 +6370,10 @@
       <c r="M78" s="11"/>
       <c r="O78" s="12"/>
       <c r="Q78" s="19"/>
-      <c r="R78" s="191"/>
-      <c r="S78" s="195"/>
-      <c r="V78" s="198"/>
-      <c r="W78" s="204"/>
+      <c r="R78" s="214"/>
+      <c r="S78" s="218"/>
+      <c r="V78" s="201"/>
+      <c r="W78" s="207"/>
       <c r="Y78" s="13"/>
       <c r="AB78" s="139"/>
       <c r="AC78" s="34" t="str">
@@ -6097,7 +6391,7 @@
       </c>
       <c r="B79" s="9"/>
       <c r="C79" s="48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D79" s="77" t="str">
         <f>IF(Q101="","",IF(LEN(Q101)&lt;=135,Q101,IF(LEN(Q101)&lt;=260,LEFT(Q101,SEARCH(" ",Q101,125)),LEFT(Q101,SEARCH(" ",Q101,130)))))</f>
@@ -6117,7 +6411,7 @@
         <v>56</v>
       </c>
       <c r="R79" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Y79" s="13"/>
       <c r="AC79" s="19"/>
@@ -6175,7 +6469,7 @@
       <c r="M81" s="11"/>
       <c r="O81" s="12"/>
       <c r="P81" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q81" s="78" t="str">
         <f>IF(Q83&lt;&gt;"",Q83,IF(AB61="","",AB61))</f>
@@ -6198,7 +6492,7 @@
       <c r="M82" s="11"/>
       <c r="O82" s="12"/>
       <c r="P82" s="80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q82" s="112"/>
       <c r="R82" s="81">
@@ -6228,10 +6522,10 @@
       </c>
       <c r="B83" s="9"/>
       <c r="C83" s="94" t="s">
+        <v>92</v>
+      </c>
+      <c r="I83" s="75" t="s">
         <v>93</v>
-      </c>
-      <c r="I83" s="75" t="s">
-        <v>94</v>
       </c>
       <c r="J83" s="75"/>
       <c r="K83" s="75"/>
@@ -6239,7 +6533,7 @@
       <c r="M83" s="11"/>
       <c r="O83" s="12"/>
       <c r="P83" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q83" s="66"/>
       <c r="R83" s="67"/>
@@ -6264,18 +6558,18 @@
       </c>
       <c r="G84" s="141" t="str">
         <f>S68</f>
-        <v>Right ()</v>
-      </c>
-      <c r="I84" s="207" t="str">
+        <v>Right (1503)</v>
+      </c>
+      <c r="I84" s="198" t="str">
         <f>R68</f>
         <v>Left ()</v>
       </c>
-      <c r="J84" s="207"/>
-      <c r="K84" s="207" t="str">
+      <c r="J84" s="198"/>
+      <c r="K84" s="198" t="str">
         <f>S68</f>
-        <v>Right ()</v>
-      </c>
-      <c r="L84" s="207"/>
+        <v>Right (1503)</v>
+      </c>
+      <c r="L84" s="198"/>
       <c r="M84" s="11"/>
       <c r="O84" s="12"/>
       <c r="Y84" s="13"/>
@@ -6295,7 +6589,7 @@
       </c>
       <c r="B85" s="9"/>
       <c r="E85" s="48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F85" s="95" t="str">
         <f t="shared" ref="F85:G87" si="15">IF(R69="","",IF(R69=1,"YES",IF(R69=2,"NO",IF(R69=3,"NA",""))))</f>
@@ -6306,24 +6600,24 @@
         <v/>
       </c>
       <c r="H85" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="I85" s="196" t="str">
+        <v>95</v>
+      </c>
+      <c r="I85" s="199" t="str">
         <f>IF(R73="","",R73)</f>
         <v/>
       </c>
-      <c r="J85" s="196"/>
-      <c r="K85" s="196" t="str">
+      <c r="J85" s="199"/>
+      <c r="K85" s="199" t="str">
         <f>IF(S73="","",S73)</f>
         <v/>
       </c>
-      <c r="L85" s="196"/>
+      <c r="L85" s="199"/>
       <c r="M85" s="11"/>
       <c r="O85" s="97" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="V85" s="60" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Y85" s="13"/>
     </row>
@@ -6333,7 +6627,7 @@
       </c>
       <c r="B86" s="9"/>
       <c r="E86" s="48" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F86" s="95" t="str">
         <f t="shared" si="15"/>
@@ -6344,28 +6638,28 @@
         <v/>
       </c>
       <c r="H86" s="48" t="s">
-        <v>98</v>
-      </c>
-      <c r="I86" s="196" t="str">
+        <v>97</v>
+      </c>
+      <c r="I86" s="199" t="str">
         <f>IF(R75="","",R75)</f>
         <v/>
       </c>
-      <c r="J86" s="196"/>
-      <c r="K86" s="196" t="str">
+      <c r="J86" s="199"/>
+      <c r="K86" s="199" t="str">
         <f>IF(S75="","",S75)</f>
         <v/>
       </c>
-      <c r="L86" s="196"/>
+      <c r="L86" s="199"/>
       <c r="M86" s="11"/>
       <c r="O86" s="12"/>
-      <c r="Q86" s="186" t="s">
+      <c r="Q86" s="209" t="s">
+        <v>116</v>
+      </c>
+      <c r="R86" s="210"/>
+      <c r="S86" s="209" t="s">
         <v>117</v>
       </c>
-      <c r="R86" s="187"/>
-      <c r="S86" s="186" t="s">
-        <v>118</v>
-      </c>
-      <c r="T86" s="187"/>
+      <c r="T86" s="210"/>
       <c r="V86" s="113" t="s">
         <v>43</v>
       </c>
@@ -6377,7 +6671,7 @@
       </c>
       <c r="B87" s="9"/>
       <c r="E87" s="48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F87" s="90" t="str">
         <f t="shared" si="15"/>
@@ -6388,18 +6682,18 @@
         <v/>
       </c>
       <c r="H87" s="48" t="s">
-        <v>101</v>
-      </c>
-      <c r="I87" s="185" t="str">
+        <v>100</v>
+      </c>
+      <c r="I87" s="208" t="str">
         <f>IF(R77="","",R77)</f>
         <v/>
       </c>
-      <c r="J87" s="185"/>
-      <c r="K87" s="185" t="str">
+      <c r="J87" s="208"/>
+      <c r="K87" s="208" t="str">
         <f>IF(S77="","",S77)</f>
         <v/>
       </c>
-      <c r="L87" s="185"/>
+      <c r="L87" s="208"/>
       <c r="M87" s="11"/>
       <c r="O87" s="12"/>
       <c r="Q87" s="114" t="str">
@@ -6408,7 +6702,7 @@
       </c>
       <c r="R87" s="115" t="str">
         <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
-        <v>Right ()</v>
+        <v>Right (1503)</v>
       </c>
       <c r="S87" s="114" t="str">
         <f>"Left ("&amp;RIGHT($V$13,4)&amp;")"</f>
@@ -6416,18 +6710,18 @@
       </c>
       <c r="T87" s="115" t="str">
         <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
-        <v>Right ()</v>
+        <v>Right (1503)</v>
       </c>
       <c r="V87" s="116"/>
       <c r="W87" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Y87" s="13"/>
       <c r="AA87" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="AC87" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="88" spans="1:30" ht="14.4" customHeight="1">
@@ -6436,7 +6730,7 @@
       </c>
       <c r="B88" s="9"/>
       <c r="C88" s="48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D88" s="77" t="str">
         <f>IF(Q81="","",IF(LEN(Q81)&lt;=135,Q81,IF(LEN(Q81)&lt;=260,LEFT(Q81,SEARCH(" ",Q81,125)),LEFT(Q81,SEARCH(" ",Q81,130)))))</f>
@@ -6453,7 +6747,7 @@
       <c r="M88" s="11"/>
       <c r="O88" s="12"/>
       <c r="P88" s="20" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="Q88" s="117" t="str">
         <f>IF(Sheet1!B9="","",Sheet1!B9+Lamb)</f>
@@ -6473,7 +6767,7 @@
       </c>
       <c r="V88" s="116"/>
       <c r="W88" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y88" s="13"/>
       <c r="AA88" s="160" t="e">
@@ -6514,7 +6808,7 @@
       <c r="M89" s="11"/>
       <c r="O89" s="12"/>
       <c r="P89" s="20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="Q89" s="151" t="str">
         <f>IF(Sheet1!B10="","",Sheet1!B10+Lamb)</f>
@@ -6534,7 +6828,7 @@
       </c>
       <c r="V89" s="116"/>
       <c r="W89" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Y89" s="13"/>
       <c r="AA89" s="160" t="e">
@@ -6575,7 +6869,7 @@
       <c r="M90" s="11"/>
       <c r="O90" s="12"/>
       <c r="P90" s="20" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="Q90" s="151" t="str">
         <f>IF(Sheet1!B11="","",Sheet1!B11+Lamb)</f>
@@ -6619,7 +6913,7 @@
       <c r="M91" s="11"/>
       <c r="O91" s="12"/>
       <c r="P91" s="20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="Q91" s="151" t="str">
         <f>IF(Sheet1!B12="","",Sheet1!B12+Lamb)</f>
@@ -6661,12 +6955,12 @@
       </c>
       <c r="B92" s="9"/>
       <c r="C92" s="72" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M92" s="11"/>
       <c r="O92" s="12"/>
       <c r="P92" s="20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="Q92" s="151" t="str">
         <f>IF(Sheet1!B13="","",Sheet1!B13+Lamb)</f>
@@ -6685,10 +6979,10 @@
         <v/>
       </c>
       <c r="W92" s="19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="X92" s="19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="Y92" s="13"/>
       <c r="AA92" s="160" t="e">
@@ -6728,7 +7022,7 @@
       <c r="M93" s="11"/>
       <c r="O93" s="12"/>
       <c r="P93" s="20" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="Q93" s="151" t="str">
         <f>IF(Sheet1!B14="","",Sheet1!B14+Lamb)</f>
@@ -6747,7 +7041,7 @@
         <v/>
       </c>
       <c r="V93" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="W93" s="174" t="e">
         <f>AVERAGE(Q88:R96)</f>
@@ -6795,7 +7089,7 @@
       <c r="M94" s="11"/>
       <c r="O94" s="12"/>
       <c r="P94" s="20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="Q94" s="151" t="str">
         <f>IF(Sheet1!B15="","",Sheet1!B15+Lamb)</f>
@@ -6814,7 +7108,7 @@
         <v/>
       </c>
       <c r="V94" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="W94" s="174" t="e">
         <f>AVERAGE(S88:T96)</f>
@@ -6862,7 +7156,7 @@
       <c r="M95" s="11"/>
       <c r="O95" s="12"/>
       <c r="P95" s="20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="Q95" s="151" t="str">
         <f>IF(Sheet1!B16="","",Sheet1!B16+Lamb)</f>
@@ -6918,7 +7212,7 @@
       <c r="M96" s="11"/>
       <c r="O96" s="12"/>
       <c r="P96" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Q96" s="154" t="str">
         <f>IF(Sheet1!B17="","",Sheet1!B17+Lamb)</f>
@@ -6974,7 +7268,7 @@
       <c r="M97" s="11"/>
       <c r="O97" s="12"/>
       <c r="P97" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q97" s="117" t="str">
         <f>IF(Q88="","",AVERAGE(Q88:Q92))</f>
@@ -7014,7 +7308,7 @@
       <c r="M98" s="11"/>
       <c r="O98" s="12"/>
       <c r="P98" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q98" s="144" t="str">
         <f>IF(Q88="","",STDEV(Q88:Q92))</f>
@@ -7054,7 +7348,7 @@
       <c r="M99" s="11"/>
       <c r="O99" s="12"/>
       <c r="P99" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q99" s="147" t="str">
         <f>IF(Q88="","",2*(MAX(Q88:Q96)-MIN(Q88:Q96))/(MIN(Q88:Q96)+MAX(Q88:Q96)))</f>
@@ -7076,7 +7370,7 @@
         <v>56</v>
       </c>
       <c r="V99" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Y99" s="13"/>
     </row>
@@ -7100,7 +7394,7 @@
       <c r="M100" s="11"/>
       <c r="O100" s="12"/>
       <c r="P100" s="20" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Q100" s="158" t="str">
         <f>IF(Q88="","",MAX(AA88:AA96))</f>
@@ -7119,7 +7413,7 @@
         <v/>
       </c>
       <c r="V100" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="Y100" s="13"/>
     </row>
@@ -7143,7 +7437,7 @@
       <c r="M101" s="11"/>
       <c r="O101" s="12"/>
       <c r="P101" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q101" s="143" t="str">
         <f>IF(Q103&lt;&gt;"",Q103,IF(AB62="","",AB62))</f>
@@ -7176,7 +7470,7 @@
       <c r="M102" s="11"/>
       <c r="O102" s="12"/>
       <c r="P102" s="80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q102" s="112"/>
       <c r="R102" s="81">
@@ -7211,7 +7505,7 @@
       <c r="M103" s="11"/>
       <c r="O103" s="12"/>
       <c r="P103" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q103" s="66"/>
       <c r="R103" s="67"/>
@@ -7291,7 +7585,7 @@
       <c r="L106" s="67"/>
       <c r="M106" s="11"/>
       <c r="T106" s="120" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="107" spans="1:25" ht="14.4" customHeight="1">
@@ -7317,7 +7611,7 @@
       <c r="Q107" s="6"/>
       <c r="R107" s="6"/>
       <c r="S107" s="121" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="T107" s="6"/>
       <c r="U107" s="6"/>
@@ -7346,7 +7640,7 @@
       <c r="M108" s="11"/>
       <c r="O108" s="12"/>
       <c r="P108" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q108" s="122"/>
       <c r="R108" s="123"/>
@@ -7379,7 +7673,7 @@
       <c r="M109" s="11"/>
       <c r="O109" s="12"/>
       <c r="P109" s="80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q109" s="112"/>
       <c r="R109" s="125">
@@ -7414,7 +7708,7 @@
       <c r="M110" s="11"/>
       <c r="O110" s="12"/>
       <c r="P110" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q110" s="122"/>
       <c r="R110" s="123"/>
@@ -7447,7 +7741,7 @@
       <c r="M111" s="11"/>
       <c r="O111" s="12"/>
       <c r="P111" s="80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q111" s="112"/>
       <c r="R111" s="125">
@@ -7482,7 +7776,7 @@
       <c r="M112" s="11"/>
       <c r="O112" s="12"/>
       <c r="P112" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q112" s="122"/>
       <c r="R112" s="123"/>
@@ -7515,7 +7809,7 @@
       <c r="M113" s="11"/>
       <c r="O113" s="12"/>
       <c r="P113" s="80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q113" s="112"/>
       <c r="R113" s="125">
@@ -7550,7 +7844,7 @@
       <c r="M114" s="11"/>
       <c r="O114" s="12"/>
       <c r="P114" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q114" s="122"/>
       <c r="R114" s="123"/>
@@ -7583,7 +7877,7 @@
       <c r="M115" s="11"/>
       <c r="O115" s="12"/>
       <c r="P115" s="80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q115" s="112"/>
       <c r="R115" s="125">
@@ -7618,7 +7912,7 @@
       <c r="M116" s="11"/>
       <c r="O116" s="12"/>
       <c r="P116" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q116" s="122"/>
       <c r="R116" s="123"/>
@@ -7651,7 +7945,7 @@
       <c r="M117" s="11"/>
       <c r="O117" s="12"/>
       <c r="P117" s="80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q117" s="112"/>
       <c r="R117" s="125">
@@ -7686,7 +7980,7 @@
       <c r="M118" s="11"/>
       <c r="O118" s="12"/>
       <c r="P118" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q118" s="122"/>
       <c r="R118" s="123"/>
@@ -7719,7 +8013,7 @@
       <c r="M119" s="11"/>
       <c r="O119" s="12"/>
       <c r="P119" s="80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q119" s="112"/>
       <c r="R119" s="125">
@@ -7754,7 +8048,7 @@
       <c r="M120" s="11"/>
       <c r="O120" s="12"/>
       <c r="P120" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q120" s="122"/>
       <c r="R120" s="123"/>
@@ -7787,7 +8081,7 @@
       <c r="M121" s="11"/>
       <c r="O121" s="12"/>
       <c r="P121" s="80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q121" s="112"/>
       <c r="R121" s="125">
@@ -7822,7 +8116,7 @@
       <c r="M122" s="11"/>
       <c r="O122" s="12"/>
       <c r="P122" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q122" s="122"/>
       <c r="R122" s="123"/>
@@ -7855,7 +8149,7 @@
       <c r="M123" s="11"/>
       <c r="O123" s="12"/>
       <c r="P123" s="80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q123" s="112"/>
       <c r="R123" s="125">
@@ -7890,7 +8184,7 @@
       <c r="M124" s="11"/>
       <c r="O124" s="12"/>
       <c r="P124" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q124" s="122"/>
       <c r="R124" s="123"/>
@@ -7923,7 +8217,7 @@
       <c r="M125" s="11"/>
       <c r="O125" s="12"/>
       <c r="P125" s="80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q125" s="112"/>
       <c r="R125" s="125">
@@ -7946,7 +8240,7 @@
       <c r="M126" s="11"/>
       <c r="O126" s="12"/>
       <c r="P126" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q126" s="122"/>
       <c r="R126" s="123"/>
@@ -7967,7 +8261,7 @@
       <c r="M127" s="11"/>
       <c r="O127" s="12"/>
       <c r="P127" s="80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q127" s="112"/>
       <c r="R127" s="125">
@@ -7990,7 +8284,7 @@
       <c r="M128" s="11"/>
       <c r="O128" s="12"/>
       <c r="P128" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q128" s="122"/>
       <c r="R128" s="123"/>
@@ -8011,7 +8305,7 @@
       <c r="M129" s="11"/>
       <c r="O129" s="12"/>
       <c r="P129" s="80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q129" s="112"/>
       <c r="R129" s="125">
@@ -8061,7 +8355,7 @@
       <c r="C131" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D131" s="223" t="str">
+      <c r="D131" s="186" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -8078,7 +8372,7 @@
         <v>66</v>
       </c>
       <c r="C132" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D132" s="99" t="str">
         <f>IF($J$12="","",$J$12)</f>
@@ -8105,35 +8399,7 @@
       </headerFooter>
     </customSheetView>
   </customSheetViews>
-  <mergeCells count="40">
-    <mergeCell ref="AG1:AJ1"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="I84:J84"/>
-    <mergeCell ref="K84:L84"/>
-    <mergeCell ref="I85:J85"/>
-    <mergeCell ref="K85:L85"/>
-    <mergeCell ref="V77:V78"/>
-    <mergeCell ref="V75:V76"/>
-    <mergeCell ref="V73:V74"/>
-    <mergeCell ref="W73:W74"/>
-    <mergeCell ref="W75:W76"/>
-    <mergeCell ref="W77:W78"/>
+  <mergeCells count="42">
     <mergeCell ref="I87:J87"/>
     <mergeCell ref="K87:L87"/>
     <mergeCell ref="Q86:R86"/>
@@ -8146,10 +8412,40 @@
     <mergeCell ref="S77:S78"/>
     <mergeCell ref="I86:J86"/>
     <mergeCell ref="K86:L86"/>
+    <mergeCell ref="V77:V78"/>
+    <mergeCell ref="V75:V76"/>
+    <mergeCell ref="V73:V74"/>
+    <mergeCell ref="W73:W74"/>
+    <mergeCell ref="W75:W76"/>
+    <mergeCell ref="W77:W78"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="I84:J84"/>
+    <mergeCell ref="K84:L84"/>
+    <mergeCell ref="I85:J85"/>
+    <mergeCell ref="K85:L85"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="AG1:AJ1"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="AG9:AH9"/>
   </mergeCells>
   <conditionalFormatting sqref="D27:D28">
     <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
-      <formula>20</formula>
+      <formula>"VLOOKUP(V13,AG10:AH16,2)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D75:G76">
@@ -8209,7 +8505,7 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="T26">
     <cfRule type="cellIs" dxfId="0" priority="7" operator="greaterThan">
-      <formula>20</formula>
+      <formula>"VLOOKUP(V13,AG10:AH16,2)"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.78740157480314965" bottom="0.94488188976377963" header="0.51181102362204722" footer="0.78740157480314965"/>
@@ -8257,7 +8553,7 @@
       <c r="K1" s="136"/>
       <c r="L1" s="176"/>
       <c r="R1" s="83" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="20.399999999999999">
@@ -8270,7 +8566,7 @@
       </c>
       <c r="L2" s="178"/>
       <c r="R2" s="83" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="20.399999999999999">
@@ -8359,19 +8655,19 @@
       <c r="D10" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="214" t="str">
+      <c r="E10" s="191" t="str">
         <f>Barco!E10</f>
         <v/>
       </c>
-      <c r="F10" s="214"/>
+      <c r="F10" s="191"/>
       <c r="I10" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="214" t="str">
+      <c r="J10" s="191" t="str">
         <f>Barco!J10</f>
         <v/>
       </c>
-      <c r="K10" s="214"/>
+      <c r="K10" s="191"/>
       <c r="L10" s="178"/>
     </row>
     <row r="11" spans="1:18">
@@ -8382,19 +8678,19 @@
       <c r="D11" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="214" t="str">
+      <c r="E11" s="191" t="str">
         <f>Barco!E11</f>
         <v/>
       </c>
-      <c r="F11" s="214"/>
+      <c r="F11" s="191"/>
       <c r="I11" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="214" t="str">
+      <c r="J11" s="191" t="str">
         <f>Barco!J11</f>
         <v/>
       </c>
-      <c r="K11" s="214"/>
+      <c r="K11" s="191"/>
       <c r="L11" s="178"/>
     </row>
     <row r="12" spans="1:18">
@@ -8405,19 +8701,19 @@
       <c r="D12" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="214" t="str">
+      <c r="E12" s="191" t="str">
         <f>Barco!E12</f>
         <v/>
       </c>
-      <c r="F12" s="214"/>
+      <c r="F12" s="191"/>
       <c r="I12" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="214" t="str">
+      <c r="J12" s="191" t="str">
         <f>Barco!J12</f>
         <v/>
       </c>
-      <c r="K12" s="214"/>
+      <c r="K12" s="191"/>
       <c r="L12" s="178"/>
     </row>
     <row r="13" spans="1:18">
@@ -8428,19 +8724,19 @@
       <c r="D13" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="214" t="str">
+      <c r="E13" s="191" t="str">
         <f>Barco!E13</f>
         <v/>
       </c>
-      <c r="F13" s="214"/>
+      <c r="F13" s="191"/>
       <c r="I13" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="214" t="str">
-        <f>Barco!J13</f>
-        <v/>
-      </c>
-      <c r="K13" s="214"/>
+      <c r="J13" s="191">
+        <f>Barco!J14</f>
+        <v>2590411503</v>
+      </c>
+      <c r="K13" s="191"/>
       <c r="L13" s="178"/>
     </row>
     <row r="14" spans="1:18">
@@ -8451,19 +8747,19 @@
       <c r="D14" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="214" t="str">
+      <c r="E14" s="191" t="str">
         <f>Barco!E14</f>
         <v/>
       </c>
-      <c r="F14" s="214"/>
+      <c r="F14" s="191"/>
       <c r="I14" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="214" t="str">
-        <f>Barco!J14</f>
-        <v/>
-      </c>
-      <c r="K14" s="214"/>
+      <c r="J14" s="191" t="str">
+        <f>Barco!J15</f>
+        <v/>
+      </c>
+      <c r="K14" s="191"/>
       <c r="L14" s="178"/>
     </row>
     <row r="15" spans="1:18">
@@ -8474,11 +8770,11 @@
       <c r="D15" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="214" t="str">
+      <c r="E15" s="191" t="str">
         <f>Barco!E15</f>
-        <v>Barco K5905277 v16</v>
-      </c>
-      <c r="F15" s="214"/>
+        <v>Barco K5905277 v18</v>
+      </c>
+      <c r="F15" s="191"/>
       <c r="L15" s="178"/>
     </row>
     <row r="16" spans="1:18" ht="16.2" thickBot="1">
@@ -8507,7 +8803,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="184" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C18" s="136"/>
       <c r="D18" s="136"/>
@@ -8532,14 +8828,14 @@
         <v>20</v>
       </c>
       <c r="B20" s="177"/>
-      <c r="F20" s="219" t="s">
-        <v>196</v>
-      </c>
-      <c r="G20" s="219"/>
-      <c r="H20" s="219" t="s">
-        <v>197</v>
-      </c>
-      <c r="I20" s="219"/>
+      <c r="F20" s="222" t="s">
+        <v>193</v>
+      </c>
+      <c r="G20" s="222"/>
+      <c r="H20" s="222" t="s">
+        <v>194</v>
+      </c>
+      <c r="I20" s="222"/>
       <c r="L20" s="178"/>
     </row>
     <row r="21" spans="1:12">
@@ -8547,16 +8843,16 @@
         <v>21</v>
       </c>
       <c r="B21" s="177"/>
-      <c r="F21" s="219" t="str">
+      <c r="F21" s="222">
         <f>J13</f>
-        <v/>
-      </c>
-      <c r="G21" s="219"/>
-      <c r="H21" s="219" t="str">
+        <v>2590411503</v>
+      </c>
+      <c r="G21" s="222"/>
+      <c r="H21" s="222" t="str">
         <f>J14</f>
         <v/>
       </c>
-      <c r="I21" s="219"/>
+      <c r="I21" s="222"/>
       <c r="L21" s="178"/>
     </row>
     <row r="22" spans="1:12">
@@ -8565,15 +8861,15 @@
       </c>
       <c r="B22" s="177"/>
       <c r="E22" s="48" t="s">
-        <v>189</v>
-      </c>
-      <c r="F22" s="218" t="str">
+        <v>186</v>
+      </c>
+      <c r="F22" s="223" t="str">
         <f>IF(Barco!E23="","",IF(Barco!E23="YES","PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="G22" s="218"/>
-      <c r="H22" s="218"/>
-      <c r="I22" s="218"/>
+      <c r="G22" s="223"/>
+      <c r="H22" s="223"/>
+      <c r="I22" s="223"/>
       <c r="L22" s="178"/>
     </row>
     <row r="23" spans="1:12">
@@ -8582,15 +8878,15 @@
       </c>
       <c r="B23" s="177"/>
       <c r="E23" s="48" t="s">
-        <v>190</v>
-      </c>
-      <c r="F23" s="218" t="str">
+        <v>187</v>
+      </c>
+      <c r="F23" s="223" t="str">
         <f>IF(Barco!E22="","",IF(Barco!E22="YES","PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="G23" s="218"/>
-      <c r="H23" s="218"/>
-      <c r="I23" s="218"/>
+      <c r="G23" s="223"/>
+      <c r="H23" s="223"/>
+      <c r="I23" s="223"/>
       <c r="L23" s="178"/>
     </row>
     <row r="24" spans="1:12">
@@ -8599,15 +8895,15 @@
       </c>
       <c r="B24" s="177"/>
       <c r="E24" s="48" t="s">
-        <v>191</v>
-      </c>
-      <c r="F24" s="218" t="str">
+        <v>188</v>
+      </c>
+      <c r="F24" s="223" t="str">
         <f>IF(OR(Barco!I72="TBD",Barco!I73="TBD"),"",IF(AND(Barco!I72="YES",Barco!I73="YES"),"PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="G24" s="218"/>
-      <c r="H24" s="218"/>
-      <c r="I24" s="218"/>
+      <c r="G24" s="223"/>
+      <c r="H24" s="223"/>
+      <c r="I24" s="223"/>
       <c r="L24" s="178"/>
     </row>
     <row r="25" spans="1:12">
@@ -8616,12 +8912,12 @@
       </c>
       <c r="B25" s="177"/>
       <c r="E25" s="48" t="s">
-        <v>192</v>
-      </c>
-      <c r="F25" s="215"/>
-      <c r="G25" s="215"/>
-      <c r="H25" s="215"/>
-      <c r="I25" s="215"/>
+        <v>189</v>
+      </c>
+      <c r="F25" s="219"/>
+      <c r="G25" s="219"/>
+      <c r="H25" s="219"/>
+      <c r="I25" s="219"/>
       <c r="L25" s="178"/>
     </row>
     <row r="26" spans="1:12">
@@ -8630,18 +8926,18 @@
       </c>
       <c r="B26" s="177"/>
       <c r="D26" s="83" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E26" s="48" t="s">
-        <v>193</v>
-      </c>
-      <c r="F26" s="218" t="str">
+        <v>190</v>
+      </c>
+      <c r="F26" s="223" t="str">
         <f>IF(Barco!F85="","",IF(Barco!F85="YES","PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="G26" s="218"/>
-      <c r="H26" s="218"/>
-      <c r="I26" s="218"/>
+      <c r="G26" s="223"/>
+      <c r="H26" s="223"/>
+      <c r="I26" s="223"/>
       <c r="L26" s="178"/>
     </row>
     <row r="27" spans="1:12">
@@ -8650,12 +8946,12 @@
       </c>
       <c r="B27" s="177"/>
       <c r="E27" s="48" t="s">
-        <v>194</v>
-      </c>
-      <c r="F27" s="215"/>
-      <c r="G27" s="215"/>
-      <c r="H27" s="215"/>
-      <c r="I27" s="215"/>
+        <v>191</v>
+      </c>
+      <c r="F27" s="219"/>
+      <c r="G27" s="219"/>
+      <c r="H27" s="219"/>
+      <c r="I27" s="219"/>
       <c r="L27" s="178"/>
     </row>
     <row r="28" spans="1:12">
@@ -8664,12 +8960,12 @@
       </c>
       <c r="B28" s="177"/>
       <c r="E28" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="F28" s="215"/>
-      <c r="G28" s="215"/>
-      <c r="H28" s="215"/>
-      <c r="I28" s="215"/>
+        <v>192</v>
+      </c>
+      <c r="F28" s="219"/>
+      <c r="G28" s="219"/>
+      <c r="H28" s="219"/>
+      <c r="I28" s="219"/>
       <c r="L28" s="178"/>
     </row>
     <row r="29" spans="1:12">
@@ -8678,18 +8974,18 @@
       </c>
       <c r="B29" s="177"/>
       <c r="E29" s="48" t="s">
-        <v>201</v>
-      </c>
-      <c r="F29" s="216" t="str">
+        <v>198</v>
+      </c>
+      <c r="F29" s="220" t="str">
         <f>IF(Barco!F86="","",IF(Barco!F86="YES","PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="G29" s="217"/>
-      <c r="H29" s="216" t="str">
+      <c r="G29" s="221"/>
+      <c r="H29" s="220" t="str">
         <f>IF(Barco!G86="","",IF(Barco!G86="YES","PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="I29" s="217"/>
+      <c r="I29" s="221"/>
       <c r="L29" s="178"/>
     </row>
     <row r="30" spans="1:12">
@@ -8841,7 +9137,7 @@
         <v>46</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D46" s="127" t="str">
         <f>Barco!D66</f>
@@ -8863,17 +9159,10 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
     <mergeCell ref="F27:G27"/>
     <mergeCell ref="F28:G28"/>
     <mergeCell ref="F29:G29"/>
@@ -8890,10 +9179,17 @@
     <mergeCell ref="F26:G26"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="J12:K12"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F25:I25 F27:I28" xr:uid="{CEAD9B4F-4A05-4883-9435-EBBC3722EE42}">
@@ -8915,225 +9211,225 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="172" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="173" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B3" s="173" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="172" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove stray monitor serial number
</commit_message>
<xml_diff>
--- a/MUSCMammoMonitor.xlsx
+++ b/MUSCMammoMonitor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA916DD7-E49E-40BF-A8DC-0931A4D97E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AD1766-3C67-49D2-AB11-277FE36AC196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3105,8 +3105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D42" activeCellId="1" sqref="D34 D42"/>
+    <sheetView tabSelected="1" topLeftCell="P80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB20" sqref="AB20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -3716,9 +3716,9 @@
       <c r="I14" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="J14" s="192">
+      <c r="J14" s="192" t="str">
         <f>IF(V14="","",V14)</f>
-        <v>2590411503</v>
+        <v/>
       </c>
       <c r="K14" s="192"/>
       <c r="M14" s="11"/>
@@ -3734,9 +3734,9 @@
       <c r="U14" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="V14" s="55">
+      <c r="V14" s="55" t="str">
         <f>IF(W14&lt;&gt;"",W14,IF(AB20="","",AB20))</f>
-        <v>2590411503</v>
+        <v/>
       </c>
       <c r="W14" s="51"/>
       <c r="Y14" s="13"/>
@@ -4014,16 +4014,14 @@
       <c r="AA20" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="AB20" s="33">
-        <v>2590411503</v>
-      </c>
+      <c r="AB20" s="33"/>
       <c r="AC20" s="34" t="str">
         <f>IF(AB20&lt;&gt;AD20,"Change","")</f>
         <v/>
       </c>
-      <c r="AD20" s="35">
+      <c r="AD20" s="35" t="str">
         <f>IF(V14="","",V14)</f>
-        <v>2590411503</v>
+        <v/>
       </c>
       <c r="AF20"/>
       <c r="AG20"/>
@@ -4611,7 +4609,7 @@
       </c>
       <c r="S34" s="19" t="str">
         <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
-        <v>Right (1503)</v>
+        <v>Right ()</v>
       </c>
       <c r="Y34" s="13"/>
       <c r="AA34" s="1" t="s">
@@ -4688,7 +4686,7 @@
       <c r="D36" s="83"/>
       <c r="E36" s="48" t="str">
         <f>S34</f>
-        <v>Right (1503)</v>
+        <v>Right ()</v>
       </c>
       <c r="F36" s="84" t="str">
         <f>IF(S35="","",S35)</f>
@@ -4955,7 +4953,7 @@
       </c>
       <c r="G42" s="141" t="str">
         <f>S45</f>
-        <v>Right (1503)</v>
+        <v>Right ()</v>
       </c>
       <c r="M42" s="11"/>
       <c r="O42" s="12"/>
@@ -5089,7 +5087,7 @@
       </c>
       <c r="S45" s="19" t="str">
         <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
-        <v>Right (1503)</v>
+        <v>Right ()</v>
       </c>
       <c r="Y45" s="13"/>
       <c r="AA45" s="20" t="s">
@@ -5319,7 +5317,7 @@
       <c r="B51" s="9"/>
       <c r="D51" s="75" t="str">
         <f>R58</f>
-        <v>Right (1503)</v>
+        <v>Right ()</v>
       </c>
       <c r="E51" s="128" t="str">
         <f>IF(R59="","",R59)</f>
@@ -5330,7 +5328,7 @@
       </c>
       <c r="I51" s="75" t="str">
         <f>R58</f>
-        <v>Right (1503)</v>
+        <v>Right ()</v>
       </c>
       <c r="J51" s="157" t="str">
         <f>IF(R60="","",R60)</f>
@@ -5408,7 +5406,7 @@
       </c>
       <c r="F53" s="83" t="str">
         <f>R58</f>
-        <v>Right (1503)</v>
+        <v>Right ()</v>
       </c>
       <c r="I53" s="48"/>
       <c r="J53" s="48"/>
@@ -5602,7 +5600,7 @@
       </c>
       <c r="R58" s="19" t="str">
         <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
-        <v>Right (1503)</v>
+        <v>Right ()</v>
       </c>
       <c r="T58" s="1" t="s">
         <v>141</v>
@@ -5613,7 +5611,7 @@
       </c>
       <c r="V58" s="19" t="str">
         <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
-        <v>Right (1503)</v>
+        <v>Right ()</v>
       </c>
       <c r="Y58" s="13"/>
       <c r="AA58" s="20" t="s">
@@ -5985,7 +5983,7 @@
       </c>
       <c r="S68" s="19" t="str">
         <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
-        <v>Right (1503)</v>
+        <v>Right ()</v>
       </c>
       <c r="Y68" s="13"/>
       <c r="AB68" s="139"/>
@@ -6089,7 +6087,7 @@
       </c>
       <c r="E72" s="84" t="str">
         <f>R87</f>
-        <v>Right (1503)</v>
+        <v>Right ()</v>
       </c>
       <c r="F72" s="84" t="str">
         <f>S87</f>
@@ -6097,7 +6095,7 @@
       </c>
       <c r="G72" s="96" t="str">
         <f>T87</f>
-        <v>Right (1503)</v>
+        <v>Right ()</v>
       </c>
       <c r="I72" s="49" t="str">
         <f>IF(V87="","TBD",IF(V87=1,"YES",IF(V87=2,"NO",IF(V87=3,"NA",""))))</f>
@@ -6558,7 +6556,7 @@
       </c>
       <c r="G84" s="141" t="str">
         <f>S68</f>
-        <v>Right (1503)</v>
+        <v>Right ()</v>
       </c>
       <c r="I84" s="198" t="str">
         <f>R68</f>
@@ -6567,7 +6565,7 @@
       <c r="J84" s="198"/>
       <c r="K84" s="198" t="str">
         <f>S68</f>
-        <v>Right (1503)</v>
+        <v>Right ()</v>
       </c>
       <c r="L84" s="198"/>
       <c r="M84" s="11"/>
@@ -6702,7 +6700,7 @@
       </c>
       <c r="R87" s="115" t="str">
         <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
-        <v>Right (1503)</v>
+        <v>Right ()</v>
       </c>
       <c r="S87" s="114" t="str">
         <f>"Left ("&amp;RIGHT($V$13,4)&amp;")"</f>
@@ -6710,7 +6708,7 @@
       </c>
       <c r="T87" s="115" t="str">
         <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
-        <v>Right (1503)</v>
+        <v>Right ()</v>
       </c>
       <c r="V87" s="116"/>
       <c r="W87" s="1" t="s">
@@ -8732,9 +8730,9 @@
       <c r="I13" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="191">
+      <c r="J13" s="191" t="str">
         <f>Barco!J14</f>
-        <v>2590411503</v>
+        <v/>
       </c>
       <c r="K13" s="191"/>
       <c r="L13" s="178"/>
@@ -8843,9 +8841,9 @@
         <v>21</v>
       </c>
       <c r="B21" s="177"/>
-      <c r="F21" s="222">
+      <c r="F21" s="222" t="str">
         <f>J13</f>
-        <v>2590411503</v>
+        <v/>
       </c>
       <c r="G21" s="222"/>
       <c r="H21" s="222" t="str">

</xml_diff>

<commit_message>
Take into account Barco monitor model for ambient illumination limits
</commit_message>
<xml_diff>
--- a/MUSCMammoMonitor.xlsx
+++ b/MUSCMammoMonitor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AD1766-3C67-49D2-AB11-277FE36AC196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3C7225-A6FA-43CD-A183-AD8D0E508F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -655,9 +655,6 @@
     <t>Waveforms</t>
   </si>
   <si>
-    <t>Revision 1.6-20220607</t>
-  </si>
-  <si>
     <t>Page1,Page2</t>
   </si>
   <si>
@@ -737,6 +734,9 @@
   </si>
   <si>
     <t>MDNG-6221</t>
+  </si>
+  <si>
+    <t>Revision 1.7-20250603</t>
   </si>
 </sst>
 </file>
@@ -2321,38 +2321,47 @@
     <xf numFmtId="167" fontId="3" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2381,38 +2390,44 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2423,26 +2438,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -2455,157 +2455,7 @@
     <cellStyle name="Result" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Result2" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3105,8 +2955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P80" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB20" sqref="AB20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -3136,7 +2986,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
       <c r="O1" s="5" t="s">
-        <v>183</v>
+        <v>210</v>
       </c>
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
@@ -3151,12 +3001,12 @@
       <c r="AA1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="AG1" s="188" t="s">
+      <c r="AG1" s="218" t="s">
         <v>1</v>
       </c>
-      <c r="AH1" s="188"/>
-      <c r="AI1" s="188"/>
-      <c r="AJ1" s="188"/>
+      <c r="AH1" s="218"/>
+      <c r="AI1" s="218"/>
+      <c r="AJ1" s="218"/>
     </row>
     <row r="2" spans="1:36" ht="14.4" customHeight="1">
       <c r="A2" s="1">
@@ -3173,16 +3023,16 @@
       </c>
       <c r="Y2" s="13"/>
       <c r="AA2" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="AG2" s="189" t="s">
+        <v>183</v>
+      </c>
+      <c r="AG2" s="219" t="s">
         <v>3</v>
       </c>
-      <c r="AH2" s="189"/>
-      <c r="AI2" s="190" t="s">
+      <c r="AH2" s="219"/>
+      <c r="AI2" s="220" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="190"/>
+      <c r="AJ2" s="220"/>
     </row>
     <row r="3" spans="1:36" ht="14.4" customHeight="1">
       <c r="A3" s="1">
@@ -3229,7 +3079,7 @@
         <v>8</v>
       </c>
       <c r="AB4" s="21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF4" s="20" t="s">
         <v>9</v>
@@ -3350,7 +3200,7 @@
       </c>
       <c r="AB7" s="33"/>
       <c r="AC7" s="34" t="str">
-        <f t="shared" ref="AC7:AC20" si="0">IF(AB7&lt;&gt;AD7,"Change","")</f>
+        <f t="shared" ref="AC7:AC18" si="0">IF(AB7&lt;&gt;AD7,"Change","")</f>
         <v>Change</v>
       </c>
       <c r="AD7" s="35" t="str">
@@ -3455,10 +3305,10 @@
         <v>Eugene Mah</v>
       </c>
       <c r="AF9"/>
-      <c r="AG9" s="226" t="s">
-        <v>202</v>
-      </c>
-      <c r="AH9" s="227"/>
+      <c r="AG9" s="222" t="s">
+        <v>201</v>
+      </c>
+      <c r="AH9" s="223"/>
     </row>
     <row r="10" spans="1:36" ht="14.4" customHeight="1">
       <c r="A10" s="1">
@@ -3468,26 +3318,26 @@
       <c r="D10" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="191" t="str">
+      <c r="E10" s="221" t="str">
         <f t="shared" ref="E10:E15" si="1">IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="F10" s="191"/>
+      <c r="F10" s="221"/>
       <c r="I10" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="191" t="str">
-        <f>IF(V10="","",V10)</f>
-        <v/>
-      </c>
-      <c r="K10" s="191"/>
+      <c r="J10" s="221" t="str">
+        <f t="shared" ref="J10:J15" si="2">IF(V10="","",V10)</f>
+        <v/>
+      </c>
+      <c r="K10" s="221"/>
       <c r="M10" s="11"/>
       <c r="O10" s="12"/>
       <c r="Q10" s="20" t="s">
         <v>31</v>
       </c>
       <c r="R10" s="50" t="str">
-        <f t="shared" ref="R10:R15" si="2">IF(S10&lt;&gt;"",S10,IF(AB10="","",AB10))</f>
+        <f t="shared" ref="R10:R15" si="3">IF(S10&lt;&gt;"",S10,IF(AB10="","",AB10))</f>
         <v/>
       </c>
       <c r="S10" s="51"/>
@@ -3495,7 +3345,7 @@
         <v>32</v>
       </c>
       <c r="V10" s="50" t="str">
-        <f>IF(W10&lt;&gt;"",W10,IF(AB16="","",AB16))</f>
+        <f t="shared" ref="V10:V15" si="4">IF(W10&lt;&gt;"",W10,IF(AB16="","",AB16))</f>
         <v/>
       </c>
       <c r="W10" s="51"/>
@@ -3509,15 +3359,15 @@
         <v/>
       </c>
       <c r="AD10" s="35" t="str">
-        <f t="shared" ref="AD10:AD15" si="3">IF(R10="","",R10)</f>
+        <f t="shared" ref="AD10:AD15" si="5">IF(R10="","",R10)</f>
         <v/>
       </c>
       <c r="AF10"/>
       <c r="AG10" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="AH10" s="189" t="s">
         <v>203</v>
-      </c>
-      <c r="AH10" s="225" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:36" ht="14.4" customHeight="1">
@@ -3528,26 +3378,26 @@
       <c r="D11" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="192" t="str">
+      <c r="E11" s="214" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F11" s="192"/>
+      <c r="F11" s="214"/>
       <c r="I11" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="193" t="str">
-        <f>IF(V11="","",V11)</f>
-        <v/>
-      </c>
-      <c r="K11" s="193"/>
+      <c r="J11" s="217" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K11" s="217"/>
       <c r="M11" s="11"/>
       <c r="O11" s="12"/>
       <c r="Q11" s="20" t="s">
         <v>33</v>
       </c>
       <c r="R11" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S11" s="51"/>
@@ -3555,7 +3405,7 @@
         <v>34</v>
       </c>
       <c r="V11" s="53" t="str">
-        <f>IF(W11&lt;&gt;"",W11,IF(AB17="","",AB17))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W11" s="54"/>
@@ -3569,12 +3419,12 @@
         <v/>
       </c>
       <c r="AD11" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AF11"/>
       <c r="AG11" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AH11" s="16">
         <v>40</v>
@@ -3588,26 +3438,26 @@
       <c r="D12" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="192" t="str">
+      <c r="E12" s="214" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F12" s="192"/>
+      <c r="F12" s="214"/>
       <c r="I12" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="192" t="str">
-        <f>IF(V12="","",V12)</f>
-        <v/>
-      </c>
-      <c r="K12" s="192"/>
+      <c r="J12" s="214" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K12" s="214"/>
       <c r="M12" s="11"/>
       <c r="O12" s="12"/>
       <c r="Q12" s="20" t="s">
         <v>35</v>
       </c>
       <c r="R12" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S12" s="51"/>
@@ -3615,7 +3465,7 @@
         <v>36</v>
       </c>
       <c r="V12" s="50" t="str">
-        <f>IF(W12&lt;&gt;"",W12,IF(AB18="","",AB18))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W12" s="51"/>
@@ -3629,12 +3479,12 @@
         <v/>
       </c>
       <c r="AD12" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AF12"/>
       <c r="AG12" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AH12" s="16">
         <v>40</v>
@@ -3648,34 +3498,34 @@
       <c r="D13" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="192" t="str">
+      <c r="E13" s="214" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F13" s="192"/>
+      <c r="F13" s="214"/>
       <c r="I13" s="48" t="s">
-        <v>200</v>
-      </c>
-      <c r="J13" s="192" t="str">
-        <f>IF(V13="","",V13)</f>
-        <v/>
-      </c>
-      <c r="K13" s="192"/>
+        <v>199</v>
+      </c>
+      <c r="J13" s="214" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K13" s="214"/>
       <c r="M13" s="11"/>
       <c r="O13" s="12"/>
       <c r="Q13" s="20" t="s">
         <v>37</v>
       </c>
       <c r="R13" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S13" s="51"/>
       <c r="U13" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V13" s="55" t="str">
-        <f>IF(W13&lt;&gt;"",W13,IF(AB19="","",AB19))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W13" s="32"/>
@@ -3689,12 +3539,12 @@
         <v/>
       </c>
       <c r="AD13" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AF13"/>
       <c r="AG13" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AH13" s="16">
         <v>20</v>
@@ -3708,26 +3558,26 @@
       <c r="D14" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="192" t="str">
+      <c r="E14" s="214" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F14" s="192"/>
+      <c r="F14" s="214"/>
       <c r="I14" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="J14" s="192" t="str">
-        <f>IF(V14="","",V14)</f>
-        <v/>
-      </c>
-      <c r="K14" s="192"/>
+      <c r="J14" s="214" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K14" s="214"/>
       <c r="M14" s="11"/>
       <c r="O14" s="12"/>
       <c r="Q14" s="20" t="s">
         <v>39</v>
       </c>
       <c r="R14" s="50" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S14" s="51"/>
@@ -3735,7 +3585,7 @@
         <v>38</v>
       </c>
       <c r="V14" s="55" t="str">
-        <f>IF(W14&lt;&gt;"",W14,IF(AB20="","",AB20))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W14" s="51"/>
@@ -3749,12 +3599,12 @@
         <v/>
       </c>
       <c r="AD14" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AF14"/>
       <c r="AG14" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AH14" s="16">
         <v>40</v>
@@ -3768,19 +3618,19 @@
       <c r="D15" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="192" t="str">
+      <c r="E15" s="214" t="str">
         <f t="shared" si="1"/>
         <v>Barco K5905277 v18</v>
       </c>
-      <c r="F15" s="192"/>
+      <c r="F15" s="214"/>
       <c r="I15" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="J15" s="192" t="str">
-        <f>IF(V15="","",V15)</f>
-        <v/>
-      </c>
-      <c r="K15" s="192"/>
+      <c r="J15" s="214" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="K15" s="214"/>
       <c r="M15" s="11"/>
       <c r="O15" s="25"/>
       <c r="P15" s="26"/>
@@ -3788,18 +3638,18 @@
         <v>41</v>
       </c>
       <c r="R15" s="57" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Barco K5905277 v18</v>
       </c>
       <c r="S15" s="58" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="T15" s="26"/>
       <c r="U15" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="V15" s="224" t="str">
-        <f>IF(W15&lt;&gt;"",W15,IF(AB21="","",AB21))</f>
+      <c r="V15" s="188" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W15" s="58"/>
@@ -3814,12 +3664,12 @@
         <v>Change</v>
       </c>
       <c r="AD15" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Barco K5905277 v18</v>
       </c>
       <c r="AF15"/>
       <c r="AG15" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AH15" s="16">
         <v>20</v>
@@ -3850,12 +3700,12 @@
         <v/>
       </c>
       <c r="AD16" s="35" t="str">
-        <f>IF(V10="","",V10)</f>
+        <f t="shared" ref="AD16:AD21" si="6">IF(V10="","",V10)</f>
         <v/>
       </c>
       <c r="AF16"/>
       <c r="AG16" s="36" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AH16" s="38">
         <v>20</v>
@@ -3882,7 +3732,7 @@
         <v/>
       </c>
       <c r="AD17" s="62" t="str">
-        <f>IF(V11="","",V11)</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AF17"/>
@@ -3918,7 +3768,7 @@
         <v/>
       </c>
       <c r="AD18" s="35" t="str">
-        <f>IF(V12="","",V12)</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AF18"/>
@@ -3939,10 +3789,10 @@
       <c r="H19" s="136"/>
       <c r="I19" s="136"/>
       <c r="J19" s="136"/>
-      <c r="K19" s="195" t="s">
+      <c r="K19" s="216" t="s">
         <v>127</v>
       </c>
-      <c r="L19" s="195"/>
+      <c r="L19" s="216"/>
       <c r="M19" s="4"/>
       <c r="O19" s="12"/>
       <c r="R19" s="1" t="s">
@@ -3953,7 +3803,7 @@
       </c>
       <c r="Y19" s="13"/>
       <c r="AA19" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AB19" s="33"/>
       <c r="AC19" s="34" t="str">
@@ -3961,7 +3811,7 @@
         <v/>
       </c>
       <c r="AD19" s="35" t="str">
-        <f>IF(V13="","",V13)</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AF19"/>
@@ -4020,7 +3870,7 @@
         <v/>
       </c>
       <c r="AD20" s="35" t="str">
-        <f>IF(V14="","",V14)</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AF20"/>
@@ -4043,14 +3893,14 @@
         <v/>
       </c>
       <c r="G21" s="1" t="str">
-        <f t="shared" ref="G21:G23" si="4">IF(R21="","",R21)</f>
+        <f t="shared" ref="G21:G23" si="7">IF(R21="","",R21)</f>
         <v/>
       </c>
       <c r="K21" s="48" t="s">
         <v>126</v>
       </c>
       <c r="L21" s="185">
-        <f t="shared" ref="L21:L22" si="5">IF(W21="","",W21)</f>
+        <f t="shared" ref="L21:L22" si="8">IF(W21="","",W21)</f>
         <v>45089</v>
       </c>
       <c r="M21" s="11"/>
@@ -4063,7 +3913,7 @@
         <v>126</v>
       </c>
       <c r="W21" s="135">
-        <f t="shared" ref="W21:W22" si="6">IF(X21&lt;&gt;"",X21,IF(AB24="","",AB24))</f>
+        <f t="shared" ref="W21:W22" si="9">IF(X21&lt;&gt;"",X21,IF(AB24="","",AB24))</f>
         <v>45089</v>
       </c>
       <c r="X21" s="187">
@@ -4074,14 +3924,14 @@
         <v>40</v>
       </c>
       <c r="AB21" s="61" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AC21" s="34" t="str">
         <f>IF(AB21&lt;&gt;AD21,"Change","")</f>
         <v/>
       </c>
       <c r="AD21" s="35" t="str">
-        <f>IF(V15="","",V15)</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AF21"/>
@@ -4104,14 +3954,14 @@
         <v/>
       </c>
       <c r="G22" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K22" s="48" t="s">
         <v>125</v>
       </c>
       <c r="L22" s="185">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>45820</v>
       </c>
       <c r="M22" s="11"/>
@@ -4124,7 +3974,7 @@
         <v>125</v>
       </c>
       <c r="W22" s="135">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>45820</v>
       </c>
       <c r="X22" s="187">
@@ -4154,7 +4004,7 @@
         <v/>
       </c>
       <c r="G23" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="M23" s="11"/>
@@ -4169,7 +4019,7 @@
       </c>
       <c r="AB23" s="33"/>
       <c r="AC23" s="34" t="str">
-        <f t="shared" ref="AC23:AC25" si="7">IF(AB23&lt;&gt;AD23,"Change","")</f>
+        <f t="shared" ref="AC23:AC25" si="10">IF(AB23&lt;&gt;AD23,"Change","")</f>
         <v>Change</v>
       </c>
       <c r="AD23" s="35" t="str">
@@ -4187,11 +4037,11 @@
       <c r="D24" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="E24" s="194" t="str">
+      <c r="E24" s="215" t="str">
         <f>IF(P52="","",P52)</f>
         <v/>
       </c>
-      <c r="F24" s="194"/>
+      <c r="F24" s="215"/>
       <c r="M24" s="11"/>
       <c r="O24" s="12"/>
       <c r="Y24" s="13"/>
@@ -4200,11 +4050,11 @@
       </c>
       <c r="AB24" s="134"/>
       <c r="AC24" s="34" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>Change</v>
       </c>
       <c r="AD24" s="133">
-        <f t="shared" ref="AD24:AD25" si="8">IF(X21="","",X21)</f>
+        <f t="shared" ref="AD24:AD25" si="11">IF(X21="","",X21)</f>
         <v>45089</v>
       </c>
       <c r="AF24"/>
@@ -4231,11 +4081,11 @@
       </c>
       <c r="AB25" s="134"/>
       <c r="AC25" s="34" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>Change</v>
       </c>
       <c r="AD25" s="133">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>45820</v>
       </c>
       <c r="AF25"/>
@@ -4505,7 +4355,7 @@
       </c>
       <c r="AB31" s="33"/>
       <c r="AC31" s="34" t="str">
-        <f t="shared" ref="AC31:AC38" si="9">IF(AB31&lt;&gt;AD31,"Change","")</f>
+        <f t="shared" ref="AC31:AC38" si="12">IF(AB31&lt;&gt;AD31,"Change","")</f>
         <v/>
       </c>
       <c r="AD31" s="35" t="str">
@@ -4528,7 +4378,7 @@
       </c>
       <c r="AB32" s="33"/>
       <c r="AC32" s="34" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD32" s="35" t="str">
@@ -4562,7 +4412,7 @@
       </c>
       <c r="AB33" s="33"/>
       <c r="AC33" s="34" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD33" s="35" t="str">
@@ -4580,7 +4430,7 @@
       <c r="C34" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="D34" s="228" t="str">
+      <c r="D34" s="190" t="str">
         <f>IF(P34="","",P34)</f>
         <v/>
       </c>
@@ -4604,11 +4454,11 @@
       </c>
       <c r="P34" s="54"/>
       <c r="R34" s="19" t="str">
-        <f>"Left ("&amp;RIGHT($V$13,4)&amp;")"</f>
+        <f>"Left ("&amp;RIGHT($V$14,4)&amp;")"</f>
         <v>Left ()</v>
       </c>
       <c r="S34" s="19" t="str">
-        <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
+        <f>"Right ("&amp;RIGHT($V$15,4)&amp;")"</f>
         <v>Right ()</v>
       </c>
       <c r="Y34" s="13"/>
@@ -4617,7 +4467,7 @@
       </c>
       <c r="AB34" s="33"/>
       <c r="AC34" s="34" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD34" s="35" t="str">
@@ -4667,7 +4517,7 @@
       </c>
       <c r="AB35" s="33"/>
       <c r="AC35" s="34" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD35" s="35" t="str">
@@ -4717,7 +4567,7 @@
       </c>
       <c r="AB36" s="33"/>
       <c r="AC36" s="34" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD36" s="35" t="str">
@@ -4766,7 +4616,7 @@
       </c>
       <c r="AB37" s="33"/>
       <c r="AC37" s="34" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD37" s="35" t="str">
@@ -4802,7 +4652,7 @@
       </c>
       <c r="AB38" s="33"/>
       <c r="AC38" s="34" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD38" s="35" t="str">
@@ -4942,7 +4792,7 @@
       <c r="C42" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="D42" s="228" t="str">
+      <c r="D42" s="190" t="str">
         <f>IF(P44="","",P44)</f>
         <v/>
       </c>
@@ -5005,7 +4855,7 @@
       </c>
       <c r="AB43" s="70"/>
       <c r="AC43" s="34" t="str">
-        <f t="shared" ref="AC43:AC46" si="10">IF(AB43&lt;&gt;AD43,"Change","")</f>
+        <f t="shared" ref="AC43:AC46" si="13">IF(AB43&lt;&gt;AD43,"Change","")</f>
         <v/>
       </c>
       <c r="AD43" s="71" t="str">
@@ -5049,7 +4899,7 @@
       </c>
       <c r="AB44" s="70"/>
       <c r="AC44" s="34" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="AD44" s="71" t="str">
@@ -5082,11 +4932,11 @@
         <v>43</v>
       </c>
       <c r="R45" s="19" t="str">
-        <f>"Left ("&amp;RIGHT($V$13,4)&amp;")"</f>
+        <f>"Left ("&amp;RIGHT($V$14,4)&amp;")"</f>
         <v>Left ()</v>
       </c>
       <c r="S45" s="19" t="str">
-        <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
+        <f>"Right ("&amp;RIGHT($V$15,4)&amp;")"</f>
         <v>Right ()</v>
       </c>
       <c r="Y45" s="13"/>
@@ -5095,7 +4945,7 @@
       </c>
       <c r="AB45" s="70"/>
       <c r="AC45" s="34" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="AD45" s="71" t="str">
@@ -5136,7 +4986,7 @@
       </c>
       <c r="AB46" s="70"/>
       <c r="AC46" s="34" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="AD46" s="71" t="str">
@@ -5205,7 +5055,7 @@
       </c>
       <c r="AB48" s="137"/>
       <c r="AC48" s="34" t="str">
-        <f t="shared" ref="AC48:AC53" si="11">IF(AB48&lt;&gt;AD48,"Change","")</f>
+        <f t="shared" ref="AC48:AC53" si="14">IF(AB48&lt;&gt;AD48,"Change","")</f>
         <v/>
       </c>
       <c r="AD48" s="71" t="str">
@@ -5253,7 +5103,7 @@
       </c>
       <c r="AB49" s="137"/>
       <c r="AC49" s="34" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AD49" s="71" t="str">
@@ -5300,7 +5150,7 @@
       </c>
       <c r="AB50" s="137"/>
       <c r="AC50" s="34" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AD50" s="71" t="str">
@@ -5353,7 +5203,7 @@
       </c>
       <c r="AB51" s="137"/>
       <c r="AC51" s="34" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AD51" s="71" t="str">
@@ -5385,7 +5235,7 @@
       </c>
       <c r="AB52" s="137"/>
       <c r="AC52" s="34" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AD52" s="71" t="str">
@@ -5430,7 +5280,7 @@
       </c>
       <c r="AB53" s="137"/>
       <c r="AC53" s="34" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AD53" s="71" t="str">
@@ -5524,7 +5374,7 @@
       </c>
       <c r="AB56" s="138"/>
       <c r="AC56" s="34" t="str">
-        <f t="shared" ref="AC56:AC62" si="12">IF(AB56&lt;&gt;AD56,"Change","")</f>
+        <f t="shared" ref="AC56:AC62" si="15">IF(AB56&lt;&gt;AD56,"Change","")</f>
         <v/>
       </c>
       <c r="AD56" s="71" t="str">
@@ -5564,7 +5414,7 @@
       </c>
       <c r="AB57" s="138"/>
       <c r="AC57" s="34" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AD57" s="71" t="str">
@@ -5595,22 +5445,22 @@
         <v>98</v>
       </c>
       <c r="Q58" s="19" t="str">
-        <f>"Left ("&amp;RIGHT($V$13,4)&amp;")"</f>
+        <f>"Left ("&amp;RIGHT($V$14,4)&amp;")"</f>
         <v>Left ()</v>
       </c>
       <c r="R58" s="19" t="str">
-        <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
+        <f>"Right ("&amp;RIGHT($V$15,4)&amp;")"</f>
         <v>Right ()</v>
       </c>
       <c r="T58" s="1" t="s">
         <v>141</v>
       </c>
       <c r="U58" s="19" t="str">
-        <f>"Left ("&amp;RIGHT($V$13,4)&amp;")"</f>
+        <f>"Left ("&amp;RIGHT($V$14,4)&amp;")"</f>
         <v>Left ()</v>
       </c>
       <c r="V58" s="19" t="str">
-        <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
+        <f>"Right ("&amp;RIGHT($V$15,4)&amp;")"</f>
         <v>Right ()</v>
       </c>
       <c r="Y58" s="13"/>
@@ -5619,7 +5469,7 @@
       </c>
       <c r="AB58" s="138"/>
       <c r="AC58" s="34" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AD58" s="71" t="str">
@@ -5675,7 +5525,7 @@
       </c>
       <c r="AB59" s="138"/>
       <c r="AC59" s="34" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AD59" s="71" t="str">
@@ -5718,7 +5568,7 @@
       </c>
       <c r="AB60" s="138"/>
       <c r="AC60" s="34" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AD60" s="71" t="str">
@@ -5761,7 +5611,7 @@
       </c>
       <c r="AB61" s="138"/>
       <c r="AC61" s="34" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AD61" s="71" t="str">
@@ -5804,7 +5654,7 @@
       </c>
       <c r="AB62" s="138"/>
       <c r="AC62" s="34" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AD62" s="71" t="str">
@@ -5978,11 +5828,11 @@
         <v>43</v>
       </c>
       <c r="R68" s="19" t="str">
-        <f>"Left ("&amp;RIGHT($V$13,4)&amp;")"</f>
+        <f>"Left ("&amp;RIGHT($V$14,4)&amp;")"</f>
         <v>Left ()</v>
       </c>
       <c r="S68" s="19" t="str">
-        <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
+        <f>"Right ("&amp;RIGHT($V$15,4)&amp;")"</f>
         <v>Right ()</v>
       </c>
       <c r="Y68" s="13"/>
@@ -6051,16 +5901,16 @@
       </c>
       <c r="B71" s="9"/>
       <c r="C71" s="83"/>
-      <c r="D71" s="196" t="str">
+      <c r="D71" s="211" t="str">
         <f>Q86</f>
         <v>UNL-10 (cd/m^2)</v>
       </c>
-      <c r="E71" s="196"/>
-      <c r="F71" s="197" t="str">
+      <c r="E71" s="211"/>
+      <c r="F71" s="212" t="str">
         <f>S86</f>
         <v>UNL-80 (cd/m^2)</v>
       </c>
-      <c r="G71" s="197"/>
+      <c r="G71" s="212"/>
       <c r="I71" s="60" t="s">
         <v>106</v>
       </c>
@@ -6136,19 +5986,19 @@
         <v>108</v>
       </c>
       <c r="D73" s="106" t="str">
-        <f t="shared" ref="D73:G76" si="13">IF(Q97="","",Q97)</f>
+        <f t="shared" ref="D73:G76" si="16">IF(Q97="","",Q97)</f>
         <v/>
       </c>
       <c r="E73" s="85" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="F73" s="85" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G73" s="107" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I73" s="52" t="str">
@@ -6163,13 +6013,13 @@
       <c r="Q73" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="R73" s="211"/>
-      <c r="S73" s="215"/>
-      <c r="V73" s="203" t="str">
+      <c r="R73" s="194"/>
+      <c r="S73" s="198"/>
+      <c r="V73" s="206" t="str">
         <f>IF(AB48="","",AB48)</f>
         <v/>
       </c>
-      <c r="W73" s="204" t="str">
+      <c r="W73" s="207" t="str">
         <f>IF(AB51="","",AB51)</f>
         <v/>
       </c>
@@ -6186,19 +6036,19 @@
         <v>110</v>
       </c>
       <c r="D74" s="106" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="E74" s="85" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="F74" s="85" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G74" s="107" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I74" s="52" t="str">
@@ -6211,10 +6061,10 @@
       <c r="M74" s="11"/>
       <c r="O74" s="12"/>
       <c r="Q74" s="19"/>
-      <c r="R74" s="212"/>
-      <c r="S74" s="216"/>
-      <c r="V74" s="202"/>
-      <c r="W74" s="205"/>
+      <c r="R74" s="195"/>
+      <c r="S74" s="199"/>
+      <c r="V74" s="205"/>
+      <c r="W74" s="208"/>
       <c r="Y74" s="13"/>
       <c r="AB74" s="139"/>
       <c r="AC74" s="34" t="str">
@@ -6235,19 +6085,19 @@
         <v>112</v>
       </c>
       <c r="D75" s="108" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="E75" s="109" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="F75" s="109" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G75" s="110" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="M75" s="11"/>
@@ -6255,13 +6105,13 @@
       <c r="Q75" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="R75" s="213"/>
-      <c r="S75" s="217"/>
-      <c r="V75" s="200" t="str">
+      <c r="R75" s="196"/>
+      <c r="S75" s="200"/>
+      <c r="V75" s="203" t="str">
         <f>IF(AB49="","",AB49)</f>
         <v/>
       </c>
-      <c r="W75" s="206" t="str">
+      <c r="W75" s="209" t="str">
         <f>IF(AB52="","",AB52)</f>
         <v/>
       </c>
@@ -6278,19 +6128,19 @@
         <v>139</v>
       </c>
       <c r="D76" s="108" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="E76" s="109" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="F76" s="109" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G76" s="110" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I76" s="28" t="s">
@@ -6302,10 +6152,10 @@
       <c r="M76" s="11"/>
       <c r="O76" s="12"/>
       <c r="Q76" s="19"/>
-      <c r="R76" s="212"/>
-      <c r="S76" s="216"/>
-      <c r="V76" s="202"/>
-      <c r="W76" s="205"/>
+      <c r="R76" s="195"/>
+      <c r="S76" s="199"/>
+      <c r="V76" s="205"/>
+      <c r="W76" s="208"/>
       <c r="Y76" s="13"/>
       <c r="AB76" s="139"/>
       <c r="AC76" s="34" t="str">
@@ -6327,15 +6177,15 @@
         <v/>
       </c>
       <c r="E77" s="111" t="str">
-        <f t="shared" ref="E77:G77" si="14">IF(OR(E75="",E76=""),"",IF(AND(E75&lt;=0.3,E76&lt;=0.3),"PASS","FAIL"))</f>
+        <f t="shared" ref="E77:G77" si="17">IF(OR(E75="",E76=""),"",IF(AND(E75&lt;=0.3,E76&lt;=0.3),"PASS","FAIL"))</f>
         <v/>
       </c>
       <c r="F77" s="111" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="G77" s="91" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J77" s="1" t="s">
@@ -6346,13 +6196,13 @@
       <c r="Q77" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="R77" s="213"/>
-      <c r="S77" s="217"/>
-      <c r="V77" s="200" t="str">
+      <c r="R77" s="196"/>
+      <c r="S77" s="200"/>
+      <c r="V77" s="203" t="str">
         <f>IF(AB50="","",AB50)</f>
         <v/>
       </c>
-      <c r="W77" s="206" t="str">
+      <c r="W77" s="209" t="str">
         <f>IF(AB53="","",AB53)</f>
         <v/>
       </c>
@@ -6368,10 +6218,10 @@
       <c r="M78" s="11"/>
       <c r="O78" s="12"/>
       <c r="Q78" s="19"/>
-      <c r="R78" s="214"/>
-      <c r="S78" s="218"/>
-      <c r="V78" s="201"/>
-      <c r="W78" s="207"/>
+      <c r="R78" s="197"/>
+      <c r="S78" s="201"/>
+      <c r="V78" s="204"/>
+      <c r="W78" s="210"/>
       <c r="Y78" s="13"/>
       <c r="AB78" s="139"/>
       <c r="AC78" s="34" t="str">
@@ -6558,16 +6408,16 @@
         <f>S68</f>
         <v>Right ()</v>
       </c>
-      <c r="I84" s="198" t="str">
+      <c r="I84" s="213" t="str">
         <f>R68</f>
         <v>Left ()</v>
       </c>
-      <c r="J84" s="198"/>
-      <c r="K84" s="198" t="str">
+      <c r="J84" s="213"/>
+      <c r="K84" s="213" t="str">
         <f>S68</f>
         <v>Right ()</v>
       </c>
-      <c r="L84" s="198"/>
+      <c r="L84" s="213"/>
       <c r="M84" s="11"/>
       <c r="O84" s="12"/>
       <c r="Y84" s="13"/>
@@ -6590,26 +6440,26 @@
         <v>94</v>
       </c>
       <c r="F85" s="95" t="str">
-        <f t="shared" ref="F85:G87" si="15">IF(R69="","",IF(R69=1,"YES",IF(R69=2,"NO",IF(R69=3,"NA",""))))</f>
+        <f t="shared" ref="F85:G87" si="18">IF(R69="","",IF(R69=1,"YES",IF(R69=2,"NO",IF(R69=3,"NA",""))))</f>
         <v/>
       </c>
       <c r="G85" s="96" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="H85" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="I85" s="199" t="str">
+      <c r="I85" s="202" t="str">
         <f>IF(R73="","",R73)</f>
         <v/>
       </c>
-      <c r="J85" s="199"/>
-      <c r="K85" s="199" t="str">
+      <c r="J85" s="202"/>
+      <c r="K85" s="202" t="str">
         <f>IF(S73="","",S73)</f>
         <v/>
       </c>
-      <c r="L85" s="199"/>
+      <c r="L85" s="202"/>
       <c r="M85" s="11"/>
       <c r="O85" s="97" t="s">
         <v>105</v>
@@ -6628,36 +6478,36 @@
         <v>96</v>
       </c>
       <c r="F86" s="95" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="G86" s="96" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="H86" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="I86" s="199" t="str">
+      <c r="I86" s="202" t="str">
         <f>IF(R75="","",R75)</f>
         <v/>
       </c>
-      <c r="J86" s="199"/>
-      <c r="K86" s="199" t="str">
+      <c r="J86" s="202"/>
+      <c r="K86" s="202" t="str">
         <f>IF(S75="","",S75)</f>
         <v/>
       </c>
-      <c r="L86" s="199"/>
+      <c r="L86" s="202"/>
       <c r="M86" s="11"/>
       <c r="O86" s="12"/>
-      <c r="Q86" s="209" t="s">
+      <c r="Q86" s="192" t="s">
         <v>116</v>
       </c>
-      <c r="R86" s="210"/>
-      <c r="S86" s="209" t="s">
+      <c r="R86" s="193"/>
+      <c r="S86" s="192" t="s">
         <v>117</v>
       </c>
-      <c r="T86" s="210"/>
+      <c r="T86" s="193"/>
       <c r="V86" s="113" t="s">
         <v>43</v>
       </c>
@@ -6672,42 +6522,42 @@
         <v>99</v>
       </c>
       <c r="F87" s="90" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="G87" s="91" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="H87" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="I87" s="208" t="str">
+      <c r="I87" s="191" t="str">
         <f>IF(R77="","",R77)</f>
         <v/>
       </c>
-      <c r="J87" s="208"/>
-      <c r="K87" s="208" t="str">
+      <c r="J87" s="191"/>
+      <c r="K87" s="191" t="str">
         <f>IF(S77="","",S77)</f>
         <v/>
       </c>
-      <c r="L87" s="208"/>
+      <c r="L87" s="191"/>
       <c r="M87" s="11"/>
       <c r="O87" s="12"/>
       <c r="Q87" s="114" t="str">
-        <f>"Left ("&amp;RIGHT($V$13,4)&amp;")"</f>
+        <f>"Left ("&amp;RIGHT($V$14,4)&amp;")"</f>
         <v>Left ()</v>
       </c>
       <c r="R87" s="115" t="str">
-        <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
+        <f>"Right ("&amp;RIGHT($V$15,4)&amp;")"</f>
         <v>Right ()</v>
       </c>
       <c r="S87" s="114" t="str">
-        <f>"Left ("&amp;RIGHT($V$13,4)&amp;")"</f>
+        <f>"Left ("&amp;RIGHT($V$14,4)&amp;")"</f>
         <v>Left ()</v>
       </c>
       <c r="T87" s="115" t="str">
-        <f>"Right ("&amp;RIGHT($V$14,4)&amp;")"</f>
+        <f>"Right ("&amp;RIGHT($V$15,4)&amp;")"</f>
         <v>Right ()</v>
       </c>
       <c r="V87" s="116"/>
@@ -6830,19 +6680,19 @@
       </c>
       <c r="Y89" s="13"/>
       <c r="AA89" s="160" t="e">
-        <f t="shared" ref="AA89:AA96" si="16">ABS(Q89-MEDIAN($Q$88:$Q$96))/MEDIAN($Q$88:$Q$96)</f>
+        <f t="shared" ref="AA89:AA96" si="19">ABS(Q89-MEDIAN($Q$88:$Q$96))/MEDIAN($Q$88:$Q$96)</f>
         <v>#VALUE!</v>
       </c>
       <c r="AB89" s="160" t="e">
-        <f t="shared" ref="AB89:AB96" si="17">ABS(R89-MEDIAN($R$88:$R$96))/MEDIAN($R$88:$R$96)</f>
+        <f t="shared" ref="AB89:AB96" si="20">ABS(R89-MEDIAN($R$88:$R$96))/MEDIAN($R$88:$R$96)</f>
         <v>#VALUE!</v>
       </c>
       <c r="AC89" s="160" t="e">
-        <f t="shared" ref="AC89:AC96" si="18">ABS(S89-MEDIAN($S$88:$S$96))/MEDIAN($S$88:$S$96)</f>
+        <f t="shared" ref="AC89:AC96" si="21">ABS(S89-MEDIAN($S$88:$S$96))/MEDIAN($S$88:$S$96)</f>
         <v>#VALUE!</v>
       </c>
       <c r="AD89" s="160" t="e">
-        <f t="shared" ref="AD89:AD96" si="19">ABS(T89-MEDIAN($T$88:$T$96))/MEDIAN($T$88:$T$96)</f>
+        <f t="shared" ref="AD89:AD96" si="22">ABS(T89-MEDIAN($T$88:$T$96))/MEDIAN($T$88:$T$96)</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -6887,19 +6737,19 @@
       </c>
       <c r="Y90" s="13"/>
       <c r="AA90" s="160" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="AB90" s="160" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
       <c r="AC90" s="160" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
       <c r="AD90" s="160" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -6931,19 +6781,19 @@
       </c>
       <c r="Y91" s="13"/>
       <c r="AA91" s="160" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="AB91" s="160" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
       <c r="AC91" s="160" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
       <c r="AD91" s="160" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -6984,19 +6834,19 @@
       </c>
       <c r="Y92" s="13"/>
       <c r="AA92" s="160" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="AB92" s="160" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
       <c r="AC92" s="160" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
       <c r="AD92" s="160" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7051,19 +6901,19 @@
       </c>
       <c r="Y93" s="13"/>
       <c r="AA93" s="160" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="AB93" s="160" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
       <c r="AC93" s="160" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
       <c r="AD93" s="160" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7118,19 +6968,19 @@
       </c>
       <c r="Y94" s="13"/>
       <c r="AA94" s="160" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="AB94" s="160" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
       <c r="AC94" s="160" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
       <c r="AD94" s="160" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7174,19 +7024,19 @@
       </c>
       <c r="Y95" s="13"/>
       <c r="AA95" s="160" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="AB95" s="160" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
       <c r="AC95" s="160" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
       <c r="AD95" s="160" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7230,19 +7080,19 @@
       </c>
       <c r="Y96" s="13"/>
       <c r="AA96" s="160" t="e">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
       <c r="AB96" s="160" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
       <c r="AC96" s="160" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>#VALUE!</v>
       </c>
       <c r="AD96" s="160" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8398,6 +8248,36 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="42">
+    <mergeCell ref="AG1:AJ1"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="AG9:AH9"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="I84:J84"/>
+    <mergeCell ref="K84:L84"/>
+    <mergeCell ref="I85:J85"/>
+    <mergeCell ref="K85:L85"/>
+    <mergeCell ref="V77:V78"/>
+    <mergeCell ref="V75:V76"/>
+    <mergeCell ref="V73:V74"/>
+    <mergeCell ref="W73:W74"/>
+    <mergeCell ref="W75:W76"/>
+    <mergeCell ref="W77:W78"/>
     <mergeCell ref="I87:J87"/>
     <mergeCell ref="K87:L87"/>
     <mergeCell ref="Q86:R86"/>
@@ -8410,36 +8290,6 @@
     <mergeCell ref="S77:S78"/>
     <mergeCell ref="I86:J86"/>
     <mergeCell ref="K86:L86"/>
-    <mergeCell ref="V77:V78"/>
-    <mergeCell ref="V75:V76"/>
-    <mergeCell ref="V73:V74"/>
-    <mergeCell ref="W73:W74"/>
-    <mergeCell ref="W75:W76"/>
-    <mergeCell ref="W77:W78"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="I84:J84"/>
-    <mergeCell ref="K84:L84"/>
-    <mergeCell ref="I85:J85"/>
-    <mergeCell ref="K85:L85"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="AG1:AJ1"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="AG9:AH9"/>
   </mergeCells>
   <conditionalFormatting sqref="D27:D28">
     <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
@@ -8551,7 +8401,7 @@
       <c r="K1" s="136"/>
       <c r="L1" s="176"/>
       <c r="R1" s="83" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="20.399999999999999">
@@ -8564,7 +8414,7 @@
       </c>
       <c r="L2" s="178"/>
       <c r="R2" s="83" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="20.399999999999999">
@@ -8653,19 +8503,19 @@
       <c r="D10" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="191" t="str">
+      <c r="E10" s="221" t="str">
         <f>Barco!E10</f>
         <v/>
       </c>
-      <c r="F10" s="191"/>
+      <c r="F10" s="221"/>
       <c r="I10" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="191" t="str">
+      <c r="J10" s="221" t="str">
         <f>Barco!J10</f>
         <v/>
       </c>
-      <c r="K10" s="191"/>
+      <c r="K10" s="221"/>
       <c r="L10" s="178"/>
     </row>
     <row r="11" spans="1:18">
@@ -8676,19 +8526,19 @@
       <c r="D11" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="191" t="str">
+      <c r="E11" s="221" t="str">
         <f>Barco!E11</f>
         <v/>
       </c>
-      <c r="F11" s="191"/>
+      <c r="F11" s="221"/>
       <c r="I11" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="191" t="str">
+      <c r="J11" s="221" t="str">
         <f>Barco!J11</f>
         <v/>
       </c>
-      <c r="K11" s="191"/>
+      <c r="K11" s="221"/>
       <c r="L11" s="178"/>
     </row>
     <row r="12" spans="1:18">
@@ -8699,19 +8549,19 @@
       <c r="D12" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="191" t="str">
+      <c r="E12" s="221" t="str">
         <f>Barco!E12</f>
         <v/>
       </c>
-      <c r="F12" s="191"/>
+      <c r="F12" s="221"/>
       <c r="I12" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="191" t="str">
+      <c r="J12" s="221" t="str">
         <f>Barco!J12</f>
         <v/>
       </c>
-      <c r="K12" s="191"/>
+      <c r="K12" s="221"/>
       <c r="L12" s="178"/>
     </row>
     <row r="13" spans="1:18">
@@ -8722,19 +8572,19 @@
       <c r="D13" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="191" t="str">
+      <c r="E13" s="221" t="str">
         <f>Barco!E13</f>
         <v/>
       </c>
-      <c r="F13" s="191"/>
+      <c r="F13" s="221"/>
       <c r="I13" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="191" t="str">
+      <c r="J13" s="221" t="str">
         <f>Barco!J14</f>
         <v/>
       </c>
-      <c r="K13" s="191"/>
+      <c r="K13" s="221"/>
       <c r="L13" s="178"/>
     </row>
     <row r="14" spans="1:18">
@@ -8745,19 +8595,19 @@
       <c r="D14" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="191" t="str">
+      <c r="E14" s="221" t="str">
         <f>Barco!E14</f>
         <v/>
       </c>
-      <c r="F14" s="191"/>
+      <c r="F14" s="221"/>
       <c r="I14" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="191" t="str">
+      <c r="J14" s="221" t="str">
         <f>Barco!J15</f>
         <v/>
       </c>
-      <c r="K14" s="191"/>
+      <c r="K14" s="221"/>
       <c r="L14" s="178"/>
     </row>
     <row r="15" spans="1:18">
@@ -8768,11 +8618,11 @@
       <c r="D15" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="191" t="str">
+      <c r="E15" s="221" t="str">
         <f>Barco!E15</f>
         <v>Barco K5905277 v18</v>
       </c>
-      <c r="F15" s="191"/>
+      <c r="F15" s="221"/>
       <c r="L15" s="178"/>
     </row>
     <row r="16" spans="1:18" ht="16.2" thickBot="1">
@@ -8801,7 +8651,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="184" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C18" s="136"/>
       <c r="D18" s="136"/>
@@ -8826,14 +8676,14 @@
         <v>20</v>
       </c>
       <c r="B20" s="177"/>
-      <c r="F20" s="222" t="s">
+      <c r="F20" s="228" t="s">
+        <v>192</v>
+      </c>
+      <c r="G20" s="228"/>
+      <c r="H20" s="228" t="s">
         <v>193</v>
       </c>
-      <c r="G20" s="222"/>
-      <c r="H20" s="222" t="s">
-        <v>194</v>
-      </c>
-      <c r="I20" s="222"/>
+      <c r="I20" s="228"/>
       <c r="L20" s="178"/>
     </row>
     <row r="21" spans="1:12">
@@ -8841,16 +8691,16 @@
         <v>21</v>
       </c>
       <c r="B21" s="177"/>
-      <c r="F21" s="222" t="str">
+      <c r="F21" s="228" t="str">
         <f>J13</f>
         <v/>
       </c>
-      <c r="G21" s="222"/>
-      <c r="H21" s="222" t="str">
+      <c r="G21" s="228"/>
+      <c r="H21" s="228" t="str">
         <f>J14</f>
         <v/>
       </c>
-      <c r="I21" s="222"/>
+      <c r="I21" s="228"/>
       <c r="L21" s="178"/>
     </row>
     <row r="22" spans="1:12">
@@ -8859,15 +8709,15 @@
       </c>
       <c r="B22" s="177"/>
       <c r="E22" s="48" t="s">
-        <v>186</v>
-      </c>
-      <c r="F22" s="223" t="str">
+        <v>185</v>
+      </c>
+      <c r="F22" s="227" t="str">
         <f>IF(Barco!E23="","",IF(Barco!E23="YES","PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="G22" s="223"/>
-      <c r="H22" s="223"/>
-      <c r="I22" s="223"/>
+      <c r="G22" s="227"/>
+      <c r="H22" s="227"/>
+      <c r="I22" s="227"/>
       <c r="L22" s="178"/>
     </row>
     <row r="23" spans="1:12">
@@ -8876,15 +8726,15 @@
       </c>
       <c r="B23" s="177"/>
       <c r="E23" s="48" t="s">
-        <v>187</v>
-      </c>
-      <c r="F23" s="223" t="str">
+        <v>186</v>
+      </c>
+      <c r="F23" s="227" t="str">
         <f>IF(Barco!E22="","",IF(Barco!E22="YES","PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="G23" s="223"/>
-      <c r="H23" s="223"/>
-      <c r="I23" s="223"/>
+      <c r="G23" s="227"/>
+      <c r="H23" s="227"/>
+      <c r="I23" s="227"/>
       <c r="L23" s="178"/>
     </row>
     <row r="24" spans="1:12">
@@ -8893,15 +8743,15 @@
       </c>
       <c r="B24" s="177"/>
       <c r="E24" s="48" t="s">
-        <v>188</v>
-      </c>
-      <c r="F24" s="223" t="str">
+        <v>187</v>
+      </c>
+      <c r="F24" s="227" t="str">
         <f>IF(OR(Barco!I72="TBD",Barco!I73="TBD"),"",IF(AND(Barco!I72="YES",Barco!I73="YES"),"PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="G24" s="223"/>
-      <c r="H24" s="223"/>
-      <c r="I24" s="223"/>
+      <c r="G24" s="227"/>
+      <c r="H24" s="227"/>
+      <c r="I24" s="227"/>
       <c r="L24" s="178"/>
     </row>
     <row r="25" spans="1:12">
@@ -8910,12 +8760,12 @@
       </c>
       <c r="B25" s="177"/>
       <c r="E25" s="48" t="s">
-        <v>189</v>
-      </c>
-      <c r="F25" s="219"/>
-      <c r="G25" s="219"/>
-      <c r="H25" s="219"/>
-      <c r="I25" s="219"/>
+        <v>188</v>
+      </c>
+      <c r="F25" s="224"/>
+      <c r="G25" s="224"/>
+      <c r="H25" s="224"/>
+      <c r="I25" s="224"/>
       <c r="L25" s="178"/>
     </row>
     <row r="26" spans="1:12">
@@ -8924,18 +8774,18 @@
       </c>
       <c r="B26" s="177"/>
       <c r="D26" s="83" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E26" s="48" t="s">
-        <v>190</v>
-      </c>
-      <c r="F26" s="223" t="str">
+        <v>189</v>
+      </c>
+      <c r="F26" s="227" t="str">
         <f>IF(Barco!F85="","",IF(Barco!F85="YES","PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="G26" s="223"/>
-      <c r="H26" s="223"/>
-      <c r="I26" s="223"/>
+      <c r="G26" s="227"/>
+      <c r="H26" s="227"/>
+      <c r="I26" s="227"/>
       <c r="L26" s="178"/>
     </row>
     <row r="27" spans="1:12">
@@ -8944,12 +8794,12 @@
       </c>
       <c r="B27" s="177"/>
       <c r="E27" s="48" t="s">
-        <v>191</v>
-      </c>
-      <c r="F27" s="219"/>
-      <c r="G27" s="219"/>
-      <c r="H27" s="219"/>
-      <c r="I27" s="219"/>
+        <v>190</v>
+      </c>
+      <c r="F27" s="224"/>
+      <c r="G27" s="224"/>
+      <c r="H27" s="224"/>
+      <c r="I27" s="224"/>
       <c r="L27" s="178"/>
     </row>
     <row r="28" spans="1:12">
@@ -8958,12 +8808,12 @@
       </c>
       <c r="B28" s="177"/>
       <c r="E28" s="48" t="s">
-        <v>192</v>
-      </c>
-      <c r="F28" s="219"/>
-      <c r="G28" s="219"/>
-      <c r="H28" s="219"/>
-      <c r="I28" s="219"/>
+        <v>191</v>
+      </c>
+      <c r="F28" s="224"/>
+      <c r="G28" s="224"/>
+      <c r="H28" s="224"/>
+      <c r="I28" s="224"/>
       <c r="L28" s="178"/>
     </row>
     <row r="29" spans="1:12">
@@ -8972,18 +8822,18 @@
       </c>
       <c r="B29" s="177"/>
       <c r="E29" s="48" t="s">
-        <v>198</v>
-      </c>
-      <c r="F29" s="220" t="str">
+        <v>197</v>
+      </c>
+      <c r="F29" s="225" t="str">
         <f>IF(Barco!F86="","",IF(Barco!F86="YES","PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="G29" s="221"/>
-      <c r="H29" s="220" t="str">
+      <c r="G29" s="226"/>
+      <c r="H29" s="225" t="str">
         <f>IF(Barco!G86="","",IF(Barco!G86="YES","PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="I29" s="221"/>
+      <c r="I29" s="226"/>
       <c r="L29" s="178"/>
     </row>
     <row r="30" spans="1:12">
@@ -9157,6 +9007,29 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="H29:I29"/>
     <mergeCell ref="H25:I25"/>
@@ -9164,30 +9037,7 @@
     <mergeCell ref="F27:G27"/>
     <mergeCell ref="F28:G28"/>
     <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
     <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="J12:K12"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F25:I25 F27:I28" xr:uid="{CEAD9B4F-4A05-4883-9435-EBBC3722EE42}">

</xml_diff>

<commit_message>
Fix incorrect monitor model in max ambient illum table
</commit_message>
<xml_diff>
--- a/MUSCMammoMonitor.xlsx
+++ b/MUSCMammoMonitor.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3C7225-A6FA-43CD-A183-AD8D0E508F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC41648A-0D69-4614-A472-0CB45631F962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -727,9 +727,6 @@
     <t>MDMG-5221</t>
   </si>
   <si>
-    <t>MDMNC-12130</t>
-  </si>
-  <si>
     <t>MDNC-6121</t>
   </si>
   <si>
@@ -737,6 +734,9 @@
   </si>
   <si>
     <t>Revision 1.7-20250603</t>
+  </si>
+  <si>
+    <t>MDNC-12130</t>
   </si>
 </sst>
 </file>
@@ -2330,6 +2330,72 @@
     <xf numFmtId="167" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2363,85 +2429,19 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2955,8 +2955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AG15" sqref="AG15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -2986,7 +2986,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
       <c r="O1" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
@@ -3001,12 +3001,12 @@
       <c r="AA1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="AG1" s="218" t="s">
+      <c r="AG1" s="191" t="s">
         <v>1</v>
       </c>
-      <c r="AH1" s="218"/>
-      <c r="AI1" s="218"/>
-      <c r="AJ1" s="218"/>
+      <c r="AH1" s="191"/>
+      <c r="AI1" s="191"/>
+      <c r="AJ1" s="191"/>
     </row>
     <row r="2" spans="1:36" ht="14.4" customHeight="1">
       <c r="A2" s="1">
@@ -3025,14 +3025,14 @@
       <c r="AA2" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="AG2" s="219" t="s">
+      <c r="AG2" s="192" t="s">
         <v>3</v>
       </c>
-      <c r="AH2" s="219"/>
-      <c r="AI2" s="220" t="s">
+      <c r="AH2" s="192"/>
+      <c r="AI2" s="193" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="220"/>
+      <c r="AJ2" s="193"/>
     </row>
     <row r="3" spans="1:36" ht="14.4" customHeight="1">
       <c r="A3" s="1">
@@ -3305,10 +3305,10 @@
         <v>Eugene Mah</v>
       </c>
       <c r="AF9"/>
-      <c r="AG9" s="222" t="s">
+      <c r="AG9" s="195" t="s">
         <v>201</v>
       </c>
-      <c r="AH9" s="223"/>
+      <c r="AH9" s="196"/>
     </row>
     <row r="10" spans="1:36" ht="14.4" customHeight="1">
       <c r="A10" s="1">
@@ -3318,19 +3318,19 @@
       <c r="D10" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="221" t="str">
+      <c r="E10" s="194" t="str">
         <f t="shared" ref="E10:E15" si="1">IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="F10" s="221"/>
+      <c r="F10" s="194"/>
       <c r="I10" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="221" t="str">
+      <c r="J10" s="194" t="str">
         <f t="shared" ref="J10:J15" si="2">IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="K10" s="221"/>
+      <c r="K10" s="194"/>
       <c r="M10" s="11"/>
       <c r="O10" s="12"/>
       <c r="Q10" s="20" t="s">
@@ -3378,19 +3378,19 @@
       <c r="D11" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="214" t="str">
+      <c r="E11" s="197" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F11" s="214"/>
+      <c r="F11" s="197"/>
       <c r="I11" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="217" t="str">
+      <c r="J11" s="198" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K11" s="217"/>
+      <c r="K11" s="198"/>
       <c r="M11" s="11"/>
       <c r="O11" s="12"/>
       <c r="Q11" s="20" t="s">
@@ -3438,19 +3438,19 @@
       <c r="D12" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="214" t="str">
+      <c r="E12" s="197" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F12" s="214"/>
+      <c r="F12" s="197"/>
       <c r="I12" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="214" t="str">
+      <c r="J12" s="197" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K12" s="214"/>
+      <c r="K12" s="197"/>
       <c r="M12" s="11"/>
       <c r="O12" s="12"/>
       <c r="Q12" s="20" t="s">
@@ -3498,19 +3498,19 @@
       <c r="D13" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="214" t="str">
+      <c r="E13" s="197" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F13" s="214"/>
+      <c r="F13" s="197"/>
       <c r="I13" s="48" t="s">
         <v>199</v>
       </c>
-      <c r="J13" s="214" t="str">
+      <c r="J13" s="197" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K13" s="214"/>
+      <c r="K13" s="197"/>
       <c r="M13" s="11"/>
       <c r="O13" s="12"/>
       <c r="Q13" s="20" t="s">
@@ -3558,19 +3558,19 @@
       <c r="D14" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="214" t="str">
+      <c r="E14" s="197" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F14" s="214"/>
+      <c r="F14" s="197"/>
       <c r="I14" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="J14" s="214" t="str">
+      <c r="J14" s="197" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K14" s="214"/>
+      <c r="K14" s="197"/>
       <c r="M14" s="11"/>
       <c r="O14" s="12"/>
       <c r="Q14" s="20" t="s">
@@ -3604,7 +3604,7 @@
       </c>
       <c r="AF14"/>
       <c r="AG14" s="15" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="AH14" s="16">
         <v>40</v>
@@ -3618,19 +3618,19 @@
       <c r="D15" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="214" t="str">
+      <c r="E15" s="197" t="str">
         <f t="shared" si="1"/>
         <v>Barco K5905277 v18</v>
       </c>
-      <c r="F15" s="214"/>
+      <c r="F15" s="197"/>
       <c r="I15" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="J15" s="214" t="str">
+      <c r="J15" s="197" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K15" s="214"/>
+      <c r="K15" s="197"/>
       <c r="M15" s="11"/>
       <c r="O15" s="25"/>
       <c r="P15" s="26"/>
@@ -3669,7 +3669,7 @@
       </c>
       <c r="AF15"/>
       <c r="AG15" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AH15" s="16">
         <v>20</v>
@@ -3705,7 +3705,7 @@
       </c>
       <c r="AF16"/>
       <c r="AG16" s="36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AH16" s="38">
         <v>20</v>
@@ -3789,10 +3789,10 @@
       <c r="H19" s="136"/>
       <c r="I19" s="136"/>
       <c r="J19" s="136"/>
-      <c r="K19" s="216" t="s">
+      <c r="K19" s="200" t="s">
         <v>127</v>
       </c>
-      <c r="L19" s="216"/>
+      <c r="L19" s="200"/>
       <c r="M19" s="4"/>
       <c r="O19" s="12"/>
       <c r="R19" s="1" t="s">
@@ -4037,11 +4037,11 @@
       <c r="D24" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="E24" s="215" t="str">
+      <c r="E24" s="199" t="str">
         <f>IF(P52="","",P52)</f>
         <v/>
       </c>
-      <c r="F24" s="215"/>
+      <c r="F24" s="199"/>
       <c r="M24" s="11"/>
       <c r="O24" s="12"/>
       <c r="Y24" s="13"/>
@@ -5901,16 +5901,16 @@
       </c>
       <c r="B71" s="9"/>
       <c r="C71" s="83"/>
-      <c r="D71" s="211" t="str">
+      <c r="D71" s="201" t="str">
         <f>Q86</f>
         <v>UNL-10 (cd/m^2)</v>
       </c>
-      <c r="E71" s="211"/>
-      <c r="F71" s="212" t="str">
+      <c r="E71" s="201"/>
+      <c r="F71" s="202" t="str">
         <f>S86</f>
         <v>UNL-80 (cd/m^2)</v>
       </c>
-      <c r="G71" s="212"/>
+      <c r="G71" s="202"/>
       <c r="I71" s="60" t="s">
         <v>106</v>
       </c>
@@ -6013,13 +6013,13 @@
       <c r="Q73" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="R73" s="194"/>
-      <c r="S73" s="198"/>
-      <c r="V73" s="206" t="str">
+      <c r="R73" s="216"/>
+      <c r="S73" s="220"/>
+      <c r="V73" s="208" t="str">
         <f>IF(AB48="","",AB48)</f>
         <v/>
       </c>
-      <c r="W73" s="207" t="str">
+      <c r="W73" s="209" t="str">
         <f>IF(AB51="","",AB51)</f>
         <v/>
       </c>
@@ -6061,10 +6061,10 @@
       <c r="M74" s="11"/>
       <c r="O74" s="12"/>
       <c r="Q74" s="19"/>
-      <c r="R74" s="195"/>
-      <c r="S74" s="199"/>
-      <c r="V74" s="205"/>
-      <c r="W74" s="208"/>
+      <c r="R74" s="217"/>
+      <c r="S74" s="221"/>
+      <c r="V74" s="207"/>
+      <c r="W74" s="210"/>
       <c r="Y74" s="13"/>
       <c r="AB74" s="139"/>
       <c r="AC74" s="34" t="str">
@@ -6105,13 +6105,13 @@
       <c r="Q75" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="R75" s="196"/>
-      <c r="S75" s="200"/>
-      <c r="V75" s="203" t="str">
+      <c r="R75" s="218"/>
+      <c r="S75" s="222"/>
+      <c r="V75" s="205" t="str">
         <f>IF(AB49="","",AB49)</f>
         <v/>
       </c>
-      <c r="W75" s="209" t="str">
+      <c r="W75" s="211" t="str">
         <f>IF(AB52="","",AB52)</f>
         <v/>
       </c>
@@ -6152,10 +6152,10 @@
       <c r="M76" s="11"/>
       <c r="O76" s="12"/>
       <c r="Q76" s="19"/>
-      <c r="R76" s="195"/>
-      <c r="S76" s="199"/>
-      <c r="V76" s="205"/>
-      <c r="W76" s="208"/>
+      <c r="R76" s="217"/>
+      <c r="S76" s="221"/>
+      <c r="V76" s="207"/>
+      <c r="W76" s="210"/>
       <c r="Y76" s="13"/>
       <c r="AB76" s="139"/>
       <c r="AC76" s="34" t="str">
@@ -6196,13 +6196,13 @@
       <c r="Q77" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="R77" s="196"/>
-      <c r="S77" s="200"/>
-      <c r="V77" s="203" t="str">
+      <c r="R77" s="218"/>
+      <c r="S77" s="222"/>
+      <c r="V77" s="205" t="str">
         <f>IF(AB50="","",AB50)</f>
         <v/>
       </c>
-      <c r="W77" s="209" t="str">
+      <c r="W77" s="211" t="str">
         <f>IF(AB53="","",AB53)</f>
         <v/>
       </c>
@@ -6218,10 +6218,10 @@
       <c r="M78" s="11"/>
       <c r="O78" s="12"/>
       <c r="Q78" s="19"/>
-      <c r="R78" s="197"/>
-      <c r="S78" s="201"/>
-      <c r="V78" s="204"/>
-      <c r="W78" s="210"/>
+      <c r="R78" s="219"/>
+      <c r="S78" s="223"/>
+      <c r="V78" s="206"/>
+      <c r="W78" s="212"/>
       <c r="Y78" s="13"/>
       <c r="AB78" s="139"/>
       <c r="AC78" s="34" t="str">
@@ -6408,16 +6408,16 @@
         <f>S68</f>
         <v>Right ()</v>
       </c>
-      <c r="I84" s="213" t="str">
+      <c r="I84" s="203" t="str">
         <f>R68</f>
         <v>Left ()</v>
       </c>
-      <c r="J84" s="213"/>
-      <c r="K84" s="213" t="str">
+      <c r="J84" s="203"/>
+      <c r="K84" s="203" t="str">
         <f>S68</f>
         <v>Right ()</v>
       </c>
-      <c r="L84" s="213"/>
+      <c r="L84" s="203"/>
       <c r="M84" s="11"/>
       <c r="O84" s="12"/>
       <c r="Y84" s="13"/>
@@ -6450,16 +6450,16 @@
       <c r="H85" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="I85" s="202" t="str">
+      <c r="I85" s="204" t="str">
         <f>IF(R73="","",R73)</f>
         <v/>
       </c>
-      <c r="J85" s="202"/>
-      <c r="K85" s="202" t="str">
+      <c r="J85" s="204"/>
+      <c r="K85" s="204" t="str">
         <f>IF(S73="","",S73)</f>
         <v/>
       </c>
-      <c r="L85" s="202"/>
+      <c r="L85" s="204"/>
       <c r="M85" s="11"/>
       <c r="O85" s="97" t="s">
         <v>105</v>
@@ -6488,26 +6488,26 @@
       <c r="H86" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="I86" s="202" t="str">
+      <c r="I86" s="204" t="str">
         <f>IF(R75="","",R75)</f>
         <v/>
       </c>
-      <c r="J86" s="202"/>
-      <c r="K86" s="202" t="str">
+      <c r="J86" s="204"/>
+      <c r="K86" s="204" t="str">
         <f>IF(S75="","",S75)</f>
         <v/>
       </c>
-      <c r="L86" s="202"/>
+      <c r="L86" s="204"/>
       <c r="M86" s="11"/>
       <c r="O86" s="12"/>
-      <c r="Q86" s="192" t="s">
+      <c r="Q86" s="214" t="s">
         <v>116</v>
       </c>
-      <c r="R86" s="193"/>
-      <c r="S86" s="192" t="s">
+      <c r="R86" s="215"/>
+      <c r="S86" s="214" t="s">
         <v>117</v>
       </c>
-      <c r="T86" s="193"/>
+      <c r="T86" s="215"/>
       <c r="V86" s="113" t="s">
         <v>43</v>
       </c>
@@ -6532,16 +6532,16 @@
       <c r="H87" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="I87" s="191" t="str">
+      <c r="I87" s="213" t="str">
         <f>IF(R77="","",R77)</f>
         <v/>
       </c>
-      <c r="J87" s="191"/>
-      <c r="K87" s="191" t="str">
+      <c r="J87" s="213"/>
+      <c r="K87" s="213" t="str">
         <f>IF(S77="","",S77)</f>
         <v/>
       </c>
-      <c r="L87" s="191"/>
+      <c r="L87" s="213"/>
       <c r="M87" s="11"/>
       <c r="O87" s="12"/>
       <c r="Q87" s="114" t="str">
@@ -8248,36 +8248,6 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="42">
-    <mergeCell ref="AG1:AJ1"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="AG9:AH9"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="I84:J84"/>
-    <mergeCell ref="K84:L84"/>
-    <mergeCell ref="I85:J85"/>
-    <mergeCell ref="K85:L85"/>
-    <mergeCell ref="V77:V78"/>
-    <mergeCell ref="V75:V76"/>
-    <mergeCell ref="V73:V74"/>
-    <mergeCell ref="W73:W74"/>
-    <mergeCell ref="W75:W76"/>
-    <mergeCell ref="W77:W78"/>
     <mergeCell ref="I87:J87"/>
     <mergeCell ref="K87:L87"/>
     <mergeCell ref="Q86:R86"/>
@@ -8290,6 +8260,36 @@
     <mergeCell ref="S77:S78"/>
     <mergeCell ref="I86:J86"/>
     <mergeCell ref="K86:L86"/>
+    <mergeCell ref="V77:V78"/>
+    <mergeCell ref="V75:V76"/>
+    <mergeCell ref="V73:V74"/>
+    <mergeCell ref="W73:W74"/>
+    <mergeCell ref="W75:W76"/>
+    <mergeCell ref="W77:W78"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="I84:J84"/>
+    <mergeCell ref="K84:L84"/>
+    <mergeCell ref="I85:J85"/>
+    <mergeCell ref="K85:L85"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="AG1:AJ1"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="AG9:AH9"/>
   </mergeCells>
   <conditionalFormatting sqref="D27:D28">
     <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
@@ -8503,19 +8503,19 @@
       <c r="D10" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="221" t="str">
+      <c r="E10" s="194" t="str">
         <f>Barco!E10</f>
         <v/>
       </c>
-      <c r="F10" s="221"/>
+      <c r="F10" s="194"/>
       <c r="I10" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="221" t="str">
+      <c r="J10" s="194" t="str">
         <f>Barco!J10</f>
         <v/>
       </c>
-      <c r="K10" s="221"/>
+      <c r="K10" s="194"/>
       <c r="L10" s="178"/>
     </row>
     <row r="11" spans="1:18">
@@ -8526,19 +8526,19 @@
       <c r="D11" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="221" t="str">
+      <c r="E11" s="194" t="str">
         <f>Barco!E11</f>
         <v/>
       </c>
-      <c r="F11" s="221"/>
+      <c r="F11" s="194"/>
       <c r="I11" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="221" t="str">
+      <c r="J11" s="194" t="str">
         <f>Barco!J11</f>
         <v/>
       </c>
-      <c r="K11" s="221"/>
+      <c r="K11" s="194"/>
       <c r="L11" s="178"/>
     </row>
     <row r="12" spans="1:18">
@@ -8549,19 +8549,19 @@
       <c r="D12" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="221" t="str">
+      <c r="E12" s="194" t="str">
         <f>Barco!E12</f>
         <v/>
       </c>
-      <c r="F12" s="221"/>
+      <c r="F12" s="194"/>
       <c r="I12" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="221" t="str">
+      <c r="J12" s="194" t="str">
         <f>Barco!J12</f>
         <v/>
       </c>
-      <c r="K12" s="221"/>
+      <c r="K12" s="194"/>
       <c r="L12" s="178"/>
     </row>
     <row r="13" spans="1:18">
@@ -8572,19 +8572,19 @@
       <c r="D13" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="221" t="str">
+      <c r="E13" s="194" t="str">
         <f>Barco!E13</f>
         <v/>
       </c>
-      <c r="F13" s="221"/>
+      <c r="F13" s="194"/>
       <c r="I13" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="221" t="str">
+      <c r="J13" s="194" t="str">
         <f>Barco!J14</f>
         <v/>
       </c>
-      <c r="K13" s="221"/>
+      <c r="K13" s="194"/>
       <c r="L13" s="178"/>
     </row>
     <row r="14" spans="1:18">
@@ -8595,19 +8595,19 @@
       <c r="D14" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="221" t="str">
+      <c r="E14" s="194" t="str">
         <f>Barco!E14</f>
         <v/>
       </c>
-      <c r="F14" s="221"/>
+      <c r="F14" s="194"/>
       <c r="I14" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="221" t="str">
+      <c r="J14" s="194" t="str">
         <f>Barco!J15</f>
         <v/>
       </c>
-      <c r="K14" s="221"/>
+      <c r="K14" s="194"/>
       <c r="L14" s="178"/>
     </row>
     <row r="15" spans="1:18">
@@ -8618,11 +8618,11 @@
       <c r="D15" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="221" t="str">
+      <c r="E15" s="194" t="str">
         <f>Barco!E15</f>
         <v>Barco K5905277 v18</v>
       </c>
-      <c r="F15" s="221"/>
+      <c r="F15" s="194"/>
       <c r="L15" s="178"/>
     </row>
     <row r="16" spans="1:18" ht="16.2" thickBot="1">
@@ -8676,14 +8676,14 @@
         <v>20</v>
       </c>
       <c r="B20" s="177"/>
-      <c r="F20" s="228" t="s">
+      <c r="F20" s="224" t="s">
         <v>192</v>
       </c>
-      <c r="G20" s="228"/>
-      <c r="H20" s="228" t="s">
+      <c r="G20" s="224"/>
+      <c r="H20" s="224" t="s">
         <v>193</v>
       </c>
-      <c r="I20" s="228"/>
+      <c r="I20" s="224"/>
       <c r="L20" s="178"/>
     </row>
     <row r="21" spans="1:12">
@@ -8691,16 +8691,16 @@
         <v>21</v>
       </c>
       <c r="B21" s="177"/>
-      <c r="F21" s="228" t="str">
+      <c r="F21" s="224" t="str">
         <f>J13</f>
         <v/>
       </c>
-      <c r="G21" s="228"/>
-      <c r="H21" s="228" t="str">
+      <c r="G21" s="224"/>
+      <c r="H21" s="224" t="str">
         <f>J14</f>
         <v/>
       </c>
-      <c r="I21" s="228"/>
+      <c r="I21" s="224"/>
       <c r="L21" s="178"/>
     </row>
     <row r="22" spans="1:12">
@@ -8711,13 +8711,13 @@
       <c r="E22" s="48" t="s">
         <v>185</v>
       </c>
-      <c r="F22" s="227" t="str">
+      <c r="F22" s="226" t="str">
         <f>IF(Barco!E23="","",IF(Barco!E23="YES","PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="G22" s="227"/>
-      <c r="H22" s="227"/>
-      <c r="I22" s="227"/>
+      <c r="G22" s="226"/>
+      <c r="H22" s="226"/>
+      <c r="I22" s="226"/>
       <c r="L22" s="178"/>
     </row>
     <row r="23" spans="1:12">
@@ -8728,13 +8728,13 @@
       <c r="E23" s="48" t="s">
         <v>186</v>
       </c>
-      <c r="F23" s="227" t="str">
+      <c r="F23" s="226" t="str">
         <f>IF(Barco!E22="","",IF(Barco!E22="YES","PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="G23" s="227"/>
-      <c r="H23" s="227"/>
-      <c r="I23" s="227"/>
+      <c r="G23" s="226"/>
+      <c r="H23" s="226"/>
+      <c r="I23" s="226"/>
       <c r="L23" s="178"/>
     </row>
     <row r="24" spans="1:12">
@@ -8745,13 +8745,13 @@
       <c r="E24" s="48" t="s">
         <v>187</v>
       </c>
-      <c r="F24" s="227" t="str">
+      <c r="F24" s="226" t="str">
         <f>IF(OR(Barco!I72="TBD",Barco!I73="TBD"),"",IF(AND(Barco!I72="YES",Barco!I73="YES"),"PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="G24" s="227"/>
-      <c r="H24" s="227"/>
-      <c r="I24" s="227"/>
+      <c r="G24" s="226"/>
+      <c r="H24" s="226"/>
+      <c r="I24" s="226"/>
       <c r="L24" s="178"/>
     </row>
     <row r="25" spans="1:12">
@@ -8762,10 +8762,10 @@
       <c r="E25" s="48" t="s">
         <v>188</v>
       </c>
-      <c r="F25" s="224"/>
-      <c r="G25" s="224"/>
-      <c r="H25" s="224"/>
-      <c r="I25" s="224"/>
+      <c r="F25" s="225"/>
+      <c r="G25" s="225"/>
+      <c r="H25" s="225"/>
+      <c r="I25" s="225"/>
       <c r="L25" s="178"/>
     </row>
     <row r="26" spans="1:12">
@@ -8779,13 +8779,13 @@
       <c r="E26" s="48" t="s">
         <v>189</v>
       </c>
-      <c r="F26" s="227" t="str">
+      <c r="F26" s="226" t="str">
         <f>IF(Barco!F85="","",IF(Barco!F85="YES","PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="G26" s="227"/>
-      <c r="H26" s="227"/>
-      <c r="I26" s="227"/>
+      <c r="G26" s="226"/>
+      <c r="H26" s="226"/>
+      <c r="I26" s="226"/>
       <c r="L26" s="178"/>
     </row>
     <row r="27" spans="1:12">
@@ -8796,10 +8796,10 @@
       <c r="E27" s="48" t="s">
         <v>190</v>
       </c>
-      <c r="F27" s="224"/>
-      <c r="G27" s="224"/>
-      <c r="H27" s="224"/>
-      <c r="I27" s="224"/>
+      <c r="F27" s="225"/>
+      <c r="G27" s="225"/>
+      <c r="H27" s="225"/>
+      <c r="I27" s="225"/>
       <c r="L27" s="178"/>
     </row>
     <row r="28" spans="1:12">
@@ -8810,10 +8810,10 @@
       <c r="E28" s="48" t="s">
         <v>191</v>
       </c>
-      <c r="F28" s="224"/>
-      <c r="G28" s="224"/>
-      <c r="H28" s="224"/>
-      <c r="I28" s="224"/>
+      <c r="F28" s="225"/>
+      <c r="G28" s="225"/>
+      <c r="H28" s="225"/>
+      <c r="I28" s="225"/>
       <c r="L28" s="178"/>
     </row>
     <row r="29" spans="1:12">
@@ -8824,16 +8824,16 @@
       <c r="E29" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="F29" s="225" t="str">
+      <c r="F29" s="227" t="str">
         <f>IF(Barco!F86="","",IF(Barco!F86="YES","PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="G29" s="226"/>
-      <c r="H29" s="225" t="str">
+      <c r="G29" s="228"/>
+      <c r="H29" s="227" t="str">
         <f>IF(Barco!G86="","",IF(Barco!G86="YES","PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="I29" s="226"/>
+      <c r="I29" s="228"/>
       <c r="L29" s="178"/>
     </row>
     <row r="30" spans="1:12">
@@ -9007,12 +9007,15 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H27:I27"/>
     <mergeCell ref="E13:F13"/>
@@ -9029,15 +9032,12 @@
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="J12:K12"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F25:I25 F27:I28" xr:uid="{CEAD9B4F-4A05-4883-9435-EBBC3722EE42}">

</xml_diff>

<commit_message>
Updates to accomodate RTI template changes
</commit_message>
<xml_diff>
--- a/MUSCMammoMonitor.xlsx
+++ b/MUSCMammoMonitor.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC41648A-0D69-4614-A472-0CB45631F962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CB544F-0450-48A3-9DC2-21A0B29942A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2330,44 +2330,38 @@
     <xf numFmtId="167" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2396,52 +2390,58 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2956,7 +2956,7 @@
   <dimension ref="A1:AJ132"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AG15" sqref="AG15"/>
+      <selection activeCell="AF7" sqref="AF7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -3001,12 +3001,12 @@
       <c r="AA1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="AG1" s="191" t="s">
+      <c r="AG1" s="218" t="s">
         <v>1</v>
       </c>
-      <c r="AH1" s="191"/>
-      <c r="AI1" s="191"/>
-      <c r="AJ1" s="191"/>
+      <c r="AH1" s="218"/>
+      <c r="AI1" s="218"/>
+      <c r="AJ1" s="218"/>
     </row>
     <row r="2" spans="1:36" ht="14.4" customHeight="1">
       <c r="A2" s="1">
@@ -3025,14 +3025,14 @@
       <c r="AA2" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="AG2" s="192" t="s">
+      <c r="AG2" s="219" t="s">
         <v>3</v>
       </c>
-      <c r="AH2" s="192"/>
-      <c r="AI2" s="193" t="s">
+      <c r="AH2" s="219"/>
+      <c r="AI2" s="220" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="193"/>
+      <c r="AJ2" s="220"/>
     </row>
     <row r="3" spans="1:36" ht="14.4" customHeight="1">
       <c r="A3" s="1">
@@ -3305,10 +3305,10 @@
         <v>Eugene Mah</v>
       </c>
       <c r="AF9"/>
-      <c r="AG9" s="195" t="s">
+      <c r="AG9" s="222" t="s">
         <v>201</v>
       </c>
-      <c r="AH9" s="196"/>
+      <c r="AH9" s="223"/>
     </row>
     <row r="10" spans="1:36" ht="14.4" customHeight="1">
       <c r="A10" s="1">
@@ -3318,19 +3318,19 @@
       <c r="D10" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="194" t="str">
+      <c r="E10" s="221" t="str">
         <f t="shared" ref="E10:E15" si="1">IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="F10" s="194"/>
+      <c r="F10" s="221"/>
       <c r="I10" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="194" t="str">
+      <c r="J10" s="221" t="str">
         <f t="shared" ref="J10:J15" si="2">IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="K10" s="194"/>
+      <c r="K10" s="221"/>
       <c r="M10" s="11"/>
       <c r="O10" s="12"/>
       <c r="Q10" s="20" t="s">
@@ -3378,19 +3378,19 @@
       <c r="D11" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="197" t="str">
+      <c r="E11" s="214" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F11" s="197"/>
+      <c r="F11" s="214"/>
       <c r="I11" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="198" t="str">
+      <c r="J11" s="217" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K11" s="198"/>
+      <c r="K11" s="217"/>
       <c r="M11" s="11"/>
       <c r="O11" s="12"/>
       <c r="Q11" s="20" t="s">
@@ -3438,19 +3438,19 @@
       <c r="D12" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="197" t="str">
+      <c r="E12" s="214" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F12" s="197"/>
+      <c r="F12" s="214"/>
       <c r="I12" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="197" t="str">
+      <c r="J12" s="214" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K12" s="197"/>
+      <c r="K12" s="214"/>
       <c r="M12" s="11"/>
       <c r="O12" s="12"/>
       <c r="Q12" s="20" t="s">
@@ -3498,19 +3498,19 @@
       <c r="D13" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="197" t="str">
+      <c r="E13" s="214" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F13" s="197"/>
+      <c r="F13" s="214"/>
       <c r="I13" s="48" t="s">
         <v>199</v>
       </c>
-      <c r="J13" s="197" t="str">
+      <c r="J13" s="214" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K13" s="197"/>
+      <c r="K13" s="214"/>
       <c r="M13" s="11"/>
       <c r="O13" s="12"/>
       <c r="Q13" s="20" t="s">
@@ -3558,19 +3558,19 @@
       <c r="D14" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="197" t="str">
+      <c r="E14" s="214" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F14" s="197"/>
+      <c r="F14" s="214"/>
       <c r="I14" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="J14" s="197" t="str">
+      <c r="J14" s="214" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K14" s="197"/>
+      <c r="K14" s="214"/>
       <c r="M14" s="11"/>
       <c r="O14" s="12"/>
       <c r="Q14" s="20" t="s">
@@ -3618,19 +3618,19 @@
       <c r="D15" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="197" t="str">
+      <c r="E15" s="214" t="str">
         <f t="shared" si="1"/>
         <v>Barco K5905277 v18</v>
       </c>
-      <c r="F15" s="197"/>
+      <c r="F15" s="214"/>
       <c r="I15" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="J15" s="197" t="str">
+      <c r="J15" s="214" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K15" s="197"/>
+      <c r="K15" s="214"/>
       <c r="M15" s="11"/>
       <c r="O15" s="25"/>
       <c r="P15" s="26"/>
@@ -3789,10 +3789,10 @@
       <c r="H19" s="136"/>
       <c r="I19" s="136"/>
       <c r="J19" s="136"/>
-      <c r="K19" s="200" t="s">
+      <c r="K19" s="216" t="s">
         <v>127</v>
       </c>
-      <c r="L19" s="200"/>
+      <c r="L19" s="216"/>
       <c r="M19" s="4"/>
       <c r="O19" s="12"/>
       <c r="R19" s="1" t="s">
@@ -4037,11 +4037,11 @@
       <c r="D24" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="E24" s="199" t="str">
+      <c r="E24" s="215" t="str">
         <f>IF(P52="","",P52)</f>
         <v/>
       </c>
-      <c r="F24" s="199"/>
+      <c r="F24" s="215"/>
       <c r="M24" s="11"/>
       <c r="O24" s="12"/>
       <c r="Y24" s="13"/>
@@ -5901,16 +5901,16 @@
       </c>
       <c r="B71" s="9"/>
       <c r="C71" s="83"/>
-      <c r="D71" s="201" t="str">
+      <c r="D71" s="211" t="str">
         <f>Q86</f>
         <v>UNL-10 (cd/m^2)</v>
       </c>
-      <c r="E71" s="201"/>
-      <c r="F71" s="202" t="str">
+      <c r="E71" s="211"/>
+      <c r="F71" s="212" t="str">
         <f>S86</f>
         <v>UNL-80 (cd/m^2)</v>
       </c>
-      <c r="G71" s="202"/>
+      <c r="G71" s="212"/>
       <c r="I71" s="60" t="s">
         <v>106</v>
       </c>
@@ -6013,13 +6013,13 @@
       <c r="Q73" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="R73" s="216"/>
-      <c r="S73" s="220"/>
-      <c r="V73" s="208" t="str">
+      <c r="R73" s="194"/>
+      <c r="S73" s="198"/>
+      <c r="V73" s="206" t="str">
         <f>IF(AB48="","",AB48)</f>
         <v/>
       </c>
-      <c r="W73" s="209" t="str">
+      <c r="W73" s="207" t="str">
         <f>IF(AB51="","",AB51)</f>
         <v/>
       </c>
@@ -6061,10 +6061,10 @@
       <c r="M74" s="11"/>
       <c r="O74" s="12"/>
       <c r="Q74" s="19"/>
-      <c r="R74" s="217"/>
-      <c r="S74" s="221"/>
-      <c r="V74" s="207"/>
-      <c r="W74" s="210"/>
+      <c r="R74" s="195"/>
+      <c r="S74" s="199"/>
+      <c r="V74" s="205"/>
+      <c r="W74" s="208"/>
       <c r="Y74" s="13"/>
       <c r="AB74" s="139"/>
       <c r="AC74" s="34" t="str">
@@ -6105,13 +6105,13 @@
       <c r="Q75" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="R75" s="218"/>
-      <c r="S75" s="222"/>
-      <c r="V75" s="205" t="str">
+      <c r="R75" s="196"/>
+      <c r="S75" s="200"/>
+      <c r="V75" s="203" t="str">
         <f>IF(AB49="","",AB49)</f>
         <v/>
       </c>
-      <c r="W75" s="211" t="str">
+      <c r="W75" s="209" t="str">
         <f>IF(AB52="","",AB52)</f>
         <v/>
       </c>
@@ -6152,10 +6152,10 @@
       <c r="M76" s="11"/>
       <c r="O76" s="12"/>
       <c r="Q76" s="19"/>
-      <c r="R76" s="217"/>
-      <c r="S76" s="221"/>
-      <c r="V76" s="207"/>
-      <c r="W76" s="210"/>
+      <c r="R76" s="195"/>
+      <c r="S76" s="199"/>
+      <c r="V76" s="205"/>
+      <c r="W76" s="208"/>
       <c r="Y76" s="13"/>
       <c r="AB76" s="139"/>
       <c r="AC76" s="34" t="str">
@@ -6196,13 +6196,13 @@
       <c r="Q77" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="R77" s="218"/>
-      <c r="S77" s="222"/>
-      <c r="V77" s="205" t="str">
+      <c r="R77" s="196"/>
+      <c r="S77" s="200"/>
+      <c r="V77" s="203" t="str">
         <f>IF(AB50="","",AB50)</f>
         <v/>
       </c>
-      <c r="W77" s="211" t="str">
+      <c r="W77" s="209" t="str">
         <f>IF(AB53="","",AB53)</f>
         <v/>
       </c>
@@ -6218,10 +6218,10 @@
       <c r="M78" s="11"/>
       <c r="O78" s="12"/>
       <c r="Q78" s="19"/>
-      <c r="R78" s="219"/>
-      <c r="S78" s="223"/>
-      <c r="V78" s="206"/>
-      <c r="W78" s="212"/>
+      <c r="R78" s="197"/>
+      <c r="S78" s="201"/>
+      <c r="V78" s="204"/>
+      <c r="W78" s="210"/>
       <c r="Y78" s="13"/>
       <c r="AB78" s="139"/>
       <c r="AC78" s="34" t="str">
@@ -6408,16 +6408,16 @@
         <f>S68</f>
         <v>Right ()</v>
       </c>
-      <c r="I84" s="203" t="str">
+      <c r="I84" s="213" t="str">
         <f>R68</f>
         <v>Left ()</v>
       </c>
-      <c r="J84" s="203"/>
-      <c r="K84" s="203" t="str">
+      <c r="J84" s="213"/>
+      <c r="K84" s="213" t="str">
         <f>S68</f>
         <v>Right ()</v>
       </c>
-      <c r="L84" s="203"/>
+      <c r="L84" s="213"/>
       <c r="M84" s="11"/>
       <c r="O84" s="12"/>
       <c r="Y84" s="13"/>
@@ -6450,16 +6450,16 @@
       <c r="H85" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="I85" s="204" t="str">
+      <c r="I85" s="202" t="str">
         <f>IF(R73="","",R73)</f>
         <v/>
       </c>
-      <c r="J85" s="204"/>
-      <c r="K85" s="204" t="str">
+      <c r="J85" s="202"/>
+      <c r="K85" s="202" t="str">
         <f>IF(S73="","",S73)</f>
         <v/>
       </c>
-      <c r="L85" s="204"/>
+      <c r="L85" s="202"/>
       <c r="M85" s="11"/>
       <c r="O85" s="97" t="s">
         <v>105</v>
@@ -6488,26 +6488,26 @@
       <c r="H86" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="I86" s="204" t="str">
+      <c r="I86" s="202" t="str">
         <f>IF(R75="","",R75)</f>
         <v/>
       </c>
-      <c r="J86" s="204"/>
-      <c r="K86" s="204" t="str">
+      <c r="J86" s="202"/>
+      <c r="K86" s="202" t="str">
         <f>IF(S75="","",S75)</f>
         <v/>
       </c>
-      <c r="L86" s="204"/>
+      <c r="L86" s="202"/>
       <c r="M86" s="11"/>
       <c r="O86" s="12"/>
-      <c r="Q86" s="214" t="s">
+      <c r="Q86" s="192" t="s">
         <v>116</v>
       </c>
-      <c r="R86" s="215"/>
-      <c r="S86" s="214" t="s">
+      <c r="R86" s="193"/>
+      <c r="S86" s="192" t="s">
         <v>117</v>
       </c>
-      <c r="T86" s="215"/>
+      <c r="T86" s="193"/>
       <c r="V86" s="113" t="s">
         <v>43</v>
       </c>
@@ -6532,16 +6532,16 @@
       <c r="H87" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="I87" s="213" t="str">
+      <c r="I87" s="191" t="str">
         <f>IF(R77="","",R77)</f>
         <v/>
       </c>
-      <c r="J87" s="213"/>
-      <c r="K87" s="213" t="str">
+      <c r="J87" s="191"/>
+      <c r="K87" s="191" t="str">
         <f>IF(S77="","",S77)</f>
         <v/>
       </c>
-      <c r="L87" s="213"/>
+      <c r="L87" s="191"/>
       <c r="M87" s="11"/>
       <c r="O87" s="12"/>
       <c r="Q87" s="114" t="str">
@@ -8248,6 +8248,36 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="42">
+    <mergeCell ref="AG1:AJ1"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="AG9:AH9"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="I84:J84"/>
+    <mergeCell ref="K84:L84"/>
+    <mergeCell ref="I85:J85"/>
+    <mergeCell ref="K85:L85"/>
+    <mergeCell ref="V77:V78"/>
+    <mergeCell ref="V75:V76"/>
+    <mergeCell ref="V73:V74"/>
+    <mergeCell ref="W73:W74"/>
+    <mergeCell ref="W75:W76"/>
+    <mergeCell ref="W77:W78"/>
     <mergeCell ref="I87:J87"/>
     <mergeCell ref="K87:L87"/>
     <mergeCell ref="Q86:R86"/>
@@ -8260,36 +8290,6 @@
     <mergeCell ref="S77:S78"/>
     <mergeCell ref="I86:J86"/>
     <mergeCell ref="K86:L86"/>
-    <mergeCell ref="V77:V78"/>
-    <mergeCell ref="V75:V76"/>
-    <mergeCell ref="V73:V74"/>
-    <mergeCell ref="W73:W74"/>
-    <mergeCell ref="W75:W76"/>
-    <mergeCell ref="W77:W78"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="I84:J84"/>
-    <mergeCell ref="K84:L84"/>
-    <mergeCell ref="I85:J85"/>
-    <mergeCell ref="K85:L85"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="AG1:AJ1"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="AG9:AH9"/>
   </mergeCells>
   <conditionalFormatting sqref="D27:D28">
     <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
@@ -8503,19 +8503,19 @@
       <c r="D10" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="194" t="str">
+      <c r="E10" s="221" t="str">
         <f>Barco!E10</f>
         <v/>
       </c>
-      <c r="F10" s="194"/>
+      <c r="F10" s="221"/>
       <c r="I10" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="194" t="str">
+      <c r="J10" s="221" t="str">
         <f>Barco!J10</f>
         <v/>
       </c>
-      <c r="K10" s="194"/>
+      <c r="K10" s="221"/>
       <c r="L10" s="178"/>
     </row>
     <row r="11" spans="1:18">
@@ -8526,19 +8526,19 @@
       <c r="D11" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="194" t="str">
+      <c r="E11" s="221" t="str">
         <f>Barco!E11</f>
         <v/>
       </c>
-      <c r="F11" s="194"/>
+      <c r="F11" s="221"/>
       <c r="I11" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="194" t="str">
+      <c r="J11" s="221" t="str">
         <f>Barco!J11</f>
         <v/>
       </c>
-      <c r="K11" s="194"/>
+      <c r="K11" s="221"/>
       <c r="L11" s="178"/>
     </row>
     <row r="12" spans="1:18">
@@ -8549,19 +8549,19 @@
       <c r="D12" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="194" t="str">
+      <c r="E12" s="221" t="str">
         <f>Barco!E12</f>
         <v/>
       </c>
-      <c r="F12" s="194"/>
+      <c r="F12" s="221"/>
       <c r="I12" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="194" t="str">
+      <c r="J12" s="221" t="str">
         <f>Barco!J12</f>
         <v/>
       </c>
-      <c r="K12" s="194"/>
+      <c r="K12" s="221"/>
       <c r="L12" s="178"/>
     </row>
     <row r="13" spans="1:18">
@@ -8572,19 +8572,19 @@
       <c r="D13" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="194" t="str">
+      <c r="E13" s="221" t="str">
         <f>Barco!E13</f>
         <v/>
       </c>
-      <c r="F13" s="194"/>
+      <c r="F13" s="221"/>
       <c r="I13" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="194" t="str">
+      <c r="J13" s="221" t="str">
         <f>Barco!J14</f>
         <v/>
       </c>
-      <c r="K13" s="194"/>
+      <c r="K13" s="221"/>
       <c r="L13" s="178"/>
     </row>
     <row r="14" spans="1:18">
@@ -8595,19 +8595,19 @@
       <c r="D14" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="194" t="str">
+      <c r="E14" s="221" t="str">
         <f>Barco!E14</f>
         <v/>
       </c>
-      <c r="F14" s="194"/>
+      <c r="F14" s="221"/>
       <c r="I14" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="194" t="str">
+      <c r="J14" s="221" t="str">
         <f>Barco!J15</f>
         <v/>
       </c>
-      <c r="K14" s="194"/>
+      <c r="K14" s="221"/>
       <c r="L14" s="178"/>
     </row>
     <row r="15" spans="1:18">
@@ -8618,11 +8618,11 @@
       <c r="D15" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="194" t="str">
+      <c r="E15" s="221" t="str">
         <f>Barco!E15</f>
         <v>Barco K5905277 v18</v>
       </c>
-      <c r="F15" s="194"/>
+      <c r="F15" s="221"/>
       <c r="L15" s="178"/>
     </row>
     <row r="16" spans="1:18" ht="16.2" thickBot="1">
@@ -8676,14 +8676,14 @@
         <v>20</v>
       </c>
       <c r="B20" s="177"/>
-      <c r="F20" s="224" t="s">
+      <c r="F20" s="228" t="s">
         <v>192</v>
       </c>
-      <c r="G20" s="224"/>
-      <c r="H20" s="224" t="s">
+      <c r="G20" s="228"/>
+      <c r="H20" s="228" t="s">
         <v>193</v>
       </c>
-      <c r="I20" s="224"/>
+      <c r="I20" s="228"/>
       <c r="L20" s="178"/>
     </row>
     <row r="21" spans="1:12">
@@ -8691,16 +8691,16 @@
         <v>21</v>
       </c>
       <c r="B21" s="177"/>
-      <c r="F21" s="224" t="str">
+      <c r="F21" s="228" t="str">
         <f>J13</f>
         <v/>
       </c>
-      <c r="G21" s="224"/>
-      <c r="H21" s="224" t="str">
+      <c r="G21" s="228"/>
+      <c r="H21" s="228" t="str">
         <f>J14</f>
         <v/>
       </c>
-      <c r="I21" s="224"/>
+      <c r="I21" s="228"/>
       <c r="L21" s="178"/>
     </row>
     <row r="22" spans="1:12">
@@ -8711,13 +8711,13 @@
       <c r="E22" s="48" t="s">
         <v>185</v>
       </c>
-      <c r="F22" s="226" t="str">
+      <c r="F22" s="227" t="str">
         <f>IF(Barco!E23="","",IF(Barco!E23="YES","PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="G22" s="226"/>
-      <c r="H22" s="226"/>
-      <c r="I22" s="226"/>
+      <c r="G22" s="227"/>
+      <c r="H22" s="227"/>
+      <c r="I22" s="227"/>
       <c r="L22" s="178"/>
     </row>
     <row r="23" spans="1:12">
@@ -8728,13 +8728,13 @@
       <c r="E23" s="48" t="s">
         <v>186</v>
       </c>
-      <c r="F23" s="226" t="str">
+      <c r="F23" s="227" t="str">
         <f>IF(Barco!E22="","",IF(Barco!E22="YES","PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="G23" s="226"/>
-      <c r="H23" s="226"/>
-      <c r="I23" s="226"/>
+      <c r="G23" s="227"/>
+      <c r="H23" s="227"/>
+      <c r="I23" s="227"/>
       <c r="L23" s="178"/>
     </row>
     <row r="24" spans="1:12">
@@ -8745,13 +8745,13 @@
       <c r="E24" s="48" t="s">
         <v>187</v>
       </c>
-      <c r="F24" s="226" t="str">
+      <c r="F24" s="227" t="str">
         <f>IF(OR(Barco!I72="TBD",Barco!I73="TBD"),"",IF(AND(Barco!I72="YES",Barco!I73="YES"),"PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="G24" s="226"/>
-      <c r="H24" s="226"/>
-      <c r="I24" s="226"/>
+      <c r="G24" s="227"/>
+      <c r="H24" s="227"/>
+      <c r="I24" s="227"/>
       <c r="L24" s="178"/>
     </row>
     <row r="25" spans="1:12">
@@ -8762,10 +8762,10 @@
       <c r="E25" s="48" t="s">
         <v>188</v>
       </c>
-      <c r="F25" s="225"/>
-      <c r="G25" s="225"/>
-      <c r="H25" s="225"/>
-      <c r="I25" s="225"/>
+      <c r="F25" s="224"/>
+      <c r="G25" s="224"/>
+      <c r="H25" s="224"/>
+      <c r="I25" s="224"/>
       <c r="L25" s="178"/>
     </row>
     <row r="26" spans="1:12">
@@ -8779,13 +8779,13 @@
       <c r="E26" s="48" t="s">
         <v>189</v>
       </c>
-      <c r="F26" s="226" t="str">
+      <c r="F26" s="227" t="str">
         <f>IF(Barco!F85="","",IF(Barco!F85="YES","PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="G26" s="226"/>
-      <c r="H26" s="226"/>
-      <c r="I26" s="226"/>
+      <c r="G26" s="227"/>
+      <c r="H26" s="227"/>
+      <c r="I26" s="227"/>
       <c r="L26" s="178"/>
     </row>
     <row r="27" spans="1:12">
@@ -8796,10 +8796,10 @@
       <c r="E27" s="48" t="s">
         <v>190</v>
       </c>
-      <c r="F27" s="225"/>
-      <c r="G27" s="225"/>
-      <c r="H27" s="225"/>
-      <c r="I27" s="225"/>
+      <c r="F27" s="224"/>
+      <c r="G27" s="224"/>
+      <c r="H27" s="224"/>
+      <c r="I27" s="224"/>
       <c r="L27" s="178"/>
     </row>
     <row r="28" spans="1:12">
@@ -8810,10 +8810,10 @@
       <c r="E28" s="48" t="s">
         <v>191</v>
       </c>
-      <c r="F28" s="225"/>
-      <c r="G28" s="225"/>
-      <c r="H28" s="225"/>
-      <c r="I28" s="225"/>
+      <c r="F28" s="224"/>
+      <c r="G28" s="224"/>
+      <c r="H28" s="224"/>
+      <c r="I28" s="224"/>
       <c r="L28" s="178"/>
     </row>
     <row r="29" spans="1:12">
@@ -8824,16 +8824,16 @@
       <c r="E29" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="F29" s="227" t="str">
+      <c r="F29" s="225" t="str">
         <f>IF(Barco!F86="","",IF(Barco!F86="YES","PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="G29" s="228"/>
-      <c r="H29" s="227" t="str">
+      <c r="G29" s="226"/>
+      <c r="H29" s="225" t="str">
         <f>IF(Barco!G86="","",IF(Barco!G86="YES","PASS","FAIL"))</f>
         <v/>
       </c>
-      <c r="I29" s="228"/>
+      <c r="I29" s="226"/>
       <c r="L29" s="178"/>
     </row>
     <row r="30" spans="1:12">
@@ -9007,15 +9007,12 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="J12:K12"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="H27:I27"/>
     <mergeCell ref="E13:F13"/>
@@ -9032,12 +9029,15 @@
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="H23:I23"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F25:I25 F27:I28" xr:uid="{CEAD9B4F-4A05-4883-9435-EBBC3722EE42}">

</xml_diff>